<commit_message>
feat: fixed a typo in krauss black excel
</commit_message>
<xml_diff>
--- a/data/Krauss KRWD64.xlsx
+++ b/data/Krauss KRWD64.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="26327"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="27425"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{37E682A1-CBF7-46D4-9231-A6014CBDB990}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7673311F-F1E9-4F71-8BFB-3E77C8530550}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" tabRatio="982" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" tabRatio="982" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Krauss до 2400 белый" sheetId="8" r:id="rId1"/>
@@ -51,7 +51,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6509" uniqueCount="458">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6509" uniqueCount="457">
   <si>
     <t>наименование</t>
   </si>
@@ -1412,9 +1412,6 @@
     <t>белый</t>
   </si>
   <si>
-    <t>Krauss до 2400 чёрный</t>
-  </si>
-  <si>
     <t>без окраса</t>
   </si>
   <si>
@@ -2104,6 +2101,51 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="4" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="8" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -2126,51 +2168,6 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="4" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="8" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="25" xfId="1" applyBorder="1" applyAlignment="1">
@@ -9911,8 +9908,8 @@
       <xdr:rowOff>38100</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>9</xdr:col>
-      <xdr:colOff>190500</xdr:colOff>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>469900</xdr:colOff>
       <xdr:row>50</xdr:row>
       <xdr:rowOff>86277</xdr:rowOff>
     </xdr:to>
@@ -9972,8 +9969,8 @@
       <xdr:rowOff>104775</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>9</xdr:col>
-      <xdr:colOff>266700</xdr:colOff>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>546100</xdr:colOff>
       <xdr:row>79</xdr:row>
       <xdr:rowOff>91034</xdr:rowOff>
     </xdr:to>
@@ -10033,8 +10030,8 @@
       <xdr:rowOff>123825</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>9</xdr:col>
-      <xdr:colOff>371475</xdr:colOff>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>41275</xdr:colOff>
       <xdr:row>104</xdr:row>
       <xdr:rowOff>95250</xdr:rowOff>
     </xdr:to>
@@ -10094,8 +10091,8 @@
       <xdr:rowOff>47625</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>9</xdr:col>
-      <xdr:colOff>386521</xdr:colOff>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>56321</xdr:colOff>
       <xdr:row>132</xdr:row>
       <xdr:rowOff>57150</xdr:rowOff>
     </xdr:to>
@@ -10155,8 +10152,8 @@
       <xdr:rowOff>180975</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>8</xdr:col>
-      <xdr:colOff>533400</xdr:colOff>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>203200</xdr:colOff>
       <xdr:row>158</xdr:row>
       <xdr:rowOff>148958</xdr:rowOff>
     </xdr:to>
@@ -10216,8 +10213,8 @@
       <xdr:rowOff>47625</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>8</xdr:col>
-      <xdr:colOff>443550</xdr:colOff>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>113350</xdr:colOff>
       <xdr:row>188</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:to>
@@ -10277,10 +10274,10 @@
       <xdr:rowOff>57150</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>8</xdr:col>
-      <xdr:colOff>542925</xdr:colOff>
-      <xdr:row>218</xdr:row>
-      <xdr:rowOff>185000</xdr:rowOff>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>212725</xdr:colOff>
+      <xdr:row>219</xdr:row>
+      <xdr:rowOff>850</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -10338,8 +10335,8 @@
       <xdr:rowOff>85725</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>8</xdr:col>
-      <xdr:colOff>438150</xdr:colOff>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>107950</xdr:colOff>
       <xdr:row>246</xdr:row>
       <xdr:rowOff>57278</xdr:rowOff>
     </xdr:to>
@@ -10399,8 +10396,8 @@
       <xdr:rowOff>171450</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>8</xdr:col>
-      <xdr:colOff>533400</xdr:colOff>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>203200</xdr:colOff>
       <xdr:row>275</xdr:row>
       <xdr:rowOff>45532</xdr:rowOff>
     </xdr:to>
@@ -10460,8 +10457,8 @@
       <xdr:rowOff>76200</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>9</xdr:col>
-      <xdr:colOff>14654</xdr:colOff>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>294054</xdr:colOff>
       <xdr:row>303</xdr:row>
       <xdr:rowOff>85725</xdr:rowOff>
     </xdr:to>
@@ -10521,8 +10518,8 @@
       <xdr:rowOff>161925</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>8</xdr:col>
-      <xdr:colOff>581025</xdr:colOff>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>250825</xdr:colOff>
       <xdr:row>331</xdr:row>
       <xdr:rowOff>64796</xdr:rowOff>
     </xdr:to>
@@ -10582,8 +10579,8 @@
       <xdr:rowOff>76200</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>9</xdr:col>
-      <xdr:colOff>228600</xdr:colOff>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>508000</xdr:colOff>
       <xdr:row>359</xdr:row>
       <xdr:rowOff>171762</xdr:rowOff>
     </xdr:to>
@@ -16225,9 +16222,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2007 - 2010">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2007 - 2010">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -16265,9 +16262,9 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2007 - 2010">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -16300,26 +16297,9 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -16352,26 +16332,9 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2007 - 2010">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -16547,16 +16510,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A5:E367"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView topLeftCell="A35" zoomScale="65" workbookViewId="0">
       <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="14.5"/>
   <cols>
-    <col min="1" max="1" width="26.21875" customWidth="1"/>
-    <col min="2" max="2" width="67.44140625" customWidth="1"/>
-    <col min="3" max="3" width="22.77734375" customWidth="1"/>
-    <col min="4" max="4" width="11.5546875" customWidth="1"/>
+    <col min="1" max="1" width="26.1796875" customWidth="1"/>
+    <col min="2" max="2" width="67.453125" customWidth="1"/>
+    <col min="3" max="3" width="22.81640625" customWidth="1"/>
+    <col min="4" max="4" width="11.54296875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="5" spans="1:5">
@@ -20117,11 +20080,11 @@
       <selection activeCell="I8" sqref="I8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="14.5"/>
   <cols>
     <col min="1" max="1" width="27" customWidth="1"/>
-    <col min="2" max="2" width="68.88671875" customWidth="1"/>
-    <col min="3" max="3" width="20.6640625" customWidth="1"/>
+    <col min="2" max="2" width="68.90625" customWidth="1"/>
+    <col min="3" max="3" width="20.6328125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="5" spans="1:6">
@@ -20137,10 +20100,10 @@
         <v>421</v>
       </c>
       <c r="E6" t="s">
+        <v>454</v>
+      </c>
+      <c r="F6" t="s">
         <v>455</v>
-      </c>
-      <c r="F6" t="s">
-        <v>456</v>
       </c>
     </row>
     <row r="7" spans="1:6">
@@ -23778,11 +23741,11 @@
       <selection activeCell="H9" sqref="H9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="14.5"/>
   <cols>
-    <col min="1" max="1" width="32.44140625" customWidth="1"/>
-    <col min="2" max="2" width="69.44140625" customWidth="1"/>
-    <col min="3" max="3" width="22.109375" customWidth="1"/>
+    <col min="1" max="1" width="32.453125" customWidth="1"/>
+    <col min="2" max="2" width="69.453125" customWidth="1"/>
+    <col min="3" max="3" width="22.08984375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="5" spans="1:6">
@@ -23801,7 +23764,7 @@
         <v>151</v>
       </c>
       <c r="F6" t="s">
-        <v>456</v>
+        <v>455</v>
       </c>
     </row>
     <row r="7" spans="1:6">
@@ -27439,12 +27402,12 @@
       <selection activeCell="H5" sqref="H5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="14.5"/>
   <cols>
-    <col min="1" max="1" width="31.44140625" customWidth="1"/>
-    <col min="2" max="2" width="68.44140625" customWidth="1"/>
-    <col min="3" max="3" width="23.109375" customWidth="1"/>
-    <col min="5" max="5" width="11.21875" customWidth="1"/>
+    <col min="1" max="1" width="31.453125" customWidth="1"/>
+    <col min="2" max="2" width="68.453125" customWidth="1"/>
+    <col min="3" max="3" width="23.08984375" customWidth="1"/>
+    <col min="5" max="5" width="11.1796875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="5" spans="1:6">
@@ -27460,10 +27423,10 @@
         <v>13</v>
       </c>
       <c r="E6" t="s">
-        <v>454</v>
+        <v>453</v>
       </c>
       <c r="F6" t="s">
-        <v>457</v>
+        <v>456</v>
       </c>
     </row>
     <row r="7" spans="1:6">
@@ -31244,13 +31207,13 @@
       <selection activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="14.5"/>
   <cols>
-    <col min="1" max="1" width="26.21875" customWidth="1"/>
-    <col min="2" max="2" width="67.44140625" customWidth="1"/>
-    <col min="3" max="3" width="22.77734375" customWidth="1"/>
-    <col min="4" max="4" width="11.5546875" customWidth="1"/>
-    <col min="5" max="5" width="10.44140625" customWidth="1"/>
+    <col min="1" max="1" width="26.1796875" customWidth="1"/>
+    <col min="2" max="2" width="67.453125" customWidth="1"/>
+    <col min="3" max="3" width="22.81640625" customWidth="1"/>
+    <col min="4" max="4" width="11.54296875" customWidth="1"/>
+    <col min="5" max="5" width="10.453125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="5" spans="1:6">
@@ -31268,10 +31231,10 @@
       <c r="C6" s="92"/>
       <c r="D6" s="92"/>
       <c r="E6" t="s">
-        <v>454</v>
+        <v>453</v>
       </c>
       <c r="F6" t="s">
-        <v>456</v>
+        <v>455</v>
       </c>
     </row>
     <row r="7" spans="1:6">
@@ -34958,11 +34921,11 @@
       <selection activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="14.5"/>
   <cols>
     <col min="1" max="1" width="32" customWidth="1"/>
-    <col min="2" max="2" width="68.88671875" customWidth="1"/>
-    <col min="3" max="3" width="20.6640625" customWidth="1"/>
+    <col min="2" max="2" width="68.90625" customWidth="1"/>
+    <col min="3" max="3" width="20.6328125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="5" spans="1:6">
@@ -34978,10 +34941,10 @@
         <v>421</v>
       </c>
       <c r="E6" t="s">
+        <v>454</v>
+      </c>
+      <c r="F6" t="s">
         <v>455</v>
-      </c>
-      <c r="F6" t="s">
-        <v>456</v>
       </c>
     </row>
     <row r="7" spans="1:6">
@@ -38619,11 +38582,11 @@
       <selection activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="14.5"/>
   <cols>
-    <col min="1" max="1" width="30.5546875" customWidth="1"/>
-    <col min="2" max="2" width="69.44140625" customWidth="1"/>
-    <col min="3" max="3" width="22.109375" customWidth="1"/>
+    <col min="1" max="1" width="30.54296875" customWidth="1"/>
+    <col min="2" max="2" width="69.453125" customWidth="1"/>
+    <col min="3" max="3" width="22.08984375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="5" spans="1:6">
@@ -38642,7 +38605,7 @@
         <v>151</v>
       </c>
       <c r="F6" t="s">
-        <v>456</v>
+        <v>455</v>
       </c>
     </row>
     <row r="7" spans="1:6">
@@ -42280,11 +42243,11 @@
       <selection activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="14.5"/>
   <cols>
-    <col min="1" max="1" width="33.33203125" customWidth="1"/>
-    <col min="2" max="2" width="68.44140625" customWidth="1"/>
-    <col min="3" max="3" width="23.109375" customWidth="1"/>
+    <col min="1" max="1" width="33.36328125" customWidth="1"/>
+    <col min="2" max="2" width="68.453125" customWidth="1"/>
+    <col min="3" max="3" width="23.08984375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="5" spans="1:6">
@@ -42300,10 +42263,10 @@
         <v>13</v>
       </c>
       <c r="E6" t="s">
-        <v>454</v>
+        <v>453</v>
       </c>
       <c r="F6" t="s">
-        <v>456</v>
+        <v>455</v>
       </c>
     </row>
     <row r="7" spans="1:6">
@@ -46091,425 +46054,425 @@
       <selection pane="topRight" activeCell="B8" sqref="B8:B22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.109375" defaultRowHeight="13.8"/>
+  <sheetFormatPr defaultColWidth="14.08984375" defaultRowHeight="14"/>
   <cols>
-    <col min="1" max="1" width="24.44140625" style="2" customWidth="1"/>
+    <col min="1" max="1" width="24.453125" style="2" customWidth="1"/>
     <col min="2" max="2" width="36" style="2" customWidth="1"/>
-    <col min="3" max="3" width="23.6640625" style="2" customWidth="1"/>
+    <col min="3" max="3" width="23.6328125" style="2" customWidth="1"/>
     <col min="4" max="4" width="16" style="2" customWidth="1"/>
-    <col min="5" max="5" width="83.88671875" style="2" customWidth="1"/>
-    <col min="6" max="256" width="14.109375" style="2"/>
-    <col min="257" max="257" width="24.44140625" style="2" customWidth="1"/>
+    <col min="5" max="5" width="83.90625" style="2" customWidth="1"/>
+    <col min="6" max="256" width="14.08984375" style="2"/>
+    <col min="257" max="257" width="24.453125" style="2" customWidth="1"/>
     <col min="258" max="258" width="36" style="2" customWidth="1"/>
-    <col min="259" max="259" width="23.6640625" style="2" customWidth="1"/>
+    <col min="259" max="259" width="23.6328125" style="2" customWidth="1"/>
     <col min="260" max="260" width="16" style="2" customWidth="1"/>
-    <col min="261" max="261" width="83.88671875" style="2" customWidth="1"/>
-    <col min="262" max="512" width="14.109375" style="2"/>
-    <col min="513" max="513" width="24.44140625" style="2" customWidth="1"/>
+    <col min="261" max="261" width="83.90625" style="2" customWidth="1"/>
+    <col min="262" max="512" width="14.08984375" style="2"/>
+    <col min="513" max="513" width="24.453125" style="2" customWidth="1"/>
     <col min="514" max="514" width="36" style="2" customWidth="1"/>
-    <col min="515" max="515" width="23.6640625" style="2" customWidth="1"/>
+    <col min="515" max="515" width="23.6328125" style="2" customWidth="1"/>
     <col min="516" max="516" width="16" style="2" customWidth="1"/>
-    <col min="517" max="517" width="83.88671875" style="2" customWidth="1"/>
-    <col min="518" max="768" width="14.109375" style="2"/>
-    <col min="769" max="769" width="24.44140625" style="2" customWidth="1"/>
+    <col min="517" max="517" width="83.90625" style="2" customWidth="1"/>
+    <col min="518" max="768" width="14.08984375" style="2"/>
+    <col min="769" max="769" width="24.453125" style="2" customWidth="1"/>
     <col min="770" max="770" width="36" style="2" customWidth="1"/>
-    <col min="771" max="771" width="23.6640625" style="2" customWidth="1"/>
+    <col min="771" max="771" width="23.6328125" style="2" customWidth="1"/>
     <col min="772" max="772" width="16" style="2" customWidth="1"/>
-    <col min="773" max="773" width="83.88671875" style="2" customWidth="1"/>
-    <col min="774" max="1024" width="14.109375" style="2"/>
-    <col min="1025" max="1025" width="24.44140625" style="2" customWidth="1"/>
+    <col min="773" max="773" width="83.90625" style="2" customWidth="1"/>
+    <col min="774" max="1024" width="14.08984375" style="2"/>
+    <col min="1025" max="1025" width="24.453125" style="2" customWidth="1"/>
     <col min="1026" max="1026" width="36" style="2" customWidth="1"/>
-    <col min="1027" max="1027" width="23.6640625" style="2" customWidth="1"/>
+    <col min="1027" max="1027" width="23.6328125" style="2" customWidth="1"/>
     <col min="1028" max="1028" width="16" style="2" customWidth="1"/>
-    <col min="1029" max="1029" width="83.88671875" style="2" customWidth="1"/>
-    <col min="1030" max="1280" width="14.109375" style="2"/>
-    <col min="1281" max="1281" width="24.44140625" style="2" customWidth="1"/>
+    <col min="1029" max="1029" width="83.90625" style="2" customWidth="1"/>
+    <col min="1030" max="1280" width="14.08984375" style="2"/>
+    <col min="1281" max="1281" width="24.453125" style="2" customWidth="1"/>
     <col min="1282" max="1282" width="36" style="2" customWidth="1"/>
-    <col min="1283" max="1283" width="23.6640625" style="2" customWidth="1"/>
+    <col min="1283" max="1283" width="23.6328125" style="2" customWidth="1"/>
     <col min="1284" max="1284" width="16" style="2" customWidth="1"/>
-    <col min="1285" max="1285" width="83.88671875" style="2" customWidth="1"/>
-    <col min="1286" max="1536" width="14.109375" style="2"/>
-    <col min="1537" max="1537" width="24.44140625" style="2" customWidth="1"/>
+    <col min="1285" max="1285" width="83.90625" style="2" customWidth="1"/>
+    <col min="1286" max="1536" width="14.08984375" style="2"/>
+    <col min="1537" max="1537" width="24.453125" style="2" customWidth="1"/>
     <col min="1538" max="1538" width="36" style="2" customWidth="1"/>
-    <col min="1539" max="1539" width="23.6640625" style="2" customWidth="1"/>
+    <col min="1539" max="1539" width="23.6328125" style="2" customWidth="1"/>
     <col min="1540" max="1540" width="16" style="2" customWidth="1"/>
-    <col min="1541" max="1541" width="83.88671875" style="2" customWidth="1"/>
-    <col min="1542" max="1792" width="14.109375" style="2"/>
-    <col min="1793" max="1793" width="24.44140625" style="2" customWidth="1"/>
+    <col min="1541" max="1541" width="83.90625" style="2" customWidth="1"/>
+    <col min="1542" max="1792" width="14.08984375" style="2"/>
+    <col min="1793" max="1793" width="24.453125" style="2" customWidth="1"/>
     <col min="1794" max="1794" width="36" style="2" customWidth="1"/>
-    <col min="1795" max="1795" width="23.6640625" style="2" customWidth="1"/>
+    <col min="1795" max="1795" width="23.6328125" style="2" customWidth="1"/>
     <col min="1796" max="1796" width="16" style="2" customWidth="1"/>
-    <col min="1797" max="1797" width="83.88671875" style="2" customWidth="1"/>
-    <col min="1798" max="2048" width="14.109375" style="2"/>
-    <col min="2049" max="2049" width="24.44140625" style="2" customWidth="1"/>
+    <col min="1797" max="1797" width="83.90625" style="2" customWidth="1"/>
+    <col min="1798" max="2048" width="14.08984375" style="2"/>
+    <col min="2049" max="2049" width="24.453125" style="2" customWidth="1"/>
     <col min="2050" max="2050" width="36" style="2" customWidth="1"/>
-    <col min="2051" max="2051" width="23.6640625" style="2" customWidth="1"/>
+    <col min="2051" max="2051" width="23.6328125" style="2" customWidth="1"/>
     <col min="2052" max="2052" width="16" style="2" customWidth="1"/>
-    <col min="2053" max="2053" width="83.88671875" style="2" customWidth="1"/>
-    <col min="2054" max="2304" width="14.109375" style="2"/>
-    <col min="2305" max="2305" width="24.44140625" style="2" customWidth="1"/>
+    <col min="2053" max="2053" width="83.90625" style="2" customWidth="1"/>
+    <col min="2054" max="2304" width="14.08984375" style="2"/>
+    <col min="2305" max="2305" width="24.453125" style="2" customWidth="1"/>
     <col min="2306" max="2306" width="36" style="2" customWidth="1"/>
-    <col min="2307" max="2307" width="23.6640625" style="2" customWidth="1"/>
+    <col min="2307" max="2307" width="23.6328125" style="2" customWidth="1"/>
     <col min="2308" max="2308" width="16" style="2" customWidth="1"/>
-    <col min="2309" max="2309" width="83.88671875" style="2" customWidth="1"/>
-    <col min="2310" max="2560" width="14.109375" style="2"/>
-    <col min="2561" max="2561" width="24.44140625" style="2" customWidth="1"/>
+    <col min="2309" max="2309" width="83.90625" style="2" customWidth="1"/>
+    <col min="2310" max="2560" width="14.08984375" style="2"/>
+    <col min="2561" max="2561" width="24.453125" style="2" customWidth="1"/>
     <col min="2562" max="2562" width="36" style="2" customWidth="1"/>
-    <col min="2563" max="2563" width="23.6640625" style="2" customWidth="1"/>
+    <col min="2563" max="2563" width="23.6328125" style="2" customWidth="1"/>
     <col min="2564" max="2564" width="16" style="2" customWidth="1"/>
-    <col min="2565" max="2565" width="83.88671875" style="2" customWidth="1"/>
-    <col min="2566" max="2816" width="14.109375" style="2"/>
-    <col min="2817" max="2817" width="24.44140625" style="2" customWidth="1"/>
+    <col min="2565" max="2565" width="83.90625" style="2" customWidth="1"/>
+    <col min="2566" max="2816" width="14.08984375" style="2"/>
+    <col min="2817" max="2817" width="24.453125" style="2" customWidth="1"/>
     <col min="2818" max="2818" width="36" style="2" customWidth="1"/>
-    <col min="2819" max="2819" width="23.6640625" style="2" customWidth="1"/>
+    <col min="2819" max="2819" width="23.6328125" style="2" customWidth="1"/>
     <col min="2820" max="2820" width="16" style="2" customWidth="1"/>
-    <col min="2821" max="2821" width="83.88671875" style="2" customWidth="1"/>
-    <col min="2822" max="3072" width="14.109375" style="2"/>
-    <col min="3073" max="3073" width="24.44140625" style="2" customWidth="1"/>
+    <col min="2821" max="2821" width="83.90625" style="2" customWidth="1"/>
+    <col min="2822" max="3072" width="14.08984375" style="2"/>
+    <col min="3073" max="3073" width="24.453125" style="2" customWidth="1"/>
     <col min="3074" max="3074" width="36" style="2" customWidth="1"/>
-    <col min="3075" max="3075" width="23.6640625" style="2" customWidth="1"/>
+    <col min="3075" max="3075" width="23.6328125" style="2" customWidth="1"/>
     <col min="3076" max="3076" width="16" style="2" customWidth="1"/>
-    <col min="3077" max="3077" width="83.88671875" style="2" customWidth="1"/>
-    <col min="3078" max="3328" width="14.109375" style="2"/>
-    <col min="3329" max="3329" width="24.44140625" style="2" customWidth="1"/>
+    <col min="3077" max="3077" width="83.90625" style="2" customWidth="1"/>
+    <col min="3078" max="3328" width="14.08984375" style="2"/>
+    <col min="3329" max="3329" width="24.453125" style="2" customWidth="1"/>
     <col min="3330" max="3330" width="36" style="2" customWidth="1"/>
-    <col min="3331" max="3331" width="23.6640625" style="2" customWidth="1"/>
+    <col min="3331" max="3331" width="23.6328125" style="2" customWidth="1"/>
     <col min="3332" max="3332" width="16" style="2" customWidth="1"/>
-    <col min="3333" max="3333" width="83.88671875" style="2" customWidth="1"/>
-    <col min="3334" max="3584" width="14.109375" style="2"/>
-    <col min="3585" max="3585" width="24.44140625" style="2" customWidth="1"/>
+    <col min="3333" max="3333" width="83.90625" style="2" customWidth="1"/>
+    <col min="3334" max="3584" width="14.08984375" style="2"/>
+    <col min="3585" max="3585" width="24.453125" style="2" customWidth="1"/>
     <col min="3586" max="3586" width="36" style="2" customWidth="1"/>
-    <col min="3587" max="3587" width="23.6640625" style="2" customWidth="1"/>
+    <col min="3587" max="3587" width="23.6328125" style="2" customWidth="1"/>
     <col min="3588" max="3588" width="16" style="2" customWidth="1"/>
-    <col min="3589" max="3589" width="83.88671875" style="2" customWidth="1"/>
-    <col min="3590" max="3840" width="14.109375" style="2"/>
-    <col min="3841" max="3841" width="24.44140625" style="2" customWidth="1"/>
+    <col min="3589" max="3589" width="83.90625" style="2" customWidth="1"/>
+    <col min="3590" max="3840" width="14.08984375" style="2"/>
+    <col min="3841" max="3841" width="24.453125" style="2" customWidth="1"/>
     <col min="3842" max="3842" width="36" style="2" customWidth="1"/>
-    <col min="3843" max="3843" width="23.6640625" style="2" customWidth="1"/>
+    <col min="3843" max="3843" width="23.6328125" style="2" customWidth="1"/>
     <col min="3844" max="3844" width="16" style="2" customWidth="1"/>
-    <col min="3845" max="3845" width="83.88671875" style="2" customWidth="1"/>
-    <col min="3846" max="4096" width="14.109375" style="2"/>
-    <col min="4097" max="4097" width="24.44140625" style="2" customWidth="1"/>
+    <col min="3845" max="3845" width="83.90625" style="2" customWidth="1"/>
+    <col min="3846" max="4096" width="14.08984375" style="2"/>
+    <col min="4097" max="4097" width="24.453125" style="2" customWidth="1"/>
     <col min="4098" max="4098" width="36" style="2" customWidth="1"/>
-    <col min="4099" max="4099" width="23.6640625" style="2" customWidth="1"/>
+    <col min="4099" max="4099" width="23.6328125" style="2" customWidth="1"/>
     <col min="4100" max="4100" width="16" style="2" customWidth="1"/>
-    <col min="4101" max="4101" width="83.88671875" style="2" customWidth="1"/>
-    <col min="4102" max="4352" width="14.109375" style="2"/>
-    <col min="4353" max="4353" width="24.44140625" style="2" customWidth="1"/>
+    <col min="4101" max="4101" width="83.90625" style="2" customWidth="1"/>
+    <col min="4102" max="4352" width="14.08984375" style="2"/>
+    <col min="4353" max="4353" width="24.453125" style="2" customWidth="1"/>
     <col min="4354" max="4354" width="36" style="2" customWidth="1"/>
-    <col min="4355" max="4355" width="23.6640625" style="2" customWidth="1"/>
+    <col min="4355" max="4355" width="23.6328125" style="2" customWidth="1"/>
     <col min="4356" max="4356" width="16" style="2" customWidth="1"/>
-    <col min="4357" max="4357" width="83.88671875" style="2" customWidth="1"/>
-    <col min="4358" max="4608" width="14.109375" style="2"/>
-    <col min="4609" max="4609" width="24.44140625" style="2" customWidth="1"/>
+    <col min="4357" max="4357" width="83.90625" style="2" customWidth="1"/>
+    <col min="4358" max="4608" width="14.08984375" style="2"/>
+    <col min="4609" max="4609" width="24.453125" style="2" customWidth="1"/>
     <col min="4610" max="4610" width="36" style="2" customWidth="1"/>
-    <col min="4611" max="4611" width="23.6640625" style="2" customWidth="1"/>
+    <col min="4611" max="4611" width="23.6328125" style="2" customWidth="1"/>
     <col min="4612" max="4612" width="16" style="2" customWidth="1"/>
-    <col min="4613" max="4613" width="83.88671875" style="2" customWidth="1"/>
-    <col min="4614" max="4864" width="14.109375" style="2"/>
-    <col min="4865" max="4865" width="24.44140625" style="2" customWidth="1"/>
+    <col min="4613" max="4613" width="83.90625" style="2" customWidth="1"/>
+    <col min="4614" max="4864" width="14.08984375" style="2"/>
+    <col min="4865" max="4865" width="24.453125" style="2" customWidth="1"/>
     <col min="4866" max="4866" width="36" style="2" customWidth="1"/>
-    <col min="4867" max="4867" width="23.6640625" style="2" customWidth="1"/>
+    <col min="4867" max="4867" width="23.6328125" style="2" customWidth="1"/>
     <col min="4868" max="4868" width="16" style="2" customWidth="1"/>
-    <col min="4869" max="4869" width="83.88671875" style="2" customWidth="1"/>
-    <col min="4870" max="5120" width="14.109375" style="2"/>
-    <col min="5121" max="5121" width="24.44140625" style="2" customWidth="1"/>
+    <col min="4869" max="4869" width="83.90625" style="2" customWidth="1"/>
+    <col min="4870" max="5120" width="14.08984375" style="2"/>
+    <col min="5121" max="5121" width="24.453125" style="2" customWidth="1"/>
     <col min="5122" max="5122" width="36" style="2" customWidth="1"/>
-    <col min="5123" max="5123" width="23.6640625" style="2" customWidth="1"/>
+    <col min="5123" max="5123" width="23.6328125" style="2" customWidth="1"/>
     <col min="5124" max="5124" width="16" style="2" customWidth="1"/>
-    <col min="5125" max="5125" width="83.88671875" style="2" customWidth="1"/>
-    <col min="5126" max="5376" width="14.109375" style="2"/>
-    <col min="5377" max="5377" width="24.44140625" style="2" customWidth="1"/>
+    <col min="5125" max="5125" width="83.90625" style="2" customWidth="1"/>
+    <col min="5126" max="5376" width="14.08984375" style="2"/>
+    <col min="5377" max="5377" width="24.453125" style="2" customWidth="1"/>
     <col min="5378" max="5378" width="36" style="2" customWidth="1"/>
-    <col min="5379" max="5379" width="23.6640625" style="2" customWidth="1"/>
+    <col min="5379" max="5379" width="23.6328125" style="2" customWidth="1"/>
     <col min="5380" max="5380" width="16" style="2" customWidth="1"/>
-    <col min="5381" max="5381" width="83.88671875" style="2" customWidth="1"/>
-    <col min="5382" max="5632" width="14.109375" style="2"/>
-    <col min="5633" max="5633" width="24.44140625" style="2" customWidth="1"/>
+    <col min="5381" max="5381" width="83.90625" style="2" customWidth="1"/>
+    <col min="5382" max="5632" width="14.08984375" style="2"/>
+    <col min="5633" max="5633" width="24.453125" style="2" customWidth="1"/>
     <col min="5634" max="5634" width="36" style="2" customWidth="1"/>
-    <col min="5635" max="5635" width="23.6640625" style="2" customWidth="1"/>
+    <col min="5635" max="5635" width="23.6328125" style="2" customWidth="1"/>
     <col min="5636" max="5636" width="16" style="2" customWidth="1"/>
-    <col min="5637" max="5637" width="83.88671875" style="2" customWidth="1"/>
-    <col min="5638" max="5888" width="14.109375" style="2"/>
-    <col min="5889" max="5889" width="24.44140625" style="2" customWidth="1"/>
+    <col min="5637" max="5637" width="83.90625" style="2" customWidth="1"/>
+    <col min="5638" max="5888" width="14.08984375" style="2"/>
+    <col min="5889" max="5889" width="24.453125" style="2" customWidth="1"/>
     <col min="5890" max="5890" width="36" style="2" customWidth="1"/>
-    <col min="5891" max="5891" width="23.6640625" style="2" customWidth="1"/>
+    <col min="5891" max="5891" width="23.6328125" style="2" customWidth="1"/>
     <col min="5892" max="5892" width="16" style="2" customWidth="1"/>
-    <col min="5893" max="5893" width="83.88671875" style="2" customWidth="1"/>
-    <col min="5894" max="6144" width="14.109375" style="2"/>
-    <col min="6145" max="6145" width="24.44140625" style="2" customWidth="1"/>
+    <col min="5893" max="5893" width="83.90625" style="2" customWidth="1"/>
+    <col min="5894" max="6144" width="14.08984375" style="2"/>
+    <col min="6145" max="6145" width="24.453125" style="2" customWidth="1"/>
     <col min="6146" max="6146" width="36" style="2" customWidth="1"/>
-    <col min="6147" max="6147" width="23.6640625" style="2" customWidth="1"/>
+    <col min="6147" max="6147" width="23.6328125" style="2" customWidth="1"/>
     <col min="6148" max="6148" width="16" style="2" customWidth="1"/>
-    <col min="6149" max="6149" width="83.88671875" style="2" customWidth="1"/>
-    <col min="6150" max="6400" width="14.109375" style="2"/>
-    <col min="6401" max="6401" width="24.44140625" style="2" customWidth="1"/>
+    <col min="6149" max="6149" width="83.90625" style="2" customWidth="1"/>
+    <col min="6150" max="6400" width="14.08984375" style="2"/>
+    <col min="6401" max="6401" width="24.453125" style="2" customWidth="1"/>
     <col min="6402" max="6402" width="36" style="2" customWidth="1"/>
-    <col min="6403" max="6403" width="23.6640625" style="2" customWidth="1"/>
+    <col min="6403" max="6403" width="23.6328125" style="2" customWidth="1"/>
     <col min="6404" max="6404" width="16" style="2" customWidth="1"/>
-    <col min="6405" max="6405" width="83.88671875" style="2" customWidth="1"/>
-    <col min="6406" max="6656" width="14.109375" style="2"/>
-    <col min="6657" max="6657" width="24.44140625" style="2" customWidth="1"/>
+    <col min="6405" max="6405" width="83.90625" style="2" customWidth="1"/>
+    <col min="6406" max="6656" width="14.08984375" style="2"/>
+    <col min="6657" max="6657" width="24.453125" style="2" customWidth="1"/>
     <col min="6658" max="6658" width="36" style="2" customWidth="1"/>
-    <col min="6659" max="6659" width="23.6640625" style="2" customWidth="1"/>
+    <col min="6659" max="6659" width="23.6328125" style="2" customWidth="1"/>
     <col min="6660" max="6660" width="16" style="2" customWidth="1"/>
-    <col min="6661" max="6661" width="83.88671875" style="2" customWidth="1"/>
-    <col min="6662" max="6912" width="14.109375" style="2"/>
-    <col min="6913" max="6913" width="24.44140625" style="2" customWidth="1"/>
+    <col min="6661" max="6661" width="83.90625" style="2" customWidth="1"/>
+    <col min="6662" max="6912" width="14.08984375" style="2"/>
+    <col min="6913" max="6913" width="24.453125" style="2" customWidth="1"/>
     <col min="6914" max="6914" width="36" style="2" customWidth="1"/>
-    <col min="6915" max="6915" width="23.6640625" style="2" customWidth="1"/>
+    <col min="6915" max="6915" width="23.6328125" style="2" customWidth="1"/>
     <col min="6916" max="6916" width="16" style="2" customWidth="1"/>
-    <col min="6917" max="6917" width="83.88671875" style="2" customWidth="1"/>
-    <col min="6918" max="7168" width="14.109375" style="2"/>
-    <col min="7169" max="7169" width="24.44140625" style="2" customWidth="1"/>
+    <col min="6917" max="6917" width="83.90625" style="2" customWidth="1"/>
+    <col min="6918" max="7168" width="14.08984375" style="2"/>
+    <col min="7169" max="7169" width="24.453125" style="2" customWidth="1"/>
     <col min="7170" max="7170" width="36" style="2" customWidth="1"/>
-    <col min="7171" max="7171" width="23.6640625" style="2" customWidth="1"/>
+    <col min="7171" max="7171" width="23.6328125" style="2" customWidth="1"/>
     <col min="7172" max="7172" width="16" style="2" customWidth="1"/>
-    <col min="7173" max="7173" width="83.88671875" style="2" customWidth="1"/>
-    <col min="7174" max="7424" width="14.109375" style="2"/>
-    <col min="7425" max="7425" width="24.44140625" style="2" customWidth="1"/>
+    <col min="7173" max="7173" width="83.90625" style="2" customWidth="1"/>
+    <col min="7174" max="7424" width="14.08984375" style="2"/>
+    <col min="7425" max="7425" width="24.453125" style="2" customWidth="1"/>
     <col min="7426" max="7426" width="36" style="2" customWidth="1"/>
-    <col min="7427" max="7427" width="23.6640625" style="2" customWidth="1"/>
+    <col min="7427" max="7427" width="23.6328125" style="2" customWidth="1"/>
     <col min="7428" max="7428" width="16" style="2" customWidth="1"/>
-    <col min="7429" max="7429" width="83.88671875" style="2" customWidth="1"/>
-    <col min="7430" max="7680" width="14.109375" style="2"/>
-    <col min="7681" max="7681" width="24.44140625" style="2" customWidth="1"/>
+    <col min="7429" max="7429" width="83.90625" style="2" customWidth="1"/>
+    <col min="7430" max="7680" width="14.08984375" style="2"/>
+    <col min="7681" max="7681" width="24.453125" style="2" customWidth="1"/>
     <col min="7682" max="7682" width="36" style="2" customWidth="1"/>
-    <col min="7683" max="7683" width="23.6640625" style="2" customWidth="1"/>
+    <col min="7683" max="7683" width="23.6328125" style="2" customWidth="1"/>
     <col min="7684" max="7684" width="16" style="2" customWidth="1"/>
-    <col min="7685" max="7685" width="83.88671875" style="2" customWidth="1"/>
-    <col min="7686" max="7936" width="14.109375" style="2"/>
-    <col min="7937" max="7937" width="24.44140625" style="2" customWidth="1"/>
+    <col min="7685" max="7685" width="83.90625" style="2" customWidth="1"/>
+    <col min="7686" max="7936" width="14.08984375" style="2"/>
+    <col min="7937" max="7937" width="24.453125" style="2" customWidth="1"/>
     <col min="7938" max="7938" width="36" style="2" customWidth="1"/>
-    <col min="7939" max="7939" width="23.6640625" style="2" customWidth="1"/>
+    <col min="7939" max="7939" width="23.6328125" style="2" customWidth="1"/>
     <col min="7940" max="7940" width="16" style="2" customWidth="1"/>
-    <col min="7941" max="7941" width="83.88671875" style="2" customWidth="1"/>
-    <col min="7942" max="8192" width="14.109375" style="2"/>
-    <col min="8193" max="8193" width="24.44140625" style="2" customWidth="1"/>
+    <col min="7941" max="7941" width="83.90625" style="2" customWidth="1"/>
+    <col min="7942" max="8192" width="14.08984375" style="2"/>
+    <col min="8193" max="8193" width="24.453125" style="2" customWidth="1"/>
     <col min="8194" max="8194" width="36" style="2" customWidth="1"/>
-    <col min="8195" max="8195" width="23.6640625" style="2" customWidth="1"/>
+    <col min="8195" max="8195" width="23.6328125" style="2" customWidth="1"/>
     <col min="8196" max="8196" width="16" style="2" customWidth="1"/>
-    <col min="8197" max="8197" width="83.88671875" style="2" customWidth="1"/>
-    <col min="8198" max="8448" width="14.109375" style="2"/>
-    <col min="8449" max="8449" width="24.44140625" style="2" customWidth="1"/>
+    <col min="8197" max="8197" width="83.90625" style="2" customWidth="1"/>
+    <col min="8198" max="8448" width="14.08984375" style="2"/>
+    <col min="8449" max="8449" width="24.453125" style="2" customWidth="1"/>
     <col min="8450" max="8450" width="36" style="2" customWidth="1"/>
-    <col min="8451" max="8451" width="23.6640625" style="2" customWidth="1"/>
+    <col min="8451" max="8451" width="23.6328125" style="2" customWidth="1"/>
     <col min="8452" max="8452" width="16" style="2" customWidth="1"/>
-    <col min="8453" max="8453" width="83.88671875" style="2" customWidth="1"/>
-    <col min="8454" max="8704" width="14.109375" style="2"/>
-    <col min="8705" max="8705" width="24.44140625" style="2" customWidth="1"/>
+    <col min="8453" max="8453" width="83.90625" style="2" customWidth="1"/>
+    <col min="8454" max="8704" width="14.08984375" style="2"/>
+    <col min="8705" max="8705" width="24.453125" style="2" customWidth="1"/>
     <col min="8706" max="8706" width="36" style="2" customWidth="1"/>
-    <col min="8707" max="8707" width="23.6640625" style="2" customWidth="1"/>
+    <col min="8707" max="8707" width="23.6328125" style="2" customWidth="1"/>
     <col min="8708" max="8708" width="16" style="2" customWidth="1"/>
-    <col min="8709" max="8709" width="83.88671875" style="2" customWidth="1"/>
-    <col min="8710" max="8960" width="14.109375" style="2"/>
-    <col min="8961" max="8961" width="24.44140625" style="2" customWidth="1"/>
+    <col min="8709" max="8709" width="83.90625" style="2" customWidth="1"/>
+    <col min="8710" max="8960" width="14.08984375" style="2"/>
+    <col min="8961" max="8961" width="24.453125" style="2" customWidth="1"/>
     <col min="8962" max="8962" width="36" style="2" customWidth="1"/>
-    <col min="8963" max="8963" width="23.6640625" style="2" customWidth="1"/>
+    <col min="8963" max="8963" width="23.6328125" style="2" customWidth="1"/>
     <col min="8964" max="8964" width="16" style="2" customWidth="1"/>
-    <col min="8965" max="8965" width="83.88671875" style="2" customWidth="1"/>
-    <col min="8966" max="9216" width="14.109375" style="2"/>
-    <col min="9217" max="9217" width="24.44140625" style="2" customWidth="1"/>
+    <col min="8965" max="8965" width="83.90625" style="2" customWidth="1"/>
+    <col min="8966" max="9216" width="14.08984375" style="2"/>
+    <col min="9217" max="9217" width="24.453125" style="2" customWidth="1"/>
     <col min="9218" max="9218" width="36" style="2" customWidth="1"/>
-    <col min="9219" max="9219" width="23.6640625" style="2" customWidth="1"/>
+    <col min="9219" max="9219" width="23.6328125" style="2" customWidth="1"/>
     <col min="9220" max="9220" width="16" style="2" customWidth="1"/>
-    <col min="9221" max="9221" width="83.88671875" style="2" customWidth="1"/>
-    <col min="9222" max="9472" width="14.109375" style="2"/>
-    <col min="9473" max="9473" width="24.44140625" style="2" customWidth="1"/>
+    <col min="9221" max="9221" width="83.90625" style="2" customWidth="1"/>
+    <col min="9222" max="9472" width="14.08984375" style="2"/>
+    <col min="9473" max="9473" width="24.453125" style="2" customWidth="1"/>
     <col min="9474" max="9474" width="36" style="2" customWidth="1"/>
-    <col min="9475" max="9475" width="23.6640625" style="2" customWidth="1"/>
+    <col min="9475" max="9475" width="23.6328125" style="2" customWidth="1"/>
     <col min="9476" max="9476" width="16" style="2" customWidth="1"/>
-    <col min="9477" max="9477" width="83.88671875" style="2" customWidth="1"/>
-    <col min="9478" max="9728" width="14.109375" style="2"/>
-    <col min="9729" max="9729" width="24.44140625" style="2" customWidth="1"/>
+    <col min="9477" max="9477" width="83.90625" style="2" customWidth="1"/>
+    <col min="9478" max="9728" width="14.08984375" style="2"/>
+    <col min="9729" max="9729" width="24.453125" style="2" customWidth="1"/>
     <col min="9730" max="9730" width="36" style="2" customWidth="1"/>
-    <col min="9731" max="9731" width="23.6640625" style="2" customWidth="1"/>
+    <col min="9731" max="9731" width="23.6328125" style="2" customWidth="1"/>
     <col min="9732" max="9732" width="16" style="2" customWidth="1"/>
-    <col min="9733" max="9733" width="83.88671875" style="2" customWidth="1"/>
-    <col min="9734" max="9984" width="14.109375" style="2"/>
-    <col min="9985" max="9985" width="24.44140625" style="2" customWidth="1"/>
+    <col min="9733" max="9733" width="83.90625" style="2" customWidth="1"/>
+    <col min="9734" max="9984" width="14.08984375" style="2"/>
+    <col min="9985" max="9985" width="24.453125" style="2" customWidth="1"/>
     <col min="9986" max="9986" width="36" style="2" customWidth="1"/>
-    <col min="9987" max="9987" width="23.6640625" style="2" customWidth="1"/>
+    <col min="9987" max="9987" width="23.6328125" style="2" customWidth="1"/>
     <col min="9988" max="9988" width="16" style="2" customWidth="1"/>
-    <col min="9989" max="9989" width="83.88671875" style="2" customWidth="1"/>
-    <col min="9990" max="10240" width="14.109375" style="2"/>
-    <col min="10241" max="10241" width="24.44140625" style="2" customWidth="1"/>
+    <col min="9989" max="9989" width="83.90625" style="2" customWidth="1"/>
+    <col min="9990" max="10240" width="14.08984375" style="2"/>
+    <col min="10241" max="10241" width="24.453125" style="2" customWidth="1"/>
     <col min="10242" max="10242" width="36" style="2" customWidth="1"/>
-    <col min="10243" max="10243" width="23.6640625" style="2" customWidth="1"/>
+    <col min="10243" max="10243" width="23.6328125" style="2" customWidth="1"/>
     <col min="10244" max="10244" width="16" style="2" customWidth="1"/>
-    <col min="10245" max="10245" width="83.88671875" style="2" customWidth="1"/>
-    <col min="10246" max="10496" width="14.109375" style="2"/>
-    <col min="10497" max="10497" width="24.44140625" style="2" customWidth="1"/>
+    <col min="10245" max="10245" width="83.90625" style="2" customWidth="1"/>
+    <col min="10246" max="10496" width="14.08984375" style="2"/>
+    <col min="10497" max="10497" width="24.453125" style="2" customWidth="1"/>
     <col min="10498" max="10498" width="36" style="2" customWidth="1"/>
-    <col min="10499" max="10499" width="23.6640625" style="2" customWidth="1"/>
+    <col min="10499" max="10499" width="23.6328125" style="2" customWidth="1"/>
     <col min="10500" max="10500" width="16" style="2" customWidth="1"/>
-    <col min="10501" max="10501" width="83.88671875" style="2" customWidth="1"/>
-    <col min="10502" max="10752" width="14.109375" style="2"/>
-    <col min="10753" max="10753" width="24.44140625" style="2" customWidth="1"/>
+    <col min="10501" max="10501" width="83.90625" style="2" customWidth="1"/>
+    <col min="10502" max="10752" width="14.08984375" style="2"/>
+    <col min="10753" max="10753" width="24.453125" style="2" customWidth="1"/>
     <col min="10754" max="10754" width="36" style="2" customWidth="1"/>
-    <col min="10755" max="10755" width="23.6640625" style="2" customWidth="1"/>
+    <col min="10755" max="10755" width="23.6328125" style="2" customWidth="1"/>
     <col min="10756" max="10756" width="16" style="2" customWidth="1"/>
-    <col min="10757" max="10757" width="83.88671875" style="2" customWidth="1"/>
-    <col min="10758" max="11008" width="14.109375" style="2"/>
-    <col min="11009" max="11009" width="24.44140625" style="2" customWidth="1"/>
+    <col min="10757" max="10757" width="83.90625" style="2" customWidth="1"/>
+    <col min="10758" max="11008" width="14.08984375" style="2"/>
+    <col min="11009" max="11009" width="24.453125" style="2" customWidth="1"/>
     <col min="11010" max="11010" width="36" style="2" customWidth="1"/>
-    <col min="11011" max="11011" width="23.6640625" style="2" customWidth="1"/>
+    <col min="11011" max="11011" width="23.6328125" style="2" customWidth="1"/>
     <col min="11012" max="11012" width="16" style="2" customWidth="1"/>
-    <col min="11013" max="11013" width="83.88671875" style="2" customWidth="1"/>
-    <col min="11014" max="11264" width="14.109375" style="2"/>
-    <col min="11265" max="11265" width="24.44140625" style="2" customWidth="1"/>
+    <col min="11013" max="11013" width="83.90625" style="2" customWidth="1"/>
+    <col min="11014" max="11264" width="14.08984375" style="2"/>
+    <col min="11265" max="11265" width="24.453125" style="2" customWidth="1"/>
     <col min="11266" max="11266" width="36" style="2" customWidth="1"/>
-    <col min="11267" max="11267" width="23.6640625" style="2" customWidth="1"/>
+    <col min="11267" max="11267" width="23.6328125" style="2" customWidth="1"/>
     <col min="11268" max="11268" width="16" style="2" customWidth="1"/>
-    <col min="11269" max="11269" width="83.88671875" style="2" customWidth="1"/>
-    <col min="11270" max="11520" width="14.109375" style="2"/>
-    <col min="11521" max="11521" width="24.44140625" style="2" customWidth="1"/>
+    <col min="11269" max="11269" width="83.90625" style="2" customWidth="1"/>
+    <col min="11270" max="11520" width="14.08984375" style="2"/>
+    <col min="11521" max="11521" width="24.453125" style="2" customWidth="1"/>
     <col min="11522" max="11522" width="36" style="2" customWidth="1"/>
-    <col min="11523" max="11523" width="23.6640625" style="2" customWidth="1"/>
+    <col min="11523" max="11523" width="23.6328125" style="2" customWidth="1"/>
     <col min="11524" max="11524" width="16" style="2" customWidth="1"/>
-    <col min="11525" max="11525" width="83.88671875" style="2" customWidth="1"/>
-    <col min="11526" max="11776" width="14.109375" style="2"/>
-    <col min="11777" max="11777" width="24.44140625" style="2" customWidth="1"/>
+    <col min="11525" max="11525" width="83.90625" style="2" customWidth="1"/>
+    <col min="11526" max="11776" width="14.08984375" style="2"/>
+    <col min="11777" max="11777" width="24.453125" style="2" customWidth="1"/>
     <col min="11778" max="11778" width="36" style="2" customWidth="1"/>
-    <col min="11779" max="11779" width="23.6640625" style="2" customWidth="1"/>
+    <col min="11779" max="11779" width="23.6328125" style="2" customWidth="1"/>
     <col min="11780" max="11780" width="16" style="2" customWidth="1"/>
-    <col min="11781" max="11781" width="83.88671875" style="2" customWidth="1"/>
-    <col min="11782" max="12032" width="14.109375" style="2"/>
-    <col min="12033" max="12033" width="24.44140625" style="2" customWidth="1"/>
+    <col min="11781" max="11781" width="83.90625" style="2" customWidth="1"/>
+    <col min="11782" max="12032" width="14.08984375" style="2"/>
+    <col min="12033" max="12033" width="24.453125" style="2" customWidth="1"/>
     <col min="12034" max="12034" width="36" style="2" customWidth="1"/>
-    <col min="12035" max="12035" width="23.6640625" style="2" customWidth="1"/>
+    <col min="12035" max="12035" width="23.6328125" style="2" customWidth="1"/>
     <col min="12036" max="12036" width="16" style="2" customWidth="1"/>
-    <col min="12037" max="12037" width="83.88671875" style="2" customWidth="1"/>
-    <col min="12038" max="12288" width="14.109375" style="2"/>
-    <col min="12289" max="12289" width="24.44140625" style="2" customWidth="1"/>
+    <col min="12037" max="12037" width="83.90625" style="2" customWidth="1"/>
+    <col min="12038" max="12288" width="14.08984375" style="2"/>
+    <col min="12289" max="12289" width="24.453125" style="2" customWidth="1"/>
     <col min="12290" max="12290" width="36" style="2" customWidth="1"/>
-    <col min="12291" max="12291" width="23.6640625" style="2" customWidth="1"/>
+    <col min="12291" max="12291" width="23.6328125" style="2" customWidth="1"/>
     <col min="12292" max="12292" width="16" style="2" customWidth="1"/>
-    <col min="12293" max="12293" width="83.88671875" style="2" customWidth="1"/>
-    <col min="12294" max="12544" width="14.109375" style="2"/>
-    <col min="12545" max="12545" width="24.44140625" style="2" customWidth="1"/>
+    <col min="12293" max="12293" width="83.90625" style="2" customWidth="1"/>
+    <col min="12294" max="12544" width="14.08984375" style="2"/>
+    <col min="12545" max="12545" width="24.453125" style="2" customWidth="1"/>
     <col min="12546" max="12546" width="36" style="2" customWidth="1"/>
-    <col min="12547" max="12547" width="23.6640625" style="2" customWidth="1"/>
+    <col min="12547" max="12547" width="23.6328125" style="2" customWidth="1"/>
     <col min="12548" max="12548" width="16" style="2" customWidth="1"/>
-    <col min="12549" max="12549" width="83.88671875" style="2" customWidth="1"/>
-    <col min="12550" max="12800" width="14.109375" style="2"/>
-    <col min="12801" max="12801" width="24.44140625" style="2" customWidth="1"/>
+    <col min="12549" max="12549" width="83.90625" style="2" customWidth="1"/>
+    <col min="12550" max="12800" width="14.08984375" style="2"/>
+    <col min="12801" max="12801" width="24.453125" style="2" customWidth="1"/>
     <col min="12802" max="12802" width="36" style="2" customWidth="1"/>
-    <col min="12803" max="12803" width="23.6640625" style="2" customWidth="1"/>
+    <col min="12803" max="12803" width="23.6328125" style="2" customWidth="1"/>
     <col min="12804" max="12804" width="16" style="2" customWidth="1"/>
-    <col min="12805" max="12805" width="83.88671875" style="2" customWidth="1"/>
-    <col min="12806" max="13056" width="14.109375" style="2"/>
-    <col min="13057" max="13057" width="24.44140625" style="2" customWidth="1"/>
+    <col min="12805" max="12805" width="83.90625" style="2" customWidth="1"/>
+    <col min="12806" max="13056" width="14.08984375" style="2"/>
+    <col min="13057" max="13057" width="24.453125" style="2" customWidth="1"/>
     <col min="13058" max="13058" width="36" style="2" customWidth="1"/>
-    <col min="13059" max="13059" width="23.6640625" style="2" customWidth="1"/>
+    <col min="13059" max="13059" width="23.6328125" style="2" customWidth="1"/>
     <col min="13060" max="13060" width="16" style="2" customWidth="1"/>
-    <col min="13061" max="13061" width="83.88671875" style="2" customWidth="1"/>
-    <col min="13062" max="13312" width="14.109375" style="2"/>
-    <col min="13313" max="13313" width="24.44140625" style="2" customWidth="1"/>
+    <col min="13061" max="13061" width="83.90625" style="2" customWidth="1"/>
+    <col min="13062" max="13312" width="14.08984375" style="2"/>
+    <col min="13313" max="13313" width="24.453125" style="2" customWidth="1"/>
     <col min="13314" max="13314" width="36" style="2" customWidth="1"/>
-    <col min="13315" max="13315" width="23.6640625" style="2" customWidth="1"/>
+    <col min="13315" max="13315" width="23.6328125" style="2" customWidth="1"/>
     <col min="13316" max="13316" width="16" style="2" customWidth="1"/>
-    <col min="13317" max="13317" width="83.88671875" style="2" customWidth="1"/>
-    <col min="13318" max="13568" width="14.109375" style="2"/>
-    <col min="13569" max="13569" width="24.44140625" style="2" customWidth="1"/>
+    <col min="13317" max="13317" width="83.90625" style="2" customWidth="1"/>
+    <col min="13318" max="13568" width="14.08984375" style="2"/>
+    <col min="13569" max="13569" width="24.453125" style="2" customWidth="1"/>
     <col min="13570" max="13570" width="36" style="2" customWidth="1"/>
-    <col min="13571" max="13571" width="23.6640625" style="2" customWidth="1"/>
+    <col min="13571" max="13571" width="23.6328125" style="2" customWidth="1"/>
     <col min="13572" max="13572" width="16" style="2" customWidth="1"/>
-    <col min="13573" max="13573" width="83.88671875" style="2" customWidth="1"/>
-    <col min="13574" max="13824" width="14.109375" style="2"/>
-    <col min="13825" max="13825" width="24.44140625" style="2" customWidth="1"/>
+    <col min="13573" max="13573" width="83.90625" style="2" customWidth="1"/>
+    <col min="13574" max="13824" width="14.08984375" style="2"/>
+    <col min="13825" max="13825" width="24.453125" style="2" customWidth="1"/>
     <col min="13826" max="13826" width="36" style="2" customWidth="1"/>
-    <col min="13827" max="13827" width="23.6640625" style="2" customWidth="1"/>
+    <col min="13827" max="13827" width="23.6328125" style="2" customWidth="1"/>
     <col min="13828" max="13828" width="16" style="2" customWidth="1"/>
-    <col min="13829" max="13829" width="83.88671875" style="2" customWidth="1"/>
-    <col min="13830" max="14080" width="14.109375" style="2"/>
-    <col min="14081" max="14081" width="24.44140625" style="2" customWidth="1"/>
+    <col min="13829" max="13829" width="83.90625" style="2" customWidth="1"/>
+    <col min="13830" max="14080" width="14.08984375" style="2"/>
+    <col min="14081" max="14081" width="24.453125" style="2" customWidth="1"/>
     <col min="14082" max="14082" width="36" style="2" customWidth="1"/>
-    <col min="14083" max="14083" width="23.6640625" style="2" customWidth="1"/>
+    <col min="14083" max="14083" width="23.6328125" style="2" customWidth="1"/>
     <col min="14084" max="14084" width="16" style="2" customWidth="1"/>
-    <col min="14085" max="14085" width="83.88671875" style="2" customWidth="1"/>
-    <col min="14086" max="14336" width="14.109375" style="2"/>
-    <col min="14337" max="14337" width="24.44140625" style="2" customWidth="1"/>
+    <col min="14085" max="14085" width="83.90625" style="2" customWidth="1"/>
+    <col min="14086" max="14336" width="14.08984375" style="2"/>
+    <col min="14337" max="14337" width="24.453125" style="2" customWidth="1"/>
     <col min="14338" max="14338" width="36" style="2" customWidth="1"/>
-    <col min="14339" max="14339" width="23.6640625" style="2" customWidth="1"/>
+    <col min="14339" max="14339" width="23.6328125" style="2" customWidth="1"/>
     <col min="14340" max="14340" width="16" style="2" customWidth="1"/>
-    <col min="14341" max="14341" width="83.88671875" style="2" customWidth="1"/>
-    <col min="14342" max="14592" width="14.109375" style="2"/>
-    <col min="14593" max="14593" width="24.44140625" style="2" customWidth="1"/>
+    <col min="14341" max="14341" width="83.90625" style="2" customWidth="1"/>
+    <col min="14342" max="14592" width="14.08984375" style="2"/>
+    <col min="14593" max="14593" width="24.453125" style="2" customWidth="1"/>
     <col min="14594" max="14594" width="36" style="2" customWidth="1"/>
-    <col min="14595" max="14595" width="23.6640625" style="2" customWidth="1"/>
+    <col min="14595" max="14595" width="23.6328125" style="2" customWidth="1"/>
     <col min="14596" max="14596" width="16" style="2" customWidth="1"/>
-    <col min="14597" max="14597" width="83.88671875" style="2" customWidth="1"/>
-    <col min="14598" max="14848" width="14.109375" style="2"/>
-    <col min="14849" max="14849" width="24.44140625" style="2" customWidth="1"/>
+    <col min="14597" max="14597" width="83.90625" style="2" customWidth="1"/>
+    <col min="14598" max="14848" width="14.08984375" style="2"/>
+    <col min="14849" max="14849" width="24.453125" style="2" customWidth="1"/>
     <col min="14850" max="14850" width="36" style="2" customWidth="1"/>
-    <col min="14851" max="14851" width="23.6640625" style="2" customWidth="1"/>
+    <col min="14851" max="14851" width="23.6328125" style="2" customWidth="1"/>
     <col min="14852" max="14852" width="16" style="2" customWidth="1"/>
-    <col min="14853" max="14853" width="83.88671875" style="2" customWidth="1"/>
-    <col min="14854" max="15104" width="14.109375" style="2"/>
-    <col min="15105" max="15105" width="24.44140625" style="2" customWidth="1"/>
+    <col min="14853" max="14853" width="83.90625" style="2" customWidth="1"/>
+    <col min="14854" max="15104" width="14.08984375" style="2"/>
+    <col min="15105" max="15105" width="24.453125" style="2" customWidth="1"/>
     <col min="15106" max="15106" width="36" style="2" customWidth="1"/>
-    <col min="15107" max="15107" width="23.6640625" style="2" customWidth="1"/>
+    <col min="15107" max="15107" width="23.6328125" style="2" customWidth="1"/>
     <col min="15108" max="15108" width="16" style="2" customWidth="1"/>
-    <col min="15109" max="15109" width="83.88671875" style="2" customWidth="1"/>
-    <col min="15110" max="15360" width="14.109375" style="2"/>
-    <col min="15361" max="15361" width="24.44140625" style="2" customWidth="1"/>
+    <col min="15109" max="15109" width="83.90625" style="2" customWidth="1"/>
+    <col min="15110" max="15360" width="14.08984375" style="2"/>
+    <col min="15361" max="15361" width="24.453125" style="2" customWidth="1"/>
     <col min="15362" max="15362" width="36" style="2" customWidth="1"/>
-    <col min="15363" max="15363" width="23.6640625" style="2" customWidth="1"/>
+    <col min="15363" max="15363" width="23.6328125" style="2" customWidth="1"/>
     <col min="15364" max="15364" width="16" style="2" customWidth="1"/>
-    <col min="15365" max="15365" width="83.88671875" style="2" customWidth="1"/>
-    <col min="15366" max="15616" width="14.109375" style="2"/>
-    <col min="15617" max="15617" width="24.44140625" style="2" customWidth="1"/>
+    <col min="15365" max="15365" width="83.90625" style="2" customWidth="1"/>
+    <col min="15366" max="15616" width="14.08984375" style="2"/>
+    <col min="15617" max="15617" width="24.453125" style="2" customWidth="1"/>
     <col min="15618" max="15618" width="36" style="2" customWidth="1"/>
-    <col min="15619" max="15619" width="23.6640625" style="2" customWidth="1"/>
+    <col min="15619" max="15619" width="23.6328125" style="2" customWidth="1"/>
     <col min="15620" max="15620" width="16" style="2" customWidth="1"/>
-    <col min="15621" max="15621" width="83.88671875" style="2" customWidth="1"/>
-    <col min="15622" max="15872" width="14.109375" style="2"/>
-    <col min="15873" max="15873" width="24.44140625" style="2" customWidth="1"/>
+    <col min="15621" max="15621" width="83.90625" style="2" customWidth="1"/>
+    <col min="15622" max="15872" width="14.08984375" style="2"/>
+    <col min="15873" max="15873" width="24.453125" style="2" customWidth="1"/>
     <col min="15874" max="15874" width="36" style="2" customWidth="1"/>
-    <col min="15875" max="15875" width="23.6640625" style="2" customWidth="1"/>
+    <col min="15875" max="15875" width="23.6328125" style="2" customWidth="1"/>
     <col min="15876" max="15876" width="16" style="2" customWidth="1"/>
-    <col min="15877" max="15877" width="83.88671875" style="2" customWidth="1"/>
-    <col min="15878" max="16128" width="14.109375" style="2"/>
-    <col min="16129" max="16129" width="24.44140625" style="2" customWidth="1"/>
+    <col min="15877" max="15877" width="83.90625" style="2" customWidth="1"/>
+    <col min="15878" max="16128" width="14.08984375" style="2"/>
+    <col min="16129" max="16129" width="24.453125" style="2" customWidth="1"/>
     <col min="16130" max="16130" width="36" style="2" customWidth="1"/>
-    <col min="16131" max="16131" width="23.6640625" style="2" customWidth="1"/>
+    <col min="16131" max="16131" width="23.6328125" style="2" customWidth="1"/>
     <col min="16132" max="16132" width="16" style="2" customWidth="1"/>
-    <col min="16133" max="16133" width="83.88671875" style="2" customWidth="1"/>
-    <col min="16134" max="16384" width="14.109375" style="2"/>
+    <col min="16133" max="16133" width="83.90625" style="2" customWidth="1"/>
+    <col min="16134" max="16384" width="14.08984375" style="2"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="9" customHeight="1"/>
     <row r="2" spans="1:5" ht="15.75" customHeight="1" thickBot="1">
-      <c r="A2" s="93"/>
-      <c r="B2" s="94"/>
-      <c r="C2" s="94"/>
-      <c r="D2" s="94"/>
-      <c r="E2" s="94"/>
+      <c r="A2" s="108"/>
+      <c r="B2" s="109"/>
+      <c r="C2" s="109"/>
+      <c r="D2" s="109"/>
+      <c r="E2" s="109"/>
     </row>
     <row r="3" spans="1:5" ht="15" customHeight="1">
-      <c r="A3" s="95" t="s">
+      <c r="A3" s="110" t="s">
         <v>64</v>
       </c>
-      <c r="B3" s="97" t="s">
+      <c r="B3" s="112" t="s">
         <v>65</v>
       </c>
-      <c r="C3" s="99" t="s">
+      <c r="C3" s="114" t="s">
         <v>66</v>
       </c>
-      <c r="D3" s="99" t="s">
+      <c r="D3" s="114" t="s">
         <v>67</v>
       </c>
-      <c r="E3" s="97" t="s">
+      <c r="E3" s="112" t="s">
         <v>68</v>
       </c>
     </row>
     <row r="4" spans="1:5" ht="45" customHeight="1" thickBot="1">
-      <c r="A4" s="96"/>
-      <c r="B4" s="98"/>
-      <c r="C4" s="100"/>
-      <c r="D4" s="100"/>
-      <c r="E4" s="98"/>
+      <c r="A4" s="111"/>
+      <c r="B4" s="113"/>
+      <c r="C4" s="115"/>
+      <c r="D4" s="115"/>
+      <c r="E4" s="113"/>
     </row>
     <row r="5" spans="1:5" ht="73.5" customHeight="1" thickBot="1">
       <c r="A5" s="3" t="s">
@@ -46541,10 +46504,10 @@
       <c r="E7" s="7"/>
     </row>
     <row r="8" spans="1:5" ht="22.5" customHeight="1">
-      <c r="A8" s="113" t="s">
+      <c r="A8" s="107" t="s">
         <v>71</v>
       </c>
-      <c r="B8" s="101"/>
+      <c r="B8" s="100"/>
       <c r="C8" s="8">
         <v>642436</v>
       </c>
@@ -46556,8 +46519,8 @@
       </c>
     </row>
     <row r="9" spans="1:5" ht="17.25" customHeight="1">
-      <c r="A9" s="105"/>
-      <c r="B9" s="102"/>
+      <c r="A9" s="93"/>
+      <c r="B9" s="101"/>
       <c r="C9" s="9">
         <v>642437</v>
       </c>
@@ -46569,8 +46532,8 @@
       </c>
     </row>
     <row r="10" spans="1:5">
-      <c r="A10" s="105"/>
-      <c r="B10" s="102"/>
+      <c r="A10" s="93"/>
+      <c r="B10" s="101"/>
       <c r="C10" s="9">
         <v>642438</v>
       </c>
@@ -46582,8 +46545,8 @@
       </c>
     </row>
     <row r="11" spans="1:5">
-      <c r="A11" s="105"/>
-      <c r="B11" s="102"/>
+      <c r="A11" s="93"/>
+      <c r="B11" s="101"/>
       <c r="C11" s="9">
         <v>642439</v>
       </c>
@@ -46595,10 +46558,10 @@
       </c>
     </row>
     <row r="12" spans="1:5">
-      <c r="A12" s="104" t="s">
+      <c r="A12" s="99" t="s">
         <v>72</v>
       </c>
-      <c r="B12" s="102"/>
+      <c r="B12" s="101"/>
       <c r="C12" s="9">
         <v>642440</v>
       </c>
@@ -46610,8 +46573,8 @@
       </c>
     </row>
     <row r="13" spans="1:5">
-      <c r="A13" s="105"/>
-      <c r="B13" s="102"/>
+      <c r="A13" s="93"/>
+      <c r="B13" s="101"/>
       <c r="C13" s="9">
         <v>642441</v>
       </c>
@@ -46623,8 +46586,8 @@
       </c>
     </row>
     <row r="14" spans="1:5">
-      <c r="A14" s="105"/>
-      <c r="B14" s="102"/>
+      <c r="A14" s="93"/>
+      <c r="B14" s="101"/>
       <c r="C14" s="9">
         <v>642442</v>
       </c>
@@ -46636,8 +46599,8 @@
       </c>
     </row>
     <row r="15" spans="1:5">
-      <c r="A15" s="105"/>
-      <c r="B15" s="102"/>
+      <c r="A15" s="93"/>
+      <c r="B15" s="101"/>
       <c r="C15" s="11">
         <v>642443</v>
       </c>
@@ -46649,10 +46612,10 @@
       </c>
     </row>
     <row r="16" spans="1:5">
-      <c r="A16" s="104" t="s">
+      <c r="A16" s="99" t="s">
         <v>73</v>
       </c>
-      <c r="B16" s="102"/>
+      <c r="B16" s="101"/>
       <c r="C16" s="9">
         <v>642444</v>
       </c>
@@ -46664,8 +46627,8 @@
       </c>
     </row>
     <row r="17" spans="1:5">
-      <c r="A17" s="105"/>
-      <c r="B17" s="102"/>
+      <c r="A17" s="93"/>
+      <c r="B17" s="101"/>
       <c r="C17" s="9">
         <v>642445</v>
       </c>
@@ -46677,8 +46640,8 @@
       </c>
     </row>
     <row r="18" spans="1:5">
-      <c r="A18" s="105"/>
-      <c r="B18" s="102"/>
+      <c r="A18" s="93"/>
+      <c r="B18" s="101"/>
       <c r="C18" s="9">
         <v>642446</v>
       </c>
@@ -46690,8 +46653,8 @@
       </c>
     </row>
     <row r="19" spans="1:5">
-      <c r="A19" s="105"/>
-      <c r="B19" s="102"/>
+      <c r="A19" s="93"/>
+      <c r="B19" s="101"/>
       <c r="C19" s="9">
         <v>642447</v>
       </c>
@@ -46703,10 +46666,10 @@
       </c>
     </row>
     <row r="20" spans="1:5">
-      <c r="A20" s="104" t="s">
+      <c r="A20" s="99" t="s">
         <v>74</v>
       </c>
-      <c r="B20" s="102"/>
+      <c r="B20" s="101"/>
       <c r="C20" s="13" t="s">
         <v>75</v>
       </c>
@@ -46718,8 +46681,8 @@
       </c>
     </row>
     <row r="21" spans="1:5">
-      <c r="A21" s="105"/>
-      <c r="B21" s="102"/>
+      <c r="A21" s="93"/>
+      <c r="B21" s="101"/>
       <c r="C21" s="13" t="s">
         <v>76</v>
       </c>
@@ -46730,9 +46693,9 @@
         <v>33</v>
       </c>
     </row>
-    <row r="22" spans="1:5" ht="14.4" thickBot="1">
-      <c r="A22" s="106"/>
-      <c r="B22" s="103"/>
+    <row r="22" spans="1:5" ht="14.5" thickBot="1">
+      <c r="A22" s="94"/>
+      <c r="B22" s="102"/>
       <c r="C22" s="14" t="s">
         <v>77</v>
       </c>
@@ -46749,17 +46712,17 @@
       <c r="D23" s="6"/>
       <c r="E23" s="7"/>
     </row>
-    <row r="24" spans="1:5" ht="14.4" thickBot="1">
+    <row r="24" spans="1:5" ht="14.5" thickBot="1">
       <c r="A24" s="5"/>
       <c r="C24" s="6"/>
       <c r="D24" s="6"/>
       <c r="E24" s="7"/>
     </row>
-    <row r="25" spans="1:5" ht="13.95" customHeight="1">
-      <c r="A25" s="113" t="s">
+    <row r="25" spans="1:5" ht="14" customHeight="1">
+      <c r="A25" s="107" t="s">
         <v>78</v>
       </c>
-      <c r="B25" s="101"/>
+      <c r="B25" s="100"/>
       <c r="C25" s="8">
         <v>312797</v>
       </c>
@@ -46771,8 +46734,8 @@
       </c>
     </row>
     <row r="26" spans="1:5">
-      <c r="A26" s="105"/>
-      <c r="B26" s="102"/>
+      <c r="A26" s="93"/>
+      <c r="B26" s="101"/>
       <c r="C26" s="9">
         <v>312798</v>
       </c>
@@ -46784,8 +46747,8 @@
       </c>
     </row>
     <row r="27" spans="1:5">
-      <c r="A27" s="105"/>
-      <c r="B27" s="102"/>
+      <c r="A27" s="93"/>
+      <c r="B27" s="101"/>
       <c r="C27" s="9">
         <v>312799</v>
       </c>
@@ -46797,8 +46760,8 @@
       </c>
     </row>
     <row r="28" spans="1:5">
-      <c r="A28" s="105"/>
-      <c r="B28" s="102"/>
+      <c r="A28" s="93"/>
+      <c r="B28" s="101"/>
       <c r="C28" s="9">
         <v>312800</v>
       </c>
@@ -46810,10 +46773,10 @@
       </c>
     </row>
     <row r="29" spans="1:5">
-      <c r="A29" s="104" t="s">
+      <c r="A29" s="99" t="s">
         <v>79</v>
       </c>
-      <c r="B29" s="102"/>
+      <c r="B29" s="101"/>
       <c r="C29" s="9">
         <v>312802</v>
       </c>
@@ -46825,8 +46788,8 @@
       </c>
     </row>
     <row r="30" spans="1:5">
-      <c r="A30" s="105"/>
-      <c r="B30" s="102"/>
+      <c r="A30" s="93"/>
+      <c r="B30" s="101"/>
       <c r="C30" s="9">
         <v>312803</v>
       </c>
@@ -46838,8 +46801,8 @@
       </c>
     </row>
     <row r="31" spans="1:5">
-      <c r="A31" s="105"/>
-      <c r="B31" s="102"/>
+      <c r="A31" s="93"/>
+      <c r="B31" s="101"/>
       <c r="C31" s="9">
         <v>312804</v>
       </c>
@@ -46851,8 +46814,8 @@
       </c>
     </row>
     <row r="32" spans="1:5">
-      <c r="A32" s="105"/>
-      <c r="B32" s="102"/>
+      <c r="A32" s="93"/>
+      <c r="B32" s="101"/>
       <c r="C32" s="9">
         <v>312805</v>
       </c>
@@ -46864,10 +46827,10 @@
       </c>
     </row>
     <row r="33" spans="1:5">
-      <c r="A33" s="104" t="s">
+      <c r="A33" s="99" t="s">
         <v>80</v>
       </c>
-      <c r="B33" s="102"/>
+      <c r="B33" s="101"/>
       <c r="C33" s="9">
         <v>312807</v>
       </c>
@@ -46879,8 +46842,8 @@
       </c>
     </row>
     <row r="34" spans="1:5">
-      <c r="A34" s="105"/>
-      <c r="B34" s="102"/>
+      <c r="A34" s="93"/>
+      <c r="B34" s="101"/>
       <c r="C34" s="9">
         <v>312808</v>
       </c>
@@ -46892,8 +46855,8 @@
       </c>
     </row>
     <row r="35" spans="1:5">
-      <c r="A35" s="105"/>
-      <c r="B35" s="102"/>
+      <c r="A35" s="93"/>
+      <c r="B35" s="101"/>
       <c r="C35" s="9">
         <v>312809</v>
       </c>
@@ -46905,8 +46868,8 @@
       </c>
     </row>
     <row r="36" spans="1:5">
-      <c r="A36" s="105"/>
-      <c r="B36" s="102"/>
+      <c r="A36" s="93"/>
+      <c r="B36" s="101"/>
       <c r="C36" s="9">
         <v>312810</v>
       </c>
@@ -46918,10 +46881,10 @@
       </c>
     </row>
     <row r="37" spans="1:5">
-      <c r="A37" s="104" t="s">
+      <c r="A37" s="99" t="s">
         <v>81</v>
       </c>
-      <c r="B37" s="102"/>
+      <c r="B37" s="101"/>
       <c r="C37" s="9">
         <v>490442</v>
       </c>
@@ -46933,8 +46896,8 @@
       </c>
     </row>
     <row r="38" spans="1:5">
-      <c r="A38" s="105"/>
-      <c r="B38" s="102"/>
+      <c r="A38" s="93"/>
+      <c r="B38" s="101"/>
       <c r="C38" s="9">
         <v>490441</v>
       </c>
@@ -46945,9 +46908,9 @@
         <v>50</v>
       </c>
     </row>
-    <row r="39" spans="1:5" ht="14.4" thickBot="1">
-      <c r="A39" s="106"/>
-      <c r="B39" s="103"/>
+    <row r="39" spans="1:5" ht="14.5" thickBot="1">
+      <c r="A39" s="94"/>
+      <c r="B39" s="102"/>
       <c r="C39" s="15">
         <v>490440</v>
       </c>
@@ -46958,7 +46921,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="40" spans="1:5" ht="14.4" thickBot="1">
+    <row r="40" spans="1:5" ht="14.5" thickBot="1">
       <c r="A40" s="5"/>
       <c r="B40" s="17"/>
       <c r="C40" s="6"/>
@@ -46966,7 +46929,7 @@
       <c r="E40" s="7"/>
     </row>
     <row r="41" spans="1:5" ht="51" customHeight="1">
-      <c r="A41" s="109" t="s">
+      <c r="A41" s="103" t="s">
         <v>82</v>
       </c>
       <c r="B41" s="18"/>
@@ -46981,7 +46944,7 @@
       </c>
     </row>
     <row r="42" spans="1:5" ht="48" customHeight="1" thickBot="1">
-      <c r="A42" s="110"/>
+      <c r="A42" s="104"/>
       <c r="B42" s="20"/>
       <c r="C42" s="15">
         <v>314417</v>
@@ -46993,17 +46956,17 @@
         <v>84</v>
       </c>
     </row>
-    <row r="43" spans="1:5" ht="14.4" thickBot="1">
+    <row r="43" spans="1:5" ht="14.5" thickBot="1">
       <c r="A43" s="5"/>
       <c r="C43" s="6"/>
       <c r="D43" s="6"/>
       <c r="E43" s="7"/>
     </row>
     <row r="44" spans="1:5" ht="20.25" customHeight="1">
-      <c r="A44" s="111" t="s">
+      <c r="A44" s="105" t="s">
         <v>85</v>
       </c>
-      <c r="B44" s="101"/>
+      <c r="B44" s="100"/>
       <c r="C44" s="8">
         <v>643863</v>
       </c>
@@ -47015,8 +46978,8 @@
       </c>
     </row>
     <row r="45" spans="1:5">
-      <c r="A45" s="112"/>
-      <c r="B45" s="102"/>
+      <c r="A45" s="106"/>
+      <c r="B45" s="101"/>
       <c r="C45" s="9">
         <v>643864</v>
       </c>
@@ -47028,8 +46991,8 @@
       </c>
     </row>
     <row r="46" spans="1:5">
-      <c r="A46" s="112"/>
-      <c r="B46" s="102"/>
+      <c r="A46" s="106"/>
+      <c r="B46" s="101"/>
       <c r="C46" s="9">
         <v>643865</v>
       </c>
@@ -47040,9 +47003,9 @@
         <v>88</v>
       </c>
     </row>
-    <row r="47" spans="1:5" ht="14.4" thickBot="1">
-      <c r="A47" s="110"/>
-      <c r="B47" s="103"/>
+    <row r="47" spans="1:5" ht="14.5" thickBot="1">
+      <c r="A47" s="104"/>
+      <c r="B47" s="102"/>
       <c r="C47" s="14" t="s">
         <v>89</v>
       </c>
@@ -47053,13 +47016,13 @@
         <v>91</v>
       </c>
     </row>
-    <row r="48" spans="1:5" ht="14.4" thickBot="1">
+    <row r="48" spans="1:5" ht="14.5" thickBot="1">
       <c r="A48" s="5"/>
       <c r="C48" s="6"/>
       <c r="D48" s="6"/>
       <c r="E48" s="7"/>
     </row>
-    <row r="49" spans="1:5" ht="57.6" customHeight="1" thickBot="1">
+    <row r="49" spans="1:5" ht="57.65" customHeight="1" thickBot="1">
       <c r="A49" s="25" t="s">
         <v>92</v>
       </c>
@@ -47073,7 +47036,7 @@
       <c r="E49" s="29"/>
     </row>
     <row r="50" spans="1:5">
-      <c r="A50" s="113" t="s">
+      <c r="A50" s="107" t="s">
         <v>95</v>
       </c>
       <c r="B50" s="30" t="s">
@@ -47083,10 +47046,10 @@
         <v>642913</v>
       </c>
       <c r="D50" s="32"/>
-      <c r="E50" s="107"/>
+      <c r="E50" s="95"/>
     </row>
     <row r="51" spans="1:5">
-      <c r="A51" s="105"/>
+      <c r="A51" s="93"/>
       <c r="B51" s="33" t="s">
         <v>97</v>
       </c>
@@ -47094,10 +47057,10 @@
         <v>643863</v>
       </c>
       <c r="D51" s="32"/>
-      <c r="E51" s="108"/>
+      <c r="E51" s="96"/>
     </row>
     <row r="52" spans="1:5">
-      <c r="A52" s="105"/>
+      <c r="A52" s="93"/>
       <c r="B52" s="35" t="s">
         <v>98</v>
       </c>
@@ -47105,10 +47068,10 @@
         <v>206878</v>
       </c>
       <c r="D52" s="32"/>
-      <c r="E52" s="108"/>
+      <c r="E52" s="96"/>
     </row>
     <row r="53" spans="1:5">
-      <c r="A53" s="105"/>
+      <c r="A53" s="93"/>
       <c r="B53" s="35" t="s">
         <v>99</v>
       </c>
@@ -47116,10 +47079,10 @@
         <v>206894</v>
       </c>
       <c r="D53" s="32"/>
-      <c r="E53" s="108"/>
+      <c r="E53" s="96"/>
     </row>
     <row r="54" spans="1:5">
-      <c r="A54" s="104" t="s">
+      <c r="A54" s="99" t="s">
         <v>100</v>
       </c>
       <c r="B54" s="35" t="s">
@@ -47129,10 +47092,10 @@
         <v>642913</v>
       </c>
       <c r="D54" s="32"/>
-      <c r="E54" s="107"/>
+      <c r="E54" s="95"/>
     </row>
     <row r="55" spans="1:5">
-      <c r="A55" s="105"/>
+      <c r="A55" s="93"/>
       <c r="B55" s="35" t="s">
         <v>101</v>
       </c>
@@ -47140,10 +47103,10 @@
         <v>643864</v>
       </c>
       <c r="D55" s="32"/>
-      <c r="E55" s="108"/>
+      <c r="E55" s="96"/>
     </row>
     <row r="56" spans="1:5">
-      <c r="A56" s="105"/>
+      <c r="A56" s="93"/>
       <c r="B56" s="33" t="s">
         <v>102</v>
       </c>
@@ -47151,10 +47114,10 @@
         <v>315577</v>
       </c>
       <c r="D56" s="32"/>
-      <c r="E56" s="108"/>
+      <c r="E56" s="96"/>
     </row>
     <row r="57" spans="1:5">
-      <c r="A57" s="105"/>
+      <c r="A57" s="93"/>
       <c r="B57" s="33" t="s">
         <v>103</v>
       </c>
@@ -47162,10 +47125,10 @@
         <v>315578</v>
       </c>
       <c r="D57" s="32"/>
-      <c r="E57" s="108"/>
+      <c r="E57" s="96"/>
     </row>
     <row r="58" spans="1:5">
-      <c r="A58" s="105" t="s">
+      <c r="A58" s="93" t="s">
         <v>104</v>
       </c>
       <c r="B58" s="35" t="s">
@@ -47175,10 +47138,10 @@
         <v>642913</v>
       </c>
       <c r="D58" s="32"/>
-      <c r="E58" s="107"/>
+      <c r="E58" s="95"/>
     </row>
     <row r="59" spans="1:5">
-      <c r="A59" s="105"/>
+      <c r="A59" s="93"/>
       <c r="B59" s="35" t="s">
         <v>105</v>
       </c>
@@ -47186,10 +47149,10 @@
         <v>643865</v>
       </c>
       <c r="D59" s="32"/>
-      <c r="E59" s="108"/>
+      <c r="E59" s="96"/>
     </row>
     <row r="60" spans="1:5">
-      <c r="A60" s="105"/>
+      <c r="A60" s="93"/>
       <c r="B60" s="35" t="s">
         <v>106</v>
       </c>
@@ -47197,10 +47160,10 @@
         <v>242080</v>
       </c>
       <c r="D60" s="32"/>
-      <c r="E60" s="108"/>
+      <c r="E60" s="96"/>
     </row>
     <row r="61" spans="1:5">
-      <c r="A61" s="105"/>
+      <c r="A61" s="93"/>
       <c r="B61" s="35" t="s">
         <v>107</v>
       </c>
@@ -47208,10 +47171,10 @@
         <v>242073</v>
       </c>
       <c r="D61" s="32"/>
-      <c r="E61" s="108"/>
+      <c r="E61" s="96"/>
     </row>
     <row r="62" spans="1:5">
-      <c r="A62" s="104" t="s">
+      <c r="A62" s="99" t="s">
         <v>108</v>
       </c>
       <c r="B62" s="35" t="s">
@@ -47221,10 +47184,10 @@
         <v>642913</v>
       </c>
       <c r="D62" s="32"/>
-      <c r="E62" s="107"/>
-    </row>
-    <row r="63" spans="1:5" ht="13.95" customHeight="1">
-      <c r="A63" s="105"/>
+      <c r="E62" s="95"/>
+    </row>
+    <row r="63" spans="1:5" ht="14" customHeight="1">
+      <c r="A63" s="93"/>
       <c r="B63" s="35" t="s">
         <v>109</v>
       </c>
@@ -47232,10 +47195,10 @@
         <v>738957</v>
       </c>
       <c r="D63" s="32"/>
-      <c r="E63" s="107"/>
+      <c r="E63" s="95"/>
     </row>
     <row r="64" spans="1:5">
-      <c r="A64" s="105"/>
+      <c r="A64" s="93"/>
       <c r="B64" s="35" t="s">
         <v>110</v>
       </c>
@@ -47243,10 +47206,10 @@
         <v>490996</v>
       </c>
       <c r="D64" s="32"/>
-      <c r="E64" s="107"/>
-    </row>
-    <row r="65" spans="1:5" ht="14.4" thickBot="1">
-      <c r="A65" s="106"/>
+      <c r="E64" s="95"/>
+    </row>
+    <row r="65" spans="1:5" ht="14.5" thickBot="1">
+      <c r="A65" s="94"/>
       <c r="B65" s="36" t="s">
         <v>111</v>
       </c>
@@ -47254,10 +47217,10 @@
         <v>490999</v>
       </c>
       <c r="D65" s="32"/>
-      <c r="E65" s="107"/>
+      <c r="E65" s="95"/>
     </row>
     <row r="66" spans="1:5">
-      <c r="A66" s="114" t="s">
+      <c r="A66" s="98" t="s">
         <v>112</v>
       </c>
       <c r="B66" s="30" t="s">
@@ -47267,10 +47230,10 @@
         <v>642914</v>
       </c>
       <c r="D66" s="32"/>
-      <c r="E66" s="107"/>
-    </row>
-    <row r="67" spans="1:5" ht="13.95" customHeight="1">
-      <c r="A67" s="105"/>
+      <c r="E66" s="95"/>
+    </row>
+    <row r="67" spans="1:5" ht="14" customHeight="1">
+      <c r="A67" s="93"/>
       <c r="B67" s="35" t="s">
         <v>97</v>
       </c>
@@ -47278,10 +47241,10 @@
         <v>643863</v>
       </c>
       <c r="D67" s="32"/>
-      <c r="E67" s="108"/>
+      <c r="E67" s="96"/>
     </row>
     <row r="68" spans="1:5">
-      <c r="A68" s="105"/>
+      <c r="A68" s="93"/>
       <c r="B68" s="35" t="s">
         <v>114</v>
       </c>
@@ -47289,10 +47252,10 @@
         <v>206880</v>
       </c>
       <c r="D68" s="32"/>
-      <c r="E68" s="108"/>
+      <c r="E68" s="96"/>
     </row>
     <row r="69" spans="1:5">
-      <c r="A69" s="105"/>
+      <c r="A69" s="93"/>
       <c r="B69" s="35" t="s">
         <v>115</v>
       </c>
@@ -47300,10 +47263,10 @@
         <v>206896</v>
       </c>
       <c r="D69" s="32"/>
-      <c r="E69" s="108"/>
+      <c r="E69" s="96"/>
     </row>
     <row r="70" spans="1:5">
-      <c r="A70" s="105" t="s">
+      <c r="A70" s="93" t="s">
         <v>116</v>
       </c>
       <c r="B70" s="35" t="s">
@@ -47313,10 +47276,10 @@
         <v>642914</v>
       </c>
       <c r="D70" s="32"/>
-      <c r="E70" s="107"/>
-    </row>
-    <row r="71" spans="1:5" ht="13.95" customHeight="1">
-      <c r="A71" s="105"/>
+      <c r="E70" s="95"/>
+    </row>
+    <row r="71" spans="1:5" ht="14" customHeight="1">
+      <c r="A71" s="93"/>
       <c r="B71" s="35" t="s">
         <v>101</v>
       </c>
@@ -47324,10 +47287,10 @@
         <v>643864</v>
       </c>
       <c r="D71" s="32"/>
-      <c r="E71" s="108"/>
+      <c r="E71" s="96"/>
     </row>
     <row r="72" spans="1:5">
-      <c r="A72" s="105"/>
+      <c r="A72" s="93"/>
       <c r="B72" s="35" t="s">
         <v>117</v>
       </c>
@@ -47335,10 +47298,10 @@
         <v>315579</v>
       </c>
       <c r="D72" s="32"/>
-      <c r="E72" s="108"/>
+      <c r="E72" s="96"/>
     </row>
     <row r="73" spans="1:5">
-      <c r="A73" s="105"/>
+      <c r="A73" s="93"/>
       <c r="B73" s="35" t="s">
         <v>118</v>
       </c>
@@ -47346,10 +47309,10 @@
         <v>315580</v>
       </c>
       <c r="D73" s="32"/>
-      <c r="E73" s="108"/>
+      <c r="E73" s="96"/>
     </row>
     <row r="74" spans="1:5">
-      <c r="A74" s="105" t="s">
+      <c r="A74" s="93" t="s">
         <v>119</v>
       </c>
       <c r="B74" s="35" t="s">
@@ -47359,10 +47322,10 @@
         <v>642914</v>
       </c>
       <c r="D74" s="32"/>
-      <c r="E74" s="107"/>
-    </row>
-    <row r="75" spans="1:5" ht="13.95" customHeight="1">
-      <c r="A75" s="105"/>
+      <c r="E74" s="95"/>
+    </row>
+    <row r="75" spans="1:5" ht="14" customHeight="1">
+      <c r="A75" s="93"/>
       <c r="B75" s="35" t="s">
         <v>105</v>
       </c>
@@ -47370,10 +47333,10 @@
         <v>643865</v>
       </c>
       <c r="D75" s="32"/>
-      <c r="E75" s="108"/>
+      <c r="E75" s="96"/>
     </row>
     <row r="76" spans="1:5">
-      <c r="A76" s="105"/>
+      <c r="A76" s="93"/>
       <c r="B76" s="35" t="s">
         <v>120</v>
       </c>
@@ -47381,10 +47344,10 @@
         <v>242081</v>
       </c>
       <c r="D76" s="32"/>
-      <c r="E76" s="108"/>
+      <c r="E76" s="96"/>
     </row>
     <row r="77" spans="1:5">
-      <c r="A77" s="105"/>
+      <c r="A77" s="93"/>
       <c r="B77" s="35" t="s">
         <v>121</v>
       </c>
@@ -47392,10 +47355,10 @@
         <v>242074</v>
       </c>
       <c r="D77" s="32"/>
-      <c r="E77" s="108"/>
+      <c r="E77" s="96"/>
     </row>
     <row r="78" spans="1:5">
-      <c r="A78" s="105" t="s">
+      <c r="A78" s="93" t="s">
         <v>122</v>
       </c>
       <c r="B78" s="35" t="s">
@@ -47405,10 +47368,10 @@
         <v>642914</v>
       </c>
       <c r="D78" s="32"/>
-      <c r="E78" s="107"/>
-    </row>
-    <row r="79" spans="1:5" ht="13.95" customHeight="1">
-      <c r="A79" s="105"/>
+      <c r="E78" s="95"/>
+    </row>
+    <row r="79" spans="1:5" ht="14" customHeight="1">
+      <c r="A79" s="93"/>
       <c r="B79" s="35" t="s">
         <v>109</v>
       </c>
@@ -47416,10 +47379,10 @@
         <v>738957</v>
       </c>
       <c r="D79" s="32"/>
-      <c r="E79" s="107"/>
+      <c r="E79" s="95"/>
     </row>
     <row r="80" spans="1:5">
-      <c r="A80" s="105"/>
+      <c r="A80" s="93"/>
       <c r="B80" s="35" t="s">
         <v>123</v>
       </c>
@@ -47427,10 +47390,10 @@
         <v>490997</v>
       </c>
       <c r="D80" s="32"/>
-      <c r="E80" s="107"/>
-    </row>
-    <row r="81" spans="1:5" ht="14.4" thickBot="1">
-      <c r="A81" s="106"/>
+      <c r="E80" s="95"/>
+    </row>
+    <row r="81" spans="1:5" ht="14.5" thickBot="1">
+      <c r="A81" s="94"/>
       <c r="B81" s="36" t="s">
         <v>124</v>
       </c>
@@ -47438,10 +47401,10 @@
         <v>491000</v>
       </c>
       <c r="D81" s="32"/>
-      <c r="E81" s="107"/>
+      <c r="E81" s="95"/>
     </row>
     <row r="82" spans="1:5">
-      <c r="A82" s="114" t="s">
+      <c r="A82" s="98" t="s">
         <v>125</v>
       </c>
       <c r="B82" s="30" t="s">
@@ -47451,10 +47414,10 @@
         <v>642915</v>
       </c>
       <c r="D82" s="32"/>
-      <c r="E82" s="107"/>
-    </row>
-    <row r="83" spans="1:5" ht="13.95" customHeight="1">
-      <c r="A83" s="105"/>
+      <c r="E82" s="95"/>
+    </row>
+    <row r="83" spans="1:5" ht="14" customHeight="1">
+      <c r="A83" s="93"/>
       <c r="B83" s="35" t="s">
         <v>97</v>
       </c>
@@ -47462,10 +47425,10 @@
         <v>643863</v>
       </c>
       <c r="D83" s="32"/>
-      <c r="E83" s="108"/>
+      <c r="E83" s="96"/>
     </row>
     <row r="84" spans="1:5">
-      <c r="A84" s="105"/>
+      <c r="A84" s="93"/>
       <c r="B84" s="35" t="s">
         <v>127</v>
       </c>
@@ -47473,10 +47436,10 @@
         <v>206884</v>
       </c>
       <c r="D84" s="32"/>
-      <c r="E84" s="108"/>
+      <c r="E84" s="96"/>
     </row>
     <row r="85" spans="1:5">
-      <c r="A85" s="105"/>
+      <c r="A85" s="93"/>
       <c r="B85" s="35" t="s">
         <v>128</v>
       </c>
@@ -47484,10 +47447,10 @@
         <v>206900</v>
       </c>
       <c r="D85" s="32"/>
-      <c r="E85" s="108"/>
+      <c r="E85" s="96"/>
     </row>
     <row r="86" spans="1:5">
-      <c r="A86" s="105" t="s">
+      <c r="A86" s="93" t="s">
         <v>129</v>
       </c>
       <c r="B86" s="35" t="s">
@@ -47497,10 +47460,10 @@
         <v>642915</v>
       </c>
       <c r="D86" s="32"/>
-      <c r="E86" s="107"/>
-    </row>
-    <row r="87" spans="1:5" ht="13.95" customHeight="1">
-      <c r="A87" s="105"/>
+      <c r="E86" s="95"/>
+    </row>
+    <row r="87" spans="1:5" ht="14" customHeight="1">
+      <c r="A87" s="93"/>
       <c r="B87" s="35" t="s">
         <v>101</v>
       </c>
@@ -47508,10 +47471,10 @@
         <v>643864</v>
       </c>
       <c r="D87" s="32"/>
-      <c r="E87" s="108"/>
+      <c r="E87" s="96"/>
     </row>
     <row r="88" spans="1:5">
-      <c r="A88" s="105"/>
+      <c r="A88" s="93"/>
       <c r="B88" s="35" t="s">
         <v>130</v>
       </c>
@@ -47519,10 +47482,10 @@
         <v>315581</v>
       </c>
       <c r="D88" s="32"/>
-      <c r="E88" s="108"/>
+      <c r="E88" s="96"/>
     </row>
     <row r="89" spans="1:5">
-      <c r="A89" s="105"/>
+      <c r="A89" s="93"/>
       <c r="B89" s="35" t="s">
         <v>131</v>
       </c>
@@ -47530,10 +47493,10 @@
         <v>315582</v>
       </c>
       <c r="D89" s="32"/>
-      <c r="E89" s="108"/>
+      <c r="E89" s="96"/>
     </row>
     <row r="90" spans="1:5">
-      <c r="A90" s="105" t="s">
+      <c r="A90" s="93" t="s">
         <v>132</v>
       </c>
       <c r="B90" s="35" t="s">
@@ -47543,10 +47506,10 @@
         <v>642915</v>
       </c>
       <c r="D90" s="32"/>
-      <c r="E90" s="107"/>
-    </row>
-    <row r="91" spans="1:5" ht="13.95" customHeight="1">
-      <c r="A91" s="105"/>
+      <c r="E90" s="95"/>
+    </row>
+    <row r="91" spans="1:5" ht="14" customHeight="1">
+      <c r="A91" s="93"/>
       <c r="B91" s="35" t="s">
         <v>105</v>
       </c>
@@ -47554,10 +47517,10 @@
         <v>643865</v>
       </c>
       <c r="D91" s="32"/>
-      <c r="E91" s="108"/>
+      <c r="E91" s="96"/>
     </row>
     <row r="92" spans="1:5">
-      <c r="A92" s="105"/>
+      <c r="A92" s="93"/>
       <c r="B92" s="35" t="s">
         <v>133</v>
       </c>
@@ -47565,10 +47528,10 @@
         <v>242082</v>
       </c>
       <c r="D92" s="32"/>
-      <c r="E92" s="108"/>
-    </row>
-    <row r="93" spans="1:5" ht="14.4" thickBot="1">
-      <c r="A93" s="106"/>
+      <c r="E92" s="96"/>
+    </row>
+    <row r="93" spans="1:5" ht="14.5" thickBot="1">
+      <c r="A93" s="94"/>
       <c r="B93" s="36" t="s">
         <v>134</v>
       </c>
@@ -47576,10 +47539,10 @@
         <v>242075</v>
       </c>
       <c r="D93" s="32"/>
-      <c r="E93" s="108"/>
+      <c r="E93" s="96"/>
     </row>
     <row r="94" spans="1:5">
-      <c r="A94" s="115" t="s">
+      <c r="A94" s="97" t="s">
         <v>135</v>
       </c>
       <c r="B94" s="38" t="s">
@@ -47589,10 +47552,10 @@
         <v>642916</v>
       </c>
       <c r="D94" s="32"/>
-      <c r="E94" s="107"/>
-    </row>
-    <row r="95" spans="1:5" ht="13.95" customHeight="1">
-      <c r="A95" s="105"/>
+      <c r="E94" s="95"/>
+    </row>
+    <row r="95" spans="1:5" ht="14" customHeight="1">
+      <c r="A95" s="93"/>
       <c r="B95" s="35" t="s">
         <v>97</v>
       </c>
@@ -47600,10 +47563,10 @@
         <v>643863</v>
       </c>
       <c r="D95" s="32"/>
-      <c r="E95" s="108"/>
+      <c r="E95" s="96"/>
     </row>
     <row r="96" spans="1:5">
-      <c r="A96" s="105"/>
+      <c r="A96" s="93"/>
       <c r="B96" s="35" t="s">
         <v>137</v>
       </c>
@@ -47611,10 +47574,10 @@
         <v>206882</v>
       </c>
       <c r="D96" s="32"/>
-      <c r="E96" s="108"/>
+      <c r="E96" s="96"/>
     </row>
     <row r="97" spans="1:5">
-      <c r="A97" s="105"/>
+      <c r="A97" s="93"/>
       <c r="B97" s="35" t="s">
         <v>138</v>
       </c>
@@ -47622,10 +47585,10 @@
         <v>206898</v>
       </c>
       <c r="D97" s="32"/>
-      <c r="E97" s="108"/>
+      <c r="E97" s="96"/>
     </row>
     <row r="98" spans="1:5">
-      <c r="A98" s="105" t="s">
+      <c r="A98" s="93" t="s">
         <v>139</v>
       </c>
       <c r="B98" s="35" t="s">
@@ -47635,10 +47598,10 @@
         <v>642916</v>
       </c>
       <c r="D98" s="32"/>
-      <c r="E98" s="107"/>
-    </row>
-    <row r="99" spans="1:5" ht="13.95" customHeight="1">
-      <c r="A99" s="105"/>
+      <c r="E98" s="95"/>
+    </row>
+    <row r="99" spans="1:5" ht="14" customHeight="1">
+      <c r="A99" s="93"/>
       <c r="B99" s="35" t="s">
         <v>101</v>
       </c>
@@ -47646,10 +47609,10 @@
         <v>643864</v>
       </c>
       <c r="D99" s="32"/>
-      <c r="E99" s="107"/>
+      <c r="E99" s="95"/>
     </row>
     <row r="100" spans="1:5">
-      <c r="A100" s="105"/>
+      <c r="A100" s="93"/>
       <c r="B100" s="35" t="s">
         <v>140</v>
       </c>
@@ -47657,10 +47620,10 @@
         <v>315584</v>
       </c>
       <c r="D100" s="32"/>
-      <c r="E100" s="107"/>
+      <c r="E100" s="95"/>
     </row>
     <row r="101" spans="1:5">
-      <c r="A101" s="105"/>
+      <c r="A101" s="93"/>
       <c r="B101" s="35" t="s">
         <v>141</v>
       </c>
@@ -47668,10 +47631,10 @@
         <v>315585</v>
       </c>
       <c r="D101" s="32"/>
-      <c r="E101" s="107"/>
+      <c r="E101" s="95"/>
     </row>
     <row r="102" spans="1:5">
-      <c r="A102" s="105" t="s">
+      <c r="A102" s="93" t="s">
         <v>142</v>
       </c>
       <c r="B102" s="35" t="s">
@@ -47681,10 +47644,10 @@
         <v>642916</v>
       </c>
       <c r="D102" s="32"/>
-      <c r="E102" s="107"/>
-    </row>
-    <row r="103" spans="1:5" ht="13.95" customHeight="1">
-      <c r="A103" s="105"/>
+      <c r="E102" s="95"/>
+    </row>
+    <row r="103" spans="1:5" ht="14" customHeight="1">
+      <c r="A103" s="93"/>
       <c r="B103" s="35" t="s">
         <v>105</v>
       </c>
@@ -47692,10 +47655,10 @@
         <v>643865</v>
       </c>
       <c r="D103" s="32"/>
-      <c r="E103" s="107"/>
+      <c r="E103" s="95"/>
     </row>
     <row r="104" spans="1:5">
-      <c r="A104" s="105"/>
+      <c r="A104" s="93"/>
       <c r="B104" s="35" t="s">
         <v>143</v>
       </c>
@@ -47703,10 +47666,10 @@
         <v>242083</v>
       </c>
       <c r="D104" s="32"/>
-      <c r="E104" s="107"/>
+      <c r="E104" s="95"/>
     </row>
     <row r="105" spans="1:5">
-      <c r="A105" s="105"/>
+      <c r="A105" s="93"/>
       <c r="B105" s="35" t="s">
         <v>144</v>
       </c>
@@ -47714,10 +47677,10 @@
         <v>242078</v>
       </c>
       <c r="D105" s="32"/>
-      <c r="E105" s="107"/>
+      <c r="E105" s="95"/>
     </row>
     <row r="106" spans="1:5">
-      <c r="A106" s="105" t="s">
+      <c r="A106" s="93" t="s">
         <v>145</v>
       </c>
       <c r="B106" s="35" t="s">
@@ -47727,10 +47690,10 @@
         <v>642916</v>
       </c>
       <c r="D106" s="32"/>
-      <c r="E106" s="107"/>
-    </row>
-    <row r="107" spans="1:5" ht="13.95" customHeight="1">
-      <c r="A107" s="105"/>
+      <c r="E106" s="95"/>
+    </row>
+    <row r="107" spans="1:5" ht="14" customHeight="1">
+      <c r="A107" s="93"/>
       <c r="B107" s="35" t="s">
         <v>109</v>
       </c>
@@ -47738,10 +47701,10 @@
         <v>738957</v>
       </c>
       <c r="D107" s="32"/>
-      <c r="E107" s="107"/>
+      <c r="E107" s="95"/>
     </row>
     <row r="108" spans="1:5">
-      <c r="A108" s="105"/>
+      <c r="A108" s="93"/>
       <c r="B108" s="35" t="s">
         <v>146</v>
       </c>
@@ -47749,10 +47712,10 @@
         <v>490998</v>
       </c>
       <c r="D108" s="32"/>
-      <c r="E108" s="107"/>
-    </row>
-    <row r="109" spans="1:5" ht="14.4" thickBot="1">
-      <c r="A109" s="106"/>
+      <c r="E108" s="95"/>
+    </row>
+    <row r="109" spans="1:5" ht="14.5" thickBot="1">
+      <c r="A109" s="94"/>
       <c r="B109" s="36" t="s">
         <v>147</v>
       </c>
@@ -47760,39 +47723,17 @@
         <v>491001</v>
       </c>
       <c r="D109" s="32"/>
-      <c r="E109" s="107"/>
+      <c r="E109" s="95"/>
     </row>
   </sheetData>
   <sheetProtection password="CC01" sheet="1" formatCells="0" formatColumns="0" formatRows="0" insertColumns="0" insertRows="0" insertHyperlinks="0" deleteColumns="0" deleteRows="0" sort="0" autoFilter="0" pivotTables="0"/>
   <mergeCells count="49">
-    <mergeCell ref="A90:A93"/>
-    <mergeCell ref="E90:E93"/>
-    <mergeCell ref="A106:A109"/>
-    <mergeCell ref="E106:E109"/>
-    <mergeCell ref="A94:A97"/>
-    <mergeCell ref="E94:E97"/>
-    <mergeCell ref="A98:A101"/>
-    <mergeCell ref="E98:E101"/>
-    <mergeCell ref="A102:A105"/>
-    <mergeCell ref="E102:E105"/>
-    <mergeCell ref="A78:A81"/>
-    <mergeCell ref="E78:E81"/>
-    <mergeCell ref="A82:A85"/>
-    <mergeCell ref="E82:E85"/>
-    <mergeCell ref="A86:A89"/>
-    <mergeCell ref="E86:E89"/>
-    <mergeCell ref="A66:A69"/>
-    <mergeCell ref="E66:E69"/>
-    <mergeCell ref="A70:A73"/>
-    <mergeCell ref="E70:E73"/>
-    <mergeCell ref="A74:A77"/>
-    <mergeCell ref="E74:E77"/>
-    <mergeCell ref="A58:A61"/>
-    <mergeCell ref="E58:E61"/>
-    <mergeCell ref="A62:A65"/>
-    <mergeCell ref="E62:E65"/>
-    <mergeCell ref="A54:A57"/>
-    <mergeCell ref="E54:E57"/>
+    <mergeCell ref="A2:E2"/>
+    <mergeCell ref="A3:A4"/>
+    <mergeCell ref="B3:B4"/>
+    <mergeCell ref="C3:C4"/>
+    <mergeCell ref="D3:D4"/>
+    <mergeCell ref="E3:E4"/>
     <mergeCell ref="B8:B22"/>
     <mergeCell ref="A12:A15"/>
     <mergeCell ref="A16:A19"/>
@@ -47808,12 +47749,34 @@
     <mergeCell ref="A33:A36"/>
     <mergeCell ref="A37:A39"/>
     <mergeCell ref="A8:A11"/>
-    <mergeCell ref="A2:E2"/>
-    <mergeCell ref="A3:A4"/>
-    <mergeCell ref="B3:B4"/>
-    <mergeCell ref="C3:C4"/>
-    <mergeCell ref="D3:D4"/>
-    <mergeCell ref="E3:E4"/>
+    <mergeCell ref="A58:A61"/>
+    <mergeCell ref="E58:E61"/>
+    <mergeCell ref="A62:A65"/>
+    <mergeCell ref="E62:E65"/>
+    <mergeCell ref="A54:A57"/>
+    <mergeCell ref="E54:E57"/>
+    <mergeCell ref="A66:A69"/>
+    <mergeCell ref="E66:E69"/>
+    <mergeCell ref="A70:A73"/>
+    <mergeCell ref="E70:E73"/>
+    <mergeCell ref="A74:A77"/>
+    <mergeCell ref="E74:E77"/>
+    <mergeCell ref="A78:A81"/>
+    <mergeCell ref="E78:E81"/>
+    <mergeCell ref="A82:A85"/>
+    <mergeCell ref="E82:E85"/>
+    <mergeCell ref="A86:A89"/>
+    <mergeCell ref="E86:E89"/>
+    <mergeCell ref="A90:A93"/>
+    <mergeCell ref="E90:E93"/>
+    <mergeCell ref="A106:A109"/>
+    <mergeCell ref="E106:E109"/>
+    <mergeCell ref="A94:A97"/>
+    <mergeCell ref="E94:E97"/>
+    <mergeCell ref="A98:A101"/>
+    <mergeCell ref="E98:E101"/>
+    <mergeCell ref="A102:A105"/>
+    <mergeCell ref="E102:E105"/>
   </mergeCells>
   <pageMargins left="0.78740157480314965" right="0.78740157480314965" top="0.98425196850393704" bottom="0.98425196850393704" header="0.51181102362204722" footer="0.51181102362204722"/>
   <pageSetup paperSize="259" scale="97" fitToHeight="0" orientation="landscape" r:id="rId1"/>
@@ -47834,406 +47797,406 @@
       <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.77734375" defaultRowHeight="13.8"/>
+  <sheetFormatPr defaultColWidth="14.81640625" defaultRowHeight="14"/>
   <cols>
-    <col min="1" max="1" width="56.6640625" style="40" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="33.6640625" style="40" customWidth="1"/>
-    <col min="3" max="3" width="26.77734375" style="40" customWidth="1"/>
-    <col min="4" max="4" width="13.44140625" style="40" customWidth="1"/>
-    <col min="5" max="5" width="87.44140625" style="40" customWidth="1"/>
-    <col min="6" max="256" width="14.77734375" style="40"/>
-    <col min="257" max="257" width="56.6640625" style="40" bestFit="1" customWidth="1"/>
-    <col min="258" max="258" width="33.6640625" style="40" customWidth="1"/>
-    <col min="259" max="259" width="14.6640625" style="40" customWidth="1"/>
-    <col min="260" max="260" width="13.44140625" style="40" customWidth="1"/>
-    <col min="261" max="261" width="74.6640625" style="40" customWidth="1"/>
-    <col min="262" max="512" width="14.77734375" style="40"/>
-    <col min="513" max="513" width="56.6640625" style="40" bestFit="1" customWidth="1"/>
-    <col min="514" max="514" width="33.6640625" style="40" customWidth="1"/>
-    <col min="515" max="515" width="14.6640625" style="40" customWidth="1"/>
-    <col min="516" max="516" width="13.44140625" style="40" customWidth="1"/>
-    <col min="517" max="517" width="74.6640625" style="40" customWidth="1"/>
-    <col min="518" max="768" width="14.77734375" style="40"/>
-    <col min="769" max="769" width="56.6640625" style="40" bestFit="1" customWidth="1"/>
-    <col min="770" max="770" width="33.6640625" style="40" customWidth="1"/>
-    <col min="771" max="771" width="14.6640625" style="40" customWidth="1"/>
-    <col min="772" max="772" width="13.44140625" style="40" customWidth="1"/>
-    <col min="773" max="773" width="74.6640625" style="40" customWidth="1"/>
-    <col min="774" max="1024" width="14.77734375" style="40"/>
-    <col min="1025" max="1025" width="56.6640625" style="40" bestFit="1" customWidth="1"/>
-    <col min="1026" max="1026" width="33.6640625" style="40" customWidth="1"/>
-    <col min="1027" max="1027" width="14.6640625" style="40" customWidth="1"/>
-    <col min="1028" max="1028" width="13.44140625" style="40" customWidth="1"/>
-    <col min="1029" max="1029" width="74.6640625" style="40" customWidth="1"/>
-    <col min="1030" max="1280" width="14.77734375" style="40"/>
-    <col min="1281" max="1281" width="56.6640625" style="40" bestFit="1" customWidth="1"/>
-    <col min="1282" max="1282" width="33.6640625" style="40" customWidth="1"/>
-    <col min="1283" max="1283" width="14.6640625" style="40" customWidth="1"/>
-    <col min="1284" max="1284" width="13.44140625" style="40" customWidth="1"/>
-    <col min="1285" max="1285" width="74.6640625" style="40" customWidth="1"/>
-    <col min="1286" max="1536" width="14.77734375" style="40"/>
-    <col min="1537" max="1537" width="56.6640625" style="40" bestFit="1" customWidth="1"/>
-    <col min="1538" max="1538" width="33.6640625" style="40" customWidth="1"/>
-    <col min="1539" max="1539" width="14.6640625" style="40" customWidth="1"/>
-    <col min="1540" max="1540" width="13.44140625" style="40" customWidth="1"/>
-    <col min="1541" max="1541" width="74.6640625" style="40" customWidth="1"/>
-    <col min="1542" max="1792" width="14.77734375" style="40"/>
-    <col min="1793" max="1793" width="56.6640625" style="40" bestFit="1" customWidth="1"/>
-    <col min="1794" max="1794" width="33.6640625" style="40" customWidth="1"/>
-    <col min="1795" max="1795" width="14.6640625" style="40" customWidth="1"/>
-    <col min="1796" max="1796" width="13.44140625" style="40" customWidth="1"/>
-    <col min="1797" max="1797" width="74.6640625" style="40" customWidth="1"/>
-    <col min="1798" max="2048" width="14.77734375" style="40"/>
-    <col min="2049" max="2049" width="56.6640625" style="40" bestFit="1" customWidth="1"/>
-    <col min="2050" max="2050" width="33.6640625" style="40" customWidth="1"/>
-    <col min="2051" max="2051" width="14.6640625" style="40" customWidth="1"/>
-    <col min="2052" max="2052" width="13.44140625" style="40" customWidth="1"/>
-    <col min="2053" max="2053" width="74.6640625" style="40" customWidth="1"/>
-    <col min="2054" max="2304" width="14.77734375" style="40"/>
-    <col min="2305" max="2305" width="56.6640625" style="40" bestFit="1" customWidth="1"/>
-    <col min="2306" max="2306" width="33.6640625" style="40" customWidth="1"/>
-    <col min="2307" max="2307" width="14.6640625" style="40" customWidth="1"/>
-    <col min="2308" max="2308" width="13.44140625" style="40" customWidth="1"/>
-    <col min="2309" max="2309" width="74.6640625" style="40" customWidth="1"/>
-    <col min="2310" max="2560" width="14.77734375" style="40"/>
-    <col min="2561" max="2561" width="56.6640625" style="40" bestFit="1" customWidth="1"/>
-    <col min="2562" max="2562" width="33.6640625" style="40" customWidth="1"/>
-    <col min="2563" max="2563" width="14.6640625" style="40" customWidth="1"/>
-    <col min="2564" max="2564" width="13.44140625" style="40" customWidth="1"/>
-    <col min="2565" max="2565" width="74.6640625" style="40" customWidth="1"/>
-    <col min="2566" max="2816" width="14.77734375" style="40"/>
-    <col min="2817" max="2817" width="56.6640625" style="40" bestFit="1" customWidth="1"/>
-    <col min="2818" max="2818" width="33.6640625" style="40" customWidth="1"/>
-    <col min="2819" max="2819" width="14.6640625" style="40" customWidth="1"/>
-    <col min="2820" max="2820" width="13.44140625" style="40" customWidth="1"/>
-    <col min="2821" max="2821" width="74.6640625" style="40" customWidth="1"/>
-    <col min="2822" max="3072" width="14.77734375" style="40"/>
-    <col min="3073" max="3073" width="56.6640625" style="40" bestFit="1" customWidth="1"/>
-    <col min="3074" max="3074" width="33.6640625" style="40" customWidth="1"/>
-    <col min="3075" max="3075" width="14.6640625" style="40" customWidth="1"/>
-    <col min="3076" max="3076" width="13.44140625" style="40" customWidth="1"/>
-    <col min="3077" max="3077" width="74.6640625" style="40" customWidth="1"/>
-    <col min="3078" max="3328" width="14.77734375" style="40"/>
-    <col min="3329" max="3329" width="56.6640625" style="40" bestFit="1" customWidth="1"/>
-    <col min="3330" max="3330" width="33.6640625" style="40" customWidth="1"/>
-    <col min="3331" max="3331" width="14.6640625" style="40" customWidth="1"/>
-    <col min="3332" max="3332" width="13.44140625" style="40" customWidth="1"/>
-    <col min="3333" max="3333" width="74.6640625" style="40" customWidth="1"/>
-    <col min="3334" max="3584" width="14.77734375" style="40"/>
-    <col min="3585" max="3585" width="56.6640625" style="40" bestFit="1" customWidth="1"/>
-    <col min="3586" max="3586" width="33.6640625" style="40" customWidth="1"/>
-    <col min="3587" max="3587" width="14.6640625" style="40" customWidth="1"/>
-    <col min="3588" max="3588" width="13.44140625" style="40" customWidth="1"/>
-    <col min="3589" max="3589" width="74.6640625" style="40" customWidth="1"/>
-    <col min="3590" max="3840" width="14.77734375" style="40"/>
-    <col min="3841" max="3841" width="56.6640625" style="40" bestFit="1" customWidth="1"/>
-    <col min="3842" max="3842" width="33.6640625" style="40" customWidth="1"/>
-    <col min="3843" max="3843" width="14.6640625" style="40" customWidth="1"/>
-    <col min="3844" max="3844" width="13.44140625" style="40" customWidth="1"/>
-    <col min="3845" max="3845" width="74.6640625" style="40" customWidth="1"/>
-    <col min="3846" max="4096" width="14.77734375" style="40"/>
-    <col min="4097" max="4097" width="56.6640625" style="40" bestFit="1" customWidth="1"/>
-    <col min="4098" max="4098" width="33.6640625" style="40" customWidth="1"/>
-    <col min="4099" max="4099" width="14.6640625" style="40" customWidth="1"/>
-    <col min="4100" max="4100" width="13.44140625" style="40" customWidth="1"/>
-    <col min="4101" max="4101" width="74.6640625" style="40" customWidth="1"/>
-    <col min="4102" max="4352" width="14.77734375" style="40"/>
-    <col min="4353" max="4353" width="56.6640625" style="40" bestFit="1" customWidth="1"/>
-    <col min="4354" max="4354" width="33.6640625" style="40" customWidth="1"/>
-    <col min="4355" max="4355" width="14.6640625" style="40" customWidth="1"/>
-    <col min="4356" max="4356" width="13.44140625" style="40" customWidth="1"/>
-    <col min="4357" max="4357" width="74.6640625" style="40" customWidth="1"/>
-    <col min="4358" max="4608" width="14.77734375" style="40"/>
-    <col min="4609" max="4609" width="56.6640625" style="40" bestFit="1" customWidth="1"/>
-    <col min="4610" max="4610" width="33.6640625" style="40" customWidth="1"/>
-    <col min="4611" max="4611" width="14.6640625" style="40" customWidth="1"/>
-    <col min="4612" max="4612" width="13.44140625" style="40" customWidth="1"/>
-    <col min="4613" max="4613" width="74.6640625" style="40" customWidth="1"/>
-    <col min="4614" max="4864" width="14.77734375" style="40"/>
-    <col min="4865" max="4865" width="56.6640625" style="40" bestFit="1" customWidth="1"/>
-    <col min="4866" max="4866" width="33.6640625" style="40" customWidth="1"/>
-    <col min="4867" max="4867" width="14.6640625" style="40" customWidth="1"/>
-    <col min="4868" max="4868" width="13.44140625" style="40" customWidth="1"/>
-    <col min="4869" max="4869" width="74.6640625" style="40" customWidth="1"/>
-    <col min="4870" max="5120" width="14.77734375" style="40"/>
-    <col min="5121" max="5121" width="56.6640625" style="40" bestFit="1" customWidth="1"/>
-    <col min="5122" max="5122" width="33.6640625" style="40" customWidth="1"/>
-    <col min="5123" max="5123" width="14.6640625" style="40" customWidth="1"/>
-    <col min="5124" max="5124" width="13.44140625" style="40" customWidth="1"/>
-    <col min="5125" max="5125" width="74.6640625" style="40" customWidth="1"/>
-    <col min="5126" max="5376" width="14.77734375" style="40"/>
-    <col min="5377" max="5377" width="56.6640625" style="40" bestFit="1" customWidth="1"/>
-    <col min="5378" max="5378" width="33.6640625" style="40" customWidth="1"/>
-    <col min="5379" max="5379" width="14.6640625" style="40" customWidth="1"/>
-    <col min="5380" max="5380" width="13.44140625" style="40" customWidth="1"/>
-    <col min="5381" max="5381" width="74.6640625" style="40" customWidth="1"/>
-    <col min="5382" max="5632" width="14.77734375" style="40"/>
-    <col min="5633" max="5633" width="56.6640625" style="40" bestFit="1" customWidth="1"/>
-    <col min="5634" max="5634" width="33.6640625" style="40" customWidth="1"/>
-    <col min="5635" max="5635" width="14.6640625" style="40" customWidth="1"/>
-    <col min="5636" max="5636" width="13.44140625" style="40" customWidth="1"/>
-    <col min="5637" max="5637" width="74.6640625" style="40" customWidth="1"/>
-    <col min="5638" max="5888" width="14.77734375" style="40"/>
-    <col min="5889" max="5889" width="56.6640625" style="40" bestFit="1" customWidth="1"/>
-    <col min="5890" max="5890" width="33.6640625" style="40" customWidth="1"/>
-    <col min="5891" max="5891" width="14.6640625" style="40" customWidth="1"/>
-    <col min="5892" max="5892" width="13.44140625" style="40" customWidth="1"/>
-    <col min="5893" max="5893" width="74.6640625" style="40" customWidth="1"/>
-    <col min="5894" max="6144" width="14.77734375" style="40"/>
-    <col min="6145" max="6145" width="56.6640625" style="40" bestFit="1" customWidth="1"/>
-    <col min="6146" max="6146" width="33.6640625" style="40" customWidth="1"/>
-    <col min="6147" max="6147" width="14.6640625" style="40" customWidth="1"/>
-    <col min="6148" max="6148" width="13.44140625" style="40" customWidth="1"/>
-    <col min="6149" max="6149" width="74.6640625" style="40" customWidth="1"/>
-    <col min="6150" max="6400" width="14.77734375" style="40"/>
-    <col min="6401" max="6401" width="56.6640625" style="40" bestFit="1" customWidth="1"/>
-    <col min="6402" max="6402" width="33.6640625" style="40" customWidth="1"/>
-    <col min="6403" max="6403" width="14.6640625" style="40" customWidth="1"/>
-    <col min="6404" max="6404" width="13.44140625" style="40" customWidth="1"/>
-    <col min="6405" max="6405" width="74.6640625" style="40" customWidth="1"/>
-    <col min="6406" max="6656" width="14.77734375" style="40"/>
-    <col min="6657" max="6657" width="56.6640625" style="40" bestFit="1" customWidth="1"/>
-    <col min="6658" max="6658" width="33.6640625" style="40" customWidth="1"/>
-    <col min="6659" max="6659" width="14.6640625" style="40" customWidth="1"/>
-    <col min="6660" max="6660" width="13.44140625" style="40" customWidth="1"/>
-    <col min="6661" max="6661" width="74.6640625" style="40" customWidth="1"/>
-    <col min="6662" max="6912" width="14.77734375" style="40"/>
-    <col min="6913" max="6913" width="56.6640625" style="40" bestFit="1" customWidth="1"/>
-    <col min="6914" max="6914" width="33.6640625" style="40" customWidth="1"/>
-    <col min="6915" max="6915" width="14.6640625" style="40" customWidth="1"/>
-    <col min="6916" max="6916" width="13.44140625" style="40" customWidth="1"/>
-    <col min="6917" max="6917" width="74.6640625" style="40" customWidth="1"/>
-    <col min="6918" max="7168" width="14.77734375" style="40"/>
-    <col min="7169" max="7169" width="56.6640625" style="40" bestFit="1" customWidth="1"/>
-    <col min="7170" max="7170" width="33.6640625" style="40" customWidth="1"/>
-    <col min="7171" max="7171" width="14.6640625" style="40" customWidth="1"/>
-    <col min="7172" max="7172" width="13.44140625" style="40" customWidth="1"/>
-    <col min="7173" max="7173" width="74.6640625" style="40" customWidth="1"/>
-    <col min="7174" max="7424" width="14.77734375" style="40"/>
-    <col min="7425" max="7425" width="56.6640625" style="40" bestFit="1" customWidth="1"/>
-    <col min="7426" max="7426" width="33.6640625" style="40" customWidth="1"/>
-    <col min="7427" max="7427" width="14.6640625" style="40" customWidth="1"/>
-    <col min="7428" max="7428" width="13.44140625" style="40" customWidth="1"/>
-    <col min="7429" max="7429" width="74.6640625" style="40" customWidth="1"/>
-    <col min="7430" max="7680" width="14.77734375" style="40"/>
-    <col min="7681" max="7681" width="56.6640625" style="40" bestFit="1" customWidth="1"/>
-    <col min="7682" max="7682" width="33.6640625" style="40" customWidth="1"/>
-    <col min="7683" max="7683" width="14.6640625" style="40" customWidth="1"/>
-    <col min="7684" max="7684" width="13.44140625" style="40" customWidth="1"/>
-    <col min="7685" max="7685" width="74.6640625" style="40" customWidth="1"/>
-    <col min="7686" max="7936" width="14.77734375" style="40"/>
-    <col min="7937" max="7937" width="56.6640625" style="40" bestFit="1" customWidth="1"/>
-    <col min="7938" max="7938" width="33.6640625" style="40" customWidth="1"/>
-    <col min="7939" max="7939" width="14.6640625" style="40" customWidth="1"/>
-    <col min="7940" max="7940" width="13.44140625" style="40" customWidth="1"/>
-    <col min="7941" max="7941" width="74.6640625" style="40" customWidth="1"/>
-    <col min="7942" max="8192" width="14.77734375" style="40"/>
-    <col min="8193" max="8193" width="56.6640625" style="40" bestFit="1" customWidth="1"/>
-    <col min="8194" max="8194" width="33.6640625" style="40" customWidth="1"/>
-    <col min="8195" max="8195" width="14.6640625" style="40" customWidth="1"/>
-    <col min="8196" max="8196" width="13.44140625" style="40" customWidth="1"/>
-    <col min="8197" max="8197" width="74.6640625" style="40" customWidth="1"/>
-    <col min="8198" max="8448" width="14.77734375" style="40"/>
-    <col min="8449" max="8449" width="56.6640625" style="40" bestFit="1" customWidth="1"/>
-    <col min="8450" max="8450" width="33.6640625" style="40" customWidth="1"/>
-    <col min="8451" max="8451" width="14.6640625" style="40" customWidth="1"/>
-    <col min="8452" max="8452" width="13.44140625" style="40" customWidth="1"/>
-    <col min="8453" max="8453" width="74.6640625" style="40" customWidth="1"/>
-    <col min="8454" max="8704" width="14.77734375" style="40"/>
-    <col min="8705" max="8705" width="56.6640625" style="40" bestFit="1" customWidth="1"/>
-    <col min="8706" max="8706" width="33.6640625" style="40" customWidth="1"/>
-    <col min="8707" max="8707" width="14.6640625" style="40" customWidth="1"/>
-    <col min="8708" max="8708" width="13.44140625" style="40" customWidth="1"/>
-    <col min="8709" max="8709" width="74.6640625" style="40" customWidth="1"/>
-    <col min="8710" max="8960" width="14.77734375" style="40"/>
-    <col min="8961" max="8961" width="56.6640625" style="40" bestFit="1" customWidth="1"/>
-    <col min="8962" max="8962" width="33.6640625" style="40" customWidth="1"/>
-    <col min="8963" max="8963" width="14.6640625" style="40" customWidth="1"/>
-    <col min="8964" max="8964" width="13.44140625" style="40" customWidth="1"/>
-    <col min="8965" max="8965" width="74.6640625" style="40" customWidth="1"/>
-    <col min="8966" max="9216" width="14.77734375" style="40"/>
-    <col min="9217" max="9217" width="56.6640625" style="40" bestFit="1" customWidth="1"/>
-    <col min="9218" max="9218" width="33.6640625" style="40" customWidth="1"/>
-    <col min="9219" max="9219" width="14.6640625" style="40" customWidth="1"/>
-    <col min="9220" max="9220" width="13.44140625" style="40" customWidth="1"/>
-    <col min="9221" max="9221" width="74.6640625" style="40" customWidth="1"/>
-    <col min="9222" max="9472" width="14.77734375" style="40"/>
-    <col min="9473" max="9473" width="56.6640625" style="40" bestFit="1" customWidth="1"/>
-    <col min="9474" max="9474" width="33.6640625" style="40" customWidth="1"/>
-    <col min="9475" max="9475" width="14.6640625" style="40" customWidth="1"/>
-    <col min="9476" max="9476" width="13.44140625" style="40" customWidth="1"/>
-    <col min="9477" max="9477" width="74.6640625" style="40" customWidth="1"/>
-    <col min="9478" max="9728" width="14.77734375" style="40"/>
-    <col min="9729" max="9729" width="56.6640625" style="40" bestFit="1" customWidth="1"/>
-    <col min="9730" max="9730" width="33.6640625" style="40" customWidth="1"/>
-    <col min="9731" max="9731" width="14.6640625" style="40" customWidth="1"/>
-    <col min="9732" max="9732" width="13.44140625" style="40" customWidth="1"/>
-    <col min="9733" max="9733" width="74.6640625" style="40" customWidth="1"/>
-    <col min="9734" max="9984" width="14.77734375" style="40"/>
-    <col min="9985" max="9985" width="56.6640625" style="40" bestFit="1" customWidth="1"/>
-    <col min="9986" max="9986" width="33.6640625" style="40" customWidth="1"/>
-    <col min="9987" max="9987" width="14.6640625" style="40" customWidth="1"/>
-    <col min="9988" max="9988" width="13.44140625" style="40" customWidth="1"/>
-    <col min="9989" max="9989" width="74.6640625" style="40" customWidth="1"/>
-    <col min="9990" max="10240" width="14.77734375" style="40"/>
-    <col min="10241" max="10241" width="56.6640625" style="40" bestFit="1" customWidth="1"/>
-    <col min="10242" max="10242" width="33.6640625" style="40" customWidth="1"/>
-    <col min="10243" max="10243" width="14.6640625" style="40" customWidth="1"/>
-    <col min="10244" max="10244" width="13.44140625" style="40" customWidth="1"/>
-    <col min="10245" max="10245" width="74.6640625" style="40" customWidth="1"/>
-    <col min="10246" max="10496" width="14.77734375" style="40"/>
-    <col min="10497" max="10497" width="56.6640625" style="40" bestFit="1" customWidth="1"/>
-    <col min="10498" max="10498" width="33.6640625" style="40" customWidth="1"/>
-    <col min="10499" max="10499" width="14.6640625" style="40" customWidth="1"/>
-    <col min="10500" max="10500" width="13.44140625" style="40" customWidth="1"/>
-    <col min="10501" max="10501" width="74.6640625" style="40" customWidth="1"/>
-    <col min="10502" max="10752" width="14.77734375" style="40"/>
-    <col min="10753" max="10753" width="56.6640625" style="40" bestFit="1" customWidth="1"/>
-    <col min="10754" max="10754" width="33.6640625" style="40" customWidth="1"/>
-    <col min="10755" max="10755" width="14.6640625" style="40" customWidth="1"/>
-    <col min="10756" max="10756" width="13.44140625" style="40" customWidth="1"/>
-    <col min="10757" max="10757" width="74.6640625" style="40" customWidth="1"/>
-    <col min="10758" max="11008" width="14.77734375" style="40"/>
-    <col min="11009" max="11009" width="56.6640625" style="40" bestFit="1" customWidth="1"/>
-    <col min="11010" max="11010" width="33.6640625" style="40" customWidth="1"/>
-    <col min="11011" max="11011" width="14.6640625" style="40" customWidth="1"/>
-    <col min="11012" max="11012" width="13.44140625" style="40" customWidth="1"/>
-    <col min="11013" max="11013" width="74.6640625" style="40" customWidth="1"/>
-    <col min="11014" max="11264" width="14.77734375" style="40"/>
-    <col min="11265" max="11265" width="56.6640625" style="40" bestFit="1" customWidth="1"/>
-    <col min="11266" max="11266" width="33.6640625" style="40" customWidth="1"/>
-    <col min="11267" max="11267" width="14.6640625" style="40" customWidth="1"/>
-    <col min="11268" max="11268" width="13.44140625" style="40" customWidth="1"/>
-    <col min="11269" max="11269" width="74.6640625" style="40" customWidth="1"/>
-    <col min="11270" max="11520" width="14.77734375" style="40"/>
-    <col min="11521" max="11521" width="56.6640625" style="40" bestFit="1" customWidth="1"/>
-    <col min="11522" max="11522" width="33.6640625" style="40" customWidth="1"/>
-    <col min="11523" max="11523" width="14.6640625" style="40" customWidth="1"/>
-    <col min="11524" max="11524" width="13.44140625" style="40" customWidth="1"/>
-    <col min="11525" max="11525" width="74.6640625" style="40" customWidth="1"/>
-    <col min="11526" max="11776" width="14.77734375" style="40"/>
-    <col min="11777" max="11777" width="56.6640625" style="40" bestFit="1" customWidth="1"/>
-    <col min="11778" max="11778" width="33.6640625" style="40" customWidth="1"/>
-    <col min="11779" max="11779" width="14.6640625" style="40" customWidth="1"/>
-    <col min="11780" max="11780" width="13.44140625" style="40" customWidth="1"/>
-    <col min="11781" max="11781" width="74.6640625" style="40" customWidth="1"/>
-    <col min="11782" max="12032" width="14.77734375" style="40"/>
-    <col min="12033" max="12033" width="56.6640625" style="40" bestFit="1" customWidth="1"/>
-    <col min="12034" max="12034" width="33.6640625" style="40" customWidth="1"/>
-    <col min="12035" max="12035" width="14.6640625" style="40" customWidth="1"/>
-    <col min="12036" max="12036" width="13.44140625" style="40" customWidth="1"/>
-    <col min="12037" max="12037" width="74.6640625" style="40" customWidth="1"/>
-    <col min="12038" max="12288" width="14.77734375" style="40"/>
-    <col min="12289" max="12289" width="56.6640625" style="40" bestFit="1" customWidth="1"/>
-    <col min="12290" max="12290" width="33.6640625" style="40" customWidth="1"/>
-    <col min="12291" max="12291" width="14.6640625" style="40" customWidth="1"/>
-    <col min="12292" max="12292" width="13.44140625" style="40" customWidth="1"/>
-    <col min="12293" max="12293" width="74.6640625" style="40" customWidth="1"/>
-    <col min="12294" max="12544" width="14.77734375" style="40"/>
-    <col min="12545" max="12545" width="56.6640625" style="40" bestFit="1" customWidth="1"/>
-    <col min="12546" max="12546" width="33.6640625" style="40" customWidth="1"/>
-    <col min="12547" max="12547" width="14.6640625" style="40" customWidth="1"/>
-    <col min="12548" max="12548" width="13.44140625" style="40" customWidth="1"/>
-    <col min="12549" max="12549" width="74.6640625" style="40" customWidth="1"/>
-    <col min="12550" max="12800" width="14.77734375" style="40"/>
-    <col min="12801" max="12801" width="56.6640625" style="40" bestFit="1" customWidth="1"/>
-    <col min="12802" max="12802" width="33.6640625" style="40" customWidth="1"/>
-    <col min="12803" max="12803" width="14.6640625" style="40" customWidth="1"/>
-    <col min="12804" max="12804" width="13.44140625" style="40" customWidth="1"/>
-    <col min="12805" max="12805" width="74.6640625" style="40" customWidth="1"/>
-    <col min="12806" max="13056" width="14.77734375" style="40"/>
-    <col min="13057" max="13057" width="56.6640625" style="40" bestFit="1" customWidth="1"/>
-    <col min="13058" max="13058" width="33.6640625" style="40" customWidth="1"/>
-    <col min="13059" max="13059" width="14.6640625" style="40" customWidth="1"/>
-    <col min="13060" max="13060" width="13.44140625" style="40" customWidth="1"/>
-    <col min="13061" max="13061" width="74.6640625" style="40" customWidth="1"/>
-    <col min="13062" max="13312" width="14.77734375" style="40"/>
-    <col min="13313" max="13313" width="56.6640625" style="40" bestFit="1" customWidth="1"/>
-    <col min="13314" max="13314" width="33.6640625" style="40" customWidth="1"/>
-    <col min="13315" max="13315" width="14.6640625" style="40" customWidth="1"/>
-    <col min="13316" max="13316" width="13.44140625" style="40" customWidth="1"/>
-    <col min="13317" max="13317" width="74.6640625" style="40" customWidth="1"/>
-    <col min="13318" max="13568" width="14.77734375" style="40"/>
-    <col min="13569" max="13569" width="56.6640625" style="40" bestFit="1" customWidth="1"/>
-    <col min="13570" max="13570" width="33.6640625" style="40" customWidth="1"/>
-    <col min="13571" max="13571" width="14.6640625" style="40" customWidth="1"/>
-    <col min="13572" max="13572" width="13.44140625" style="40" customWidth="1"/>
-    <col min="13573" max="13573" width="74.6640625" style="40" customWidth="1"/>
-    <col min="13574" max="13824" width="14.77734375" style="40"/>
-    <col min="13825" max="13825" width="56.6640625" style="40" bestFit="1" customWidth="1"/>
-    <col min="13826" max="13826" width="33.6640625" style="40" customWidth="1"/>
-    <col min="13827" max="13827" width="14.6640625" style="40" customWidth="1"/>
-    <col min="13828" max="13828" width="13.44140625" style="40" customWidth="1"/>
-    <col min="13829" max="13829" width="74.6640625" style="40" customWidth="1"/>
-    <col min="13830" max="14080" width="14.77734375" style="40"/>
-    <col min="14081" max="14081" width="56.6640625" style="40" bestFit="1" customWidth="1"/>
-    <col min="14082" max="14082" width="33.6640625" style="40" customWidth="1"/>
-    <col min="14083" max="14083" width="14.6640625" style="40" customWidth="1"/>
-    <col min="14084" max="14084" width="13.44140625" style="40" customWidth="1"/>
-    <col min="14085" max="14085" width="74.6640625" style="40" customWidth="1"/>
-    <col min="14086" max="14336" width="14.77734375" style="40"/>
-    <col min="14337" max="14337" width="56.6640625" style="40" bestFit="1" customWidth="1"/>
-    <col min="14338" max="14338" width="33.6640625" style="40" customWidth="1"/>
-    <col min="14339" max="14339" width="14.6640625" style="40" customWidth="1"/>
-    <col min="14340" max="14340" width="13.44140625" style="40" customWidth="1"/>
-    <col min="14341" max="14341" width="74.6640625" style="40" customWidth="1"/>
-    <col min="14342" max="14592" width="14.77734375" style="40"/>
-    <col min="14593" max="14593" width="56.6640625" style="40" bestFit="1" customWidth="1"/>
-    <col min="14594" max="14594" width="33.6640625" style="40" customWidth="1"/>
-    <col min="14595" max="14595" width="14.6640625" style="40" customWidth="1"/>
-    <col min="14596" max="14596" width="13.44140625" style="40" customWidth="1"/>
-    <col min="14597" max="14597" width="74.6640625" style="40" customWidth="1"/>
-    <col min="14598" max="14848" width="14.77734375" style="40"/>
-    <col min="14849" max="14849" width="56.6640625" style="40" bestFit="1" customWidth="1"/>
-    <col min="14850" max="14850" width="33.6640625" style="40" customWidth="1"/>
-    <col min="14851" max="14851" width="14.6640625" style="40" customWidth="1"/>
-    <col min="14852" max="14852" width="13.44140625" style="40" customWidth="1"/>
-    <col min="14853" max="14853" width="74.6640625" style="40" customWidth="1"/>
-    <col min="14854" max="15104" width="14.77734375" style="40"/>
-    <col min="15105" max="15105" width="56.6640625" style="40" bestFit="1" customWidth="1"/>
-    <col min="15106" max="15106" width="33.6640625" style="40" customWidth="1"/>
-    <col min="15107" max="15107" width="14.6640625" style="40" customWidth="1"/>
-    <col min="15108" max="15108" width="13.44140625" style="40" customWidth="1"/>
-    <col min="15109" max="15109" width="74.6640625" style="40" customWidth="1"/>
-    <col min="15110" max="15360" width="14.77734375" style="40"/>
-    <col min="15361" max="15361" width="56.6640625" style="40" bestFit="1" customWidth="1"/>
-    <col min="15362" max="15362" width="33.6640625" style="40" customWidth="1"/>
-    <col min="15363" max="15363" width="14.6640625" style="40" customWidth="1"/>
-    <col min="15364" max="15364" width="13.44140625" style="40" customWidth="1"/>
-    <col min="15365" max="15365" width="74.6640625" style="40" customWidth="1"/>
-    <col min="15366" max="15616" width="14.77734375" style="40"/>
-    <col min="15617" max="15617" width="56.6640625" style="40" bestFit="1" customWidth="1"/>
-    <col min="15618" max="15618" width="33.6640625" style="40" customWidth="1"/>
-    <col min="15619" max="15619" width="14.6640625" style="40" customWidth="1"/>
-    <col min="15620" max="15620" width="13.44140625" style="40" customWidth="1"/>
-    <col min="15621" max="15621" width="74.6640625" style="40" customWidth="1"/>
-    <col min="15622" max="15872" width="14.77734375" style="40"/>
-    <col min="15873" max="15873" width="56.6640625" style="40" bestFit="1" customWidth="1"/>
-    <col min="15874" max="15874" width="33.6640625" style="40" customWidth="1"/>
-    <col min="15875" max="15875" width="14.6640625" style="40" customWidth="1"/>
-    <col min="15876" max="15876" width="13.44140625" style="40" customWidth="1"/>
-    <col min="15877" max="15877" width="74.6640625" style="40" customWidth="1"/>
-    <col min="15878" max="16128" width="14.77734375" style="40"/>
-    <col min="16129" max="16129" width="56.6640625" style="40" bestFit="1" customWidth="1"/>
-    <col min="16130" max="16130" width="33.6640625" style="40" customWidth="1"/>
-    <col min="16131" max="16131" width="14.6640625" style="40" customWidth="1"/>
-    <col min="16132" max="16132" width="13.44140625" style="40" customWidth="1"/>
-    <col min="16133" max="16133" width="74.6640625" style="40" customWidth="1"/>
-    <col min="16134" max="16384" width="14.77734375" style="40"/>
+    <col min="1" max="1" width="56.6328125" style="40" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="33.6328125" style="40" customWidth="1"/>
+    <col min="3" max="3" width="26.81640625" style="40" customWidth="1"/>
+    <col min="4" max="4" width="13.453125" style="40" customWidth="1"/>
+    <col min="5" max="5" width="87.453125" style="40" customWidth="1"/>
+    <col min="6" max="256" width="14.81640625" style="40"/>
+    <col min="257" max="257" width="56.6328125" style="40" bestFit="1" customWidth="1"/>
+    <col min="258" max="258" width="33.6328125" style="40" customWidth="1"/>
+    <col min="259" max="259" width="14.6328125" style="40" customWidth="1"/>
+    <col min="260" max="260" width="13.453125" style="40" customWidth="1"/>
+    <col min="261" max="261" width="74.6328125" style="40" customWidth="1"/>
+    <col min="262" max="512" width="14.81640625" style="40"/>
+    <col min="513" max="513" width="56.6328125" style="40" bestFit="1" customWidth="1"/>
+    <col min="514" max="514" width="33.6328125" style="40" customWidth="1"/>
+    <col min="515" max="515" width="14.6328125" style="40" customWidth="1"/>
+    <col min="516" max="516" width="13.453125" style="40" customWidth="1"/>
+    <col min="517" max="517" width="74.6328125" style="40" customWidth="1"/>
+    <col min="518" max="768" width="14.81640625" style="40"/>
+    <col min="769" max="769" width="56.6328125" style="40" bestFit="1" customWidth="1"/>
+    <col min="770" max="770" width="33.6328125" style="40" customWidth="1"/>
+    <col min="771" max="771" width="14.6328125" style="40" customWidth="1"/>
+    <col min="772" max="772" width="13.453125" style="40" customWidth="1"/>
+    <col min="773" max="773" width="74.6328125" style="40" customWidth="1"/>
+    <col min="774" max="1024" width="14.81640625" style="40"/>
+    <col min="1025" max="1025" width="56.6328125" style="40" bestFit="1" customWidth="1"/>
+    <col min="1026" max="1026" width="33.6328125" style="40" customWidth="1"/>
+    <col min="1027" max="1027" width="14.6328125" style="40" customWidth="1"/>
+    <col min="1028" max="1028" width="13.453125" style="40" customWidth="1"/>
+    <col min="1029" max="1029" width="74.6328125" style="40" customWidth="1"/>
+    <col min="1030" max="1280" width="14.81640625" style="40"/>
+    <col min="1281" max="1281" width="56.6328125" style="40" bestFit="1" customWidth="1"/>
+    <col min="1282" max="1282" width="33.6328125" style="40" customWidth="1"/>
+    <col min="1283" max="1283" width="14.6328125" style="40" customWidth="1"/>
+    <col min="1284" max="1284" width="13.453125" style="40" customWidth="1"/>
+    <col min="1285" max="1285" width="74.6328125" style="40" customWidth="1"/>
+    <col min="1286" max="1536" width="14.81640625" style="40"/>
+    <col min="1537" max="1537" width="56.6328125" style="40" bestFit="1" customWidth="1"/>
+    <col min="1538" max="1538" width="33.6328125" style="40" customWidth="1"/>
+    <col min="1539" max="1539" width="14.6328125" style="40" customWidth="1"/>
+    <col min="1540" max="1540" width="13.453125" style="40" customWidth="1"/>
+    <col min="1541" max="1541" width="74.6328125" style="40" customWidth="1"/>
+    <col min="1542" max="1792" width="14.81640625" style="40"/>
+    <col min="1793" max="1793" width="56.6328125" style="40" bestFit="1" customWidth="1"/>
+    <col min="1794" max="1794" width="33.6328125" style="40" customWidth="1"/>
+    <col min="1795" max="1795" width="14.6328125" style="40" customWidth="1"/>
+    <col min="1796" max="1796" width="13.453125" style="40" customWidth="1"/>
+    <col min="1797" max="1797" width="74.6328125" style="40" customWidth="1"/>
+    <col min="1798" max="2048" width="14.81640625" style="40"/>
+    <col min="2049" max="2049" width="56.6328125" style="40" bestFit="1" customWidth="1"/>
+    <col min="2050" max="2050" width="33.6328125" style="40" customWidth="1"/>
+    <col min="2051" max="2051" width="14.6328125" style="40" customWidth="1"/>
+    <col min="2052" max="2052" width="13.453125" style="40" customWidth="1"/>
+    <col min="2053" max="2053" width="74.6328125" style="40" customWidth="1"/>
+    <col min="2054" max="2304" width="14.81640625" style="40"/>
+    <col min="2305" max="2305" width="56.6328125" style="40" bestFit="1" customWidth="1"/>
+    <col min="2306" max="2306" width="33.6328125" style="40" customWidth="1"/>
+    <col min="2307" max="2307" width="14.6328125" style="40" customWidth="1"/>
+    <col min="2308" max="2308" width="13.453125" style="40" customWidth="1"/>
+    <col min="2309" max="2309" width="74.6328125" style="40" customWidth="1"/>
+    <col min="2310" max="2560" width="14.81640625" style="40"/>
+    <col min="2561" max="2561" width="56.6328125" style="40" bestFit="1" customWidth="1"/>
+    <col min="2562" max="2562" width="33.6328125" style="40" customWidth="1"/>
+    <col min="2563" max="2563" width="14.6328125" style="40" customWidth="1"/>
+    <col min="2564" max="2564" width="13.453125" style="40" customWidth="1"/>
+    <col min="2565" max="2565" width="74.6328125" style="40" customWidth="1"/>
+    <col min="2566" max="2816" width="14.81640625" style="40"/>
+    <col min="2817" max="2817" width="56.6328125" style="40" bestFit="1" customWidth="1"/>
+    <col min="2818" max="2818" width="33.6328125" style="40" customWidth="1"/>
+    <col min="2819" max="2819" width="14.6328125" style="40" customWidth="1"/>
+    <col min="2820" max="2820" width="13.453125" style="40" customWidth="1"/>
+    <col min="2821" max="2821" width="74.6328125" style="40" customWidth="1"/>
+    <col min="2822" max="3072" width="14.81640625" style="40"/>
+    <col min="3073" max="3073" width="56.6328125" style="40" bestFit="1" customWidth="1"/>
+    <col min="3074" max="3074" width="33.6328125" style="40" customWidth="1"/>
+    <col min="3075" max="3075" width="14.6328125" style="40" customWidth="1"/>
+    <col min="3076" max="3076" width="13.453125" style="40" customWidth="1"/>
+    <col min="3077" max="3077" width="74.6328125" style="40" customWidth="1"/>
+    <col min="3078" max="3328" width="14.81640625" style="40"/>
+    <col min="3329" max="3329" width="56.6328125" style="40" bestFit="1" customWidth="1"/>
+    <col min="3330" max="3330" width="33.6328125" style="40" customWidth="1"/>
+    <col min="3331" max="3331" width="14.6328125" style="40" customWidth="1"/>
+    <col min="3332" max="3332" width="13.453125" style="40" customWidth="1"/>
+    <col min="3333" max="3333" width="74.6328125" style="40" customWidth="1"/>
+    <col min="3334" max="3584" width="14.81640625" style="40"/>
+    <col min="3585" max="3585" width="56.6328125" style="40" bestFit="1" customWidth="1"/>
+    <col min="3586" max="3586" width="33.6328125" style="40" customWidth="1"/>
+    <col min="3587" max="3587" width="14.6328125" style="40" customWidth="1"/>
+    <col min="3588" max="3588" width="13.453125" style="40" customWidth="1"/>
+    <col min="3589" max="3589" width="74.6328125" style="40" customWidth="1"/>
+    <col min="3590" max="3840" width="14.81640625" style="40"/>
+    <col min="3841" max="3841" width="56.6328125" style="40" bestFit="1" customWidth="1"/>
+    <col min="3842" max="3842" width="33.6328125" style="40" customWidth="1"/>
+    <col min="3843" max="3843" width="14.6328125" style="40" customWidth="1"/>
+    <col min="3844" max="3844" width="13.453125" style="40" customWidth="1"/>
+    <col min="3845" max="3845" width="74.6328125" style="40" customWidth="1"/>
+    <col min="3846" max="4096" width="14.81640625" style="40"/>
+    <col min="4097" max="4097" width="56.6328125" style="40" bestFit="1" customWidth="1"/>
+    <col min="4098" max="4098" width="33.6328125" style="40" customWidth="1"/>
+    <col min="4099" max="4099" width="14.6328125" style="40" customWidth="1"/>
+    <col min="4100" max="4100" width="13.453125" style="40" customWidth="1"/>
+    <col min="4101" max="4101" width="74.6328125" style="40" customWidth="1"/>
+    <col min="4102" max="4352" width="14.81640625" style="40"/>
+    <col min="4353" max="4353" width="56.6328125" style="40" bestFit="1" customWidth="1"/>
+    <col min="4354" max="4354" width="33.6328125" style="40" customWidth="1"/>
+    <col min="4355" max="4355" width="14.6328125" style="40" customWidth="1"/>
+    <col min="4356" max="4356" width="13.453125" style="40" customWidth="1"/>
+    <col min="4357" max="4357" width="74.6328125" style="40" customWidth="1"/>
+    <col min="4358" max="4608" width="14.81640625" style="40"/>
+    <col min="4609" max="4609" width="56.6328125" style="40" bestFit="1" customWidth="1"/>
+    <col min="4610" max="4610" width="33.6328125" style="40" customWidth="1"/>
+    <col min="4611" max="4611" width="14.6328125" style="40" customWidth="1"/>
+    <col min="4612" max="4612" width="13.453125" style="40" customWidth="1"/>
+    <col min="4613" max="4613" width="74.6328125" style="40" customWidth="1"/>
+    <col min="4614" max="4864" width="14.81640625" style="40"/>
+    <col min="4865" max="4865" width="56.6328125" style="40" bestFit="1" customWidth="1"/>
+    <col min="4866" max="4866" width="33.6328125" style="40" customWidth="1"/>
+    <col min="4867" max="4867" width="14.6328125" style="40" customWidth="1"/>
+    <col min="4868" max="4868" width="13.453125" style="40" customWidth="1"/>
+    <col min="4869" max="4869" width="74.6328125" style="40" customWidth="1"/>
+    <col min="4870" max="5120" width="14.81640625" style="40"/>
+    <col min="5121" max="5121" width="56.6328125" style="40" bestFit="1" customWidth="1"/>
+    <col min="5122" max="5122" width="33.6328125" style="40" customWidth="1"/>
+    <col min="5123" max="5123" width="14.6328125" style="40" customWidth="1"/>
+    <col min="5124" max="5124" width="13.453125" style="40" customWidth="1"/>
+    <col min="5125" max="5125" width="74.6328125" style="40" customWidth="1"/>
+    <col min="5126" max="5376" width="14.81640625" style="40"/>
+    <col min="5377" max="5377" width="56.6328125" style="40" bestFit="1" customWidth="1"/>
+    <col min="5378" max="5378" width="33.6328125" style="40" customWidth="1"/>
+    <col min="5379" max="5379" width="14.6328125" style="40" customWidth="1"/>
+    <col min="5380" max="5380" width="13.453125" style="40" customWidth="1"/>
+    <col min="5381" max="5381" width="74.6328125" style="40" customWidth="1"/>
+    <col min="5382" max="5632" width="14.81640625" style="40"/>
+    <col min="5633" max="5633" width="56.6328125" style="40" bestFit="1" customWidth="1"/>
+    <col min="5634" max="5634" width="33.6328125" style="40" customWidth="1"/>
+    <col min="5635" max="5635" width="14.6328125" style="40" customWidth="1"/>
+    <col min="5636" max="5636" width="13.453125" style="40" customWidth="1"/>
+    <col min="5637" max="5637" width="74.6328125" style="40" customWidth="1"/>
+    <col min="5638" max="5888" width="14.81640625" style="40"/>
+    <col min="5889" max="5889" width="56.6328125" style="40" bestFit="1" customWidth="1"/>
+    <col min="5890" max="5890" width="33.6328125" style="40" customWidth="1"/>
+    <col min="5891" max="5891" width="14.6328125" style="40" customWidth="1"/>
+    <col min="5892" max="5892" width="13.453125" style="40" customWidth="1"/>
+    <col min="5893" max="5893" width="74.6328125" style="40" customWidth="1"/>
+    <col min="5894" max="6144" width="14.81640625" style="40"/>
+    <col min="6145" max="6145" width="56.6328125" style="40" bestFit="1" customWidth="1"/>
+    <col min="6146" max="6146" width="33.6328125" style="40" customWidth="1"/>
+    <col min="6147" max="6147" width="14.6328125" style="40" customWidth="1"/>
+    <col min="6148" max="6148" width="13.453125" style="40" customWidth="1"/>
+    <col min="6149" max="6149" width="74.6328125" style="40" customWidth="1"/>
+    <col min="6150" max="6400" width="14.81640625" style="40"/>
+    <col min="6401" max="6401" width="56.6328125" style="40" bestFit="1" customWidth="1"/>
+    <col min="6402" max="6402" width="33.6328125" style="40" customWidth="1"/>
+    <col min="6403" max="6403" width="14.6328125" style="40" customWidth="1"/>
+    <col min="6404" max="6404" width="13.453125" style="40" customWidth="1"/>
+    <col min="6405" max="6405" width="74.6328125" style="40" customWidth="1"/>
+    <col min="6406" max="6656" width="14.81640625" style="40"/>
+    <col min="6657" max="6657" width="56.6328125" style="40" bestFit="1" customWidth="1"/>
+    <col min="6658" max="6658" width="33.6328125" style="40" customWidth="1"/>
+    <col min="6659" max="6659" width="14.6328125" style="40" customWidth="1"/>
+    <col min="6660" max="6660" width="13.453125" style="40" customWidth="1"/>
+    <col min="6661" max="6661" width="74.6328125" style="40" customWidth="1"/>
+    <col min="6662" max="6912" width="14.81640625" style="40"/>
+    <col min="6913" max="6913" width="56.6328125" style="40" bestFit="1" customWidth="1"/>
+    <col min="6914" max="6914" width="33.6328125" style="40" customWidth="1"/>
+    <col min="6915" max="6915" width="14.6328125" style="40" customWidth="1"/>
+    <col min="6916" max="6916" width="13.453125" style="40" customWidth="1"/>
+    <col min="6917" max="6917" width="74.6328125" style="40" customWidth="1"/>
+    <col min="6918" max="7168" width="14.81640625" style="40"/>
+    <col min="7169" max="7169" width="56.6328125" style="40" bestFit="1" customWidth="1"/>
+    <col min="7170" max="7170" width="33.6328125" style="40" customWidth="1"/>
+    <col min="7171" max="7171" width="14.6328125" style="40" customWidth="1"/>
+    <col min="7172" max="7172" width="13.453125" style="40" customWidth="1"/>
+    <col min="7173" max="7173" width="74.6328125" style="40" customWidth="1"/>
+    <col min="7174" max="7424" width="14.81640625" style="40"/>
+    <col min="7425" max="7425" width="56.6328125" style="40" bestFit="1" customWidth="1"/>
+    <col min="7426" max="7426" width="33.6328125" style="40" customWidth="1"/>
+    <col min="7427" max="7427" width="14.6328125" style="40" customWidth="1"/>
+    <col min="7428" max="7428" width="13.453125" style="40" customWidth="1"/>
+    <col min="7429" max="7429" width="74.6328125" style="40" customWidth="1"/>
+    <col min="7430" max="7680" width="14.81640625" style="40"/>
+    <col min="7681" max="7681" width="56.6328125" style="40" bestFit="1" customWidth="1"/>
+    <col min="7682" max="7682" width="33.6328125" style="40" customWidth="1"/>
+    <col min="7683" max="7683" width="14.6328125" style="40" customWidth="1"/>
+    <col min="7684" max="7684" width="13.453125" style="40" customWidth="1"/>
+    <col min="7685" max="7685" width="74.6328125" style="40" customWidth="1"/>
+    <col min="7686" max="7936" width="14.81640625" style="40"/>
+    <col min="7937" max="7937" width="56.6328125" style="40" bestFit="1" customWidth="1"/>
+    <col min="7938" max="7938" width="33.6328125" style="40" customWidth="1"/>
+    <col min="7939" max="7939" width="14.6328125" style="40" customWidth="1"/>
+    <col min="7940" max="7940" width="13.453125" style="40" customWidth="1"/>
+    <col min="7941" max="7941" width="74.6328125" style="40" customWidth="1"/>
+    <col min="7942" max="8192" width="14.81640625" style="40"/>
+    <col min="8193" max="8193" width="56.6328125" style="40" bestFit="1" customWidth="1"/>
+    <col min="8194" max="8194" width="33.6328125" style="40" customWidth="1"/>
+    <col min="8195" max="8195" width="14.6328125" style="40" customWidth="1"/>
+    <col min="8196" max="8196" width="13.453125" style="40" customWidth="1"/>
+    <col min="8197" max="8197" width="74.6328125" style="40" customWidth="1"/>
+    <col min="8198" max="8448" width="14.81640625" style="40"/>
+    <col min="8449" max="8449" width="56.6328125" style="40" bestFit="1" customWidth="1"/>
+    <col min="8450" max="8450" width="33.6328125" style="40" customWidth="1"/>
+    <col min="8451" max="8451" width="14.6328125" style="40" customWidth="1"/>
+    <col min="8452" max="8452" width="13.453125" style="40" customWidth="1"/>
+    <col min="8453" max="8453" width="74.6328125" style="40" customWidth="1"/>
+    <col min="8454" max="8704" width="14.81640625" style="40"/>
+    <col min="8705" max="8705" width="56.6328125" style="40" bestFit="1" customWidth="1"/>
+    <col min="8706" max="8706" width="33.6328125" style="40" customWidth="1"/>
+    <col min="8707" max="8707" width="14.6328125" style="40" customWidth="1"/>
+    <col min="8708" max="8708" width="13.453125" style="40" customWidth="1"/>
+    <col min="8709" max="8709" width="74.6328125" style="40" customWidth="1"/>
+    <col min="8710" max="8960" width="14.81640625" style="40"/>
+    <col min="8961" max="8961" width="56.6328125" style="40" bestFit="1" customWidth="1"/>
+    <col min="8962" max="8962" width="33.6328125" style="40" customWidth="1"/>
+    <col min="8963" max="8963" width="14.6328125" style="40" customWidth="1"/>
+    <col min="8964" max="8964" width="13.453125" style="40" customWidth="1"/>
+    <col min="8965" max="8965" width="74.6328125" style="40" customWidth="1"/>
+    <col min="8966" max="9216" width="14.81640625" style="40"/>
+    <col min="9217" max="9217" width="56.6328125" style="40" bestFit="1" customWidth="1"/>
+    <col min="9218" max="9218" width="33.6328125" style="40" customWidth="1"/>
+    <col min="9219" max="9219" width="14.6328125" style="40" customWidth="1"/>
+    <col min="9220" max="9220" width="13.453125" style="40" customWidth="1"/>
+    <col min="9221" max="9221" width="74.6328125" style="40" customWidth="1"/>
+    <col min="9222" max="9472" width="14.81640625" style="40"/>
+    <col min="9473" max="9473" width="56.6328125" style="40" bestFit="1" customWidth="1"/>
+    <col min="9474" max="9474" width="33.6328125" style="40" customWidth="1"/>
+    <col min="9475" max="9475" width="14.6328125" style="40" customWidth="1"/>
+    <col min="9476" max="9476" width="13.453125" style="40" customWidth="1"/>
+    <col min="9477" max="9477" width="74.6328125" style="40" customWidth="1"/>
+    <col min="9478" max="9728" width="14.81640625" style="40"/>
+    <col min="9729" max="9729" width="56.6328125" style="40" bestFit="1" customWidth="1"/>
+    <col min="9730" max="9730" width="33.6328125" style="40" customWidth="1"/>
+    <col min="9731" max="9731" width="14.6328125" style="40" customWidth="1"/>
+    <col min="9732" max="9732" width="13.453125" style="40" customWidth="1"/>
+    <col min="9733" max="9733" width="74.6328125" style="40" customWidth="1"/>
+    <col min="9734" max="9984" width="14.81640625" style="40"/>
+    <col min="9985" max="9985" width="56.6328125" style="40" bestFit="1" customWidth="1"/>
+    <col min="9986" max="9986" width="33.6328125" style="40" customWidth="1"/>
+    <col min="9987" max="9987" width="14.6328125" style="40" customWidth="1"/>
+    <col min="9988" max="9988" width="13.453125" style="40" customWidth="1"/>
+    <col min="9989" max="9989" width="74.6328125" style="40" customWidth="1"/>
+    <col min="9990" max="10240" width="14.81640625" style="40"/>
+    <col min="10241" max="10241" width="56.6328125" style="40" bestFit="1" customWidth="1"/>
+    <col min="10242" max="10242" width="33.6328125" style="40" customWidth="1"/>
+    <col min="10243" max="10243" width="14.6328125" style="40" customWidth="1"/>
+    <col min="10244" max="10244" width="13.453125" style="40" customWidth="1"/>
+    <col min="10245" max="10245" width="74.6328125" style="40" customWidth="1"/>
+    <col min="10246" max="10496" width="14.81640625" style="40"/>
+    <col min="10497" max="10497" width="56.6328125" style="40" bestFit="1" customWidth="1"/>
+    <col min="10498" max="10498" width="33.6328125" style="40" customWidth="1"/>
+    <col min="10499" max="10499" width="14.6328125" style="40" customWidth="1"/>
+    <col min="10500" max="10500" width="13.453125" style="40" customWidth="1"/>
+    <col min="10501" max="10501" width="74.6328125" style="40" customWidth="1"/>
+    <col min="10502" max="10752" width="14.81640625" style="40"/>
+    <col min="10753" max="10753" width="56.6328125" style="40" bestFit="1" customWidth="1"/>
+    <col min="10754" max="10754" width="33.6328125" style="40" customWidth="1"/>
+    <col min="10755" max="10755" width="14.6328125" style="40" customWidth="1"/>
+    <col min="10756" max="10756" width="13.453125" style="40" customWidth="1"/>
+    <col min="10757" max="10757" width="74.6328125" style="40" customWidth="1"/>
+    <col min="10758" max="11008" width="14.81640625" style="40"/>
+    <col min="11009" max="11009" width="56.6328125" style="40" bestFit="1" customWidth="1"/>
+    <col min="11010" max="11010" width="33.6328125" style="40" customWidth="1"/>
+    <col min="11011" max="11011" width="14.6328125" style="40" customWidth="1"/>
+    <col min="11012" max="11012" width="13.453125" style="40" customWidth="1"/>
+    <col min="11013" max="11013" width="74.6328125" style="40" customWidth="1"/>
+    <col min="11014" max="11264" width="14.81640625" style="40"/>
+    <col min="11265" max="11265" width="56.6328125" style="40" bestFit="1" customWidth="1"/>
+    <col min="11266" max="11266" width="33.6328125" style="40" customWidth="1"/>
+    <col min="11267" max="11267" width="14.6328125" style="40" customWidth="1"/>
+    <col min="11268" max="11268" width="13.453125" style="40" customWidth="1"/>
+    <col min="11269" max="11269" width="74.6328125" style="40" customWidth="1"/>
+    <col min="11270" max="11520" width="14.81640625" style="40"/>
+    <col min="11521" max="11521" width="56.6328125" style="40" bestFit="1" customWidth="1"/>
+    <col min="11522" max="11522" width="33.6328125" style="40" customWidth="1"/>
+    <col min="11523" max="11523" width="14.6328125" style="40" customWidth="1"/>
+    <col min="11524" max="11524" width="13.453125" style="40" customWidth="1"/>
+    <col min="11525" max="11525" width="74.6328125" style="40" customWidth="1"/>
+    <col min="11526" max="11776" width="14.81640625" style="40"/>
+    <col min="11777" max="11777" width="56.6328125" style="40" bestFit="1" customWidth="1"/>
+    <col min="11778" max="11778" width="33.6328125" style="40" customWidth="1"/>
+    <col min="11779" max="11779" width="14.6328125" style="40" customWidth="1"/>
+    <col min="11780" max="11780" width="13.453125" style="40" customWidth="1"/>
+    <col min="11781" max="11781" width="74.6328125" style="40" customWidth="1"/>
+    <col min="11782" max="12032" width="14.81640625" style="40"/>
+    <col min="12033" max="12033" width="56.6328125" style="40" bestFit="1" customWidth="1"/>
+    <col min="12034" max="12034" width="33.6328125" style="40" customWidth="1"/>
+    <col min="12035" max="12035" width="14.6328125" style="40" customWidth="1"/>
+    <col min="12036" max="12036" width="13.453125" style="40" customWidth="1"/>
+    <col min="12037" max="12037" width="74.6328125" style="40" customWidth="1"/>
+    <col min="12038" max="12288" width="14.81640625" style="40"/>
+    <col min="12289" max="12289" width="56.6328125" style="40" bestFit="1" customWidth="1"/>
+    <col min="12290" max="12290" width="33.6328125" style="40" customWidth="1"/>
+    <col min="12291" max="12291" width="14.6328125" style="40" customWidth="1"/>
+    <col min="12292" max="12292" width="13.453125" style="40" customWidth="1"/>
+    <col min="12293" max="12293" width="74.6328125" style="40" customWidth="1"/>
+    <col min="12294" max="12544" width="14.81640625" style="40"/>
+    <col min="12545" max="12545" width="56.6328125" style="40" bestFit="1" customWidth="1"/>
+    <col min="12546" max="12546" width="33.6328125" style="40" customWidth="1"/>
+    <col min="12547" max="12547" width="14.6328125" style="40" customWidth="1"/>
+    <col min="12548" max="12548" width="13.453125" style="40" customWidth="1"/>
+    <col min="12549" max="12549" width="74.6328125" style="40" customWidth="1"/>
+    <col min="12550" max="12800" width="14.81640625" style="40"/>
+    <col min="12801" max="12801" width="56.6328125" style="40" bestFit="1" customWidth="1"/>
+    <col min="12802" max="12802" width="33.6328125" style="40" customWidth="1"/>
+    <col min="12803" max="12803" width="14.6328125" style="40" customWidth="1"/>
+    <col min="12804" max="12804" width="13.453125" style="40" customWidth="1"/>
+    <col min="12805" max="12805" width="74.6328125" style="40" customWidth="1"/>
+    <col min="12806" max="13056" width="14.81640625" style="40"/>
+    <col min="13057" max="13057" width="56.6328125" style="40" bestFit="1" customWidth="1"/>
+    <col min="13058" max="13058" width="33.6328125" style="40" customWidth="1"/>
+    <col min="13059" max="13059" width="14.6328125" style="40" customWidth="1"/>
+    <col min="13060" max="13060" width="13.453125" style="40" customWidth="1"/>
+    <col min="13061" max="13061" width="74.6328125" style="40" customWidth="1"/>
+    <col min="13062" max="13312" width="14.81640625" style="40"/>
+    <col min="13313" max="13313" width="56.6328125" style="40" bestFit="1" customWidth="1"/>
+    <col min="13314" max="13314" width="33.6328125" style="40" customWidth="1"/>
+    <col min="13315" max="13315" width="14.6328125" style="40" customWidth="1"/>
+    <col min="13316" max="13316" width="13.453125" style="40" customWidth="1"/>
+    <col min="13317" max="13317" width="74.6328125" style="40" customWidth="1"/>
+    <col min="13318" max="13568" width="14.81640625" style="40"/>
+    <col min="13569" max="13569" width="56.6328125" style="40" bestFit="1" customWidth="1"/>
+    <col min="13570" max="13570" width="33.6328125" style="40" customWidth="1"/>
+    <col min="13571" max="13571" width="14.6328125" style="40" customWidth="1"/>
+    <col min="13572" max="13572" width="13.453125" style="40" customWidth="1"/>
+    <col min="13573" max="13573" width="74.6328125" style="40" customWidth="1"/>
+    <col min="13574" max="13824" width="14.81640625" style="40"/>
+    <col min="13825" max="13825" width="56.6328125" style="40" bestFit="1" customWidth="1"/>
+    <col min="13826" max="13826" width="33.6328125" style="40" customWidth="1"/>
+    <col min="13827" max="13827" width="14.6328125" style="40" customWidth="1"/>
+    <col min="13828" max="13828" width="13.453125" style="40" customWidth="1"/>
+    <col min="13829" max="13829" width="74.6328125" style="40" customWidth="1"/>
+    <col min="13830" max="14080" width="14.81640625" style="40"/>
+    <col min="14081" max="14081" width="56.6328125" style="40" bestFit="1" customWidth="1"/>
+    <col min="14082" max="14082" width="33.6328125" style="40" customWidth="1"/>
+    <col min="14083" max="14083" width="14.6328125" style="40" customWidth="1"/>
+    <col min="14084" max="14084" width="13.453125" style="40" customWidth="1"/>
+    <col min="14085" max="14085" width="74.6328125" style="40" customWidth="1"/>
+    <col min="14086" max="14336" width="14.81640625" style="40"/>
+    <col min="14337" max="14337" width="56.6328125" style="40" bestFit="1" customWidth="1"/>
+    <col min="14338" max="14338" width="33.6328125" style="40" customWidth="1"/>
+    <col min="14339" max="14339" width="14.6328125" style="40" customWidth="1"/>
+    <col min="14340" max="14340" width="13.453125" style="40" customWidth="1"/>
+    <col min="14341" max="14341" width="74.6328125" style="40" customWidth="1"/>
+    <col min="14342" max="14592" width="14.81640625" style="40"/>
+    <col min="14593" max="14593" width="56.6328125" style="40" bestFit="1" customWidth="1"/>
+    <col min="14594" max="14594" width="33.6328125" style="40" customWidth="1"/>
+    <col min="14595" max="14595" width="14.6328125" style="40" customWidth="1"/>
+    <col min="14596" max="14596" width="13.453125" style="40" customWidth="1"/>
+    <col min="14597" max="14597" width="74.6328125" style="40" customWidth="1"/>
+    <col min="14598" max="14848" width="14.81640625" style="40"/>
+    <col min="14849" max="14849" width="56.6328125" style="40" bestFit="1" customWidth="1"/>
+    <col min="14850" max="14850" width="33.6328125" style="40" customWidth="1"/>
+    <col min="14851" max="14851" width="14.6328125" style="40" customWidth="1"/>
+    <col min="14852" max="14852" width="13.453125" style="40" customWidth="1"/>
+    <col min="14853" max="14853" width="74.6328125" style="40" customWidth="1"/>
+    <col min="14854" max="15104" width="14.81640625" style="40"/>
+    <col min="15105" max="15105" width="56.6328125" style="40" bestFit="1" customWidth="1"/>
+    <col min="15106" max="15106" width="33.6328125" style="40" customWidth="1"/>
+    <col min="15107" max="15107" width="14.6328125" style="40" customWidth="1"/>
+    <col min="15108" max="15108" width="13.453125" style="40" customWidth="1"/>
+    <col min="15109" max="15109" width="74.6328125" style="40" customWidth="1"/>
+    <col min="15110" max="15360" width="14.81640625" style="40"/>
+    <col min="15361" max="15361" width="56.6328125" style="40" bestFit="1" customWidth="1"/>
+    <col min="15362" max="15362" width="33.6328125" style="40" customWidth="1"/>
+    <col min="15363" max="15363" width="14.6328125" style="40" customWidth="1"/>
+    <col min="15364" max="15364" width="13.453125" style="40" customWidth="1"/>
+    <col min="15365" max="15365" width="74.6328125" style="40" customWidth="1"/>
+    <col min="15366" max="15616" width="14.81640625" style="40"/>
+    <col min="15617" max="15617" width="56.6328125" style="40" bestFit="1" customWidth="1"/>
+    <col min="15618" max="15618" width="33.6328125" style="40" customWidth="1"/>
+    <col min="15619" max="15619" width="14.6328125" style="40" customWidth="1"/>
+    <col min="15620" max="15620" width="13.453125" style="40" customWidth="1"/>
+    <col min="15621" max="15621" width="74.6328125" style="40" customWidth="1"/>
+    <col min="15622" max="15872" width="14.81640625" style="40"/>
+    <col min="15873" max="15873" width="56.6328125" style="40" bestFit="1" customWidth="1"/>
+    <col min="15874" max="15874" width="33.6328125" style="40" customWidth="1"/>
+    <col min="15875" max="15875" width="14.6328125" style="40" customWidth="1"/>
+    <col min="15876" max="15876" width="13.453125" style="40" customWidth="1"/>
+    <col min="15877" max="15877" width="74.6328125" style="40" customWidth="1"/>
+    <col min="15878" max="16128" width="14.81640625" style="40"/>
+    <col min="16129" max="16129" width="56.6328125" style="40" bestFit="1" customWidth="1"/>
+    <col min="16130" max="16130" width="33.6328125" style="40" customWidth="1"/>
+    <col min="16131" max="16131" width="14.6328125" style="40" customWidth="1"/>
+    <col min="16132" max="16132" width="13.453125" style="40" customWidth="1"/>
+    <col min="16133" max="16133" width="74.6328125" style="40" customWidth="1"/>
+    <col min="16134" max="16384" width="14.81640625" style="40"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" s="2" customFormat="1" ht="40.200000000000003" customHeight="1" thickBot="1">
-      <c r="A1" s="93"/>
-      <c r="B1" s="94"/>
-      <c r="C1" s="94"/>
-      <c r="D1" s="94"/>
-      <c r="E1" s="94"/>
-    </row>
-    <row r="2" spans="1:5" ht="13.95" customHeight="1">
+    <row r="1" spans="1:5" s="2" customFormat="1" ht="40.25" customHeight="1" thickBot="1">
+      <c r="A1" s="108"/>
+      <c r="B1" s="109"/>
+      <c r="C1" s="109"/>
+      <c r="D1" s="109"/>
+      <c r="E1" s="109"/>
+    </row>
+    <row r="2" spans="1:5" ht="14" customHeight="1">
       <c r="A2" s="118" t="s">
         <v>64</v>
       </c>
-      <c r="B2" s="97" t="s">
+      <c r="B2" s="112" t="s">
         <v>65</v>
       </c>
       <c r="C2" s="119" t="s">
@@ -48242,16 +48205,16 @@
       <c r="D2" s="119" t="s">
         <v>67</v>
       </c>
-      <c r="E2" s="97" t="s">
+      <c r="E2" s="112" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="3" spans="1:5" ht="14.4" thickBot="1">
-      <c r="A3" s="96"/>
-      <c r="B3" s="98"/>
-      <c r="C3" s="100"/>
-      <c r="D3" s="100"/>
-      <c r="E3" s="98"/>
+    <row r="3" spans="1:5" ht="14.5" thickBot="1">
+      <c r="A3" s="111"/>
+      <c r="B3" s="113"/>
+      <c r="C3" s="115"/>
+      <c r="D3" s="115"/>
+      <c r="E3" s="113"/>
     </row>
     <row r="4" spans="1:5">
       <c r="A4" s="41" t="s">
@@ -48324,7 +48287,7 @@
         <v>389</v>
       </c>
     </row>
-    <row r="9" spans="1:5" ht="14.4" thickBot="1">
+    <row r="9" spans="1:5" ht="14.5" thickBot="1">
       <c r="A9" s="45" t="s">
         <v>153</v>
       </c>
@@ -48339,7 +48302,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="10" spans="1:5" ht="14.4" thickBot="1">
+    <row r="10" spans="1:5" ht="14.5" thickBot="1">
       <c r="A10" s="5"/>
       <c r="B10" s="5"/>
       <c r="C10" s="6"/>
@@ -48365,7 +48328,7 @@
       <c r="A12" s="49" t="s">
         <v>156</v>
       </c>
-      <c r="B12" s="102"/>
+      <c r="B12" s="101"/>
       <c r="C12" s="10" t="s">
         <v>228</v>
       </c>
@@ -48380,7 +48343,7 @@
       <c r="A13" s="51" t="s">
         <v>151</v>
       </c>
-      <c r="B13" s="102"/>
+      <c r="B13" s="101"/>
       <c r="C13" s="10" t="s">
         <v>229</v>
       </c>
@@ -48417,7 +48380,7 @@
         <v>391</v>
       </c>
     </row>
-    <row r="16" spans="1:5" ht="14.4" thickBot="1">
+    <row r="16" spans="1:5" ht="14.5" thickBot="1">
       <c r="A16" s="54" t="s">
         <v>153</v>
       </c>
@@ -48451,7 +48414,7 @@
       <c r="A18" s="51" t="s">
         <v>156</v>
       </c>
-      <c r="B18" s="102"/>
+      <c r="B18" s="101"/>
       <c r="C18" s="10">
         <v>737261</v>
       </c>
@@ -48466,7 +48429,7 @@
       <c r="A19" s="51" t="s">
         <v>151</v>
       </c>
-      <c r="B19" s="102"/>
+      <c r="B19" s="101"/>
       <c r="C19" s="10">
         <v>737262</v>
       </c>
@@ -48492,11 +48455,11 @@
         <v>162</v>
       </c>
     </row>
-    <row r="21" spans="1:5" ht="14.4" thickBot="1">
+    <row r="21" spans="1:5" ht="14.5" thickBot="1">
       <c r="A21" s="45" t="s">
         <v>153</v>
       </c>
-      <c r="B21" s="103"/>
+      <c r="B21" s="102"/>
       <c r="C21" s="16">
         <v>737263</v>
       </c>
@@ -48507,7 +48470,7 @@
         <v>163</v>
       </c>
     </row>
-    <row r="22" spans="1:5" ht="14.4" thickBot="1">
+    <row r="22" spans="1:5" ht="14.5" thickBot="1">
       <c r="A22" s="58"/>
       <c r="B22" s="59"/>
       <c r="C22" s="60"/>
@@ -48633,7 +48596,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="32" spans="1:5" ht="14.4" thickBot="1">
+    <row r="32" spans="1:5" ht="14.5" thickBot="1">
       <c r="A32" s="127"/>
       <c r="B32" s="130"/>
       <c r="C32" s="14">
@@ -48646,15 +48609,15 @@
         <v>174</v>
       </c>
     </row>
-    <row r="33" spans="1:5" ht="14.4" thickBot="1">
+    <row r="33" spans="1:5" ht="14.5" thickBot="1">
       <c r="A33" s="5"/>
       <c r="B33" s="68"/>
       <c r="C33" s="69"/>
       <c r="D33" s="69"/>
       <c r="E33" s="70"/>
     </row>
-    <row r="34" spans="1:5" ht="39.6" customHeight="1">
-      <c r="A34" s="113" t="s">
+    <row r="34" spans="1:5" ht="39.65" customHeight="1">
+      <c r="A34" s="107" t="s">
         <v>175</v>
       </c>
       <c r="B34" s="116"/>
@@ -48669,7 +48632,7 @@
       </c>
     </row>
     <row r="35" spans="1:5" ht="42" customHeight="1" thickBot="1">
-      <c r="A35" s="106"/>
+      <c r="A35" s="94"/>
       <c r="B35" s="117"/>
       <c r="C35" s="73">
         <v>734493</v>
@@ -48718,345 +48681,345 @@
       <selection activeCell="C17" sqref="C17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.77734375" defaultRowHeight="13.8"/>
+  <sheetFormatPr defaultColWidth="14.81640625" defaultRowHeight="14"/>
   <cols>
-    <col min="1" max="1" width="23.5546875" style="40" customWidth="1"/>
-    <col min="2" max="2" width="33.6640625" style="40" customWidth="1"/>
-    <col min="3" max="4" width="14.77734375" style="40" customWidth="1"/>
-    <col min="5" max="5" width="82.44140625" style="40" customWidth="1"/>
-    <col min="6" max="256" width="14.77734375" style="40"/>
-    <col min="257" max="257" width="23.5546875" style="40" customWidth="1"/>
-    <col min="258" max="258" width="33.6640625" style="40" customWidth="1"/>
-    <col min="259" max="260" width="14.77734375" style="40" customWidth="1"/>
-    <col min="261" max="261" width="82.44140625" style="40" customWidth="1"/>
-    <col min="262" max="512" width="14.77734375" style="40"/>
-    <col min="513" max="513" width="23.5546875" style="40" customWidth="1"/>
-    <col min="514" max="514" width="33.6640625" style="40" customWidth="1"/>
-    <col min="515" max="516" width="14.77734375" style="40" customWidth="1"/>
-    <col min="517" max="517" width="82.44140625" style="40" customWidth="1"/>
-    <col min="518" max="768" width="14.77734375" style="40"/>
-    <col min="769" max="769" width="23.5546875" style="40" customWidth="1"/>
-    <col min="770" max="770" width="33.6640625" style="40" customWidth="1"/>
-    <col min="771" max="772" width="14.77734375" style="40" customWidth="1"/>
-    <col min="773" max="773" width="82.44140625" style="40" customWidth="1"/>
-    <col min="774" max="1024" width="14.77734375" style="40"/>
-    <col min="1025" max="1025" width="23.5546875" style="40" customWidth="1"/>
-    <col min="1026" max="1026" width="33.6640625" style="40" customWidth="1"/>
-    <col min="1027" max="1028" width="14.77734375" style="40" customWidth="1"/>
-    <col min="1029" max="1029" width="82.44140625" style="40" customWidth="1"/>
-    <col min="1030" max="1280" width="14.77734375" style="40"/>
-    <col min="1281" max="1281" width="23.5546875" style="40" customWidth="1"/>
-    <col min="1282" max="1282" width="33.6640625" style="40" customWidth="1"/>
-    <col min="1283" max="1284" width="14.77734375" style="40" customWidth="1"/>
-    <col min="1285" max="1285" width="82.44140625" style="40" customWidth="1"/>
-    <col min="1286" max="1536" width="14.77734375" style="40"/>
-    <col min="1537" max="1537" width="23.5546875" style="40" customWidth="1"/>
-    <col min="1538" max="1538" width="33.6640625" style="40" customWidth="1"/>
-    <col min="1539" max="1540" width="14.77734375" style="40" customWidth="1"/>
-    <col min="1541" max="1541" width="82.44140625" style="40" customWidth="1"/>
-    <col min="1542" max="1792" width="14.77734375" style="40"/>
-    <col min="1793" max="1793" width="23.5546875" style="40" customWidth="1"/>
-    <col min="1794" max="1794" width="33.6640625" style="40" customWidth="1"/>
-    <col min="1795" max="1796" width="14.77734375" style="40" customWidth="1"/>
-    <col min="1797" max="1797" width="82.44140625" style="40" customWidth="1"/>
-    <col min="1798" max="2048" width="14.77734375" style="40"/>
-    <col min="2049" max="2049" width="23.5546875" style="40" customWidth="1"/>
-    <col min="2050" max="2050" width="33.6640625" style="40" customWidth="1"/>
-    <col min="2051" max="2052" width="14.77734375" style="40" customWidth="1"/>
-    <col min="2053" max="2053" width="82.44140625" style="40" customWidth="1"/>
-    <col min="2054" max="2304" width="14.77734375" style="40"/>
-    <col min="2305" max="2305" width="23.5546875" style="40" customWidth="1"/>
-    <col min="2306" max="2306" width="33.6640625" style="40" customWidth="1"/>
-    <col min="2307" max="2308" width="14.77734375" style="40" customWidth="1"/>
-    <col min="2309" max="2309" width="82.44140625" style="40" customWidth="1"/>
-    <col min="2310" max="2560" width="14.77734375" style="40"/>
-    <col min="2561" max="2561" width="23.5546875" style="40" customWidth="1"/>
-    <col min="2562" max="2562" width="33.6640625" style="40" customWidth="1"/>
-    <col min="2563" max="2564" width="14.77734375" style="40" customWidth="1"/>
-    <col min="2565" max="2565" width="82.44140625" style="40" customWidth="1"/>
-    <col min="2566" max="2816" width="14.77734375" style="40"/>
-    <col min="2817" max="2817" width="23.5546875" style="40" customWidth="1"/>
-    <col min="2818" max="2818" width="33.6640625" style="40" customWidth="1"/>
-    <col min="2819" max="2820" width="14.77734375" style="40" customWidth="1"/>
-    <col min="2821" max="2821" width="82.44140625" style="40" customWidth="1"/>
-    <col min="2822" max="3072" width="14.77734375" style="40"/>
-    <col min="3073" max="3073" width="23.5546875" style="40" customWidth="1"/>
-    <col min="3074" max="3074" width="33.6640625" style="40" customWidth="1"/>
-    <col min="3075" max="3076" width="14.77734375" style="40" customWidth="1"/>
-    <col min="3077" max="3077" width="82.44140625" style="40" customWidth="1"/>
-    <col min="3078" max="3328" width="14.77734375" style="40"/>
-    <col min="3329" max="3329" width="23.5546875" style="40" customWidth="1"/>
-    <col min="3330" max="3330" width="33.6640625" style="40" customWidth="1"/>
-    <col min="3331" max="3332" width="14.77734375" style="40" customWidth="1"/>
-    <col min="3333" max="3333" width="82.44140625" style="40" customWidth="1"/>
-    <col min="3334" max="3584" width="14.77734375" style="40"/>
-    <col min="3585" max="3585" width="23.5546875" style="40" customWidth="1"/>
-    <col min="3586" max="3586" width="33.6640625" style="40" customWidth="1"/>
-    <col min="3587" max="3588" width="14.77734375" style="40" customWidth="1"/>
-    <col min="3589" max="3589" width="82.44140625" style="40" customWidth="1"/>
-    <col min="3590" max="3840" width="14.77734375" style="40"/>
-    <col min="3841" max="3841" width="23.5546875" style="40" customWidth="1"/>
-    <col min="3842" max="3842" width="33.6640625" style="40" customWidth="1"/>
-    <col min="3843" max="3844" width="14.77734375" style="40" customWidth="1"/>
-    <col min="3845" max="3845" width="82.44140625" style="40" customWidth="1"/>
-    <col min="3846" max="4096" width="14.77734375" style="40"/>
-    <col min="4097" max="4097" width="23.5546875" style="40" customWidth="1"/>
-    <col min="4098" max="4098" width="33.6640625" style="40" customWidth="1"/>
-    <col min="4099" max="4100" width="14.77734375" style="40" customWidth="1"/>
-    <col min="4101" max="4101" width="82.44140625" style="40" customWidth="1"/>
-    <col min="4102" max="4352" width="14.77734375" style="40"/>
-    <col min="4353" max="4353" width="23.5546875" style="40" customWidth="1"/>
-    <col min="4354" max="4354" width="33.6640625" style="40" customWidth="1"/>
-    <col min="4355" max="4356" width="14.77734375" style="40" customWidth="1"/>
-    <col min="4357" max="4357" width="82.44140625" style="40" customWidth="1"/>
-    <col min="4358" max="4608" width="14.77734375" style="40"/>
-    <col min="4609" max="4609" width="23.5546875" style="40" customWidth="1"/>
-    <col min="4610" max="4610" width="33.6640625" style="40" customWidth="1"/>
-    <col min="4611" max="4612" width="14.77734375" style="40" customWidth="1"/>
-    <col min="4613" max="4613" width="82.44140625" style="40" customWidth="1"/>
-    <col min="4614" max="4864" width="14.77734375" style="40"/>
-    <col min="4865" max="4865" width="23.5546875" style="40" customWidth="1"/>
-    <col min="4866" max="4866" width="33.6640625" style="40" customWidth="1"/>
-    <col min="4867" max="4868" width="14.77734375" style="40" customWidth="1"/>
-    <col min="4869" max="4869" width="82.44140625" style="40" customWidth="1"/>
-    <col min="4870" max="5120" width="14.77734375" style="40"/>
-    <col min="5121" max="5121" width="23.5546875" style="40" customWidth="1"/>
-    <col min="5122" max="5122" width="33.6640625" style="40" customWidth="1"/>
-    <col min="5123" max="5124" width="14.77734375" style="40" customWidth="1"/>
-    <col min="5125" max="5125" width="82.44140625" style="40" customWidth="1"/>
-    <col min="5126" max="5376" width="14.77734375" style="40"/>
-    <col min="5377" max="5377" width="23.5546875" style="40" customWidth="1"/>
-    <col min="5378" max="5378" width="33.6640625" style="40" customWidth="1"/>
-    <col min="5379" max="5380" width="14.77734375" style="40" customWidth="1"/>
-    <col min="5381" max="5381" width="82.44140625" style="40" customWidth="1"/>
-    <col min="5382" max="5632" width="14.77734375" style="40"/>
-    <col min="5633" max="5633" width="23.5546875" style="40" customWidth="1"/>
-    <col min="5634" max="5634" width="33.6640625" style="40" customWidth="1"/>
-    <col min="5635" max="5636" width="14.77734375" style="40" customWidth="1"/>
-    <col min="5637" max="5637" width="82.44140625" style="40" customWidth="1"/>
-    <col min="5638" max="5888" width="14.77734375" style="40"/>
-    <col min="5889" max="5889" width="23.5546875" style="40" customWidth="1"/>
-    <col min="5890" max="5890" width="33.6640625" style="40" customWidth="1"/>
-    <col min="5891" max="5892" width="14.77734375" style="40" customWidth="1"/>
-    <col min="5893" max="5893" width="82.44140625" style="40" customWidth="1"/>
-    <col min="5894" max="6144" width="14.77734375" style="40"/>
-    <col min="6145" max="6145" width="23.5546875" style="40" customWidth="1"/>
-    <col min="6146" max="6146" width="33.6640625" style="40" customWidth="1"/>
-    <col min="6147" max="6148" width="14.77734375" style="40" customWidth="1"/>
-    <col min="6149" max="6149" width="82.44140625" style="40" customWidth="1"/>
-    <col min="6150" max="6400" width="14.77734375" style="40"/>
-    <col min="6401" max="6401" width="23.5546875" style="40" customWidth="1"/>
-    <col min="6402" max="6402" width="33.6640625" style="40" customWidth="1"/>
-    <col min="6403" max="6404" width="14.77734375" style="40" customWidth="1"/>
-    <col min="6405" max="6405" width="82.44140625" style="40" customWidth="1"/>
-    <col min="6406" max="6656" width="14.77734375" style="40"/>
-    <col min="6657" max="6657" width="23.5546875" style="40" customWidth="1"/>
-    <col min="6658" max="6658" width="33.6640625" style="40" customWidth="1"/>
-    <col min="6659" max="6660" width="14.77734375" style="40" customWidth="1"/>
-    <col min="6661" max="6661" width="82.44140625" style="40" customWidth="1"/>
-    <col min="6662" max="6912" width="14.77734375" style="40"/>
-    <col min="6913" max="6913" width="23.5546875" style="40" customWidth="1"/>
-    <col min="6914" max="6914" width="33.6640625" style="40" customWidth="1"/>
-    <col min="6915" max="6916" width="14.77734375" style="40" customWidth="1"/>
-    <col min="6917" max="6917" width="82.44140625" style="40" customWidth="1"/>
-    <col min="6918" max="7168" width="14.77734375" style="40"/>
-    <col min="7169" max="7169" width="23.5546875" style="40" customWidth="1"/>
-    <col min="7170" max="7170" width="33.6640625" style="40" customWidth="1"/>
-    <col min="7171" max="7172" width="14.77734375" style="40" customWidth="1"/>
-    <col min="7173" max="7173" width="82.44140625" style="40" customWidth="1"/>
-    <col min="7174" max="7424" width="14.77734375" style="40"/>
-    <col min="7425" max="7425" width="23.5546875" style="40" customWidth="1"/>
-    <col min="7426" max="7426" width="33.6640625" style="40" customWidth="1"/>
-    <col min="7427" max="7428" width="14.77734375" style="40" customWidth="1"/>
-    <col min="7429" max="7429" width="82.44140625" style="40" customWidth="1"/>
-    <col min="7430" max="7680" width="14.77734375" style="40"/>
-    <col min="7681" max="7681" width="23.5546875" style="40" customWidth="1"/>
-    <col min="7682" max="7682" width="33.6640625" style="40" customWidth="1"/>
-    <col min="7683" max="7684" width="14.77734375" style="40" customWidth="1"/>
-    <col min="7685" max="7685" width="82.44140625" style="40" customWidth="1"/>
-    <col min="7686" max="7936" width="14.77734375" style="40"/>
-    <col min="7937" max="7937" width="23.5546875" style="40" customWidth="1"/>
-    <col min="7938" max="7938" width="33.6640625" style="40" customWidth="1"/>
-    <col min="7939" max="7940" width="14.77734375" style="40" customWidth="1"/>
-    <col min="7941" max="7941" width="82.44140625" style="40" customWidth="1"/>
-    <col min="7942" max="8192" width="14.77734375" style="40"/>
-    <col min="8193" max="8193" width="23.5546875" style="40" customWidth="1"/>
-    <col min="8194" max="8194" width="33.6640625" style="40" customWidth="1"/>
-    <col min="8195" max="8196" width="14.77734375" style="40" customWidth="1"/>
-    <col min="8197" max="8197" width="82.44140625" style="40" customWidth="1"/>
-    <col min="8198" max="8448" width="14.77734375" style="40"/>
-    <col min="8449" max="8449" width="23.5546875" style="40" customWidth="1"/>
-    <col min="8450" max="8450" width="33.6640625" style="40" customWidth="1"/>
-    <col min="8451" max="8452" width="14.77734375" style="40" customWidth="1"/>
-    <col min="8453" max="8453" width="82.44140625" style="40" customWidth="1"/>
-    <col min="8454" max="8704" width="14.77734375" style="40"/>
-    <col min="8705" max="8705" width="23.5546875" style="40" customWidth="1"/>
-    <col min="8706" max="8706" width="33.6640625" style="40" customWidth="1"/>
-    <col min="8707" max="8708" width="14.77734375" style="40" customWidth="1"/>
-    <col min="8709" max="8709" width="82.44140625" style="40" customWidth="1"/>
-    <col min="8710" max="8960" width="14.77734375" style="40"/>
-    <col min="8961" max="8961" width="23.5546875" style="40" customWidth="1"/>
-    <col min="8962" max="8962" width="33.6640625" style="40" customWidth="1"/>
-    <col min="8963" max="8964" width="14.77734375" style="40" customWidth="1"/>
-    <col min="8965" max="8965" width="82.44140625" style="40" customWidth="1"/>
-    <col min="8966" max="9216" width="14.77734375" style="40"/>
-    <col min="9217" max="9217" width="23.5546875" style="40" customWidth="1"/>
-    <col min="9218" max="9218" width="33.6640625" style="40" customWidth="1"/>
-    <col min="9219" max="9220" width="14.77734375" style="40" customWidth="1"/>
-    <col min="9221" max="9221" width="82.44140625" style="40" customWidth="1"/>
-    <col min="9222" max="9472" width="14.77734375" style="40"/>
-    <col min="9473" max="9473" width="23.5546875" style="40" customWidth="1"/>
-    <col min="9474" max="9474" width="33.6640625" style="40" customWidth="1"/>
-    <col min="9475" max="9476" width="14.77734375" style="40" customWidth="1"/>
-    <col min="9477" max="9477" width="82.44140625" style="40" customWidth="1"/>
-    <col min="9478" max="9728" width="14.77734375" style="40"/>
-    <col min="9729" max="9729" width="23.5546875" style="40" customWidth="1"/>
-    <col min="9730" max="9730" width="33.6640625" style="40" customWidth="1"/>
-    <col min="9731" max="9732" width="14.77734375" style="40" customWidth="1"/>
-    <col min="9733" max="9733" width="82.44140625" style="40" customWidth="1"/>
-    <col min="9734" max="9984" width="14.77734375" style="40"/>
-    <col min="9985" max="9985" width="23.5546875" style="40" customWidth="1"/>
-    <col min="9986" max="9986" width="33.6640625" style="40" customWidth="1"/>
-    <col min="9987" max="9988" width="14.77734375" style="40" customWidth="1"/>
-    <col min="9989" max="9989" width="82.44140625" style="40" customWidth="1"/>
-    <col min="9990" max="10240" width="14.77734375" style="40"/>
-    <col min="10241" max="10241" width="23.5546875" style="40" customWidth="1"/>
-    <col min="10242" max="10242" width="33.6640625" style="40" customWidth="1"/>
-    <col min="10243" max="10244" width="14.77734375" style="40" customWidth="1"/>
-    <col min="10245" max="10245" width="82.44140625" style="40" customWidth="1"/>
-    <col min="10246" max="10496" width="14.77734375" style="40"/>
-    <col min="10497" max="10497" width="23.5546875" style="40" customWidth="1"/>
-    <col min="10498" max="10498" width="33.6640625" style="40" customWidth="1"/>
-    <col min="10499" max="10500" width="14.77734375" style="40" customWidth="1"/>
-    <col min="10501" max="10501" width="82.44140625" style="40" customWidth="1"/>
-    <col min="10502" max="10752" width="14.77734375" style="40"/>
-    <col min="10753" max="10753" width="23.5546875" style="40" customWidth="1"/>
-    <col min="10754" max="10754" width="33.6640625" style="40" customWidth="1"/>
-    <col min="10755" max="10756" width="14.77734375" style="40" customWidth="1"/>
-    <col min="10757" max="10757" width="82.44140625" style="40" customWidth="1"/>
-    <col min="10758" max="11008" width="14.77734375" style="40"/>
-    <col min="11009" max="11009" width="23.5546875" style="40" customWidth="1"/>
-    <col min="11010" max="11010" width="33.6640625" style="40" customWidth="1"/>
-    <col min="11011" max="11012" width="14.77734375" style="40" customWidth="1"/>
-    <col min="11013" max="11013" width="82.44140625" style="40" customWidth="1"/>
-    <col min="11014" max="11264" width="14.77734375" style="40"/>
-    <col min="11265" max="11265" width="23.5546875" style="40" customWidth="1"/>
-    <col min="11266" max="11266" width="33.6640625" style="40" customWidth="1"/>
-    <col min="11267" max="11268" width="14.77734375" style="40" customWidth="1"/>
-    <col min="11269" max="11269" width="82.44140625" style="40" customWidth="1"/>
-    <col min="11270" max="11520" width="14.77734375" style="40"/>
-    <col min="11521" max="11521" width="23.5546875" style="40" customWidth="1"/>
-    <col min="11522" max="11522" width="33.6640625" style="40" customWidth="1"/>
-    <col min="11523" max="11524" width="14.77734375" style="40" customWidth="1"/>
-    <col min="11525" max="11525" width="82.44140625" style="40" customWidth="1"/>
-    <col min="11526" max="11776" width="14.77734375" style="40"/>
-    <col min="11777" max="11777" width="23.5546875" style="40" customWidth="1"/>
-    <col min="11778" max="11778" width="33.6640625" style="40" customWidth="1"/>
-    <col min="11779" max="11780" width="14.77734375" style="40" customWidth="1"/>
-    <col min="11781" max="11781" width="82.44140625" style="40" customWidth="1"/>
-    <col min="11782" max="12032" width="14.77734375" style="40"/>
-    <col min="12033" max="12033" width="23.5546875" style="40" customWidth="1"/>
-    <col min="12034" max="12034" width="33.6640625" style="40" customWidth="1"/>
-    <col min="12035" max="12036" width="14.77734375" style="40" customWidth="1"/>
-    <col min="12037" max="12037" width="82.44140625" style="40" customWidth="1"/>
-    <col min="12038" max="12288" width="14.77734375" style="40"/>
-    <col min="12289" max="12289" width="23.5546875" style="40" customWidth="1"/>
-    <col min="12290" max="12290" width="33.6640625" style="40" customWidth="1"/>
-    <col min="12291" max="12292" width="14.77734375" style="40" customWidth="1"/>
-    <col min="12293" max="12293" width="82.44140625" style="40" customWidth="1"/>
-    <col min="12294" max="12544" width="14.77734375" style="40"/>
-    <col min="12545" max="12545" width="23.5546875" style="40" customWidth="1"/>
-    <col min="12546" max="12546" width="33.6640625" style="40" customWidth="1"/>
-    <col min="12547" max="12548" width="14.77734375" style="40" customWidth="1"/>
-    <col min="12549" max="12549" width="82.44140625" style="40" customWidth="1"/>
-    <col min="12550" max="12800" width="14.77734375" style="40"/>
-    <col min="12801" max="12801" width="23.5546875" style="40" customWidth="1"/>
-    <col min="12802" max="12802" width="33.6640625" style="40" customWidth="1"/>
-    <col min="12803" max="12804" width="14.77734375" style="40" customWidth="1"/>
-    <col min="12805" max="12805" width="82.44140625" style="40" customWidth="1"/>
-    <col min="12806" max="13056" width="14.77734375" style="40"/>
-    <col min="13057" max="13057" width="23.5546875" style="40" customWidth="1"/>
-    <col min="13058" max="13058" width="33.6640625" style="40" customWidth="1"/>
-    <col min="13059" max="13060" width="14.77734375" style="40" customWidth="1"/>
-    <col min="13061" max="13061" width="82.44140625" style="40" customWidth="1"/>
-    <col min="13062" max="13312" width="14.77734375" style="40"/>
-    <col min="13313" max="13313" width="23.5546875" style="40" customWidth="1"/>
-    <col min="13314" max="13314" width="33.6640625" style="40" customWidth="1"/>
-    <col min="13315" max="13316" width="14.77734375" style="40" customWidth="1"/>
-    <col min="13317" max="13317" width="82.44140625" style="40" customWidth="1"/>
-    <col min="13318" max="13568" width="14.77734375" style="40"/>
-    <col min="13569" max="13569" width="23.5546875" style="40" customWidth="1"/>
-    <col min="13570" max="13570" width="33.6640625" style="40" customWidth="1"/>
-    <col min="13571" max="13572" width="14.77734375" style="40" customWidth="1"/>
-    <col min="13573" max="13573" width="82.44140625" style="40" customWidth="1"/>
-    <col min="13574" max="13824" width="14.77734375" style="40"/>
-    <col min="13825" max="13825" width="23.5546875" style="40" customWidth="1"/>
-    <col min="13826" max="13826" width="33.6640625" style="40" customWidth="1"/>
-    <col min="13827" max="13828" width="14.77734375" style="40" customWidth="1"/>
-    <col min="13829" max="13829" width="82.44140625" style="40" customWidth="1"/>
-    <col min="13830" max="14080" width="14.77734375" style="40"/>
-    <col min="14081" max="14081" width="23.5546875" style="40" customWidth="1"/>
-    <col min="14082" max="14082" width="33.6640625" style="40" customWidth="1"/>
-    <col min="14083" max="14084" width="14.77734375" style="40" customWidth="1"/>
-    <col min="14085" max="14085" width="82.44140625" style="40" customWidth="1"/>
-    <col min="14086" max="14336" width="14.77734375" style="40"/>
-    <col min="14337" max="14337" width="23.5546875" style="40" customWidth="1"/>
-    <col min="14338" max="14338" width="33.6640625" style="40" customWidth="1"/>
-    <col min="14339" max="14340" width="14.77734375" style="40" customWidth="1"/>
-    <col min="14341" max="14341" width="82.44140625" style="40" customWidth="1"/>
-    <col min="14342" max="14592" width="14.77734375" style="40"/>
-    <col min="14593" max="14593" width="23.5546875" style="40" customWidth="1"/>
-    <col min="14594" max="14594" width="33.6640625" style="40" customWidth="1"/>
-    <col min="14595" max="14596" width="14.77734375" style="40" customWidth="1"/>
-    <col min="14597" max="14597" width="82.44140625" style="40" customWidth="1"/>
-    <col min="14598" max="14848" width="14.77734375" style="40"/>
-    <col min="14849" max="14849" width="23.5546875" style="40" customWidth="1"/>
-    <col min="14850" max="14850" width="33.6640625" style="40" customWidth="1"/>
-    <col min="14851" max="14852" width="14.77734375" style="40" customWidth="1"/>
-    <col min="14853" max="14853" width="82.44140625" style="40" customWidth="1"/>
-    <col min="14854" max="15104" width="14.77734375" style="40"/>
-    <col min="15105" max="15105" width="23.5546875" style="40" customWidth="1"/>
-    <col min="15106" max="15106" width="33.6640625" style="40" customWidth="1"/>
-    <col min="15107" max="15108" width="14.77734375" style="40" customWidth="1"/>
-    <col min="15109" max="15109" width="82.44140625" style="40" customWidth="1"/>
-    <col min="15110" max="15360" width="14.77734375" style="40"/>
-    <col min="15361" max="15361" width="23.5546875" style="40" customWidth="1"/>
-    <col min="15362" max="15362" width="33.6640625" style="40" customWidth="1"/>
-    <col min="15363" max="15364" width="14.77734375" style="40" customWidth="1"/>
-    <col min="15365" max="15365" width="82.44140625" style="40" customWidth="1"/>
-    <col min="15366" max="15616" width="14.77734375" style="40"/>
-    <col min="15617" max="15617" width="23.5546875" style="40" customWidth="1"/>
-    <col min="15618" max="15618" width="33.6640625" style="40" customWidth="1"/>
-    <col min="15619" max="15620" width="14.77734375" style="40" customWidth="1"/>
-    <col min="15621" max="15621" width="82.44140625" style="40" customWidth="1"/>
-    <col min="15622" max="15872" width="14.77734375" style="40"/>
-    <col min="15873" max="15873" width="23.5546875" style="40" customWidth="1"/>
-    <col min="15874" max="15874" width="33.6640625" style="40" customWidth="1"/>
-    <col min="15875" max="15876" width="14.77734375" style="40" customWidth="1"/>
-    <col min="15877" max="15877" width="82.44140625" style="40" customWidth="1"/>
-    <col min="15878" max="16128" width="14.77734375" style="40"/>
-    <col min="16129" max="16129" width="23.5546875" style="40" customWidth="1"/>
-    <col min="16130" max="16130" width="33.6640625" style="40" customWidth="1"/>
-    <col min="16131" max="16132" width="14.77734375" style="40" customWidth="1"/>
-    <col min="16133" max="16133" width="82.44140625" style="40" customWidth="1"/>
-    <col min="16134" max="16384" width="14.77734375" style="40"/>
+    <col min="1" max="1" width="23.54296875" style="40" customWidth="1"/>
+    <col min="2" max="2" width="33.6328125" style="40" customWidth="1"/>
+    <col min="3" max="4" width="14.81640625" style="40" customWidth="1"/>
+    <col min="5" max="5" width="82.453125" style="40" customWidth="1"/>
+    <col min="6" max="256" width="14.81640625" style="40"/>
+    <col min="257" max="257" width="23.54296875" style="40" customWidth="1"/>
+    <col min="258" max="258" width="33.6328125" style="40" customWidth="1"/>
+    <col min="259" max="260" width="14.81640625" style="40" customWidth="1"/>
+    <col min="261" max="261" width="82.453125" style="40" customWidth="1"/>
+    <col min="262" max="512" width="14.81640625" style="40"/>
+    <col min="513" max="513" width="23.54296875" style="40" customWidth="1"/>
+    <col min="514" max="514" width="33.6328125" style="40" customWidth="1"/>
+    <col min="515" max="516" width="14.81640625" style="40" customWidth="1"/>
+    <col min="517" max="517" width="82.453125" style="40" customWidth="1"/>
+    <col min="518" max="768" width="14.81640625" style="40"/>
+    <col min="769" max="769" width="23.54296875" style="40" customWidth="1"/>
+    <col min="770" max="770" width="33.6328125" style="40" customWidth="1"/>
+    <col min="771" max="772" width="14.81640625" style="40" customWidth="1"/>
+    <col min="773" max="773" width="82.453125" style="40" customWidth="1"/>
+    <col min="774" max="1024" width="14.81640625" style="40"/>
+    <col min="1025" max="1025" width="23.54296875" style="40" customWidth="1"/>
+    <col min="1026" max="1026" width="33.6328125" style="40" customWidth="1"/>
+    <col min="1027" max="1028" width="14.81640625" style="40" customWidth="1"/>
+    <col min="1029" max="1029" width="82.453125" style="40" customWidth="1"/>
+    <col min="1030" max="1280" width="14.81640625" style="40"/>
+    <col min="1281" max="1281" width="23.54296875" style="40" customWidth="1"/>
+    <col min="1282" max="1282" width="33.6328125" style="40" customWidth="1"/>
+    <col min="1283" max="1284" width="14.81640625" style="40" customWidth="1"/>
+    <col min="1285" max="1285" width="82.453125" style="40" customWidth="1"/>
+    <col min="1286" max="1536" width="14.81640625" style="40"/>
+    <col min="1537" max="1537" width="23.54296875" style="40" customWidth="1"/>
+    <col min="1538" max="1538" width="33.6328125" style="40" customWidth="1"/>
+    <col min="1539" max="1540" width="14.81640625" style="40" customWidth="1"/>
+    <col min="1541" max="1541" width="82.453125" style="40" customWidth="1"/>
+    <col min="1542" max="1792" width="14.81640625" style="40"/>
+    <col min="1793" max="1793" width="23.54296875" style="40" customWidth="1"/>
+    <col min="1794" max="1794" width="33.6328125" style="40" customWidth="1"/>
+    <col min="1795" max="1796" width="14.81640625" style="40" customWidth="1"/>
+    <col min="1797" max="1797" width="82.453125" style="40" customWidth="1"/>
+    <col min="1798" max="2048" width="14.81640625" style="40"/>
+    <col min="2049" max="2049" width="23.54296875" style="40" customWidth="1"/>
+    <col min="2050" max="2050" width="33.6328125" style="40" customWidth="1"/>
+    <col min="2051" max="2052" width="14.81640625" style="40" customWidth="1"/>
+    <col min="2053" max="2053" width="82.453125" style="40" customWidth="1"/>
+    <col min="2054" max="2304" width="14.81640625" style="40"/>
+    <col min="2305" max="2305" width="23.54296875" style="40" customWidth="1"/>
+    <col min="2306" max="2306" width="33.6328125" style="40" customWidth="1"/>
+    <col min="2307" max="2308" width="14.81640625" style="40" customWidth="1"/>
+    <col min="2309" max="2309" width="82.453125" style="40" customWidth="1"/>
+    <col min="2310" max="2560" width="14.81640625" style="40"/>
+    <col min="2561" max="2561" width="23.54296875" style="40" customWidth="1"/>
+    <col min="2562" max="2562" width="33.6328125" style="40" customWidth="1"/>
+    <col min="2563" max="2564" width="14.81640625" style="40" customWidth="1"/>
+    <col min="2565" max="2565" width="82.453125" style="40" customWidth="1"/>
+    <col min="2566" max="2816" width="14.81640625" style="40"/>
+    <col min="2817" max="2817" width="23.54296875" style="40" customWidth="1"/>
+    <col min="2818" max="2818" width="33.6328125" style="40" customWidth="1"/>
+    <col min="2819" max="2820" width="14.81640625" style="40" customWidth="1"/>
+    <col min="2821" max="2821" width="82.453125" style="40" customWidth="1"/>
+    <col min="2822" max="3072" width="14.81640625" style="40"/>
+    <col min="3073" max="3073" width="23.54296875" style="40" customWidth="1"/>
+    <col min="3074" max="3074" width="33.6328125" style="40" customWidth="1"/>
+    <col min="3075" max="3076" width="14.81640625" style="40" customWidth="1"/>
+    <col min="3077" max="3077" width="82.453125" style="40" customWidth="1"/>
+    <col min="3078" max="3328" width="14.81640625" style="40"/>
+    <col min="3329" max="3329" width="23.54296875" style="40" customWidth="1"/>
+    <col min="3330" max="3330" width="33.6328125" style="40" customWidth="1"/>
+    <col min="3331" max="3332" width="14.81640625" style="40" customWidth="1"/>
+    <col min="3333" max="3333" width="82.453125" style="40" customWidth="1"/>
+    <col min="3334" max="3584" width="14.81640625" style="40"/>
+    <col min="3585" max="3585" width="23.54296875" style="40" customWidth="1"/>
+    <col min="3586" max="3586" width="33.6328125" style="40" customWidth="1"/>
+    <col min="3587" max="3588" width="14.81640625" style="40" customWidth="1"/>
+    <col min="3589" max="3589" width="82.453125" style="40" customWidth="1"/>
+    <col min="3590" max="3840" width="14.81640625" style="40"/>
+    <col min="3841" max="3841" width="23.54296875" style="40" customWidth="1"/>
+    <col min="3842" max="3842" width="33.6328125" style="40" customWidth="1"/>
+    <col min="3843" max="3844" width="14.81640625" style="40" customWidth="1"/>
+    <col min="3845" max="3845" width="82.453125" style="40" customWidth="1"/>
+    <col min="3846" max="4096" width="14.81640625" style="40"/>
+    <col min="4097" max="4097" width="23.54296875" style="40" customWidth="1"/>
+    <col min="4098" max="4098" width="33.6328125" style="40" customWidth="1"/>
+    <col min="4099" max="4100" width="14.81640625" style="40" customWidth="1"/>
+    <col min="4101" max="4101" width="82.453125" style="40" customWidth="1"/>
+    <col min="4102" max="4352" width="14.81640625" style="40"/>
+    <col min="4353" max="4353" width="23.54296875" style="40" customWidth="1"/>
+    <col min="4354" max="4354" width="33.6328125" style="40" customWidth="1"/>
+    <col min="4355" max="4356" width="14.81640625" style="40" customWidth="1"/>
+    <col min="4357" max="4357" width="82.453125" style="40" customWidth="1"/>
+    <col min="4358" max="4608" width="14.81640625" style="40"/>
+    <col min="4609" max="4609" width="23.54296875" style="40" customWidth="1"/>
+    <col min="4610" max="4610" width="33.6328125" style="40" customWidth="1"/>
+    <col min="4611" max="4612" width="14.81640625" style="40" customWidth="1"/>
+    <col min="4613" max="4613" width="82.453125" style="40" customWidth="1"/>
+    <col min="4614" max="4864" width="14.81640625" style="40"/>
+    <col min="4865" max="4865" width="23.54296875" style="40" customWidth="1"/>
+    <col min="4866" max="4866" width="33.6328125" style="40" customWidth="1"/>
+    <col min="4867" max="4868" width="14.81640625" style="40" customWidth="1"/>
+    <col min="4869" max="4869" width="82.453125" style="40" customWidth="1"/>
+    <col min="4870" max="5120" width="14.81640625" style="40"/>
+    <col min="5121" max="5121" width="23.54296875" style="40" customWidth="1"/>
+    <col min="5122" max="5122" width="33.6328125" style="40" customWidth="1"/>
+    <col min="5123" max="5124" width="14.81640625" style="40" customWidth="1"/>
+    <col min="5125" max="5125" width="82.453125" style="40" customWidth="1"/>
+    <col min="5126" max="5376" width="14.81640625" style="40"/>
+    <col min="5377" max="5377" width="23.54296875" style="40" customWidth="1"/>
+    <col min="5378" max="5378" width="33.6328125" style="40" customWidth="1"/>
+    <col min="5379" max="5380" width="14.81640625" style="40" customWidth="1"/>
+    <col min="5381" max="5381" width="82.453125" style="40" customWidth="1"/>
+    <col min="5382" max="5632" width="14.81640625" style="40"/>
+    <col min="5633" max="5633" width="23.54296875" style="40" customWidth="1"/>
+    <col min="5634" max="5634" width="33.6328125" style="40" customWidth="1"/>
+    <col min="5635" max="5636" width="14.81640625" style="40" customWidth="1"/>
+    <col min="5637" max="5637" width="82.453125" style="40" customWidth="1"/>
+    <col min="5638" max="5888" width="14.81640625" style="40"/>
+    <col min="5889" max="5889" width="23.54296875" style="40" customWidth="1"/>
+    <col min="5890" max="5890" width="33.6328125" style="40" customWidth="1"/>
+    <col min="5891" max="5892" width="14.81640625" style="40" customWidth="1"/>
+    <col min="5893" max="5893" width="82.453125" style="40" customWidth="1"/>
+    <col min="5894" max="6144" width="14.81640625" style="40"/>
+    <col min="6145" max="6145" width="23.54296875" style="40" customWidth="1"/>
+    <col min="6146" max="6146" width="33.6328125" style="40" customWidth="1"/>
+    <col min="6147" max="6148" width="14.81640625" style="40" customWidth="1"/>
+    <col min="6149" max="6149" width="82.453125" style="40" customWidth="1"/>
+    <col min="6150" max="6400" width="14.81640625" style="40"/>
+    <col min="6401" max="6401" width="23.54296875" style="40" customWidth="1"/>
+    <col min="6402" max="6402" width="33.6328125" style="40" customWidth="1"/>
+    <col min="6403" max="6404" width="14.81640625" style="40" customWidth="1"/>
+    <col min="6405" max="6405" width="82.453125" style="40" customWidth="1"/>
+    <col min="6406" max="6656" width="14.81640625" style="40"/>
+    <col min="6657" max="6657" width="23.54296875" style="40" customWidth="1"/>
+    <col min="6658" max="6658" width="33.6328125" style="40" customWidth="1"/>
+    <col min="6659" max="6660" width="14.81640625" style="40" customWidth="1"/>
+    <col min="6661" max="6661" width="82.453125" style="40" customWidth="1"/>
+    <col min="6662" max="6912" width="14.81640625" style="40"/>
+    <col min="6913" max="6913" width="23.54296875" style="40" customWidth="1"/>
+    <col min="6914" max="6914" width="33.6328125" style="40" customWidth="1"/>
+    <col min="6915" max="6916" width="14.81640625" style="40" customWidth="1"/>
+    <col min="6917" max="6917" width="82.453125" style="40" customWidth="1"/>
+    <col min="6918" max="7168" width="14.81640625" style="40"/>
+    <col min="7169" max="7169" width="23.54296875" style="40" customWidth="1"/>
+    <col min="7170" max="7170" width="33.6328125" style="40" customWidth="1"/>
+    <col min="7171" max="7172" width="14.81640625" style="40" customWidth="1"/>
+    <col min="7173" max="7173" width="82.453125" style="40" customWidth="1"/>
+    <col min="7174" max="7424" width="14.81640625" style="40"/>
+    <col min="7425" max="7425" width="23.54296875" style="40" customWidth="1"/>
+    <col min="7426" max="7426" width="33.6328125" style="40" customWidth="1"/>
+    <col min="7427" max="7428" width="14.81640625" style="40" customWidth="1"/>
+    <col min="7429" max="7429" width="82.453125" style="40" customWidth="1"/>
+    <col min="7430" max="7680" width="14.81640625" style="40"/>
+    <col min="7681" max="7681" width="23.54296875" style="40" customWidth="1"/>
+    <col min="7682" max="7682" width="33.6328125" style="40" customWidth="1"/>
+    <col min="7683" max="7684" width="14.81640625" style="40" customWidth="1"/>
+    <col min="7685" max="7685" width="82.453125" style="40" customWidth="1"/>
+    <col min="7686" max="7936" width="14.81640625" style="40"/>
+    <col min="7937" max="7937" width="23.54296875" style="40" customWidth="1"/>
+    <col min="7938" max="7938" width="33.6328125" style="40" customWidth="1"/>
+    <col min="7939" max="7940" width="14.81640625" style="40" customWidth="1"/>
+    <col min="7941" max="7941" width="82.453125" style="40" customWidth="1"/>
+    <col min="7942" max="8192" width="14.81640625" style="40"/>
+    <col min="8193" max="8193" width="23.54296875" style="40" customWidth="1"/>
+    <col min="8194" max="8194" width="33.6328125" style="40" customWidth="1"/>
+    <col min="8195" max="8196" width="14.81640625" style="40" customWidth="1"/>
+    <col min="8197" max="8197" width="82.453125" style="40" customWidth="1"/>
+    <col min="8198" max="8448" width="14.81640625" style="40"/>
+    <col min="8449" max="8449" width="23.54296875" style="40" customWidth="1"/>
+    <col min="8450" max="8450" width="33.6328125" style="40" customWidth="1"/>
+    <col min="8451" max="8452" width="14.81640625" style="40" customWidth="1"/>
+    <col min="8453" max="8453" width="82.453125" style="40" customWidth="1"/>
+    <col min="8454" max="8704" width="14.81640625" style="40"/>
+    <col min="8705" max="8705" width="23.54296875" style="40" customWidth="1"/>
+    <col min="8706" max="8706" width="33.6328125" style="40" customWidth="1"/>
+    <col min="8707" max="8708" width="14.81640625" style="40" customWidth="1"/>
+    <col min="8709" max="8709" width="82.453125" style="40" customWidth="1"/>
+    <col min="8710" max="8960" width="14.81640625" style="40"/>
+    <col min="8961" max="8961" width="23.54296875" style="40" customWidth="1"/>
+    <col min="8962" max="8962" width="33.6328125" style="40" customWidth="1"/>
+    <col min="8963" max="8964" width="14.81640625" style="40" customWidth="1"/>
+    <col min="8965" max="8965" width="82.453125" style="40" customWidth="1"/>
+    <col min="8966" max="9216" width="14.81640625" style="40"/>
+    <col min="9217" max="9217" width="23.54296875" style="40" customWidth="1"/>
+    <col min="9218" max="9218" width="33.6328125" style="40" customWidth="1"/>
+    <col min="9219" max="9220" width="14.81640625" style="40" customWidth="1"/>
+    <col min="9221" max="9221" width="82.453125" style="40" customWidth="1"/>
+    <col min="9222" max="9472" width="14.81640625" style="40"/>
+    <col min="9473" max="9473" width="23.54296875" style="40" customWidth="1"/>
+    <col min="9474" max="9474" width="33.6328125" style="40" customWidth="1"/>
+    <col min="9475" max="9476" width="14.81640625" style="40" customWidth="1"/>
+    <col min="9477" max="9477" width="82.453125" style="40" customWidth="1"/>
+    <col min="9478" max="9728" width="14.81640625" style="40"/>
+    <col min="9729" max="9729" width="23.54296875" style="40" customWidth="1"/>
+    <col min="9730" max="9730" width="33.6328125" style="40" customWidth="1"/>
+    <col min="9731" max="9732" width="14.81640625" style="40" customWidth="1"/>
+    <col min="9733" max="9733" width="82.453125" style="40" customWidth="1"/>
+    <col min="9734" max="9984" width="14.81640625" style="40"/>
+    <col min="9985" max="9985" width="23.54296875" style="40" customWidth="1"/>
+    <col min="9986" max="9986" width="33.6328125" style="40" customWidth="1"/>
+    <col min="9987" max="9988" width="14.81640625" style="40" customWidth="1"/>
+    <col min="9989" max="9989" width="82.453125" style="40" customWidth="1"/>
+    <col min="9990" max="10240" width="14.81640625" style="40"/>
+    <col min="10241" max="10241" width="23.54296875" style="40" customWidth="1"/>
+    <col min="10242" max="10242" width="33.6328125" style="40" customWidth="1"/>
+    <col min="10243" max="10244" width="14.81640625" style="40" customWidth="1"/>
+    <col min="10245" max="10245" width="82.453125" style="40" customWidth="1"/>
+    <col min="10246" max="10496" width="14.81640625" style="40"/>
+    <col min="10497" max="10497" width="23.54296875" style="40" customWidth="1"/>
+    <col min="10498" max="10498" width="33.6328125" style="40" customWidth="1"/>
+    <col min="10499" max="10500" width="14.81640625" style="40" customWidth="1"/>
+    <col min="10501" max="10501" width="82.453125" style="40" customWidth="1"/>
+    <col min="10502" max="10752" width="14.81640625" style="40"/>
+    <col min="10753" max="10753" width="23.54296875" style="40" customWidth="1"/>
+    <col min="10754" max="10754" width="33.6328125" style="40" customWidth="1"/>
+    <col min="10755" max="10756" width="14.81640625" style="40" customWidth="1"/>
+    <col min="10757" max="10757" width="82.453125" style="40" customWidth="1"/>
+    <col min="10758" max="11008" width="14.81640625" style="40"/>
+    <col min="11009" max="11009" width="23.54296875" style="40" customWidth="1"/>
+    <col min="11010" max="11010" width="33.6328125" style="40" customWidth="1"/>
+    <col min="11011" max="11012" width="14.81640625" style="40" customWidth="1"/>
+    <col min="11013" max="11013" width="82.453125" style="40" customWidth="1"/>
+    <col min="11014" max="11264" width="14.81640625" style="40"/>
+    <col min="11265" max="11265" width="23.54296875" style="40" customWidth="1"/>
+    <col min="11266" max="11266" width="33.6328125" style="40" customWidth="1"/>
+    <col min="11267" max="11268" width="14.81640625" style="40" customWidth="1"/>
+    <col min="11269" max="11269" width="82.453125" style="40" customWidth="1"/>
+    <col min="11270" max="11520" width="14.81640625" style="40"/>
+    <col min="11521" max="11521" width="23.54296875" style="40" customWidth="1"/>
+    <col min="11522" max="11522" width="33.6328125" style="40" customWidth="1"/>
+    <col min="11523" max="11524" width="14.81640625" style="40" customWidth="1"/>
+    <col min="11525" max="11525" width="82.453125" style="40" customWidth="1"/>
+    <col min="11526" max="11776" width="14.81640625" style="40"/>
+    <col min="11777" max="11777" width="23.54296875" style="40" customWidth="1"/>
+    <col min="11778" max="11778" width="33.6328125" style="40" customWidth="1"/>
+    <col min="11779" max="11780" width="14.81640625" style="40" customWidth="1"/>
+    <col min="11781" max="11781" width="82.453125" style="40" customWidth="1"/>
+    <col min="11782" max="12032" width="14.81640625" style="40"/>
+    <col min="12033" max="12033" width="23.54296875" style="40" customWidth="1"/>
+    <col min="12034" max="12034" width="33.6328125" style="40" customWidth="1"/>
+    <col min="12035" max="12036" width="14.81640625" style="40" customWidth="1"/>
+    <col min="12037" max="12037" width="82.453125" style="40" customWidth="1"/>
+    <col min="12038" max="12288" width="14.81640625" style="40"/>
+    <col min="12289" max="12289" width="23.54296875" style="40" customWidth="1"/>
+    <col min="12290" max="12290" width="33.6328125" style="40" customWidth="1"/>
+    <col min="12291" max="12292" width="14.81640625" style="40" customWidth="1"/>
+    <col min="12293" max="12293" width="82.453125" style="40" customWidth="1"/>
+    <col min="12294" max="12544" width="14.81640625" style="40"/>
+    <col min="12545" max="12545" width="23.54296875" style="40" customWidth="1"/>
+    <col min="12546" max="12546" width="33.6328125" style="40" customWidth="1"/>
+    <col min="12547" max="12548" width="14.81640625" style="40" customWidth="1"/>
+    <col min="12549" max="12549" width="82.453125" style="40" customWidth="1"/>
+    <col min="12550" max="12800" width="14.81640625" style="40"/>
+    <col min="12801" max="12801" width="23.54296875" style="40" customWidth="1"/>
+    <col min="12802" max="12802" width="33.6328125" style="40" customWidth="1"/>
+    <col min="12803" max="12804" width="14.81640625" style="40" customWidth="1"/>
+    <col min="12805" max="12805" width="82.453125" style="40" customWidth="1"/>
+    <col min="12806" max="13056" width="14.81640625" style="40"/>
+    <col min="13057" max="13057" width="23.54296875" style="40" customWidth="1"/>
+    <col min="13058" max="13058" width="33.6328125" style="40" customWidth="1"/>
+    <col min="13059" max="13060" width="14.81640625" style="40" customWidth="1"/>
+    <col min="13061" max="13061" width="82.453125" style="40" customWidth="1"/>
+    <col min="13062" max="13312" width="14.81640625" style="40"/>
+    <col min="13313" max="13313" width="23.54296875" style="40" customWidth="1"/>
+    <col min="13314" max="13314" width="33.6328125" style="40" customWidth="1"/>
+    <col min="13315" max="13316" width="14.81640625" style="40" customWidth="1"/>
+    <col min="13317" max="13317" width="82.453125" style="40" customWidth="1"/>
+    <col min="13318" max="13568" width="14.81640625" style="40"/>
+    <col min="13569" max="13569" width="23.54296875" style="40" customWidth="1"/>
+    <col min="13570" max="13570" width="33.6328125" style="40" customWidth="1"/>
+    <col min="13571" max="13572" width="14.81640625" style="40" customWidth="1"/>
+    <col min="13573" max="13573" width="82.453125" style="40" customWidth="1"/>
+    <col min="13574" max="13824" width="14.81640625" style="40"/>
+    <col min="13825" max="13825" width="23.54296875" style="40" customWidth="1"/>
+    <col min="13826" max="13826" width="33.6328125" style="40" customWidth="1"/>
+    <col min="13827" max="13828" width="14.81640625" style="40" customWidth="1"/>
+    <col min="13829" max="13829" width="82.453125" style="40" customWidth="1"/>
+    <col min="13830" max="14080" width="14.81640625" style="40"/>
+    <col min="14081" max="14081" width="23.54296875" style="40" customWidth="1"/>
+    <col min="14082" max="14082" width="33.6328125" style="40" customWidth="1"/>
+    <col min="14083" max="14084" width="14.81640625" style="40" customWidth="1"/>
+    <col min="14085" max="14085" width="82.453125" style="40" customWidth="1"/>
+    <col min="14086" max="14336" width="14.81640625" style="40"/>
+    <col min="14337" max="14337" width="23.54296875" style="40" customWidth="1"/>
+    <col min="14338" max="14338" width="33.6328125" style="40" customWidth="1"/>
+    <col min="14339" max="14340" width="14.81640625" style="40" customWidth="1"/>
+    <col min="14341" max="14341" width="82.453125" style="40" customWidth="1"/>
+    <col min="14342" max="14592" width="14.81640625" style="40"/>
+    <col min="14593" max="14593" width="23.54296875" style="40" customWidth="1"/>
+    <col min="14594" max="14594" width="33.6328125" style="40" customWidth="1"/>
+    <col min="14595" max="14596" width="14.81640625" style="40" customWidth="1"/>
+    <col min="14597" max="14597" width="82.453125" style="40" customWidth="1"/>
+    <col min="14598" max="14848" width="14.81640625" style="40"/>
+    <col min="14849" max="14849" width="23.54296875" style="40" customWidth="1"/>
+    <col min="14850" max="14850" width="33.6328125" style="40" customWidth="1"/>
+    <col min="14851" max="14852" width="14.81640625" style="40" customWidth="1"/>
+    <col min="14853" max="14853" width="82.453125" style="40" customWidth="1"/>
+    <col min="14854" max="15104" width="14.81640625" style="40"/>
+    <col min="15105" max="15105" width="23.54296875" style="40" customWidth="1"/>
+    <col min="15106" max="15106" width="33.6328125" style="40" customWidth="1"/>
+    <col min="15107" max="15108" width="14.81640625" style="40" customWidth="1"/>
+    <col min="15109" max="15109" width="82.453125" style="40" customWidth="1"/>
+    <col min="15110" max="15360" width="14.81640625" style="40"/>
+    <col min="15361" max="15361" width="23.54296875" style="40" customWidth="1"/>
+    <col min="15362" max="15362" width="33.6328125" style="40" customWidth="1"/>
+    <col min="15363" max="15364" width="14.81640625" style="40" customWidth="1"/>
+    <col min="15365" max="15365" width="82.453125" style="40" customWidth="1"/>
+    <col min="15366" max="15616" width="14.81640625" style="40"/>
+    <col min="15617" max="15617" width="23.54296875" style="40" customWidth="1"/>
+    <col min="15618" max="15618" width="33.6328125" style="40" customWidth="1"/>
+    <col min="15619" max="15620" width="14.81640625" style="40" customWidth="1"/>
+    <col min="15621" max="15621" width="82.453125" style="40" customWidth="1"/>
+    <col min="15622" max="15872" width="14.81640625" style="40"/>
+    <col min="15873" max="15873" width="23.54296875" style="40" customWidth="1"/>
+    <col min="15874" max="15874" width="33.6328125" style="40" customWidth="1"/>
+    <col min="15875" max="15876" width="14.81640625" style="40" customWidth="1"/>
+    <col min="15877" max="15877" width="82.453125" style="40" customWidth="1"/>
+    <col min="15878" max="16128" width="14.81640625" style="40"/>
+    <col min="16129" max="16129" width="23.54296875" style="40" customWidth="1"/>
+    <col min="16130" max="16130" width="33.6328125" style="40" customWidth="1"/>
+    <col min="16131" max="16132" width="14.81640625" style="40" customWidth="1"/>
+    <col min="16133" max="16133" width="82.453125" style="40" customWidth="1"/>
+    <col min="16134" max="16384" width="14.81640625" style="40"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="17.399999999999999">
+    <row r="1" spans="1:5" ht="18">
       <c r="A1" s="76"/>
       <c r="B1" s="77"/>
       <c r="C1" s="77"/>
       <c r="D1" s="77"/>
       <c r="E1" s="77"/>
     </row>
-    <row r="2" spans="1:5" ht="14.4" thickBot="1">
+    <row r="2" spans="1:5" ht="14.5" thickBot="1">
       <c r="A2" s="77"/>
       <c r="B2" s="77"/>
       <c r="C2" s="77"/>
       <c r="D2" s="77"/>
       <c r="E2" s="77"/>
     </row>
-    <row r="3" spans="1:5" ht="13.95" customHeight="1">
+    <row r="3" spans="1:5" ht="14" customHeight="1">
       <c r="A3" s="160" t="s">
         <v>64</v>
       </c>
@@ -49073,14 +49036,14 @@
         <v>68</v>
       </c>
     </row>
-    <row r="4" spans="1:5" ht="14.4" thickBot="1">
+    <row r="4" spans="1:5" ht="14.5" thickBot="1">
       <c r="A4" s="161"/>
       <c r="B4" s="134"/>
       <c r="C4" s="134"/>
       <c r="D4" s="132"/>
       <c r="E4" s="134"/>
     </row>
-    <row r="5" spans="1:5" ht="13.95" customHeight="1">
+    <row r="5" spans="1:5" ht="14" customHeight="1">
       <c r="A5" s="153" t="s">
         <v>178</v>
       </c>
@@ -49134,7 +49097,7 @@
         <v>182</v>
       </c>
     </row>
-    <row r="9" spans="1:5" ht="13.95" customHeight="1">
+    <row r="9" spans="1:5" ht="14" customHeight="1">
       <c r="A9" s="137"/>
       <c r="B9" s="139"/>
       <c r="C9" s="79">
@@ -49292,7 +49255,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="21" spans="1:5" ht="14.4" thickBot="1">
+    <row r="21" spans="1:5" ht="14.5" thickBot="1">
       <c r="A21" s="138"/>
       <c r="B21" s="140"/>
       <c r="C21" s="81">
@@ -49305,7 +49268,7 @@
         <v>195</v>
       </c>
     </row>
-    <row r="22" spans="1:5" ht="13.95" customHeight="1">
+    <row r="22" spans="1:5" ht="14" customHeight="1">
       <c r="A22" s="141" t="s">
         <v>196</v>
       </c>
@@ -49385,7 +49348,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="28" spans="1:5" ht="14.4" thickBot="1">
+    <row r="28" spans="1:5" ht="14.5" thickBot="1">
       <c r="A28" s="142"/>
       <c r="B28" s="144"/>
       <c r="C28" s="80">
@@ -49621,7 +49584,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="46" spans="1:5" ht="14.4" thickBot="1">
+    <row r="46" spans="1:5" ht="14.5" thickBot="1">
       <c r="A46" s="148"/>
       <c r="B46" s="152"/>
       <c r="C46" s="81">
@@ -49650,8 +49613,8 @@
       </c>
     </row>
     <row r="48" spans="1:5">
-      <c r="A48" s="105"/>
-      <c r="B48" s="102"/>
+      <c r="A48" s="93"/>
+      <c r="B48" s="101"/>
       <c r="C48" s="79">
         <v>312832</v>
       </c>
@@ -49663,8 +49626,8 @@
       </c>
     </row>
     <row r="49" spans="1:5">
-      <c r="A49" s="105"/>
-      <c r="B49" s="102"/>
+      <c r="A49" s="93"/>
+      <c r="B49" s="101"/>
       <c r="C49" s="79">
         <v>312833</v>
       </c>
@@ -49676,8 +49639,8 @@
       </c>
     </row>
     <row r="50" spans="1:5">
-      <c r="A50" s="105"/>
-      <c r="B50" s="102"/>
+      <c r="A50" s="93"/>
+      <c r="B50" s="101"/>
       <c r="C50" s="79">
         <v>337802</v>
       </c>
@@ -49689,8 +49652,8 @@
       </c>
     </row>
     <row r="51" spans="1:5">
-      <c r="A51" s="105"/>
-      <c r="B51" s="102"/>
+      <c r="A51" s="93"/>
+      <c r="B51" s="101"/>
       <c r="C51" s="79">
         <v>312834</v>
       </c>
@@ -49702,8 +49665,8 @@
       </c>
     </row>
     <row r="52" spans="1:5">
-      <c r="A52" s="105"/>
-      <c r="B52" s="102"/>
+      <c r="A52" s="93"/>
+      <c r="B52" s="101"/>
       <c r="C52" s="79">
         <v>312835</v>
       </c>
@@ -49715,8 +49678,8 @@
       </c>
     </row>
     <row r="53" spans="1:5">
-      <c r="A53" s="105"/>
-      <c r="B53" s="102"/>
+      <c r="A53" s="93"/>
+      <c r="B53" s="101"/>
       <c r="C53" s="79">
         <v>312836</v>
       </c>
@@ -49727,9 +49690,9 @@
         <v>221</v>
       </c>
     </row>
-    <row r="54" spans="1:5" ht="14.4" thickBot="1">
-      <c r="A54" s="106"/>
-      <c r="B54" s="103"/>
+    <row r="54" spans="1:5" ht="14.5" thickBot="1">
+      <c r="A54" s="94"/>
+      <c r="B54" s="102"/>
       <c r="C54" s="81">
         <v>337803</v>
       </c>
@@ -49774,15 +49737,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A5:E367"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E6" sqref="E6"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="14.5"/>
   <cols>
-    <col min="1" max="1" width="29.21875" customWidth="1"/>
-    <col min="2" max="2" width="68.88671875" customWidth="1"/>
-    <col min="3" max="3" width="20.6640625" customWidth="1"/>
+    <col min="1" max="1" width="29.1796875" customWidth="1"/>
+    <col min="2" max="2" width="68.90625" customWidth="1"/>
+    <col min="3" max="3" width="20.6328125" customWidth="1"/>
+    <col min="5" max="5" width="22.1796875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="5" spans="1:5">
@@ -49798,7 +49762,7 @@
         <v>421</v>
       </c>
       <c r="E6" t="s">
-        <v>453</v>
+        <v>454</v>
       </c>
     </row>
     <row r="7" spans="1:5">
@@ -53293,10 +53257,10 @@
       <selection activeCell="D75" sqref="D75"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="14.5"/>
   <cols>
-    <col min="3" max="3" width="28.33203125" customWidth="1"/>
-    <col min="4" max="4" width="79.21875" customWidth="1"/>
+    <col min="3" max="3" width="28.36328125" customWidth="1"/>
+    <col min="4" max="4" width="79.1796875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="4" spans="3:4">
@@ -54125,10 +54089,10 @@
       <selection activeCell="G16" sqref="G16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="14.5"/>
   <cols>
-    <col min="4" max="4" width="21.6640625" customWidth="1"/>
-    <col min="5" max="5" width="84.88671875" customWidth="1"/>
+    <col min="4" max="4" width="21.6328125" customWidth="1"/>
+    <col min="5" max="5" width="84.90625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="6" spans="4:5">
@@ -54433,11 +54397,11 @@
       <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="14.5"/>
   <cols>
-    <col min="1" max="1" width="24.33203125" customWidth="1"/>
-    <col min="2" max="2" width="69.44140625" customWidth="1"/>
-    <col min="3" max="3" width="22.109375" customWidth="1"/>
+    <col min="1" max="1" width="24.36328125" customWidth="1"/>
+    <col min="2" max="2" width="69.453125" customWidth="1"/>
+    <col min="3" max="3" width="22.08984375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="5" spans="1:5">
@@ -57948,12 +57912,12 @@
       <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="14.5"/>
   <cols>
-    <col min="1" max="1" width="32.33203125" customWidth="1"/>
-    <col min="2" max="2" width="68.44140625" customWidth="1"/>
-    <col min="3" max="3" width="23.109375" customWidth="1"/>
-    <col min="5" max="5" width="10.5546875" customWidth="1"/>
+    <col min="1" max="1" width="32.36328125" customWidth="1"/>
+    <col min="2" max="2" width="68.453125" customWidth="1"/>
+    <col min="3" max="3" width="23.08984375" customWidth="1"/>
+    <col min="5" max="5" width="10.54296875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="5" spans="1:5">
@@ -57969,7 +57933,7 @@
         <v>13</v>
       </c>
       <c r="E6" t="s">
-        <v>454</v>
+        <v>453</v>
       </c>
     </row>
     <row r="7" spans="1:5">
@@ -61321,12 +61285,12 @@
       <selection activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="14.5"/>
   <cols>
-    <col min="1" max="1" width="25.77734375" customWidth="1"/>
-    <col min="2" max="2" width="67.44140625" customWidth="1"/>
-    <col min="3" max="3" width="22.77734375" customWidth="1"/>
-    <col min="4" max="4" width="11.5546875" customWidth="1"/>
+    <col min="1" max="1" width="25.81640625" customWidth="1"/>
+    <col min="2" max="2" width="67.453125" customWidth="1"/>
+    <col min="3" max="3" width="22.81640625" customWidth="1"/>
+    <col min="4" max="4" width="11.54296875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="5" spans="1:5">
@@ -64889,11 +64853,11 @@
       <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="14.5"/>
   <cols>
-    <col min="1" max="1" width="22.88671875" customWidth="1"/>
-    <col min="2" max="2" width="68.88671875" customWidth="1"/>
-    <col min="3" max="3" width="20.6640625" customWidth="1"/>
+    <col min="1" max="1" width="22.90625" customWidth="1"/>
+    <col min="2" max="2" width="68.90625" customWidth="1"/>
+    <col min="3" max="3" width="20.6328125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="5" spans="1:5">
@@ -64909,7 +64873,7 @@
         <v>421</v>
       </c>
       <c r="E6" t="s">
-        <v>455</v>
+        <v>454</v>
       </c>
     </row>
     <row r="7" spans="1:5">
@@ -68404,11 +68368,11 @@
       <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="14.5"/>
   <cols>
-    <col min="1" max="1" width="24.44140625" customWidth="1"/>
-    <col min="2" max="2" width="69.44140625" customWidth="1"/>
-    <col min="3" max="3" width="22.109375" customWidth="1"/>
+    <col min="1" max="1" width="24.453125" customWidth="1"/>
+    <col min="2" max="2" width="69.453125" customWidth="1"/>
+    <col min="3" max="3" width="22.08984375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="5" spans="1:5">
@@ -71919,12 +71883,12 @@
       <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="14.5"/>
   <cols>
-    <col min="1" max="1" width="27.21875" customWidth="1"/>
-    <col min="2" max="2" width="68.44140625" customWidth="1"/>
-    <col min="3" max="3" width="23.109375" customWidth="1"/>
-    <col min="5" max="5" width="10.44140625" customWidth="1"/>
+    <col min="1" max="1" width="27.1796875" customWidth="1"/>
+    <col min="2" max="2" width="68.453125" customWidth="1"/>
+    <col min="3" max="3" width="23.08984375" customWidth="1"/>
+    <col min="5" max="5" width="10.453125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="5" spans="1:5">
@@ -71940,7 +71904,7 @@
         <v>13</v>
       </c>
       <c r="E6" t="s">
-        <v>454</v>
+        <v>453</v>
       </c>
     </row>
     <row r="7" spans="1:5">
@@ -75292,12 +75256,12 @@
       <selection activeCell="H7" sqref="H7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="14.5"/>
   <cols>
-    <col min="1" max="1" width="32.44140625" customWidth="1"/>
-    <col min="2" max="2" width="67.44140625" customWidth="1"/>
-    <col min="3" max="3" width="22.77734375" customWidth="1"/>
-    <col min="4" max="4" width="11.5546875" customWidth="1"/>
+    <col min="1" max="1" width="32.453125" customWidth="1"/>
+    <col min="2" max="2" width="67.453125" customWidth="1"/>
+    <col min="3" max="3" width="22.81640625" customWidth="1"/>
+    <col min="4" max="4" width="11.54296875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="5" spans="1:6">
@@ -75318,7 +75282,7 @@
         <v>452</v>
       </c>
       <c r="F6" t="s">
-        <v>456</v>
+        <v>455</v>
       </c>
     </row>
     <row r="7" spans="1:6">

</xml_diff>

<commit_message>
typo: fixed typo error
</commit_message>
<xml_diff>
--- a/data/Krauss KRWD64.xlsx
+++ b/data/Krauss KRWD64.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="27425"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="26327"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8D3C6C7F-8B8C-4508-B1A9-0DCB461251B2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2E17AF42-3CD7-4334-8021-1EAB3CA78512}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" tabRatio="982" firstSheet="12" activeTab="12" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" tabRatio="982" firstSheet="4" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Krauss до 2400 белый" sheetId="8" r:id="rId1"/>
@@ -51,7 +51,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6509" uniqueCount="457">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6509" uniqueCount="458">
   <si>
     <t>наименование</t>
   </si>
@@ -1423,6 +1423,9 @@
   <si>
     <t>2-ст ру</t>
   </si>
+  <si>
+    <t>Опора (пара)  ALU WEISS R07.2 чёрный PATIO FOLD</t>
+  </si>
 </sst>
 </file>
 
@@ -2101,51 +2104,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="4" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="8" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -2168,6 +2126,51 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="4" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="8" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="25" xfId="1" applyBorder="1" applyAlignment="1">
@@ -16222,9 +16225,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2007 - 2010">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
-    <a:clrScheme name="Office 2007 - 2010">
+    <a:clrScheme name="Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -16262,9 +16265,9 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office 2007 - 2010">
+    <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -16297,9 +16300,26 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -16332,9 +16352,26 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office 2007 - 2010">
+    <a:fmtScheme name="Office">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -16514,12 +16551,12 @@
       <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="26.1796875" customWidth="1"/>
-    <col min="2" max="2" width="67.453125" customWidth="1"/>
-    <col min="3" max="3" width="22.81640625" customWidth="1"/>
-    <col min="4" max="4" width="11.54296875" customWidth="1"/>
+    <col min="1" max="1" width="26.21875" customWidth="1"/>
+    <col min="2" max="2" width="67.44140625" customWidth="1"/>
+    <col min="3" max="3" width="22.77734375" customWidth="1"/>
+    <col min="4" max="4" width="11.5546875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="5" spans="1:5">
@@ -20076,15 +20113,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
   <dimension ref="A5:F380"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="I8" sqref="I8"/>
+    <sheetView topLeftCell="A352" workbookViewId="0">
+      <selection activeCell="B369" sqref="B369"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
     <col min="1" max="1" width="27" customWidth="1"/>
-    <col min="2" max="2" width="68.90625" customWidth="1"/>
-    <col min="3" max="3" width="20.6328125" customWidth="1"/>
+    <col min="2" max="2" width="68.88671875" customWidth="1"/>
+    <col min="3" max="3" width="20.6640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="5" spans="1:6">
@@ -23476,7 +23513,7 @@
     </row>
     <row r="358" spans="1:4">
       <c r="B358" s="1" t="s">
-        <v>149</v>
+        <v>457</v>
       </c>
       <c r="C358" s="1">
         <v>768893</v>
@@ -23741,11 +23778,11 @@
       <selection activeCell="H9" sqref="H9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="32.453125" customWidth="1"/>
-    <col min="2" max="2" width="69.453125" customWidth="1"/>
-    <col min="3" max="3" width="22.08984375" customWidth="1"/>
+    <col min="1" max="1" width="32.44140625" customWidth="1"/>
+    <col min="2" max="2" width="69.44140625" customWidth="1"/>
+    <col min="3" max="3" width="22.109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="5" spans="1:6">
@@ -27402,12 +27439,12 @@
       <selection activeCell="H5" sqref="H5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="31.453125" customWidth="1"/>
-    <col min="2" max="2" width="68.453125" customWidth="1"/>
-    <col min="3" max="3" width="23.08984375" customWidth="1"/>
-    <col min="5" max="5" width="11.1796875" customWidth="1"/>
+    <col min="1" max="1" width="31.44140625" customWidth="1"/>
+    <col min="2" max="2" width="68.44140625" customWidth="1"/>
+    <col min="3" max="3" width="23.109375" customWidth="1"/>
+    <col min="5" max="5" width="11.21875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="5" spans="1:6">
@@ -31203,17 +31240,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0C00-000000000000}">
   <dimension ref="A5:F380"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="26.1796875" customWidth="1"/>
-    <col min="2" max="2" width="67.453125" customWidth="1"/>
-    <col min="3" max="3" width="22.81640625" customWidth="1"/>
-    <col min="4" max="4" width="11.54296875" customWidth="1"/>
-    <col min="5" max="5" width="10.453125" customWidth="1"/>
+    <col min="1" max="1" width="26.21875" customWidth="1"/>
+    <col min="2" max="2" width="67.44140625" customWidth="1"/>
+    <col min="3" max="3" width="22.77734375" customWidth="1"/>
+    <col min="4" max="4" width="11.5546875" customWidth="1"/>
+    <col min="5" max="5" width="10.44140625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="5" spans="1:6">
@@ -34918,14 +34955,14 @@
   <dimension ref="A5:F380"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F6" sqref="F6"/>
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
     <col min="1" max="1" width="32" customWidth="1"/>
-    <col min="2" max="2" width="68.90625" customWidth="1"/>
-    <col min="3" max="3" width="20.6328125" customWidth="1"/>
+    <col min="2" max="2" width="68.88671875" customWidth="1"/>
+    <col min="3" max="3" width="20.6640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="5" spans="1:6">
@@ -38317,7 +38354,7 @@
     </row>
     <row r="358" spans="1:4">
       <c r="B358" s="1" t="s">
-        <v>149</v>
+        <v>457</v>
       </c>
       <c r="C358" s="1">
         <v>768893</v>
@@ -38582,11 +38619,11 @@
       <selection activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="30.54296875" customWidth="1"/>
-    <col min="2" max="2" width="69.453125" customWidth="1"/>
-    <col min="3" max="3" width="22.08984375" customWidth="1"/>
+    <col min="1" max="1" width="30.5546875" customWidth="1"/>
+    <col min="2" max="2" width="69.44140625" customWidth="1"/>
+    <col min="3" max="3" width="22.109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="5" spans="1:6">
@@ -42243,12 +42280,12 @@
       <selection activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="33.36328125" customWidth="1"/>
-    <col min="2" max="2" width="68.453125" customWidth="1"/>
-    <col min="3" max="3" width="23.08984375" customWidth="1"/>
-    <col min="5" max="5" width="15.6328125" customWidth="1"/>
+    <col min="1" max="1" width="33.33203125" customWidth="1"/>
+    <col min="2" max="2" width="68.44140625" customWidth="1"/>
+    <col min="3" max="3" width="23.109375" customWidth="1"/>
+    <col min="5" max="5" width="15.6640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="5" spans="1:6">
@@ -46055,425 +46092,425 @@
       <selection pane="topRight" activeCell="B8" sqref="B8:B22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.08984375" defaultRowHeight="14"/>
+  <sheetFormatPr defaultColWidth="14.109375" defaultRowHeight="13.8"/>
   <cols>
-    <col min="1" max="1" width="24.453125" style="2" customWidth="1"/>
+    <col min="1" max="1" width="24.44140625" style="2" customWidth="1"/>
     <col min="2" max="2" width="36" style="2" customWidth="1"/>
-    <col min="3" max="3" width="23.6328125" style="2" customWidth="1"/>
+    <col min="3" max="3" width="23.6640625" style="2" customWidth="1"/>
     <col min="4" max="4" width="16" style="2" customWidth="1"/>
-    <col min="5" max="5" width="83.90625" style="2" customWidth="1"/>
-    <col min="6" max="256" width="14.08984375" style="2"/>
-    <col min="257" max="257" width="24.453125" style="2" customWidth="1"/>
+    <col min="5" max="5" width="83.88671875" style="2" customWidth="1"/>
+    <col min="6" max="256" width="14.109375" style="2"/>
+    <col min="257" max="257" width="24.44140625" style="2" customWidth="1"/>
     <col min="258" max="258" width="36" style="2" customWidth="1"/>
-    <col min="259" max="259" width="23.6328125" style="2" customWidth="1"/>
+    <col min="259" max="259" width="23.6640625" style="2" customWidth="1"/>
     <col min="260" max="260" width="16" style="2" customWidth="1"/>
-    <col min="261" max="261" width="83.90625" style="2" customWidth="1"/>
-    <col min="262" max="512" width="14.08984375" style="2"/>
-    <col min="513" max="513" width="24.453125" style="2" customWidth="1"/>
+    <col min="261" max="261" width="83.88671875" style="2" customWidth="1"/>
+    <col min="262" max="512" width="14.109375" style="2"/>
+    <col min="513" max="513" width="24.44140625" style="2" customWidth="1"/>
     <col min="514" max="514" width="36" style="2" customWidth="1"/>
-    <col min="515" max="515" width="23.6328125" style="2" customWidth="1"/>
+    <col min="515" max="515" width="23.6640625" style="2" customWidth="1"/>
     <col min="516" max="516" width="16" style="2" customWidth="1"/>
-    <col min="517" max="517" width="83.90625" style="2" customWidth="1"/>
-    <col min="518" max="768" width="14.08984375" style="2"/>
-    <col min="769" max="769" width="24.453125" style="2" customWidth="1"/>
+    <col min="517" max="517" width="83.88671875" style="2" customWidth="1"/>
+    <col min="518" max="768" width="14.109375" style="2"/>
+    <col min="769" max="769" width="24.44140625" style="2" customWidth="1"/>
     <col min="770" max="770" width="36" style="2" customWidth="1"/>
-    <col min="771" max="771" width="23.6328125" style="2" customWidth="1"/>
+    <col min="771" max="771" width="23.6640625" style="2" customWidth="1"/>
     <col min="772" max="772" width="16" style="2" customWidth="1"/>
-    <col min="773" max="773" width="83.90625" style="2" customWidth="1"/>
-    <col min="774" max="1024" width="14.08984375" style="2"/>
-    <col min="1025" max="1025" width="24.453125" style="2" customWidth="1"/>
+    <col min="773" max="773" width="83.88671875" style="2" customWidth="1"/>
+    <col min="774" max="1024" width="14.109375" style="2"/>
+    <col min="1025" max="1025" width="24.44140625" style="2" customWidth="1"/>
     <col min="1026" max="1026" width="36" style="2" customWidth="1"/>
-    <col min="1027" max="1027" width="23.6328125" style="2" customWidth="1"/>
+    <col min="1027" max="1027" width="23.6640625" style="2" customWidth="1"/>
     <col min="1028" max="1028" width="16" style="2" customWidth="1"/>
-    <col min="1029" max="1029" width="83.90625" style="2" customWidth="1"/>
-    <col min="1030" max="1280" width="14.08984375" style="2"/>
-    <col min="1281" max="1281" width="24.453125" style="2" customWidth="1"/>
+    <col min="1029" max="1029" width="83.88671875" style="2" customWidth="1"/>
+    <col min="1030" max="1280" width="14.109375" style="2"/>
+    <col min="1281" max="1281" width="24.44140625" style="2" customWidth="1"/>
     <col min="1282" max="1282" width="36" style="2" customWidth="1"/>
-    <col min="1283" max="1283" width="23.6328125" style="2" customWidth="1"/>
+    <col min="1283" max="1283" width="23.6640625" style="2" customWidth="1"/>
     <col min="1284" max="1284" width="16" style="2" customWidth="1"/>
-    <col min="1285" max="1285" width="83.90625" style="2" customWidth="1"/>
-    <col min="1286" max="1536" width="14.08984375" style="2"/>
-    <col min="1537" max="1537" width="24.453125" style="2" customWidth="1"/>
+    <col min="1285" max="1285" width="83.88671875" style="2" customWidth="1"/>
+    <col min="1286" max="1536" width="14.109375" style="2"/>
+    <col min="1537" max="1537" width="24.44140625" style="2" customWidth="1"/>
     <col min="1538" max="1538" width="36" style="2" customWidth="1"/>
-    <col min="1539" max="1539" width="23.6328125" style="2" customWidth="1"/>
+    <col min="1539" max="1539" width="23.6640625" style="2" customWidth="1"/>
     <col min="1540" max="1540" width="16" style="2" customWidth="1"/>
-    <col min="1541" max="1541" width="83.90625" style="2" customWidth="1"/>
-    <col min="1542" max="1792" width="14.08984375" style="2"/>
-    <col min="1793" max="1793" width="24.453125" style="2" customWidth="1"/>
+    <col min="1541" max="1541" width="83.88671875" style="2" customWidth="1"/>
+    <col min="1542" max="1792" width="14.109375" style="2"/>
+    <col min="1793" max="1793" width="24.44140625" style="2" customWidth="1"/>
     <col min="1794" max="1794" width="36" style="2" customWidth="1"/>
-    <col min="1795" max="1795" width="23.6328125" style="2" customWidth="1"/>
+    <col min="1795" max="1795" width="23.6640625" style="2" customWidth="1"/>
     <col min="1796" max="1796" width="16" style="2" customWidth="1"/>
-    <col min="1797" max="1797" width="83.90625" style="2" customWidth="1"/>
-    <col min="1798" max="2048" width="14.08984375" style="2"/>
-    <col min="2049" max="2049" width="24.453125" style="2" customWidth="1"/>
+    <col min="1797" max="1797" width="83.88671875" style="2" customWidth="1"/>
+    <col min="1798" max="2048" width="14.109375" style="2"/>
+    <col min="2049" max="2049" width="24.44140625" style="2" customWidth="1"/>
     <col min="2050" max="2050" width="36" style="2" customWidth="1"/>
-    <col min="2051" max="2051" width="23.6328125" style="2" customWidth="1"/>
+    <col min="2051" max="2051" width="23.6640625" style="2" customWidth="1"/>
     <col min="2052" max="2052" width="16" style="2" customWidth="1"/>
-    <col min="2053" max="2053" width="83.90625" style="2" customWidth="1"/>
-    <col min="2054" max="2304" width="14.08984375" style="2"/>
-    <col min="2305" max="2305" width="24.453125" style="2" customWidth="1"/>
+    <col min="2053" max="2053" width="83.88671875" style="2" customWidth="1"/>
+    <col min="2054" max="2304" width="14.109375" style="2"/>
+    <col min="2305" max="2305" width="24.44140625" style="2" customWidth="1"/>
     <col min="2306" max="2306" width="36" style="2" customWidth="1"/>
-    <col min="2307" max="2307" width="23.6328125" style="2" customWidth="1"/>
+    <col min="2307" max="2307" width="23.6640625" style="2" customWidth="1"/>
     <col min="2308" max="2308" width="16" style="2" customWidth="1"/>
-    <col min="2309" max="2309" width="83.90625" style="2" customWidth="1"/>
-    <col min="2310" max="2560" width="14.08984375" style="2"/>
-    <col min="2561" max="2561" width="24.453125" style="2" customWidth="1"/>
+    <col min="2309" max="2309" width="83.88671875" style="2" customWidth="1"/>
+    <col min="2310" max="2560" width="14.109375" style="2"/>
+    <col min="2561" max="2561" width="24.44140625" style="2" customWidth="1"/>
     <col min="2562" max="2562" width="36" style="2" customWidth="1"/>
-    <col min="2563" max="2563" width="23.6328125" style="2" customWidth="1"/>
+    <col min="2563" max="2563" width="23.6640625" style="2" customWidth="1"/>
     <col min="2564" max="2564" width="16" style="2" customWidth="1"/>
-    <col min="2565" max="2565" width="83.90625" style="2" customWidth="1"/>
-    <col min="2566" max="2816" width="14.08984375" style="2"/>
-    <col min="2817" max="2817" width="24.453125" style="2" customWidth="1"/>
+    <col min="2565" max="2565" width="83.88671875" style="2" customWidth="1"/>
+    <col min="2566" max="2816" width="14.109375" style="2"/>
+    <col min="2817" max="2817" width="24.44140625" style="2" customWidth="1"/>
     <col min="2818" max="2818" width="36" style="2" customWidth="1"/>
-    <col min="2819" max="2819" width="23.6328125" style="2" customWidth="1"/>
+    <col min="2819" max="2819" width="23.6640625" style="2" customWidth="1"/>
     <col min="2820" max="2820" width="16" style="2" customWidth="1"/>
-    <col min="2821" max="2821" width="83.90625" style="2" customWidth="1"/>
-    <col min="2822" max="3072" width="14.08984375" style="2"/>
-    <col min="3073" max="3073" width="24.453125" style="2" customWidth="1"/>
+    <col min="2821" max="2821" width="83.88671875" style="2" customWidth="1"/>
+    <col min="2822" max="3072" width="14.109375" style="2"/>
+    <col min="3073" max="3073" width="24.44140625" style="2" customWidth="1"/>
     <col min="3074" max="3074" width="36" style="2" customWidth="1"/>
-    <col min="3075" max="3075" width="23.6328125" style="2" customWidth="1"/>
+    <col min="3075" max="3075" width="23.6640625" style="2" customWidth="1"/>
     <col min="3076" max="3076" width="16" style="2" customWidth="1"/>
-    <col min="3077" max="3077" width="83.90625" style="2" customWidth="1"/>
-    <col min="3078" max="3328" width="14.08984375" style="2"/>
-    <col min="3329" max="3329" width="24.453125" style="2" customWidth="1"/>
+    <col min="3077" max="3077" width="83.88671875" style="2" customWidth="1"/>
+    <col min="3078" max="3328" width="14.109375" style="2"/>
+    <col min="3329" max="3329" width="24.44140625" style="2" customWidth="1"/>
     <col min="3330" max="3330" width="36" style="2" customWidth="1"/>
-    <col min="3331" max="3331" width="23.6328125" style="2" customWidth="1"/>
+    <col min="3331" max="3331" width="23.6640625" style="2" customWidth="1"/>
     <col min="3332" max="3332" width="16" style="2" customWidth="1"/>
-    <col min="3333" max="3333" width="83.90625" style="2" customWidth="1"/>
-    <col min="3334" max="3584" width="14.08984375" style="2"/>
-    <col min="3585" max="3585" width="24.453125" style="2" customWidth="1"/>
+    <col min="3333" max="3333" width="83.88671875" style="2" customWidth="1"/>
+    <col min="3334" max="3584" width="14.109375" style="2"/>
+    <col min="3585" max="3585" width="24.44140625" style="2" customWidth="1"/>
     <col min="3586" max="3586" width="36" style="2" customWidth="1"/>
-    <col min="3587" max="3587" width="23.6328125" style="2" customWidth="1"/>
+    <col min="3587" max="3587" width="23.6640625" style="2" customWidth="1"/>
     <col min="3588" max="3588" width="16" style="2" customWidth="1"/>
-    <col min="3589" max="3589" width="83.90625" style="2" customWidth="1"/>
-    <col min="3590" max="3840" width="14.08984375" style="2"/>
-    <col min="3841" max="3841" width="24.453125" style="2" customWidth="1"/>
+    <col min="3589" max="3589" width="83.88671875" style="2" customWidth="1"/>
+    <col min="3590" max="3840" width="14.109375" style="2"/>
+    <col min="3841" max="3841" width="24.44140625" style="2" customWidth="1"/>
     <col min="3842" max="3842" width="36" style="2" customWidth="1"/>
-    <col min="3843" max="3843" width="23.6328125" style="2" customWidth="1"/>
+    <col min="3843" max="3843" width="23.6640625" style="2" customWidth="1"/>
     <col min="3844" max="3844" width="16" style="2" customWidth="1"/>
-    <col min="3845" max="3845" width="83.90625" style="2" customWidth="1"/>
-    <col min="3846" max="4096" width="14.08984375" style="2"/>
-    <col min="4097" max="4097" width="24.453125" style="2" customWidth="1"/>
+    <col min="3845" max="3845" width="83.88671875" style="2" customWidth="1"/>
+    <col min="3846" max="4096" width="14.109375" style="2"/>
+    <col min="4097" max="4097" width="24.44140625" style="2" customWidth="1"/>
     <col min="4098" max="4098" width="36" style="2" customWidth="1"/>
-    <col min="4099" max="4099" width="23.6328125" style="2" customWidth="1"/>
+    <col min="4099" max="4099" width="23.6640625" style="2" customWidth="1"/>
     <col min="4100" max="4100" width="16" style="2" customWidth="1"/>
-    <col min="4101" max="4101" width="83.90625" style="2" customWidth="1"/>
-    <col min="4102" max="4352" width="14.08984375" style="2"/>
-    <col min="4353" max="4353" width="24.453125" style="2" customWidth="1"/>
+    <col min="4101" max="4101" width="83.88671875" style="2" customWidth="1"/>
+    <col min="4102" max="4352" width="14.109375" style="2"/>
+    <col min="4353" max="4353" width="24.44140625" style="2" customWidth="1"/>
     <col min="4354" max="4354" width="36" style="2" customWidth="1"/>
-    <col min="4355" max="4355" width="23.6328125" style="2" customWidth="1"/>
+    <col min="4355" max="4355" width="23.6640625" style="2" customWidth="1"/>
     <col min="4356" max="4356" width="16" style="2" customWidth="1"/>
-    <col min="4357" max="4357" width="83.90625" style="2" customWidth="1"/>
-    <col min="4358" max="4608" width="14.08984375" style="2"/>
-    <col min="4609" max="4609" width="24.453125" style="2" customWidth="1"/>
+    <col min="4357" max="4357" width="83.88671875" style="2" customWidth="1"/>
+    <col min="4358" max="4608" width="14.109375" style="2"/>
+    <col min="4609" max="4609" width="24.44140625" style="2" customWidth="1"/>
     <col min="4610" max="4610" width="36" style="2" customWidth="1"/>
-    <col min="4611" max="4611" width="23.6328125" style="2" customWidth="1"/>
+    <col min="4611" max="4611" width="23.6640625" style="2" customWidth="1"/>
     <col min="4612" max="4612" width="16" style="2" customWidth="1"/>
-    <col min="4613" max="4613" width="83.90625" style="2" customWidth="1"/>
-    <col min="4614" max="4864" width="14.08984375" style="2"/>
-    <col min="4865" max="4865" width="24.453125" style="2" customWidth="1"/>
+    <col min="4613" max="4613" width="83.88671875" style="2" customWidth="1"/>
+    <col min="4614" max="4864" width="14.109375" style="2"/>
+    <col min="4865" max="4865" width="24.44140625" style="2" customWidth="1"/>
     <col min="4866" max="4866" width="36" style="2" customWidth="1"/>
-    <col min="4867" max="4867" width="23.6328125" style="2" customWidth="1"/>
+    <col min="4867" max="4867" width="23.6640625" style="2" customWidth="1"/>
     <col min="4868" max="4868" width="16" style="2" customWidth="1"/>
-    <col min="4869" max="4869" width="83.90625" style="2" customWidth="1"/>
-    <col min="4870" max="5120" width="14.08984375" style="2"/>
-    <col min="5121" max="5121" width="24.453125" style="2" customWidth="1"/>
+    <col min="4869" max="4869" width="83.88671875" style="2" customWidth="1"/>
+    <col min="4870" max="5120" width="14.109375" style="2"/>
+    <col min="5121" max="5121" width="24.44140625" style="2" customWidth="1"/>
     <col min="5122" max="5122" width="36" style="2" customWidth="1"/>
-    <col min="5123" max="5123" width="23.6328125" style="2" customWidth="1"/>
+    <col min="5123" max="5123" width="23.6640625" style="2" customWidth="1"/>
     <col min="5124" max="5124" width="16" style="2" customWidth="1"/>
-    <col min="5125" max="5125" width="83.90625" style="2" customWidth="1"/>
-    <col min="5126" max="5376" width="14.08984375" style="2"/>
-    <col min="5377" max="5377" width="24.453125" style="2" customWidth="1"/>
+    <col min="5125" max="5125" width="83.88671875" style="2" customWidth="1"/>
+    <col min="5126" max="5376" width="14.109375" style="2"/>
+    <col min="5377" max="5377" width="24.44140625" style="2" customWidth="1"/>
     <col min="5378" max="5378" width="36" style="2" customWidth="1"/>
-    <col min="5379" max="5379" width="23.6328125" style="2" customWidth="1"/>
+    <col min="5379" max="5379" width="23.6640625" style="2" customWidth="1"/>
     <col min="5380" max="5380" width="16" style="2" customWidth="1"/>
-    <col min="5381" max="5381" width="83.90625" style="2" customWidth="1"/>
-    <col min="5382" max="5632" width="14.08984375" style="2"/>
-    <col min="5633" max="5633" width="24.453125" style="2" customWidth="1"/>
+    <col min="5381" max="5381" width="83.88671875" style="2" customWidth="1"/>
+    <col min="5382" max="5632" width="14.109375" style="2"/>
+    <col min="5633" max="5633" width="24.44140625" style="2" customWidth="1"/>
     <col min="5634" max="5634" width="36" style="2" customWidth="1"/>
-    <col min="5635" max="5635" width="23.6328125" style="2" customWidth="1"/>
+    <col min="5635" max="5635" width="23.6640625" style="2" customWidth="1"/>
     <col min="5636" max="5636" width="16" style="2" customWidth="1"/>
-    <col min="5637" max="5637" width="83.90625" style="2" customWidth="1"/>
-    <col min="5638" max="5888" width="14.08984375" style="2"/>
-    <col min="5889" max="5889" width="24.453125" style="2" customWidth="1"/>
+    <col min="5637" max="5637" width="83.88671875" style="2" customWidth="1"/>
+    <col min="5638" max="5888" width="14.109375" style="2"/>
+    <col min="5889" max="5889" width="24.44140625" style="2" customWidth="1"/>
     <col min="5890" max="5890" width="36" style="2" customWidth="1"/>
-    <col min="5891" max="5891" width="23.6328125" style="2" customWidth="1"/>
+    <col min="5891" max="5891" width="23.6640625" style="2" customWidth="1"/>
     <col min="5892" max="5892" width="16" style="2" customWidth="1"/>
-    <col min="5893" max="5893" width="83.90625" style="2" customWidth="1"/>
-    <col min="5894" max="6144" width="14.08984375" style="2"/>
-    <col min="6145" max="6145" width="24.453125" style="2" customWidth="1"/>
+    <col min="5893" max="5893" width="83.88671875" style="2" customWidth="1"/>
+    <col min="5894" max="6144" width="14.109375" style="2"/>
+    <col min="6145" max="6145" width="24.44140625" style="2" customWidth="1"/>
     <col min="6146" max="6146" width="36" style="2" customWidth="1"/>
-    <col min="6147" max="6147" width="23.6328125" style="2" customWidth="1"/>
+    <col min="6147" max="6147" width="23.6640625" style="2" customWidth="1"/>
     <col min="6148" max="6148" width="16" style="2" customWidth="1"/>
-    <col min="6149" max="6149" width="83.90625" style="2" customWidth="1"/>
-    <col min="6150" max="6400" width="14.08984375" style="2"/>
-    <col min="6401" max="6401" width="24.453125" style="2" customWidth="1"/>
+    <col min="6149" max="6149" width="83.88671875" style="2" customWidth="1"/>
+    <col min="6150" max="6400" width="14.109375" style="2"/>
+    <col min="6401" max="6401" width="24.44140625" style="2" customWidth="1"/>
     <col min="6402" max="6402" width="36" style="2" customWidth="1"/>
-    <col min="6403" max="6403" width="23.6328125" style="2" customWidth="1"/>
+    <col min="6403" max="6403" width="23.6640625" style="2" customWidth="1"/>
     <col min="6404" max="6404" width="16" style="2" customWidth="1"/>
-    <col min="6405" max="6405" width="83.90625" style="2" customWidth="1"/>
-    <col min="6406" max="6656" width="14.08984375" style="2"/>
-    <col min="6657" max="6657" width="24.453125" style="2" customWidth="1"/>
+    <col min="6405" max="6405" width="83.88671875" style="2" customWidth="1"/>
+    <col min="6406" max="6656" width="14.109375" style="2"/>
+    <col min="6657" max="6657" width="24.44140625" style="2" customWidth="1"/>
     <col min="6658" max="6658" width="36" style="2" customWidth="1"/>
-    <col min="6659" max="6659" width="23.6328125" style="2" customWidth="1"/>
+    <col min="6659" max="6659" width="23.6640625" style="2" customWidth="1"/>
     <col min="6660" max="6660" width="16" style="2" customWidth="1"/>
-    <col min="6661" max="6661" width="83.90625" style="2" customWidth="1"/>
-    <col min="6662" max="6912" width="14.08984375" style="2"/>
-    <col min="6913" max="6913" width="24.453125" style="2" customWidth="1"/>
+    <col min="6661" max="6661" width="83.88671875" style="2" customWidth="1"/>
+    <col min="6662" max="6912" width="14.109375" style="2"/>
+    <col min="6913" max="6913" width="24.44140625" style="2" customWidth="1"/>
     <col min="6914" max="6914" width="36" style="2" customWidth="1"/>
-    <col min="6915" max="6915" width="23.6328125" style="2" customWidth="1"/>
+    <col min="6915" max="6915" width="23.6640625" style="2" customWidth="1"/>
     <col min="6916" max="6916" width="16" style="2" customWidth="1"/>
-    <col min="6917" max="6917" width="83.90625" style="2" customWidth="1"/>
-    <col min="6918" max="7168" width="14.08984375" style="2"/>
-    <col min="7169" max="7169" width="24.453125" style="2" customWidth="1"/>
+    <col min="6917" max="6917" width="83.88671875" style="2" customWidth="1"/>
+    <col min="6918" max="7168" width="14.109375" style="2"/>
+    <col min="7169" max="7169" width="24.44140625" style="2" customWidth="1"/>
     <col min="7170" max="7170" width="36" style="2" customWidth="1"/>
-    <col min="7171" max="7171" width="23.6328125" style="2" customWidth="1"/>
+    <col min="7171" max="7171" width="23.6640625" style="2" customWidth="1"/>
     <col min="7172" max="7172" width="16" style="2" customWidth="1"/>
-    <col min="7173" max="7173" width="83.90625" style="2" customWidth="1"/>
-    <col min="7174" max="7424" width="14.08984375" style="2"/>
-    <col min="7425" max="7425" width="24.453125" style="2" customWidth="1"/>
+    <col min="7173" max="7173" width="83.88671875" style="2" customWidth="1"/>
+    <col min="7174" max="7424" width="14.109375" style="2"/>
+    <col min="7425" max="7425" width="24.44140625" style="2" customWidth="1"/>
     <col min="7426" max="7426" width="36" style="2" customWidth="1"/>
-    <col min="7427" max="7427" width="23.6328125" style="2" customWidth="1"/>
+    <col min="7427" max="7427" width="23.6640625" style="2" customWidth="1"/>
     <col min="7428" max="7428" width="16" style="2" customWidth="1"/>
-    <col min="7429" max="7429" width="83.90625" style="2" customWidth="1"/>
-    <col min="7430" max="7680" width="14.08984375" style="2"/>
-    <col min="7681" max="7681" width="24.453125" style="2" customWidth="1"/>
+    <col min="7429" max="7429" width="83.88671875" style="2" customWidth="1"/>
+    <col min="7430" max="7680" width="14.109375" style="2"/>
+    <col min="7681" max="7681" width="24.44140625" style="2" customWidth="1"/>
     <col min="7682" max="7682" width="36" style="2" customWidth="1"/>
-    <col min="7683" max="7683" width="23.6328125" style="2" customWidth="1"/>
+    <col min="7683" max="7683" width="23.6640625" style="2" customWidth="1"/>
     <col min="7684" max="7684" width="16" style="2" customWidth="1"/>
-    <col min="7685" max="7685" width="83.90625" style="2" customWidth="1"/>
-    <col min="7686" max="7936" width="14.08984375" style="2"/>
-    <col min="7937" max="7937" width="24.453125" style="2" customWidth="1"/>
+    <col min="7685" max="7685" width="83.88671875" style="2" customWidth="1"/>
+    <col min="7686" max="7936" width="14.109375" style="2"/>
+    <col min="7937" max="7937" width="24.44140625" style="2" customWidth="1"/>
     <col min="7938" max="7938" width="36" style="2" customWidth="1"/>
-    <col min="7939" max="7939" width="23.6328125" style="2" customWidth="1"/>
+    <col min="7939" max="7939" width="23.6640625" style="2" customWidth="1"/>
     <col min="7940" max="7940" width="16" style="2" customWidth="1"/>
-    <col min="7941" max="7941" width="83.90625" style="2" customWidth="1"/>
-    <col min="7942" max="8192" width="14.08984375" style="2"/>
-    <col min="8193" max="8193" width="24.453125" style="2" customWidth="1"/>
+    <col min="7941" max="7941" width="83.88671875" style="2" customWidth="1"/>
+    <col min="7942" max="8192" width="14.109375" style="2"/>
+    <col min="8193" max="8193" width="24.44140625" style="2" customWidth="1"/>
     <col min="8194" max="8194" width="36" style="2" customWidth="1"/>
-    <col min="8195" max="8195" width="23.6328125" style="2" customWidth="1"/>
+    <col min="8195" max="8195" width="23.6640625" style="2" customWidth="1"/>
     <col min="8196" max="8196" width="16" style="2" customWidth="1"/>
-    <col min="8197" max="8197" width="83.90625" style="2" customWidth="1"/>
-    <col min="8198" max="8448" width="14.08984375" style="2"/>
-    <col min="8449" max="8449" width="24.453125" style="2" customWidth="1"/>
+    <col min="8197" max="8197" width="83.88671875" style="2" customWidth="1"/>
+    <col min="8198" max="8448" width="14.109375" style="2"/>
+    <col min="8449" max="8449" width="24.44140625" style="2" customWidth="1"/>
     <col min="8450" max="8450" width="36" style="2" customWidth="1"/>
-    <col min="8451" max="8451" width="23.6328125" style="2" customWidth="1"/>
+    <col min="8451" max="8451" width="23.6640625" style="2" customWidth="1"/>
     <col min="8452" max="8452" width="16" style="2" customWidth="1"/>
-    <col min="8453" max="8453" width="83.90625" style="2" customWidth="1"/>
-    <col min="8454" max="8704" width="14.08984375" style="2"/>
-    <col min="8705" max="8705" width="24.453125" style="2" customWidth="1"/>
+    <col min="8453" max="8453" width="83.88671875" style="2" customWidth="1"/>
+    <col min="8454" max="8704" width="14.109375" style="2"/>
+    <col min="8705" max="8705" width="24.44140625" style="2" customWidth="1"/>
     <col min="8706" max="8706" width="36" style="2" customWidth="1"/>
-    <col min="8707" max="8707" width="23.6328125" style="2" customWidth="1"/>
+    <col min="8707" max="8707" width="23.6640625" style="2" customWidth="1"/>
     <col min="8708" max="8708" width="16" style="2" customWidth="1"/>
-    <col min="8709" max="8709" width="83.90625" style="2" customWidth="1"/>
-    <col min="8710" max="8960" width="14.08984375" style="2"/>
-    <col min="8961" max="8961" width="24.453125" style="2" customWidth="1"/>
+    <col min="8709" max="8709" width="83.88671875" style="2" customWidth="1"/>
+    <col min="8710" max="8960" width="14.109375" style="2"/>
+    <col min="8961" max="8961" width="24.44140625" style="2" customWidth="1"/>
     <col min="8962" max="8962" width="36" style="2" customWidth="1"/>
-    <col min="8963" max="8963" width="23.6328125" style="2" customWidth="1"/>
+    <col min="8963" max="8963" width="23.6640625" style="2" customWidth="1"/>
     <col min="8964" max="8964" width="16" style="2" customWidth="1"/>
-    <col min="8965" max="8965" width="83.90625" style="2" customWidth="1"/>
-    <col min="8966" max="9216" width="14.08984375" style="2"/>
-    <col min="9217" max="9217" width="24.453125" style="2" customWidth="1"/>
+    <col min="8965" max="8965" width="83.88671875" style="2" customWidth="1"/>
+    <col min="8966" max="9216" width="14.109375" style="2"/>
+    <col min="9217" max="9217" width="24.44140625" style="2" customWidth="1"/>
     <col min="9218" max="9218" width="36" style="2" customWidth="1"/>
-    <col min="9219" max="9219" width="23.6328125" style="2" customWidth="1"/>
+    <col min="9219" max="9219" width="23.6640625" style="2" customWidth="1"/>
     <col min="9220" max="9220" width="16" style="2" customWidth="1"/>
-    <col min="9221" max="9221" width="83.90625" style="2" customWidth="1"/>
-    <col min="9222" max="9472" width="14.08984375" style="2"/>
-    <col min="9473" max="9473" width="24.453125" style="2" customWidth="1"/>
+    <col min="9221" max="9221" width="83.88671875" style="2" customWidth="1"/>
+    <col min="9222" max="9472" width="14.109375" style="2"/>
+    <col min="9473" max="9473" width="24.44140625" style="2" customWidth="1"/>
     <col min="9474" max="9474" width="36" style="2" customWidth="1"/>
-    <col min="9475" max="9475" width="23.6328125" style="2" customWidth="1"/>
+    <col min="9475" max="9475" width="23.6640625" style="2" customWidth="1"/>
     <col min="9476" max="9476" width="16" style="2" customWidth="1"/>
-    <col min="9477" max="9477" width="83.90625" style="2" customWidth="1"/>
-    <col min="9478" max="9728" width="14.08984375" style="2"/>
-    <col min="9729" max="9729" width="24.453125" style="2" customWidth="1"/>
+    <col min="9477" max="9477" width="83.88671875" style="2" customWidth="1"/>
+    <col min="9478" max="9728" width="14.109375" style="2"/>
+    <col min="9729" max="9729" width="24.44140625" style="2" customWidth="1"/>
     <col min="9730" max="9730" width="36" style="2" customWidth="1"/>
-    <col min="9731" max="9731" width="23.6328125" style="2" customWidth="1"/>
+    <col min="9731" max="9731" width="23.6640625" style="2" customWidth="1"/>
     <col min="9732" max="9732" width="16" style="2" customWidth="1"/>
-    <col min="9733" max="9733" width="83.90625" style="2" customWidth="1"/>
-    <col min="9734" max="9984" width="14.08984375" style="2"/>
-    <col min="9985" max="9985" width="24.453125" style="2" customWidth="1"/>
+    <col min="9733" max="9733" width="83.88671875" style="2" customWidth="1"/>
+    <col min="9734" max="9984" width="14.109375" style="2"/>
+    <col min="9985" max="9985" width="24.44140625" style="2" customWidth="1"/>
     <col min="9986" max="9986" width="36" style="2" customWidth="1"/>
-    <col min="9987" max="9987" width="23.6328125" style="2" customWidth="1"/>
+    <col min="9987" max="9987" width="23.6640625" style="2" customWidth="1"/>
     <col min="9988" max="9988" width="16" style="2" customWidth="1"/>
-    <col min="9989" max="9989" width="83.90625" style="2" customWidth="1"/>
-    <col min="9990" max="10240" width="14.08984375" style="2"/>
-    <col min="10241" max="10241" width="24.453125" style="2" customWidth="1"/>
+    <col min="9989" max="9989" width="83.88671875" style="2" customWidth="1"/>
+    <col min="9990" max="10240" width="14.109375" style="2"/>
+    <col min="10241" max="10241" width="24.44140625" style="2" customWidth="1"/>
     <col min="10242" max="10242" width="36" style="2" customWidth="1"/>
-    <col min="10243" max="10243" width="23.6328125" style="2" customWidth="1"/>
+    <col min="10243" max="10243" width="23.6640625" style="2" customWidth="1"/>
     <col min="10244" max="10244" width="16" style="2" customWidth="1"/>
-    <col min="10245" max="10245" width="83.90625" style="2" customWidth="1"/>
-    <col min="10246" max="10496" width="14.08984375" style="2"/>
-    <col min="10497" max="10497" width="24.453125" style="2" customWidth="1"/>
+    <col min="10245" max="10245" width="83.88671875" style="2" customWidth="1"/>
+    <col min="10246" max="10496" width="14.109375" style="2"/>
+    <col min="10497" max="10497" width="24.44140625" style="2" customWidth="1"/>
     <col min="10498" max="10498" width="36" style="2" customWidth="1"/>
-    <col min="10499" max="10499" width="23.6328125" style="2" customWidth="1"/>
+    <col min="10499" max="10499" width="23.6640625" style="2" customWidth="1"/>
     <col min="10500" max="10500" width="16" style="2" customWidth="1"/>
-    <col min="10501" max="10501" width="83.90625" style="2" customWidth="1"/>
-    <col min="10502" max="10752" width="14.08984375" style="2"/>
-    <col min="10753" max="10753" width="24.453125" style="2" customWidth="1"/>
+    <col min="10501" max="10501" width="83.88671875" style="2" customWidth="1"/>
+    <col min="10502" max="10752" width="14.109375" style="2"/>
+    <col min="10753" max="10753" width="24.44140625" style="2" customWidth="1"/>
     <col min="10754" max="10754" width="36" style="2" customWidth="1"/>
-    <col min="10755" max="10755" width="23.6328125" style="2" customWidth="1"/>
+    <col min="10755" max="10755" width="23.6640625" style="2" customWidth="1"/>
     <col min="10756" max="10756" width="16" style="2" customWidth="1"/>
-    <col min="10757" max="10757" width="83.90625" style="2" customWidth="1"/>
-    <col min="10758" max="11008" width="14.08984375" style="2"/>
-    <col min="11009" max="11009" width="24.453125" style="2" customWidth="1"/>
+    <col min="10757" max="10757" width="83.88671875" style="2" customWidth="1"/>
+    <col min="10758" max="11008" width="14.109375" style="2"/>
+    <col min="11009" max="11009" width="24.44140625" style="2" customWidth="1"/>
     <col min="11010" max="11010" width="36" style="2" customWidth="1"/>
-    <col min="11011" max="11011" width="23.6328125" style="2" customWidth="1"/>
+    <col min="11011" max="11011" width="23.6640625" style="2" customWidth="1"/>
     <col min="11012" max="11012" width="16" style="2" customWidth="1"/>
-    <col min="11013" max="11013" width="83.90625" style="2" customWidth="1"/>
-    <col min="11014" max="11264" width="14.08984375" style="2"/>
-    <col min="11265" max="11265" width="24.453125" style="2" customWidth="1"/>
+    <col min="11013" max="11013" width="83.88671875" style="2" customWidth="1"/>
+    <col min="11014" max="11264" width="14.109375" style="2"/>
+    <col min="11265" max="11265" width="24.44140625" style="2" customWidth="1"/>
     <col min="11266" max="11266" width="36" style="2" customWidth="1"/>
-    <col min="11267" max="11267" width="23.6328125" style="2" customWidth="1"/>
+    <col min="11267" max="11267" width="23.6640625" style="2" customWidth="1"/>
     <col min="11268" max="11268" width="16" style="2" customWidth="1"/>
-    <col min="11269" max="11269" width="83.90625" style="2" customWidth="1"/>
-    <col min="11270" max="11520" width="14.08984375" style="2"/>
-    <col min="11521" max="11521" width="24.453125" style="2" customWidth="1"/>
+    <col min="11269" max="11269" width="83.88671875" style="2" customWidth="1"/>
+    <col min="11270" max="11520" width="14.109375" style="2"/>
+    <col min="11521" max="11521" width="24.44140625" style="2" customWidth="1"/>
     <col min="11522" max="11522" width="36" style="2" customWidth="1"/>
-    <col min="11523" max="11523" width="23.6328125" style="2" customWidth="1"/>
+    <col min="11523" max="11523" width="23.6640625" style="2" customWidth="1"/>
     <col min="11524" max="11524" width="16" style="2" customWidth="1"/>
-    <col min="11525" max="11525" width="83.90625" style="2" customWidth="1"/>
-    <col min="11526" max="11776" width="14.08984375" style="2"/>
-    <col min="11777" max="11777" width="24.453125" style="2" customWidth="1"/>
+    <col min="11525" max="11525" width="83.88671875" style="2" customWidth="1"/>
+    <col min="11526" max="11776" width="14.109375" style="2"/>
+    <col min="11777" max="11777" width="24.44140625" style="2" customWidth="1"/>
     <col min="11778" max="11778" width="36" style="2" customWidth="1"/>
-    <col min="11779" max="11779" width="23.6328125" style="2" customWidth="1"/>
+    <col min="11779" max="11779" width="23.6640625" style="2" customWidth="1"/>
     <col min="11780" max="11780" width="16" style="2" customWidth="1"/>
-    <col min="11781" max="11781" width="83.90625" style="2" customWidth="1"/>
-    <col min="11782" max="12032" width="14.08984375" style="2"/>
-    <col min="12033" max="12033" width="24.453125" style="2" customWidth="1"/>
+    <col min="11781" max="11781" width="83.88671875" style="2" customWidth="1"/>
+    <col min="11782" max="12032" width="14.109375" style="2"/>
+    <col min="12033" max="12033" width="24.44140625" style="2" customWidth="1"/>
     <col min="12034" max="12034" width="36" style="2" customWidth="1"/>
-    <col min="12035" max="12035" width="23.6328125" style="2" customWidth="1"/>
+    <col min="12035" max="12035" width="23.6640625" style="2" customWidth="1"/>
     <col min="12036" max="12036" width="16" style="2" customWidth="1"/>
-    <col min="12037" max="12037" width="83.90625" style="2" customWidth="1"/>
-    <col min="12038" max="12288" width="14.08984375" style="2"/>
-    <col min="12289" max="12289" width="24.453125" style="2" customWidth="1"/>
+    <col min="12037" max="12037" width="83.88671875" style="2" customWidth="1"/>
+    <col min="12038" max="12288" width="14.109375" style="2"/>
+    <col min="12289" max="12289" width="24.44140625" style="2" customWidth="1"/>
     <col min="12290" max="12290" width="36" style="2" customWidth="1"/>
-    <col min="12291" max="12291" width="23.6328125" style="2" customWidth="1"/>
+    <col min="12291" max="12291" width="23.6640625" style="2" customWidth="1"/>
     <col min="12292" max="12292" width="16" style="2" customWidth="1"/>
-    <col min="12293" max="12293" width="83.90625" style="2" customWidth="1"/>
-    <col min="12294" max="12544" width="14.08984375" style="2"/>
-    <col min="12545" max="12545" width="24.453125" style="2" customWidth="1"/>
+    <col min="12293" max="12293" width="83.88671875" style="2" customWidth="1"/>
+    <col min="12294" max="12544" width="14.109375" style="2"/>
+    <col min="12545" max="12545" width="24.44140625" style="2" customWidth="1"/>
     <col min="12546" max="12546" width="36" style="2" customWidth="1"/>
-    <col min="12547" max="12547" width="23.6328125" style="2" customWidth="1"/>
+    <col min="12547" max="12547" width="23.6640625" style="2" customWidth="1"/>
     <col min="12548" max="12548" width="16" style="2" customWidth="1"/>
-    <col min="12549" max="12549" width="83.90625" style="2" customWidth="1"/>
-    <col min="12550" max="12800" width="14.08984375" style="2"/>
-    <col min="12801" max="12801" width="24.453125" style="2" customWidth="1"/>
+    <col min="12549" max="12549" width="83.88671875" style="2" customWidth="1"/>
+    <col min="12550" max="12800" width="14.109375" style="2"/>
+    <col min="12801" max="12801" width="24.44140625" style="2" customWidth="1"/>
     <col min="12802" max="12802" width="36" style="2" customWidth="1"/>
-    <col min="12803" max="12803" width="23.6328125" style="2" customWidth="1"/>
+    <col min="12803" max="12803" width="23.6640625" style="2" customWidth="1"/>
     <col min="12804" max="12804" width="16" style="2" customWidth="1"/>
-    <col min="12805" max="12805" width="83.90625" style="2" customWidth="1"/>
-    <col min="12806" max="13056" width="14.08984375" style="2"/>
-    <col min="13057" max="13057" width="24.453125" style="2" customWidth="1"/>
+    <col min="12805" max="12805" width="83.88671875" style="2" customWidth="1"/>
+    <col min="12806" max="13056" width="14.109375" style="2"/>
+    <col min="13057" max="13057" width="24.44140625" style="2" customWidth="1"/>
     <col min="13058" max="13058" width="36" style="2" customWidth="1"/>
-    <col min="13059" max="13059" width="23.6328125" style="2" customWidth="1"/>
+    <col min="13059" max="13059" width="23.6640625" style="2" customWidth="1"/>
     <col min="13060" max="13060" width="16" style="2" customWidth="1"/>
-    <col min="13061" max="13061" width="83.90625" style="2" customWidth="1"/>
-    <col min="13062" max="13312" width="14.08984375" style="2"/>
-    <col min="13313" max="13313" width="24.453125" style="2" customWidth="1"/>
+    <col min="13061" max="13061" width="83.88671875" style="2" customWidth="1"/>
+    <col min="13062" max="13312" width="14.109375" style="2"/>
+    <col min="13313" max="13313" width="24.44140625" style="2" customWidth="1"/>
     <col min="13314" max="13314" width="36" style="2" customWidth="1"/>
-    <col min="13315" max="13315" width="23.6328125" style="2" customWidth="1"/>
+    <col min="13315" max="13315" width="23.6640625" style="2" customWidth="1"/>
     <col min="13316" max="13316" width="16" style="2" customWidth="1"/>
-    <col min="13317" max="13317" width="83.90625" style="2" customWidth="1"/>
-    <col min="13318" max="13568" width="14.08984375" style="2"/>
-    <col min="13569" max="13569" width="24.453125" style="2" customWidth="1"/>
+    <col min="13317" max="13317" width="83.88671875" style="2" customWidth="1"/>
+    <col min="13318" max="13568" width="14.109375" style="2"/>
+    <col min="13569" max="13569" width="24.44140625" style="2" customWidth="1"/>
     <col min="13570" max="13570" width="36" style="2" customWidth="1"/>
-    <col min="13571" max="13571" width="23.6328125" style="2" customWidth="1"/>
+    <col min="13571" max="13571" width="23.6640625" style="2" customWidth="1"/>
     <col min="13572" max="13572" width="16" style="2" customWidth="1"/>
-    <col min="13573" max="13573" width="83.90625" style="2" customWidth="1"/>
-    <col min="13574" max="13824" width="14.08984375" style="2"/>
-    <col min="13825" max="13825" width="24.453125" style="2" customWidth="1"/>
+    <col min="13573" max="13573" width="83.88671875" style="2" customWidth="1"/>
+    <col min="13574" max="13824" width="14.109375" style="2"/>
+    <col min="13825" max="13825" width="24.44140625" style="2" customWidth="1"/>
     <col min="13826" max="13826" width="36" style="2" customWidth="1"/>
-    <col min="13827" max="13827" width="23.6328125" style="2" customWidth="1"/>
+    <col min="13827" max="13827" width="23.6640625" style="2" customWidth="1"/>
     <col min="13828" max="13828" width="16" style="2" customWidth="1"/>
-    <col min="13829" max="13829" width="83.90625" style="2" customWidth="1"/>
-    <col min="13830" max="14080" width="14.08984375" style="2"/>
-    <col min="14081" max="14081" width="24.453125" style="2" customWidth="1"/>
+    <col min="13829" max="13829" width="83.88671875" style="2" customWidth="1"/>
+    <col min="13830" max="14080" width="14.109375" style="2"/>
+    <col min="14081" max="14081" width="24.44140625" style="2" customWidth="1"/>
     <col min="14082" max="14082" width="36" style="2" customWidth="1"/>
-    <col min="14083" max="14083" width="23.6328125" style="2" customWidth="1"/>
+    <col min="14083" max="14083" width="23.6640625" style="2" customWidth="1"/>
     <col min="14084" max="14084" width="16" style="2" customWidth="1"/>
-    <col min="14085" max="14085" width="83.90625" style="2" customWidth="1"/>
-    <col min="14086" max="14336" width="14.08984375" style="2"/>
-    <col min="14337" max="14337" width="24.453125" style="2" customWidth="1"/>
+    <col min="14085" max="14085" width="83.88671875" style="2" customWidth="1"/>
+    <col min="14086" max="14336" width="14.109375" style="2"/>
+    <col min="14337" max="14337" width="24.44140625" style="2" customWidth="1"/>
     <col min="14338" max="14338" width="36" style="2" customWidth="1"/>
-    <col min="14339" max="14339" width="23.6328125" style="2" customWidth="1"/>
+    <col min="14339" max="14339" width="23.6640625" style="2" customWidth="1"/>
     <col min="14340" max="14340" width="16" style="2" customWidth="1"/>
-    <col min="14341" max="14341" width="83.90625" style="2" customWidth="1"/>
-    <col min="14342" max="14592" width="14.08984375" style="2"/>
-    <col min="14593" max="14593" width="24.453125" style="2" customWidth="1"/>
+    <col min="14341" max="14341" width="83.88671875" style="2" customWidth="1"/>
+    <col min="14342" max="14592" width="14.109375" style="2"/>
+    <col min="14593" max="14593" width="24.44140625" style="2" customWidth="1"/>
     <col min="14594" max="14594" width="36" style="2" customWidth="1"/>
-    <col min="14595" max="14595" width="23.6328125" style="2" customWidth="1"/>
+    <col min="14595" max="14595" width="23.6640625" style="2" customWidth="1"/>
     <col min="14596" max="14596" width="16" style="2" customWidth="1"/>
-    <col min="14597" max="14597" width="83.90625" style="2" customWidth="1"/>
-    <col min="14598" max="14848" width="14.08984375" style="2"/>
-    <col min="14849" max="14849" width="24.453125" style="2" customWidth="1"/>
+    <col min="14597" max="14597" width="83.88671875" style="2" customWidth="1"/>
+    <col min="14598" max="14848" width="14.109375" style="2"/>
+    <col min="14849" max="14849" width="24.44140625" style="2" customWidth="1"/>
     <col min="14850" max="14850" width="36" style="2" customWidth="1"/>
-    <col min="14851" max="14851" width="23.6328125" style="2" customWidth="1"/>
+    <col min="14851" max="14851" width="23.6640625" style="2" customWidth="1"/>
     <col min="14852" max="14852" width="16" style="2" customWidth="1"/>
-    <col min="14853" max="14853" width="83.90625" style="2" customWidth="1"/>
-    <col min="14854" max="15104" width="14.08984375" style="2"/>
-    <col min="15105" max="15105" width="24.453125" style="2" customWidth="1"/>
+    <col min="14853" max="14853" width="83.88671875" style="2" customWidth="1"/>
+    <col min="14854" max="15104" width="14.109375" style="2"/>
+    <col min="15105" max="15105" width="24.44140625" style="2" customWidth="1"/>
     <col min="15106" max="15106" width="36" style="2" customWidth="1"/>
-    <col min="15107" max="15107" width="23.6328125" style="2" customWidth="1"/>
+    <col min="15107" max="15107" width="23.6640625" style="2" customWidth="1"/>
     <col min="15108" max="15108" width="16" style="2" customWidth="1"/>
-    <col min="15109" max="15109" width="83.90625" style="2" customWidth="1"/>
-    <col min="15110" max="15360" width="14.08984375" style="2"/>
-    <col min="15361" max="15361" width="24.453125" style="2" customWidth="1"/>
+    <col min="15109" max="15109" width="83.88671875" style="2" customWidth="1"/>
+    <col min="15110" max="15360" width="14.109375" style="2"/>
+    <col min="15361" max="15361" width="24.44140625" style="2" customWidth="1"/>
     <col min="15362" max="15362" width="36" style="2" customWidth="1"/>
-    <col min="15363" max="15363" width="23.6328125" style="2" customWidth="1"/>
+    <col min="15363" max="15363" width="23.6640625" style="2" customWidth="1"/>
     <col min="15364" max="15364" width="16" style="2" customWidth="1"/>
-    <col min="15365" max="15365" width="83.90625" style="2" customWidth="1"/>
-    <col min="15366" max="15616" width="14.08984375" style="2"/>
-    <col min="15617" max="15617" width="24.453125" style="2" customWidth="1"/>
+    <col min="15365" max="15365" width="83.88671875" style="2" customWidth="1"/>
+    <col min="15366" max="15616" width="14.109375" style="2"/>
+    <col min="15617" max="15617" width="24.44140625" style="2" customWidth="1"/>
     <col min="15618" max="15618" width="36" style="2" customWidth="1"/>
-    <col min="15619" max="15619" width="23.6328125" style="2" customWidth="1"/>
+    <col min="15619" max="15619" width="23.6640625" style="2" customWidth="1"/>
     <col min="15620" max="15620" width="16" style="2" customWidth="1"/>
-    <col min="15621" max="15621" width="83.90625" style="2" customWidth="1"/>
-    <col min="15622" max="15872" width="14.08984375" style="2"/>
-    <col min="15873" max="15873" width="24.453125" style="2" customWidth="1"/>
+    <col min="15621" max="15621" width="83.88671875" style="2" customWidth="1"/>
+    <col min="15622" max="15872" width="14.109375" style="2"/>
+    <col min="15873" max="15873" width="24.44140625" style="2" customWidth="1"/>
     <col min="15874" max="15874" width="36" style="2" customWidth="1"/>
-    <col min="15875" max="15875" width="23.6328125" style="2" customWidth="1"/>
+    <col min="15875" max="15875" width="23.6640625" style="2" customWidth="1"/>
     <col min="15876" max="15876" width="16" style="2" customWidth="1"/>
-    <col min="15877" max="15877" width="83.90625" style="2" customWidth="1"/>
-    <col min="15878" max="16128" width="14.08984375" style="2"/>
-    <col min="16129" max="16129" width="24.453125" style="2" customWidth="1"/>
+    <col min="15877" max="15877" width="83.88671875" style="2" customWidth="1"/>
+    <col min="15878" max="16128" width="14.109375" style="2"/>
+    <col min="16129" max="16129" width="24.44140625" style="2" customWidth="1"/>
     <col min="16130" max="16130" width="36" style="2" customWidth="1"/>
-    <col min="16131" max="16131" width="23.6328125" style="2" customWidth="1"/>
+    <col min="16131" max="16131" width="23.6640625" style="2" customWidth="1"/>
     <col min="16132" max="16132" width="16" style="2" customWidth="1"/>
-    <col min="16133" max="16133" width="83.90625" style="2" customWidth="1"/>
-    <col min="16134" max="16384" width="14.08984375" style="2"/>
+    <col min="16133" max="16133" width="83.88671875" style="2" customWidth="1"/>
+    <col min="16134" max="16384" width="14.109375" style="2"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="9" customHeight="1"/>
     <row r="2" spans="1:5" ht="15.75" customHeight="1" thickBot="1">
-      <c r="A2" s="108"/>
-      <c r="B2" s="109"/>
-      <c r="C2" s="109"/>
-      <c r="D2" s="109"/>
-      <c r="E2" s="109"/>
+      <c r="A2" s="93"/>
+      <c r="B2" s="94"/>
+      <c r="C2" s="94"/>
+      <c r="D2" s="94"/>
+      <c r="E2" s="94"/>
     </row>
     <row r="3" spans="1:5" ht="15" customHeight="1">
-      <c r="A3" s="110" t="s">
+      <c r="A3" s="95" t="s">
         <v>64</v>
       </c>
-      <c r="B3" s="112" t="s">
+      <c r="B3" s="97" t="s">
         <v>65</v>
       </c>
-      <c r="C3" s="114" t="s">
+      <c r="C3" s="99" t="s">
         <v>66</v>
       </c>
-      <c r="D3" s="114" t="s">
+      <c r="D3" s="99" t="s">
         <v>67</v>
       </c>
-      <c r="E3" s="112" t="s">
+      <c r="E3" s="97" t="s">
         <v>68</v>
       </c>
     </row>
     <row r="4" spans="1:5" ht="45" customHeight="1" thickBot="1">
-      <c r="A4" s="111"/>
-      <c r="B4" s="113"/>
-      <c r="C4" s="115"/>
-      <c r="D4" s="115"/>
-      <c r="E4" s="113"/>
+      <c r="A4" s="96"/>
+      <c r="B4" s="98"/>
+      <c r="C4" s="100"/>
+      <c r="D4" s="100"/>
+      <c r="E4" s="98"/>
     </row>
     <row r="5" spans="1:5" ht="73.5" customHeight="1" thickBot="1">
       <c r="A5" s="3" t="s">
@@ -46505,10 +46542,10 @@
       <c r="E7" s="7"/>
     </row>
     <row r="8" spans="1:5" ht="22.5" customHeight="1">
-      <c r="A8" s="107" t="s">
+      <c r="A8" s="113" t="s">
         <v>71</v>
       </c>
-      <c r="B8" s="100"/>
+      <c r="B8" s="101"/>
       <c r="C8" s="8">
         <v>642436</v>
       </c>
@@ -46520,8 +46557,8 @@
       </c>
     </row>
     <row r="9" spans="1:5" ht="17.25" customHeight="1">
-      <c r="A9" s="93"/>
-      <c r="B9" s="101"/>
+      <c r="A9" s="105"/>
+      <c r="B9" s="102"/>
       <c r="C9" s="9">
         <v>642437</v>
       </c>
@@ -46533,8 +46570,8 @@
       </c>
     </row>
     <row r="10" spans="1:5">
-      <c r="A10" s="93"/>
-      <c r="B10" s="101"/>
+      <c r="A10" s="105"/>
+      <c r="B10" s="102"/>
       <c r="C10" s="9">
         <v>642438</v>
       </c>
@@ -46546,8 +46583,8 @@
       </c>
     </row>
     <row r="11" spans="1:5">
-      <c r="A11" s="93"/>
-      <c r="B11" s="101"/>
+      <c r="A11" s="105"/>
+      <c r="B11" s="102"/>
       <c r="C11" s="9">
         <v>642439</v>
       </c>
@@ -46559,10 +46596,10 @@
       </c>
     </row>
     <row r="12" spans="1:5">
-      <c r="A12" s="99" t="s">
+      <c r="A12" s="104" t="s">
         <v>72</v>
       </c>
-      <c r="B12" s="101"/>
+      <c r="B12" s="102"/>
       <c r="C12" s="9">
         <v>642440</v>
       </c>
@@ -46574,8 +46611,8 @@
       </c>
     </row>
     <row r="13" spans="1:5">
-      <c r="A13" s="93"/>
-      <c r="B13" s="101"/>
+      <c r="A13" s="105"/>
+      <c r="B13" s="102"/>
       <c r="C13" s="9">
         <v>642441</v>
       </c>
@@ -46587,8 +46624,8 @@
       </c>
     </row>
     <row r="14" spans="1:5">
-      <c r="A14" s="93"/>
-      <c r="B14" s="101"/>
+      <c r="A14" s="105"/>
+      <c r="B14" s="102"/>
       <c r="C14" s="9">
         <v>642442</v>
       </c>
@@ -46600,8 +46637,8 @@
       </c>
     </row>
     <row r="15" spans="1:5">
-      <c r="A15" s="93"/>
-      <c r="B15" s="101"/>
+      <c r="A15" s="105"/>
+      <c r="B15" s="102"/>
       <c r="C15" s="11">
         <v>642443</v>
       </c>
@@ -46613,10 +46650,10 @@
       </c>
     </row>
     <row r="16" spans="1:5">
-      <c r="A16" s="99" t="s">
+      <c r="A16" s="104" t="s">
         <v>73</v>
       </c>
-      <c r="B16" s="101"/>
+      <c r="B16" s="102"/>
       <c r="C16" s="9">
         <v>642444</v>
       </c>
@@ -46628,8 +46665,8 @@
       </c>
     </row>
     <row r="17" spans="1:5">
-      <c r="A17" s="93"/>
-      <c r="B17" s="101"/>
+      <c r="A17" s="105"/>
+      <c r="B17" s="102"/>
       <c r="C17" s="9">
         <v>642445</v>
       </c>
@@ -46641,8 +46678,8 @@
       </c>
     </row>
     <row r="18" spans="1:5">
-      <c r="A18" s="93"/>
-      <c r="B18" s="101"/>
+      <c r="A18" s="105"/>
+      <c r="B18" s="102"/>
       <c r="C18" s="9">
         <v>642446</v>
       </c>
@@ -46654,8 +46691,8 @@
       </c>
     </row>
     <row r="19" spans="1:5">
-      <c r="A19" s="93"/>
-      <c r="B19" s="101"/>
+      <c r="A19" s="105"/>
+      <c r="B19" s="102"/>
       <c r="C19" s="9">
         <v>642447</v>
       </c>
@@ -46667,10 +46704,10 @@
       </c>
     </row>
     <row r="20" spans="1:5">
-      <c r="A20" s="99" t="s">
+      <c r="A20" s="104" t="s">
         <v>74</v>
       </c>
-      <c r="B20" s="101"/>
+      <c r="B20" s="102"/>
       <c r="C20" s="13" t="s">
         <v>75</v>
       </c>
@@ -46682,8 +46719,8 @@
       </c>
     </row>
     <row r="21" spans="1:5">
-      <c r="A21" s="93"/>
-      <c r="B21" s="101"/>
+      <c r="A21" s="105"/>
+      <c r="B21" s="102"/>
       <c r="C21" s="13" t="s">
         <v>76</v>
       </c>
@@ -46694,9 +46731,9 @@
         <v>33</v>
       </c>
     </row>
-    <row r="22" spans="1:5" ht="14.5" thickBot="1">
-      <c r="A22" s="94"/>
-      <c r="B22" s="102"/>
+    <row r="22" spans="1:5" ht="14.4" thickBot="1">
+      <c r="A22" s="106"/>
+      <c r="B22" s="103"/>
       <c r="C22" s="14" t="s">
         <v>77</v>
       </c>
@@ -46713,17 +46750,17 @@
       <c r="D23" s="6"/>
       <c r="E23" s="7"/>
     </row>
-    <row r="24" spans="1:5" ht="14.5" thickBot="1">
+    <row r="24" spans="1:5" ht="14.4" thickBot="1">
       <c r="A24" s="5"/>
       <c r="C24" s="6"/>
       <c r="D24" s="6"/>
       <c r="E24" s="7"/>
     </row>
-    <row r="25" spans="1:5" ht="14" customHeight="1">
-      <c r="A25" s="107" t="s">
+    <row r="25" spans="1:5" ht="13.95" customHeight="1">
+      <c r="A25" s="113" t="s">
         <v>78</v>
       </c>
-      <c r="B25" s="100"/>
+      <c r="B25" s="101"/>
       <c r="C25" s="8">
         <v>312797</v>
       </c>
@@ -46735,8 +46772,8 @@
       </c>
     </row>
     <row r="26" spans="1:5">
-      <c r="A26" s="93"/>
-      <c r="B26" s="101"/>
+      <c r="A26" s="105"/>
+      <c r="B26" s="102"/>
       <c r="C26" s="9">
         <v>312798</v>
       </c>
@@ -46748,8 +46785,8 @@
       </c>
     </row>
     <row r="27" spans="1:5">
-      <c r="A27" s="93"/>
-      <c r="B27" s="101"/>
+      <c r="A27" s="105"/>
+      <c r="B27" s="102"/>
       <c r="C27" s="9">
         <v>312799</v>
       </c>
@@ -46761,8 +46798,8 @@
       </c>
     </row>
     <row r="28" spans="1:5">
-      <c r="A28" s="93"/>
-      <c r="B28" s="101"/>
+      <c r="A28" s="105"/>
+      <c r="B28" s="102"/>
       <c r="C28" s="9">
         <v>312800</v>
       </c>
@@ -46774,10 +46811,10 @@
       </c>
     </row>
     <row r="29" spans="1:5">
-      <c r="A29" s="99" t="s">
+      <c r="A29" s="104" t="s">
         <v>79</v>
       </c>
-      <c r="B29" s="101"/>
+      <c r="B29" s="102"/>
       <c r="C29" s="9">
         <v>312802</v>
       </c>
@@ -46789,8 +46826,8 @@
       </c>
     </row>
     <row r="30" spans="1:5">
-      <c r="A30" s="93"/>
-      <c r="B30" s="101"/>
+      <c r="A30" s="105"/>
+      <c r="B30" s="102"/>
       <c r="C30" s="9">
         <v>312803</v>
       </c>
@@ -46802,8 +46839,8 @@
       </c>
     </row>
     <row r="31" spans="1:5">
-      <c r="A31" s="93"/>
-      <c r="B31" s="101"/>
+      <c r="A31" s="105"/>
+      <c r="B31" s="102"/>
       <c r="C31" s="9">
         <v>312804</v>
       </c>
@@ -46815,8 +46852,8 @@
       </c>
     </row>
     <row r="32" spans="1:5">
-      <c r="A32" s="93"/>
-      <c r="B32" s="101"/>
+      <c r="A32" s="105"/>
+      <c r="B32" s="102"/>
       <c r="C32" s="9">
         <v>312805</v>
       </c>
@@ -46828,10 +46865,10 @@
       </c>
     </row>
     <row r="33" spans="1:5">
-      <c r="A33" s="99" t="s">
+      <c r="A33" s="104" t="s">
         <v>80</v>
       </c>
-      <c r="B33" s="101"/>
+      <c r="B33" s="102"/>
       <c r="C33" s="9">
         <v>312807</v>
       </c>
@@ -46843,8 +46880,8 @@
       </c>
     </row>
     <row r="34" spans="1:5">
-      <c r="A34" s="93"/>
-      <c r="B34" s="101"/>
+      <c r="A34" s="105"/>
+      <c r="B34" s="102"/>
       <c r="C34" s="9">
         <v>312808</v>
       </c>
@@ -46856,8 +46893,8 @@
       </c>
     </row>
     <row r="35" spans="1:5">
-      <c r="A35" s="93"/>
-      <c r="B35" s="101"/>
+      <c r="A35" s="105"/>
+      <c r="B35" s="102"/>
       <c r="C35" s="9">
         <v>312809</v>
       </c>
@@ -46869,8 +46906,8 @@
       </c>
     </row>
     <row r="36" spans="1:5">
-      <c r="A36" s="93"/>
-      <c r="B36" s="101"/>
+      <c r="A36" s="105"/>
+      <c r="B36" s="102"/>
       <c r="C36" s="9">
         <v>312810</v>
       </c>
@@ -46882,10 +46919,10 @@
       </c>
     </row>
     <row r="37" spans="1:5">
-      <c r="A37" s="99" t="s">
+      <c r="A37" s="104" t="s">
         <v>81</v>
       </c>
-      <c r="B37" s="101"/>
+      <c r="B37" s="102"/>
       <c r="C37" s="9">
         <v>490442</v>
       </c>
@@ -46897,8 +46934,8 @@
       </c>
     </row>
     <row r="38" spans="1:5">
-      <c r="A38" s="93"/>
-      <c r="B38" s="101"/>
+      <c r="A38" s="105"/>
+      <c r="B38" s="102"/>
       <c r="C38" s="9">
         <v>490441</v>
       </c>
@@ -46909,9 +46946,9 @@
         <v>50</v>
       </c>
     </row>
-    <row r="39" spans="1:5" ht="14.5" thickBot="1">
-      <c r="A39" s="94"/>
-      <c r="B39" s="102"/>
+    <row r="39" spans="1:5" ht="14.4" thickBot="1">
+      <c r="A39" s="106"/>
+      <c r="B39" s="103"/>
       <c r="C39" s="15">
         <v>490440</v>
       </c>
@@ -46922,7 +46959,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="40" spans="1:5" ht="14.5" thickBot="1">
+    <row r="40" spans="1:5" ht="14.4" thickBot="1">
       <c r="A40" s="5"/>
       <c r="B40" s="17"/>
       <c r="C40" s="6"/>
@@ -46930,7 +46967,7 @@
       <c r="E40" s="7"/>
     </row>
     <row r="41" spans="1:5" ht="51" customHeight="1">
-      <c r="A41" s="103" t="s">
+      <c r="A41" s="109" t="s">
         <v>82</v>
       </c>
       <c r="B41" s="18"/>
@@ -46945,7 +46982,7 @@
       </c>
     </row>
     <row r="42" spans="1:5" ht="48" customHeight="1" thickBot="1">
-      <c r="A42" s="104"/>
+      <c r="A42" s="110"/>
       <c r="B42" s="20"/>
       <c r="C42" s="15">
         <v>314417</v>
@@ -46957,17 +46994,17 @@
         <v>84</v>
       </c>
     </row>
-    <row r="43" spans="1:5" ht="14.5" thickBot="1">
+    <row r="43" spans="1:5" ht="14.4" thickBot="1">
       <c r="A43" s="5"/>
       <c r="C43" s="6"/>
       <c r="D43" s="6"/>
       <c r="E43" s="7"/>
     </row>
     <row r="44" spans="1:5" ht="20.25" customHeight="1">
-      <c r="A44" s="105" t="s">
+      <c r="A44" s="111" t="s">
         <v>85</v>
       </c>
-      <c r="B44" s="100"/>
+      <c r="B44" s="101"/>
       <c r="C44" s="8">
         <v>643863</v>
       </c>
@@ -46979,8 +47016,8 @@
       </c>
     </row>
     <row r="45" spans="1:5">
-      <c r="A45" s="106"/>
-      <c r="B45" s="101"/>
+      <c r="A45" s="112"/>
+      <c r="B45" s="102"/>
       <c r="C45" s="9">
         <v>643864</v>
       </c>
@@ -46992,8 +47029,8 @@
       </c>
     </row>
     <row r="46" spans="1:5">
-      <c r="A46" s="106"/>
-      <c r="B46" s="101"/>
+      <c r="A46" s="112"/>
+      <c r="B46" s="102"/>
       <c r="C46" s="9">
         <v>643865</v>
       </c>
@@ -47004,9 +47041,9 @@
         <v>88</v>
       </c>
     </row>
-    <row r="47" spans="1:5" ht="14.5" thickBot="1">
-      <c r="A47" s="104"/>
-      <c r="B47" s="102"/>
+    <row r="47" spans="1:5" ht="14.4" thickBot="1">
+      <c r="A47" s="110"/>
+      <c r="B47" s="103"/>
       <c r="C47" s="14" t="s">
         <v>89</v>
       </c>
@@ -47017,13 +47054,13 @@
         <v>91</v>
       </c>
     </row>
-    <row r="48" spans="1:5" ht="14.5" thickBot="1">
+    <row r="48" spans="1:5" ht="14.4" thickBot="1">
       <c r="A48" s="5"/>
       <c r="C48" s="6"/>
       <c r="D48" s="6"/>
       <c r="E48" s="7"/>
     </row>
-    <row r="49" spans="1:5" ht="57.65" customHeight="1" thickBot="1">
+    <row r="49" spans="1:5" ht="57.6" customHeight="1" thickBot="1">
       <c r="A49" s="25" t="s">
         <v>92</v>
       </c>
@@ -47037,7 +47074,7 @@
       <c r="E49" s="29"/>
     </row>
     <row r="50" spans="1:5">
-      <c r="A50" s="107" t="s">
+      <c r="A50" s="113" t="s">
         <v>95</v>
       </c>
       <c r="B50" s="30" t="s">
@@ -47047,10 +47084,10 @@
         <v>642913</v>
       </c>
       <c r="D50" s="32"/>
-      <c r="E50" s="95"/>
+      <c r="E50" s="107"/>
     </row>
     <row r="51" spans="1:5">
-      <c r="A51" s="93"/>
+      <c r="A51" s="105"/>
       <c r="B51" s="33" t="s">
         <v>97</v>
       </c>
@@ -47058,10 +47095,10 @@
         <v>643863</v>
       </c>
       <c r="D51" s="32"/>
-      <c r="E51" s="96"/>
+      <c r="E51" s="108"/>
     </row>
     <row r="52" spans="1:5">
-      <c r="A52" s="93"/>
+      <c r="A52" s="105"/>
       <c r="B52" s="35" t="s">
         <v>98</v>
       </c>
@@ -47069,10 +47106,10 @@
         <v>206878</v>
       </c>
       <c r="D52" s="32"/>
-      <c r="E52" s="96"/>
+      <c r="E52" s="108"/>
     </row>
     <row r="53" spans="1:5">
-      <c r="A53" s="93"/>
+      <c r="A53" s="105"/>
       <c r="B53" s="35" t="s">
         <v>99</v>
       </c>
@@ -47080,10 +47117,10 @@
         <v>206894</v>
       </c>
       <c r="D53" s="32"/>
-      <c r="E53" s="96"/>
+      <c r="E53" s="108"/>
     </row>
     <row r="54" spans="1:5">
-      <c r="A54" s="99" t="s">
+      <c r="A54" s="104" t="s">
         <v>100</v>
       </c>
       <c r="B54" s="35" t="s">
@@ -47093,10 +47130,10 @@
         <v>642913</v>
       </c>
       <c r="D54" s="32"/>
-      <c r="E54" s="95"/>
+      <c r="E54" s="107"/>
     </row>
     <row r="55" spans="1:5">
-      <c r="A55" s="93"/>
+      <c r="A55" s="105"/>
       <c r="B55" s="35" t="s">
         <v>101</v>
       </c>
@@ -47104,10 +47141,10 @@
         <v>643864</v>
       </c>
       <c r="D55" s="32"/>
-      <c r="E55" s="96"/>
+      <c r="E55" s="108"/>
     </row>
     <row r="56" spans="1:5">
-      <c r="A56" s="93"/>
+      <c r="A56" s="105"/>
       <c r="B56" s="33" t="s">
         <v>102</v>
       </c>
@@ -47115,10 +47152,10 @@
         <v>315577</v>
       </c>
       <c r="D56" s="32"/>
-      <c r="E56" s="96"/>
+      <c r="E56" s="108"/>
     </row>
     <row r="57" spans="1:5">
-      <c r="A57" s="93"/>
+      <c r="A57" s="105"/>
       <c r="B57" s="33" t="s">
         <v>103</v>
       </c>
@@ -47126,10 +47163,10 @@
         <v>315578</v>
       </c>
       <c r="D57" s="32"/>
-      <c r="E57" s="96"/>
+      <c r="E57" s="108"/>
     </row>
     <row r="58" spans="1:5">
-      <c r="A58" s="93" t="s">
+      <c r="A58" s="105" t="s">
         <v>104</v>
       </c>
       <c r="B58" s="35" t="s">
@@ -47139,10 +47176,10 @@
         <v>642913</v>
       </c>
       <c r="D58" s="32"/>
-      <c r="E58" s="95"/>
+      <c r="E58" s="107"/>
     </row>
     <row r="59" spans="1:5">
-      <c r="A59" s="93"/>
+      <c r="A59" s="105"/>
       <c r="B59" s="35" t="s">
         <v>105</v>
       </c>
@@ -47150,10 +47187,10 @@
         <v>643865</v>
       </c>
       <c r="D59" s="32"/>
-      <c r="E59" s="96"/>
+      <c r="E59" s="108"/>
     </row>
     <row r="60" spans="1:5">
-      <c r="A60" s="93"/>
+      <c r="A60" s="105"/>
       <c r="B60" s="35" t="s">
         <v>106</v>
       </c>
@@ -47161,10 +47198,10 @@
         <v>242080</v>
       </c>
       <c r="D60" s="32"/>
-      <c r="E60" s="96"/>
+      <c r="E60" s="108"/>
     </row>
     <row r="61" spans="1:5">
-      <c r="A61" s="93"/>
+      <c r="A61" s="105"/>
       <c r="B61" s="35" t="s">
         <v>107</v>
       </c>
@@ -47172,10 +47209,10 @@
         <v>242073</v>
       </c>
       <c r="D61" s="32"/>
-      <c r="E61" s="96"/>
+      <c r="E61" s="108"/>
     </row>
     <row r="62" spans="1:5">
-      <c r="A62" s="99" t="s">
+      <c r="A62" s="104" t="s">
         <v>108</v>
       </c>
       <c r="B62" s="35" t="s">
@@ -47185,10 +47222,10 @@
         <v>642913</v>
       </c>
       <c r="D62" s="32"/>
-      <c r="E62" s="95"/>
-    </row>
-    <row r="63" spans="1:5" ht="14" customHeight="1">
-      <c r="A63" s="93"/>
+      <c r="E62" s="107"/>
+    </row>
+    <row r="63" spans="1:5" ht="13.95" customHeight="1">
+      <c r="A63" s="105"/>
       <c r="B63" s="35" t="s">
         <v>109</v>
       </c>
@@ -47196,10 +47233,10 @@
         <v>738957</v>
       </c>
       <c r="D63" s="32"/>
-      <c r="E63" s="95"/>
+      <c r="E63" s="107"/>
     </row>
     <row r="64" spans="1:5">
-      <c r="A64" s="93"/>
+      <c r="A64" s="105"/>
       <c r="B64" s="35" t="s">
         <v>110</v>
       </c>
@@ -47207,10 +47244,10 @@
         <v>490996</v>
       </c>
       <c r="D64" s="32"/>
-      <c r="E64" s="95"/>
-    </row>
-    <row r="65" spans="1:5" ht="14.5" thickBot="1">
-      <c r="A65" s="94"/>
+      <c r="E64" s="107"/>
+    </row>
+    <row r="65" spans="1:5" ht="14.4" thickBot="1">
+      <c r="A65" s="106"/>
       <c r="B65" s="36" t="s">
         <v>111</v>
       </c>
@@ -47218,10 +47255,10 @@
         <v>490999</v>
       </c>
       <c r="D65" s="32"/>
-      <c r="E65" s="95"/>
+      <c r="E65" s="107"/>
     </row>
     <row r="66" spans="1:5">
-      <c r="A66" s="98" t="s">
+      <c r="A66" s="114" t="s">
         <v>112</v>
       </c>
       <c r="B66" s="30" t="s">
@@ -47231,10 +47268,10 @@
         <v>642914</v>
       </c>
       <c r="D66" s="32"/>
-      <c r="E66" s="95"/>
-    </row>
-    <row r="67" spans="1:5" ht="14" customHeight="1">
-      <c r="A67" s="93"/>
+      <c r="E66" s="107"/>
+    </row>
+    <row r="67" spans="1:5" ht="13.95" customHeight="1">
+      <c r="A67" s="105"/>
       <c r="B67" s="35" t="s">
         <v>97</v>
       </c>
@@ -47242,10 +47279,10 @@
         <v>643863</v>
       </c>
       <c r="D67" s="32"/>
-      <c r="E67" s="96"/>
+      <c r="E67" s="108"/>
     </row>
     <row r="68" spans="1:5">
-      <c r="A68" s="93"/>
+      <c r="A68" s="105"/>
       <c r="B68" s="35" t="s">
         <v>114</v>
       </c>
@@ -47253,10 +47290,10 @@
         <v>206880</v>
       </c>
       <c r="D68" s="32"/>
-      <c r="E68" s="96"/>
+      <c r="E68" s="108"/>
     </row>
     <row r="69" spans="1:5">
-      <c r="A69" s="93"/>
+      <c r="A69" s="105"/>
       <c r="B69" s="35" t="s">
         <v>115</v>
       </c>
@@ -47264,10 +47301,10 @@
         <v>206896</v>
       </c>
       <c r="D69" s="32"/>
-      <c r="E69" s="96"/>
+      <c r="E69" s="108"/>
     </row>
     <row r="70" spans="1:5">
-      <c r="A70" s="93" t="s">
+      <c r="A70" s="105" t="s">
         <v>116</v>
       </c>
       <c r="B70" s="35" t="s">
@@ -47277,10 +47314,10 @@
         <v>642914</v>
       </c>
       <c r="D70" s="32"/>
-      <c r="E70" s="95"/>
-    </row>
-    <row r="71" spans="1:5" ht="14" customHeight="1">
-      <c r="A71" s="93"/>
+      <c r="E70" s="107"/>
+    </row>
+    <row r="71" spans="1:5" ht="13.95" customHeight="1">
+      <c r="A71" s="105"/>
       <c r="B71" s="35" t="s">
         <v>101</v>
       </c>
@@ -47288,10 +47325,10 @@
         <v>643864</v>
       </c>
       <c r="D71" s="32"/>
-      <c r="E71" s="96"/>
+      <c r="E71" s="108"/>
     </row>
     <row r="72" spans="1:5">
-      <c r="A72" s="93"/>
+      <c r="A72" s="105"/>
       <c r="B72" s="35" t="s">
         <v>117</v>
       </c>
@@ -47299,10 +47336,10 @@
         <v>315579</v>
       </c>
       <c r="D72" s="32"/>
-      <c r="E72" s="96"/>
+      <c r="E72" s="108"/>
     </row>
     <row r="73" spans="1:5">
-      <c r="A73" s="93"/>
+      <c r="A73" s="105"/>
       <c r="B73" s="35" t="s">
         <v>118</v>
       </c>
@@ -47310,10 +47347,10 @@
         <v>315580</v>
       </c>
       <c r="D73" s="32"/>
-      <c r="E73" s="96"/>
+      <c r="E73" s="108"/>
     </row>
     <row r="74" spans="1:5">
-      <c r="A74" s="93" t="s">
+      <c r="A74" s="105" t="s">
         <v>119</v>
       </c>
       <c r="B74" s="35" t="s">
@@ -47323,10 +47360,10 @@
         <v>642914</v>
       </c>
       <c r="D74" s="32"/>
-      <c r="E74" s="95"/>
-    </row>
-    <row r="75" spans="1:5" ht="14" customHeight="1">
-      <c r="A75" s="93"/>
+      <c r="E74" s="107"/>
+    </row>
+    <row r="75" spans="1:5" ht="13.95" customHeight="1">
+      <c r="A75" s="105"/>
       <c r="B75" s="35" t="s">
         <v>105</v>
       </c>
@@ -47334,10 +47371,10 @@
         <v>643865</v>
       </c>
       <c r="D75" s="32"/>
-      <c r="E75" s="96"/>
+      <c r="E75" s="108"/>
     </row>
     <row r="76" spans="1:5">
-      <c r="A76" s="93"/>
+      <c r="A76" s="105"/>
       <c r="B76" s="35" t="s">
         <v>120</v>
       </c>
@@ -47345,10 +47382,10 @@
         <v>242081</v>
       </c>
       <c r="D76" s="32"/>
-      <c r="E76" s="96"/>
+      <c r="E76" s="108"/>
     </row>
     <row r="77" spans="1:5">
-      <c r="A77" s="93"/>
+      <c r="A77" s="105"/>
       <c r="B77" s="35" t="s">
         <v>121</v>
       </c>
@@ -47356,10 +47393,10 @@
         <v>242074</v>
       </c>
       <c r="D77" s="32"/>
-      <c r="E77" s="96"/>
+      <c r="E77" s="108"/>
     </row>
     <row r="78" spans="1:5">
-      <c r="A78" s="93" t="s">
+      <c r="A78" s="105" t="s">
         <v>122</v>
       </c>
       <c r="B78" s="35" t="s">
@@ -47369,10 +47406,10 @@
         <v>642914</v>
       </c>
       <c r="D78" s="32"/>
-      <c r="E78" s="95"/>
-    </row>
-    <row r="79" spans="1:5" ht="14" customHeight="1">
-      <c r="A79" s="93"/>
+      <c r="E78" s="107"/>
+    </row>
+    <row r="79" spans="1:5" ht="13.95" customHeight="1">
+      <c r="A79" s="105"/>
       <c r="B79" s="35" t="s">
         <v>109</v>
       </c>
@@ -47380,10 +47417,10 @@
         <v>738957</v>
       </c>
       <c r="D79" s="32"/>
-      <c r="E79" s="95"/>
+      <c r="E79" s="107"/>
     </row>
     <row r="80" spans="1:5">
-      <c r="A80" s="93"/>
+      <c r="A80" s="105"/>
       <c r="B80" s="35" t="s">
         <v>123</v>
       </c>
@@ -47391,10 +47428,10 @@
         <v>490997</v>
       </c>
       <c r="D80" s="32"/>
-      <c r="E80" s="95"/>
-    </row>
-    <row r="81" spans="1:5" ht="14.5" thickBot="1">
-      <c r="A81" s="94"/>
+      <c r="E80" s="107"/>
+    </row>
+    <row r="81" spans="1:5" ht="14.4" thickBot="1">
+      <c r="A81" s="106"/>
       <c r="B81" s="36" t="s">
         <v>124</v>
       </c>
@@ -47402,10 +47439,10 @@
         <v>491000</v>
       </c>
       <c r="D81" s="32"/>
-      <c r="E81" s="95"/>
+      <c r="E81" s="107"/>
     </row>
     <row r="82" spans="1:5">
-      <c r="A82" s="98" t="s">
+      <c r="A82" s="114" t="s">
         <v>125</v>
       </c>
       <c r="B82" s="30" t="s">
@@ -47415,10 +47452,10 @@
         <v>642915</v>
       </c>
       <c r="D82" s="32"/>
-      <c r="E82" s="95"/>
-    </row>
-    <row r="83" spans="1:5" ht="14" customHeight="1">
-      <c r="A83" s="93"/>
+      <c r="E82" s="107"/>
+    </row>
+    <row r="83" spans="1:5" ht="13.95" customHeight="1">
+      <c r="A83" s="105"/>
       <c r="B83" s="35" t="s">
         <v>97</v>
       </c>
@@ -47426,10 +47463,10 @@
         <v>643863</v>
       </c>
       <c r="D83" s="32"/>
-      <c r="E83" s="96"/>
+      <c r="E83" s="108"/>
     </row>
     <row r="84" spans="1:5">
-      <c r="A84" s="93"/>
+      <c r="A84" s="105"/>
       <c r="B84" s="35" t="s">
         <v>127</v>
       </c>
@@ -47437,10 +47474,10 @@
         <v>206884</v>
       </c>
       <c r="D84" s="32"/>
-      <c r="E84" s="96"/>
+      <c r="E84" s="108"/>
     </row>
     <row r="85" spans="1:5">
-      <c r="A85" s="93"/>
+      <c r="A85" s="105"/>
       <c r="B85" s="35" t="s">
         <v>128</v>
       </c>
@@ -47448,10 +47485,10 @@
         <v>206900</v>
       </c>
       <c r="D85" s="32"/>
-      <c r="E85" s="96"/>
+      <c r="E85" s="108"/>
     </row>
     <row r="86" spans="1:5">
-      <c r="A86" s="93" t="s">
+      <c r="A86" s="105" t="s">
         <v>129</v>
       </c>
       <c r="B86" s="35" t="s">
@@ -47461,10 +47498,10 @@
         <v>642915</v>
       </c>
       <c r="D86" s="32"/>
-      <c r="E86" s="95"/>
-    </row>
-    <row r="87" spans="1:5" ht="14" customHeight="1">
-      <c r="A87" s="93"/>
+      <c r="E86" s="107"/>
+    </row>
+    <row r="87" spans="1:5" ht="13.95" customHeight="1">
+      <c r="A87" s="105"/>
       <c r="B87" s="35" t="s">
         <v>101</v>
       </c>
@@ -47472,10 +47509,10 @@
         <v>643864</v>
       </c>
       <c r="D87" s="32"/>
-      <c r="E87" s="96"/>
+      <c r="E87" s="108"/>
     </row>
     <row r="88" spans="1:5">
-      <c r="A88" s="93"/>
+      <c r="A88" s="105"/>
       <c r="B88" s="35" t="s">
         <v>130</v>
       </c>
@@ -47483,10 +47520,10 @@
         <v>315581</v>
       </c>
       <c r="D88" s="32"/>
-      <c r="E88" s="96"/>
+      <c r="E88" s="108"/>
     </row>
     <row r="89" spans="1:5">
-      <c r="A89" s="93"/>
+      <c r="A89" s="105"/>
       <c r="B89" s="35" t="s">
         <v>131</v>
       </c>
@@ -47494,10 +47531,10 @@
         <v>315582</v>
       </c>
       <c r="D89" s="32"/>
-      <c r="E89" s="96"/>
+      <c r="E89" s="108"/>
     </row>
     <row r="90" spans="1:5">
-      <c r="A90" s="93" t="s">
+      <c r="A90" s="105" t="s">
         <v>132</v>
       </c>
       <c r="B90" s="35" t="s">
@@ -47507,10 +47544,10 @@
         <v>642915</v>
       </c>
       <c r="D90" s="32"/>
-      <c r="E90" s="95"/>
-    </row>
-    <row r="91" spans="1:5" ht="14" customHeight="1">
-      <c r="A91" s="93"/>
+      <c r="E90" s="107"/>
+    </row>
+    <row r="91" spans="1:5" ht="13.95" customHeight="1">
+      <c r="A91" s="105"/>
       <c r="B91" s="35" t="s">
         <v>105</v>
       </c>
@@ -47518,10 +47555,10 @@
         <v>643865</v>
       </c>
       <c r="D91" s="32"/>
-      <c r="E91" s="96"/>
+      <c r="E91" s="108"/>
     </row>
     <row r="92" spans="1:5">
-      <c r="A92" s="93"/>
+      <c r="A92" s="105"/>
       <c r="B92" s="35" t="s">
         <v>133</v>
       </c>
@@ -47529,10 +47566,10 @@
         <v>242082</v>
       </c>
       <c r="D92" s="32"/>
-      <c r="E92" s="96"/>
-    </row>
-    <row r="93" spans="1:5" ht="14.5" thickBot="1">
-      <c r="A93" s="94"/>
+      <c r="E92" s="108"/>
+    </row>
+    <row r="93" spans="1:5" ht="14.4" thickBot="1">
+      <c r="A93" s="106"/>
       <c r="B93" s="36" t="s">
         <v>134</v>
       </c>
@@ -47540,10 +47577,10 @@
         <v>242075</v>
       </c>
       <c r="D93" s="32"/>
-      <c r="E93" s="96"/>
+      <c r="E93" s="108"/>
     </row>
     <row r="94" spans="1:5">
-      <c r="A94" s="97" t="s">
+      <c r="A94" s="115" t="s">
         <v>135</v>
       </c>
       <c r="B94" s="38" t="s">
@@ -47553,10 +47590,10 @@
         <v>642916</v>
       </c>
       <c r="D94" s="32"/>
-      <c r="E94" s="95"/>
-    </row>
-    <row r="95" spans="1:5" ht="14" customHeight="1">
-      <c r="A95" s="93"/>
+      <c r="E94" s="107"/>
+    </row>
+    <row r="95" spans="1:5" ht="13.95" customHeight="1">
+      <c r="A95" s="105"/>
       <c r="B95" s="35" t="s">
         <v>97</v>
       </c>
@@ -47564,10 +47601,10 @@
         <v>643863</v>
       </c>
       <c r="D95" s="32"/>
-      <c r="E95" s="96"/>
+      <c r="E95" s="108"/>
     </row>
     <row r="96" spans="1:5">
-      <c r="A96" s="93"/>
+      <c r="A96" s="105"/>
       <c r="B96" s="35" t="s">
         <v>137</v>
       </c>
@@ -47575,10 +47612,10 @@
         <v>206882</v>
       </c>
       <c r="D96" s="32"/>
-      <c r="E96" s="96"/>
+      <c r="E96" s="108"/>
     </row>
     <row r="97" spans="1:5">
-      <c r="A97" s="93"/>
+      <c r="A97" s="105"/>
       <c r="B97" s="35" t="s">
         <v>138</v>
       </c>
@@ -47586,10 +47623,10 @@
         <v>206898</v>
       </c>
       <c r="D97" s="32"/>
-      <c r="E97" s="96"/>
+      <c r="E97" s="108"/>
     </row>
     <row r="98" spans="1:5">
-      <c r="A98" s="93" t="s">
+      <c r="A98" s="105" t="s">
         <v>139</v>
       </c>
       <c r="B98" s="35" t="s">
@@ -47599,10 +47636,10 @@
         <v>642916</v>
       </c>
       <c r="D98" s="32"/>
-      <c r="E98" s="95"/>
-    </row>
-    <row r="99" spans="1:5" ht="14" customHeight="1">
-      <c r="A99" s="93"/>
+      <c r="E98" s="107"/>
+    </row>
+    <row r="99" spans="1:5" ht="13.95" customHeight="1">
+      <c r="A99" s="105"/>
       <c r="B99" s="35" t="s">
         <v>101</v>
       </c>
@@ -47610,10 +47647,10 @@
         <v>643864</v>
       </c>
       <c r="D99" s="32"/>
-      <c r="E99" s="95"/>
+      <c r="E99" s="107"/>
     </row>
     <row r="100" spans="1:5">
-      <c r="A100" s="93"/>
+      <c r="A100" s="105"/>
       <c r="B100" s="35" t="s">
         <v>140</v>
       </c>
@@ -47621,10 +47658,10 @@
         <v>315584</v>
       </c>
       <c r="D100" s="32"/>
-      <c r="E100" s="95"/>
+      <c r="E100" s="107"/>
     </row>
     <row r="101" spans="1:5">
-      <c r="A101" s="93"/>
+      <c r="A101" s="105"/>
       <c r="B101" s="35" t="s">
         <v>141</v>
       </c>
@@ -47632,10 +47669,10 @@
         <v>315585</v>
       </c>
       <c r="D101" s="32"/>
-      <c r="E101" s="95"/>
+      <c r="E101" s="107"/>
     </row>
     <row r="102" spans="1:5">
-      <c r="A102" s="93" t="s">
+      <c r="A102" s="105" t="s">
         <v>142</v>
       </c>
       <c r="B102" s="35" t="s">
@@ -47645,10 +47682,10 @@
         <v>642916</v>
       </c>
       <c r="D102" s="32"/>
-      <c r="E102" s="95"/>
-    </row>
-    <row r="103" spans="1:5" ht="14" customHeight="1">
-      <c r="A103" s="93"/>
+      <c r="E102" s="107"/>
+    </row>
+    <row r="103" spans="1:5" ht="13.95" customHeight="1">
+      <c r="A103" s="105"/>
       <c r="B103" s="35" t="s">
         <v>105</v>
       </c>
@@ -47656,10 +47693,10 @@
         <v>643865</v>
       </c>
       <c r="D103" s="32"/>
-      <c r="E103" s="95"/>
+      <c r="E103" s="107"/>
     </row>
     <row r="104" spans="1:5">
-      <c r="A104" s="93"/>
+      <c r="A104" s="105"/>
       <c r="B104" s="35" t="s">
         <v>143</v>
       </c>
@@ -47667,10 +47704,10 @@
         <v>242083</v>
       </c>
       <c r="D104" s="32"/>
-      <c r="E104" s="95"/>
+      <c r="E104" s="107"/>
     </row>
     <row r="105" spans="1:5">
-      <c r="A105" s="93"/>
+      <c r="A105" s="105"/>
       <c r="B105" s="35" t="s">
         <v>144</v>
       </c>
@@ -47678,10 +47715,10 @@
         <v>242078</v>
       </c>
       <c r="D105" s="32"/>
-      <c r="E105" s="95"/>
+      <c r="E105" s="107"/>
     </row>
     <row r="106" spans="1:5">
-      <c r="A106" s="93" t="s">
+      <c r="A106" s="105" t="s">
         <v>145</v>
       </c>
       <c r="B106" s="35" t="s">
@@ -47691,10 +47728,10 @@
         <v>642916</v>
       </c>
       <c r="D106" s="32"/>
-      <c r="E106" s="95"/>
-    </row>
-    <row r="107" spans="1:5" ht="14" customHeight="1">
-      <c r="A107" s="93"/>
+      <c r="E106" s="107"/>
+    </row>
+    <row r="107" spans="1:5" ht="13.95" customHeight="1">
+      <c r="A107" s="105"/>
       <c r="B107" s="35" t="s">
         <v>109</v>
       </c>
@@ -47702,10 +47739,10 @@
         <v>738957</v>
       </c>
       <c r="D107" s="32"/>
-      <c r="E107" s="95"/>
+      <c r="E107" s="107"/>
     </row>
     <row r="108" spans="1:5">
-      <c r="A108" s="93"/>
+      <c r="A108" s="105"/>
       <c r="B108" s="35" t="s">
         <v>146</v>
       </c>
@@ -47713,10 +47750,10 @@
         <v>490998</v>
       </c>
       <c r="D108" s="32"/>
-      <c r="E108" s="95"/>
-    </row>
-    <row r="109" spans="1:5" ht="14.5" thickBot="1">
-      <c r="A109" s="94"/>
+      <c r="E108" s="107"/>
+    </row>
+    <row r="109" spans="1:5" ht="14.4" thickBot="1">
+      <c r="A109" s="106"/>
       <c r="B109" s="36" t="s">
         <v>147</v>
       </c>
@@ -47724,17 +47761,39 @@
         <v>491001</v>
       </c>
       <c r="D109" s="32"/>
-      <c r="E109" s="95"/>
+      <c r="E109" s="107"/>
     </row>
   </sheetData>
   <sheetProtection password="CC01" sheet="1" formatCells="0" formatColumns="0" formatRows="0" insertColumns="0" insertRows="0" insertHyperlinks="0" deleteColumns="0" deleteRows="0" sort="0" autoFilter="0" pivotTables="0"/>
   <mergeCells count="49">
-    <mergeCell ref="A2:E2"/>
-    <mergeCell ref="A3:A4"/>
-    <mergeCell ref="B3:B4"/>
-    <mergeCell ref="C3:C4"/>
-    <mergeCell ref="D3:D4"/>
-    <mergeCell ref="E3:E4"/>
+    <mergeCell ref="A90:A93"/>
+    <mergeCell ref="E90:E93"/>
+    <mergeCell ref="A106:A109"/>
+    <mergeCell ref="E106:E109"/>
+    <mergeCell ref="A94:A97"/>
+    <mergeCell ref="E94:E97"/>
+    <mergeCell ref="A98:A101"/>
+    <mergeCell ref="E98:E101"/>
+    <mergeCell ref="A102:A105"/>
+    <mergeCell ref="E102:E105"/>
+    <mergeCell ref="A78:A81"/>
+    <mergeCell ref="E78:E81"/>
+    <mergeCell ref="A82:A85"/>
+    <mergeCell ref="E82:E85"/>
+    <mergeCell ref="A86:A89"/>
+    <mergeCell ref="E86:E89"/>
+    <mergeCell ref="A66:A69"/>
+    <mergeCell ref="E66:E69"/>
+    <mergeCell ref="A70:A73"/>
+    <mergeCell ref="E70:E73"/>
+    <mergeCell ref="A74:A77"/>
+    <mergeCell ref="E74:E77"/>
+    <mergeCell ref="A58:A61"/>
+    <mergeCell ref="E58:E61"/>
+    <mergeCell ref="A62:A65"/>
+    <mergeCell ref="E62:E65"/>
+    <mergeCell ref="A54:A57"/>
+    <mergeCell ref="E54:E57"/>
     <mergeCell ref="B8:B22"/>
     <mergeCell ref="A12:A15"/>
     <mergeCell ref="A16:A19"/>
@@ -47750,34 +47809,12 @@
     <mergeCell ref="A33:A36"/>
     <mergeCell ref="A37:A39"/>
     <mergeCell ref="A8:A11"/>
-    <mergeCell ref="A58:A61"/>
-    <mergeCell ref="E58:E61"/>
-    <mergeCell ref="A62:A65"/>
-    <mergeCell ref="E62:E65"/>
-    <mergeCell ref="A54:A57"/>
-    <mergeCell ref="E54:E57"/>
-    <mergeCell ref="A66:A69"/>
-    <mergeCell ref="E66:E69"/>
-    <mergeCell ref="A70:A73"/>
-    <mergeCell ref="E70:E73"/>
-    <mergeCell ref="A74:A77"/>
-    <mergeCell ref="E74:E77"/>
-    <mergeCell ref="A78:A81"/>
-    <mergeCell ref="E78:E81"/>
-    <mergeCell ref="A82:A85"/>
-    <mergeCell ref="E82:E85"/>
-    <mergeCell ref="A86:A89"/>
-    <mergeCell ref="E86:E89"/>
-    <mergeCell ref="A90:A93"/>
-    <mergeCell ref="E90:E93"/>
-    <mergeCell ref="A106:A109"/>
-    <mergeCell ref="E106:E109"/>
-    <mergeCell ref="A94:A97"/>
-    <mergeCell ref="E94:E97"/>
-    <mergeCell ref="A98:A101"/>
-    <mergeCell ref="E98:E101"/>
-    <mergeCell ref="A102:A105"/>
-    <mergeCell ref="E102:E105"/>
+    <mergeCell ref="A2:E2"/>
+    <mergeCell ref="A3:A4"/>
+    <mergeCell ref="B3:B4"/>
+    <mergeCell ref="C3:C4"/>
+    <mergeCell ref="D3:D4"/>
+    <mergeCell ref="E3:E4"/>
   </mergeCells>
   <pageMargins left="0.78740157480314965" right="0.78740157480314965" top="0.98425196850393704" bottom="0.98425196850393704" header="0.51181102362204722" footer="0.51181102362204722"/>
   <pageSetup paperSize="259" scale="97" fitToHeight="0" orientation="landscape" r:id="rId1"/>
@@ -47798,406 +47835,406 @@
       <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.81640625" defaultRowHeight="14"/>
+  <sheetFormatPr defaultColWidth="14.77734375" defaultRowHeight="13.8"/>
   <cols>
-    <col min="1" max="1" width="56.6328125" style="40" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="33.6328125" style="40" customWidth="1"/>
-    <col min="3" max="3" width="26.81640625" style="40" customWidth="1"/>
-    <col min="4" max="4" width="13.453125" style="40" customWidth="1"/>
-    <col min="5" max="5" width="87.453125" style="40" customWidth="1"/>
-    <col min="6" max="256" width="14.81640625" style="40"/>
-    <col min="257" max="257" width="56.6328125" style="40" bestFit="1" customWidth="1"/>
-    <col min="258" max="258" width="33.6328125" style="40" customWidth="1"/>
-    <col min="259" max="259" width="14.6328125" style="40" customWidth="1"/>
-    <col min="260" max="260" width="13.453125" style="40" customWidth="1"/>
-    <col min="261" max="261" width="74.6328125" style="40" customWidth="1"/>
-    <col min="262" max="512" width="14.81640625" style="40"/>
-    <col min="513" max="513" width="56.6328125" style="40" bestFit="1" customWidth="1"/>
-    <col min="514" max="514" width="33.6328125" style="40" customWidth="1"/>
-    <col min="515" max="515" width="14.6328125" style="40" customWidth="1"/>
-    <col min="516" max="516" width="13.453125" style="40" customWidth="1"/>
-    <col min="517" max="517" width="74.6328125" style="40" customWidth="1"/>
-    <col min="518" max="768" width="14.81640625" style="40"/>
-    <col min="769" max="769" width="56.6328125" style="40" bestFit="1" customWidth="1"/>
-    <col min="770" max="770" width="33.6328125" style="40" customWidth="1"/>
-    <col min="771" max="771" width="14.6328125" style="40" customWidth="1"/>
-    <col min="772" max="772" width="13.453125" style="40" customWidth="1"/>
-    <col min="773" max="773" width="74.6328125" style="40" customWidth="1"/>
-    <col min="774" max="1024" width="14.81640625" style="40"/>
-    <col min="1025" max="1025" width="56.6328125" style="40" bestFit="1" customWidth="1"/>
-    <col min="1026" max="1026" width="33.6328125" style="40" customWidth="1"/>
-    <col min="1027" max="1027" width="14.6328125" style="40" customWidth="1"/>
-    <col min="1028" max="1028" width="13.453125" style="40" customWidth="1"/>
-    <col min="1029" max="1029" width="74.6328125" style="40" customWidth="1"/>
-    <col min="1030" max="1280" width="14.81640625" style="40"/>
-    <col min="1281" max="1281" width="56.6328125" style="40" bestFit="1" customWidth="1"/>
-    <col min="1282" max="1282" width="33.6328125" style="40" customWidth="1"/>
-    <col min="1283" max="1283" width="14.6328125" style="40" customWidth="1"/>
-    <col min="1284" max="1284" width="13.453125" style="40" customWidth="1"/>
-    <col min="1285" max="1285" width="74.6328125" style="40" customWidth="1"/>
-    <col min="1286" max="1536" width="14.81640625" style="40"/>
-    <col min="1537" max="1537" width="56.6328125" style="40" bestFit="1" customWidth="1"/>
-    <col min="1538" max="1538" width="33.6328125" style="40" customWidth="1"/>
-    <col min="1539" max="1539" width="14.6328125" style="40" customWidth="1"/>
-    <col min="1540" max="1540" width="13.453125" style="40" customWidth="1"/>
-    <col min="1541" max="1541" width="74.6328125" style="40" customWidth="1"/>
-    <col min="1542" max="1792" width="14.81640625" style="40"/>
-    <col min="1793" max="1793" width="56.6328125" style="40" bestFit="1" customWidth="1"/>
-    <col min="1794" max="1794" width="33.6328125" style="40" customWidth="1"/>
-    <col min="1795" max="1795" width="14.6328125" style="40" customWidth="1"/>
-    <col min="1796" max="1796" width="13.453125" style="40" customWidth="1"/>
-    <col min="1797" max="1797" width="74.6328125" style="40" customWidth="1"/>
-    <col min="1798" max="2048" width="14.81640625" style="40"/>
-    <col min="2049" max="2049" width="56.6328125" style="40" bestFit="1" customWidth="1"/>
-    <col min="2050" max="2050" width="33.6328125" style="40" customWidth="1"/>
-    <col min="2051" max="2051" width="14.6328125" style="40" customWidth="1"/>
-    <col min="2052" max="2052" width="13.453125" style="40" customWidth="1"/>
-    <col min="2053" max="2053" width="74.6328125" style="40" customWidth="1"/>
-    <col min="2054" max="2304" width="14.81640625" style="40"/>
-    <col min="2305" max="2305" width="56.6328125" style="40" bestFit="1" customWidth="1"/>
-    <col min="2306" max="2306" width="33.6328125" style="40" customWidth="1"/>
-    <col min="2307" max="2307" width="14.6328125" style="40" customWidth="1"/>
-    <col min="2308" max="2308" width="13.453125" style="40" customWidth="1"/>
-    <col min="2309" max="2309" width="74.6328125" style="40" customWidth="1"/>
-    <col min="2310" max="2560" width="14.81640625" style="40"/>
-    <col min="2561" max="2561" width="56.6328125" style="40" bestFit="1" customWidth="1"/>
-    <col min="2562" max="2562" width="33.6328125" style="40" customWidth="1"/>
-    <col min="2563" max="2563" width="14.6328125" style="40" customWidth="1"/>
-    <col min="2564" max="2564" width="13.453125" style="40" customWidth="1"/>
-    <col min="2565" max="2565" width="74.6328125" style="40" customWidth="1"/>
-    <col min="2566" max="2816" width="14.81640625" style="40"/>
-    <col min="2817" max="2817" width="56.6328125" style="40" bestFit="1" customWidth="1"/>
-    <col min="2818" max="2818" width="33.6328125" style="40" customWidth="1"/>
-    <col min="2819" max="2819" width="14.6328125" style="40" customWidth="1"/>
-    <col min="2820" max="2820" width="13.453125" style="40" customWidth="1"/>
-    <col min="2821" max="2821" width="74.6328125" style="40" customWidth="1"/>
-    <col min="2822" max="3072" width="14.81640625" style="40"/>
-    <col min="3073" max="3073" width="56.6328125" style="40" bestFit="1" customWidth="1"/>
-    <col min="3074" max="3074" width="33.6328125" style="40" customWidth="1"/>
-    <col min="3075" max="3075" width="14.6328125" style="40" customWidth="1"/>
-    <col min="3076" max="3076" width="13.453125" style="40" customWidth="1"/>
-    <col min="3077" max="3077" width="74.6328125" style="40" customWidth="1"/>
-    <col min="3078" max="3328" width="14.81640625" style="40"/>
-    <col min="3329" max="3329" width="56.6328125" style="40" bestFit="1" customWidth="1"/>
-    <col min="3330" max="3330" width="33.6328125" style="40" customWidth="1"/>
-    <col min="3331" max="3331" width="14.6328125" style="40" customWidth="1"/>
-    <col min="3332" max="3332" width="13.453125" style="40" customWidth="1"/>
-    <col min="3333" max="3333" width="74.6328125" style="40" customWidth="1"/>
-    <col min="3334" max="3584" width="14.81640625" style="40"/>
-    <col min="3585" max="3585" width="56.6328125" style="40" bestFit="1" customWidth="1"/>
-    <col min="3586" max="3586" width="33.6328125" style="40" customWidth="1"/>
-    <col min="3587" max="3587" width="14.6328125" style="40" customWidth="1"/>
-    <col min="3588" max="3588" width="13.453125" style="40" customWidth="1"/>
-    <col min="3589" max="3589" width="74.6328125" style="40" customWidth="1"/>
-    <col min="3590" max="3840" width="14.81640625" style="40"/>
-    <col min="3841" max="3841" width="56.6328125" style="40" bestFit="1" customWidth="1"/>
-    <col min="3842" max="3842" width="33.6328125" style="40" customWidth="1"/>
-    <col min="3843" max="3843" width="14.6328125" style="40" customWidth="1"/>
-    <col min="3844" max="3844" width="13.453125" style="40" customWidth="1"/>
-    <col min="3845" max="3845" width="74.6328125" style="40" customWidth="1"/>
-    <col min="3846" max="4096" width="14.81640625" style="40"/>
-    <col min="4097" max="4097" width="56.6328125" style="40" bestFit="1" customWidth="1"/>
-    <col min="4098" max="4098" width="33.6328125" style="40" customWidth="1"/>
-    <col min="4099" max="4099" width="14.6328125" style="40" customWidth="1"/>
-    <col min="4100" max="4100" width="13.453125" style="40" customWidth="1"/>
-    <col min="4101" max="4101" width="74.6328125" style="40" customWidth="1"/>
-    <col min="4102" max="4352" width="14.81640625" style="40"/>
-    <col min="4353" max="4353" width="56.6328125" style="40" bestFit="1" customWidth="1"/>
-    <col min="4354" max="4354" width="33.6328125" style="40" customWidth="1"/>
-    <col min="4355" max="4355" width="14.6328125" style="40" customWidth="1"/>
-    <col min="4356" max="4356" width="13.453125" style="40" customWidth="1"/>
-    <col min="4357" max="4357" width="74.6328125" style="40" customWidth="1"/>
-    <col min="4358" max="4608" width="14.81640625" style="40"/>
-    <col min="4609" max="4609" width="56.6328125" style="40" bestFit="1" customWidth="1"/>
-    <col min="4610" max="4610" width="33.6328125" style="40" customWidth="1"/>
-    <col min="4611" max="4611" width="14.6328125" style="40" customWidth="1"/>
-    <col min="4612" max="4612" width="13.453125" style="40" customWidth="1"/>
-    <col min="4613" max="4613" width="74.6328125" style="40" customWidth="1"/>
-    <col min="4614" max="4864" width="14.81640625" style="40"/>
-    <col min="4865" max="4865" width="56.6328125" style="40" bestFit="1" customWidth="1"/>
-    <col min="4866" max="4866" width="33.6328125" style="40" customWidth="1"/>
-    <col min="4867" max="4867" width="14.6328125" style="40" customWidth="1"/>
-    <col min="4868" max="4868" width="13.453125" style="40" customWidth="1"/>
-    <col min="4869" max="4869" width="74.6328125" style="40" customWidth="1"/>
-    <col min="4870" max="5120" width="14.81640625" style="40"/>
-    <col min="5121" max="5121" width="56.6328125" style="40" bestFit="1" customWidth="1"/>
-    <col min="5122" max="5122" width="33.6328125" style="40" customWidth="1"/>
-    <col min="5123" max="5123" width="14.6328125" style="40" customWidth="1"/>
-    <col min="5124" max="5124" width="13.453125" style="40" customWidth="1"/>
-    <col min="5125" max="5125" width="74.6328125" style="40" customWidth="1"/>
-    <col min="5126" max="5376" width="14.81640625" style="40"/>
-    <col min="5377" max="5377" width="56.6328125" style="40" bestFit="1" customWidth="1"/>
-    <col min="5378" max="5378" width="33.6328125" style="40" customWidth="1"/>
-    <col min="5379" max="5379" width="14.6328125" style="40" customWidth="1"/>
-    <col min="5380" max="5380" width="13.453125" style="40" customWidth="1"/>
-    <col min="5381" max="5381" width="74.6328125" style="40" customWidth="1"/>
-    <col min="5382" max="5632" width="14.81640625" style="40"/>
-    <col min="5633" max="5633" width="56.6328125" style="40" bestFit="1" customWidth="1"/>
-    <col min="5634" max="5634" width="33.6328125" style="40" customWidth="1"/>
-    <col min="5635" max="5635" width="14.6328125" style="40" customWidth="1"/>
-    <col min="5636" max="5636" width="13.453125" style="40" customWidth="1"/>
-    <col min="5637" max="5637" width="74.6328125" style="40" customWidth="1"/>
-    <col min="5638" max="5888" width="14.81640625" style="40"/>
-    <col min="5889" max="5889" width="56.6328125" style="40" bestFit="1" customWidth="1"/>
-    <col min="5890" max="5890" width="33.6328125" style="40" customWidth="1"/>
-    <col min="5891" max="5891" width="14.6328125" style="40" customWidth="1"/>
-    <col min="5892" max="5892" width="13.453125" style="40" customWidth="1"/>
-    <col min="5893" max="5893" width="74.6328125" style="40" customWidth="1"/>
-    <col min="5894" max="6144" width="14.81640625" style="40"/>
-    <col min="6145" max="6145" width="56.6328125" style="40" bestFit="1" customWidth="1"/>
-    <col min="6146" max="6146" width="33.6328125" style="40" customWidth="1"/>
-    <col min="6147" max="6147" width="14.6328125" style="40" customWidth="1"/>
-    <col min="6148" max="6148" width="13.453125" style="40" customWidth="1"/>
-    <col min="6149" max="6149" width="74.6328125" style="40" customWidth="1"/>
-    <col min="6150" max="6400" width="14.81640625" style="40"/>
-    <col min="6401" max="6401" width="56.6328125" style="40" bestFit="1" customWidth="1"/>
-    <col min="6402" max="6402" width="33.6328125" style="40" customWidth="1"/>
-    <col min="6403" max="6403" width="14.6328125" style="40" customWidth="1"/>
-    <col min="6404" max="6404" width="13.453125" style="40" customWidth="1"/>
-    <col min="6405" max="6405" width="74.6328125" style="40" customWidth="1"/>
-    <col min="6406" max="6656" width="14.81640625" style="40"/>
-    <col min="6657" max="6657" width="56.6328125" style="40" bestFit="1" customWidth="1"/>
-    <col min="6658" max="6658" width="33.6328125" style="40" customWidth="1"/>
-    <col min="6659" max="6659" width="14.6328125" style="40" customWidth="1"/>
-    <col min="6660" max="6660" width="13.453125" style="40" customWidth="1"/>
-    <col min="6661" max="6661" width="74.6328125" style="40" customWidth="1"/>
-    <col min="6662" max="6912" width="14.81640625" style="40"/>
-    <col min="6913" max="6913" width="56.6328125" style="40" bestFit="1" customWidth="1"/>
-    <col min="6914" max="6914" width="33.6328125" style="40" customWidth="1"/>
-    <col min="6915" max="6915" width="14.6328125" style="40" customWidth="1"/>
-    <col min="6916" max="6916" width="13.453125" style="40" customWidth="1"/>
-    <col min="6917" max="6917" width="74.6328125" style="40" customWidth="1"/>
-    <col min="6918" max="7168" width="14.81640625" style="40"/>
-    <col min="7169" max="7169" width="56.6328125" style="40" bestFit="1" customWidth="1"/>
-    <col min="7170" max="7170" width="33.6328125" style="40" customWidth="1"/>
-    <col min="7171" max="7171" width="14.6328125" style="40" customWidth="1"/>
-    <col min="7172" max="7172" width="13.453125" style="40" customWidth="1"/>
-    <col min="7173" max="7173" width="74.6328125" style="40" customWidth="1"/>
-    <col min="7174" max="7424" width="14.81640625" style="40"/>
-    <col min="7425" max="7425" width="56.6328125" style="40" bestFit="1" customWidth="1"/>
-    <col min="7426" max="7426" width="33.6328125" style="40" customWidth="1"/>
-    <col min="7427" max="7427" width="14.6328125" style="40" customWidth="1"/>
-    <col min="7428" max="7428" width="13.453125" style="40" customWidth="1"/>
-    <col min="7429" max="7429" width="74.6328125" style="40" customWidth="1"/>
-    <col min="7430" max="7680" width="14.81640625" style="40"/>
-    <col min="7681" max="7681" width="56.6328125" style="40" bestFit="1" customWidth="1"/>
-    <col min="7682" max="7682" width="33.6328125" style="40" customWidth="1"/>
-    <col min="7683" max="7683" width="14.6328125" style="40" customWidth="1"/>
-    <col min="7684" max="7684" width="13.453125" style="40" customWidth="1"/>
-    <col min="7685" max="7685" width="74.6328125" style="40" customWidth="1"/>
-    <col min="7686" max="7936" width="14.81640625" style="40"/>
-    <col min="7937" max="7937" width="56.6328125" style="40" bestFit="1" customWidth="1"/>
-    <col min="7938" max="7938" width="33.6328125" style="40" customWidth="1"/>
-    <col min="7939" max="7939" width="14.6328125" style="40" customWidth="1"/>
-    <col min="7940" max="7940" width="13.453125" style="40" customWidth="1"/>
-    <col min="7941" max="7941" width="74.6328125" style="40" customWidth="1"/>
-    <col min="7942" max="8192" width="14.81640625" style="40"/>
-    <col min="8193" max="8193" width="56.6328125" style="40" bestFit="1" customWidth="1"/>
-    <col min="8194" max="8194" width="33.6328125" style="40" customWidth="1"/>
-    <col min="8195" max="8195" width="14.6328125" style="40" customWidth="1"/>
-    <col min="8196" max="8196" width="13.453125" style="40" customWidth="1"/>
-    <col min="8197" max="8197" width="74.6328125" style="40" customWidth="1"/>
-    <col min="8198" max="8448" width="14.81640625" style="40"/>
-    <col min="8449" max="8449" width="56.6328125" style="40" bestFit="1" customWidth="1"/>
-    <col min="8450" max="8450" width="33.6328125" style="40" customWidth="1"/>
-    <col min="8451" max="8451" width="14.6328125" style="40" customWidth="1"/>
-    <col min="8452" max="8452" width="13.453125" style="40" customWidth="1"/>
-    <col min="8453" max="8453" width="74.6328125" style="40" customWidth="1"/>
-    <col min="8454" max="8704" width="14.81640625" style="40"/>
-    <col min="8705" max="8705" width="56.6328125" style="40" bestFit="1" customWidth="1"/>
-    <col min="8706" max="8706" width="33.6328125" style="40" customWidth="1"/>
-    <col min="8707" max="8707" width="14.6328125" style="40" customWidth="1"/>
-    <col min="8708" max="8708" width="13.453125" style="40" customWidth="1"/>
-    <col min="8709" max="8709" width="74.6328125" style="40" customWidth="1"/>
-    <col min="8710" max="8960" width="14.81640625" style="40"/>
-    <col min="8961" max="8961" width="56.6328125" style="40" bestFit="1" customWidth="1"/>
-    <col min="8962" max="8962" width="33.6328125" style="40" customWidth="1"/>
-    <col min="8963" max="8963" width="14.6328125" style="40" customWidth="1"/>
-    <col min="8964" max="8964" width="13.453125" style="40" customWidth="1"/>
-    <col min="8965" max="8965" width="74.6328125" style="40" customWidth="1"/>
-    <col min="8966" max="9216" width="14.81640625" style="40"/>
-    <col min="9217" max="9217" width="56.6328125" style="40" bestFit="1" customWidth="1"/>
-    <col min="9218" max="9218" width="33.6328125" style="40" customWidth="1"/>
-    <col min="9219" max="9219" width="14.6328125" style="40" customWidth="1"/>
-    <col min="9220" max="9220" width="13.453125" style="40" customWidth="1"/>
-    <col min="9221" max="9221" width="74.6328125" style="40" customWidth="1"/>
-    <col min="9222" max="9472" width="14.81640625" style="40"/>
-    <col min="9473" max="9473" width="56.6328125" style="40" bestFit="1" customWidth="1"/>
-    <col min="9474" max="9474" width="33.6328125" style="40" customWidth="1"/>
-    <col min="9475" max="9475" width="14.6328125" style="40" customWidth="1"/>
-    <col min="9476" max="9476" width="13.453125" style="40" customWidth="1"/>
-    <col min="9477" max="9477" width="74.6328125" style="40" customWidth="1"/>
-    <col min="9478" max="9728" width="14.81640625" style="40"/>
-    <col min="9729" max="9729" width="56.6328125" style="40" bestFit="1" customWidth="1"/>
-    <col min="9730" max="9730" width="33.6328125" style="40" customWidth="1"/>
-    <col min="9731" max="9731" width="14.6328125" style="40" customWidth="1"/>
-    <col min="9732" max="9732" width="13.453125" style="40" customWidth="1"/>
-    <col min="9733" max="9733" width="74.6328125" style="40" customWidth="1"/>
-    <col min="9734" max="9984" width="14.81640625" style="40"/>
-    <col min="9985" max="9985" width="56.6328125" style="40" bestFit="1" customWidth="1"/>
-    <col min="9986" max="9986" width="33.6328125" style="40" customWidth="1"/>
-    <col min="9987" max="9987" width="14.6328125" style="40" customWidth="1"/>
-    <col min="9988" max="9988" width="13.453125" style="40" customWidth="1"/>
-    <col min="9989" max="9989" width="74.6328125" style="40" customWidth="1"/>
-    <col min="9990" max="10240" width="14.81640625" style="40"/>
-    <col min="10241" max="10241" width="56.6328125" style="40" bestFit="1" customWidth="1"/>
-    <col min="10242" max="10242" width="33.6328125" style="40" customWidth="1"/>
-    <col min="10243" max="10243" width="14.6328125" style="40" customWidth="1"/>
-    <col min="10244" max="10244" width="13.453125" style="40" customWidth="1"/>
-    <col min="10245" max="10245" width="74.6328125" style="40" customWidth="1"/>
-    <col min="10246" max="10496" width="14.81640625" style="40"/>
-    <col min="10497" max="10497" width="56.6328125" style="40" bestFit="1" customWidth="1"/>
-    <col min="10498" max="10498" width="33.6328125" style="40" customWidth="1"/>
-    <col min="10499" max="10499" width="14.6328125" style="40" customWidth="1"/>
-    <col min="10500" max="10500" width="13.453125" style="40" customWidth="1"/>
-    <col min="10501" max="10501" width="74.6328125" style="40" customWidth="1"/>
-    <col min="10502" max="10752" width="14.81640625" style="40"/>
-    <col min="10753" max="10753" width="56.6328125" style="40" bestFit="1" customWidth="1"/>
-    <col min="10754" max="10754" width="33.6328125" style="40" customWidth="1"/>
-    <col min="10755" max="10755" width="14.6328125" style="40" customWidth="1"/>
-    <col min="10756" max="10756" width="13.453125" style="40" customWidth="1"/>
-    <col min="10757" max="10757" width="74.6328125" style="40" customWidth="1"/>
-    <col min="10758" max="11008" width="14.81640625" style="40"/>
-    <col min="11009" max="11009" width="56.6328125" style="40" bestFit="1" customWidth="1"/>
-    <col min="11010" max="11010" width="33.6328125" style="40" customWidth="1"/>
-    <col min="11011" max="11011" width="14.6328125" style="40" customWidth="1"/>
-    <col min="11012" max="11012" width="13.453125" style="40" customWidth="1"/>
-    <col min="11013" max="11013" width="74.6328125" style="40" customWidth="1"/>
-    <col min="11014" max="11264" width="14.81640625" style="40"/>
-    <col min="11265" max="11265" width="56.6328125" style="40" bestFit="1" customWidth="1"/>
-    <col min="11266" max="11266" width="33.6328125" style="40" customWidth="1"/>
-    <col min="11267" max="11267" width="14.6328125" style="40" customWidth="1"/>
-    <col min="11268" max="11268" width="13.453125" style="40" customWidth="1"/>
-    <col min="11269" max="11269" width="74.6328125" style="40" customWidth="1"/>
-    <col min="11270" max="11520" width="14.81640625" style="40"/>
-    <col min="11521" max="11521" width="56.6328125" style="40" bestFit="1" customWidth="1"/>
-    <col min="11522" max="11522" width="33.6328125" style="40" customWidth="1"/>
-    <col min="11523" max="11523" width="14.6328125" style="40" customWidth="1"/>
-    <col min="11524" max="11524" width="13.453125" style="40" customWidth="1"/>
-    <col min="11525" max="11525" width="74.6328125" style="40" customWidth="1"/>
-    <col min="11526" max="11776" width="14.81640625" style="40"/>
-    <col min="11777" max="11777" width="56.6328125" style="40" bestFit="1" customWidth="1"/>
-    <col min="11778" max="11778" width="33.6328125" style="40" customWidth="1"/>
-    <col min="11779" max="11779" width="14.6328125" style="40" customWidth="1"/>
-    <col min="11780" max="11780" width="13.453125" style="40" customWidth="1"/>
-    <col min="11781" max="11781" width="74.6328125" style="40" customWidth="1"/>
-    <col min="11782" max="12032" width="14.81640625" style="40"/>
-    <col min="12033" max="12033" width="56.6328125" style="40" bestFit="1" customWidth="1"/>
-    <col min="12034" max="12034" width="33.6328125" style="40" customWidth="1"/>
-    <col min="12035" max="12035" width="14.6328125" style="40" customWidth="1"/>
-    <col min="12036" max="12036" width="13.453125" style="40" customWidth="1"/>
-    <col min="12037" max="12037" width="74.6328125" style="40" customWidth="1"/>
-    <col min="12038" max="12288" width="14.81640625" style="40"/>
-    <col min="12289" max="12289" width="56.6328125" style="40" bestFit="1" customWidth="1"/>
-    <col min="12290" max="12290" width="33.6328125" style="40" customWidth="1"/>
-    <col min="12291" max="12291" width="14.6328125" style="40" customWidth="1"/>
-    <col min="12292" max="12292" width="13.453125" style="40" customWidth="1"/>
-    <col min="12293" max="12293" width="74.6328125" style="40" customWidth="1"/>
-    <col min="12294" max="12544" width="14.81640625" style="40"/>
-    <col min="12545" max="12545" width="56.6328125" style="40" bestFit="1" customWidth="1"/>
-    <col min="12546" max="12546" width="33.6328125" style="40" customWidth="1"/>
-    <col min="12547" max="12547" width="14.6328125" style="40" customWidth="1"/>
-    <col min="12548" max="12548" width="13.453125" style="40" customWidth="1"/>
-    <col min="12549" max="12549" width="74.6328125" style="40" customWidth="1"/>
-    <col min="12550" max="12800" width="14.81640625" style="40"/>
-    <col min="12801" max="12801" width="56.6328125" style="40" bestFit="1" customWidth="1"/>
-    <col min="12802" max="12802" width="33.6328125" style="40" customWidth="1"/>
-    <col min="12803" max="12803" width="14.6328125" style="40" customWidth="1"/>
-    <col min="12804" max="12804" width="13.453125" style="40" customWidth="1"/>
-    <col min="12805" max="12805" width="74.6328125" style="40" customWidth="1"/>
-    <col min="12806" max="13056" width="14.81640625" style="40"/>
-    <col min="13057" max="13057" width="56.6328125" style="40" bestFit="1" customWidth="1"/>
-    <col min="13058" max="13058" width="33.6328125" style="40" customWidth="1"/>
-    <col min="13059" max="13059" width="14.6328125" style="40" customWidth="1"/>
-    <col min="13060" max="13060" width="13.453125" style="40" customWidth="1"/>
-    <col min="13061" max="13061" width="74.6328125" style="40" customWidth="1"/>
-    <col min="13062" max="13312" width="14.81640625" style="40"/>
-    <col min="13313" max="13313" width="56.6328125" style="40" bestFit="1" customWidth="1"/>
-    <col min="13314" max="13314" width="33.6328125" style="40" customWidth="1"/>
-    <col min="13315" max="13315" width="14.6328125" style="40" customWidth="1"/>
-    <col min="13316" max="13316" width="13.453125" style="40" customWidth="1"/>
-    <col min="13317" max="13317" width="74.6328125" style="40" customWidth="1"/>
-    <col min="13318" max="13568" width="14.81640625" style="40"/>
-    <col min="13569" max="13569" width="56.6328125" style="40" bestFit="1" customWidth="1"/>
-    <col min="13570" max="13570" width="33.6328125" style="40" customWidth="1"/>
-    <col min="13571" max="13571" width="14.6328125" style="40" customWidth="1"/>
-    <col min="13572" max="13572" width="13.453125" style="40" customWidth="1"/>
-    <col min="13573" max="13573" width="74.6328125" style="40" customWidth="1"/>
-    <col min="13574" max="13824" width="14.81640625" style="40"/>
-    <col min="13825" max="13825" width="56.6328125" style="40" bestFit="1" customWidth="1"/>
-    <col min="13826" max="13826" width="33.6328125" style="40" customWidth="1"/>
-    <col min="13827" max="13827" width="14.6328125" style="40" customWidth="1"/>
-    <col min="13828" max="13828" width="13.453125" style="40" customWidth="1"/>
-    <col min="13829" max="13829" width="74.6328125" style="40" customWidth="1"/>
-    <col min="13830" max="14080" width="14.81640625" style="40"/>
-    <col min="14081" max="14081" width="56.6328125" style="40" bestFit="1" customWidth="1"/>
-    <col min="14082" max="14082" width="33.6328125" style="40" customWidth="1"/>
-    <col min="14083" max="14083" width="14.6328125" style="40" customWidth="1"/>
-    <col min="14084" max="14084" width="13.453125" style="40" customWidth="1"/>
-    <col min="14085" max="14085" width="74.6328125" style="40" customWidth="1"/>
-    <col min="14086" max="14336" width="14.81640625" style="40"/>
-    <col min="14337" max="14337" width="56.6328125" style="40" bestFit="1" customWidth="1"/>
-    <col min="14338" max="14338" width="33.6328125" style="40" customWidth="1"/>
-    <col min="14339" max="14339" width="14.6328125" style="40" customWidth="1"/>
-    <col min="14340" max="14340" width="13.453125" style="40" customWidth="1"/>
-    <col min="14341" max="14341" width="74.6328125" style="40" customWidth="1"/>
-    <col min="14342" max="14592" width="14.81640625" style="40"/>
-    <col min="14593" max="14593" width="56.6328125" style="40" bestFit="1" customWidth="1"/>
-    <col min="14594" max="14594" width="33.6328125" style="40" customWidth="1"/>
-    <col min="14595" max="14595" width="14.6328125" style="40" customWidth="1"/>
-    <col min="14596" max="14596" width="13.453125" style="40" customWidth="1"/>
-    <col min="14597" max="14597" width="74.6328125" style="40" customWidth="1"/>
-    <col min="14598" max="14848" width="14.81640625" style="40"/>
-    <col min="14849" max="14849" width="56.6328125" style="40" bestFit="1" customWidth="1"/>
-    <col min="14850" max="14850" width="33.6328125" style="40" customWidth="1"/>
-    <col min="14851" max="14851" width="14.6328125" style="40" customWidth="1"/>
-    <col min="14852" max="14852" width="13.453125" style="40" customWidth="1"/>
-    <col min="14853" max="14853" width="74.6328125" style="40" customWidth="1"/>
-    <col min="14854" max="15104" width="14.81640625" style="40"/>
-    <col min="15105" max="15105" width="56.6328125" style="40" bestFit="1" customWidth="1"/>
-    <col min="15106" max="15106" width="33.6328125" style="40" customWidth="1"/>
-    <col min="15107" max="15107" width="14.6328125" style="40" customWidth="1"/>
-    <col min="15108" max="15108" width="13.453125" style="40" customWidth="1"/>
-    <col min="15109" max="15109" width="74.6328125" style="40" customWidth="1"/>
-    <col min="15110" max="15360" width="14.81640625" style="40"/>
-    <col min="15361" max="15361" width="56.6328125" style="40" bestFit="1" customWidth="1"/>
-    <col min="15362" max="15362" width="33.6328125" style="40" customWidth="1"/>
-    <col min="15363" max="15363" width="14.6328125" style="40" customWidth="1"/>
-    <col min="15364" max="15364" width="13.453125" style="40" customWidth="1"/>
-    <col min="15365" max="15365" width="74.6328125" style="40" customWidth="1"/>
-    <col min="15366" max="15616" width="14.81640625" style="40"/>
-    <col min="15617" max="15617" width="56.6328125" style="40" bestFit="1" customWidth="1"/>
-    <col min="15618" max="15618" width="33.6328125" style="40" customWidth="1"/>
-    <col min="15619" max="15619" width="14.6328125" style="40" customWidth="1"/>
-    <col min="15620" max="15620" width="13.453125" style="40" customWidth="1"/>
-    <col min="15621" max="15621" width="74.6328125" style="40" customWidth="1"/>
-    <col min="15622" max="15872" width="14.81640625" style="40"/>
-    <col min="15873" max="15873" width="56.6328125" style="40" bestFit="1" customWidth="1"/>
-    <col min="15874" max="15874" width="33.6328125" style="40" customWidth="1"/>
-    <col min="15875" max="15875" width="14.6328125" style="40" customWidth="1"/>
-    <col min="15876" max="15876" width="13.453125" style="40" customWidth="1"/>
-    <col min="15877" max="15877" width="74.6328125" style="40" customWidth="1"/>
-    <col min="15878" max="16128" width="14.81640625" style="40"/>
-    <col min="16129" max="16129" width="56.6328125" style="40" bestFit="1" customWidth="1"/>
-    <col min="16130" max="16130" width="33.6328125" style="40" customWidth="1"/>
-    <col min="16131" max="16131" width="14.6328125" style="40" customWidth="1"/>
-    <col min="16132" max="16132" width="13.453125" style="40" customWidth="1"/>
-    <col min="16133" max="16133" width="74.6328125" style="40" customWidth="1"/>
-    <col min="16134" max="16384" width="14.81640625" style="40"/>
+    <col min="1" max="1" width="56.6640625" style="40" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="33.6640625" style="40" customWidth="1"/>
+    <col min="3" max="3" width="26.77734375" style="40" customWidth="1"/>
+    <col min="4" max="4" width="13.44140625" style="40" customWidth="1"/>
+    <col min="5" max="5" width="87.44140625" style="40" customWidth="1"/>
+    <col min="6" max="256" width="14.77734375" style="40"/>
+    <col min="257" max="257" width="56.6640625" style="40" bestFit="1" customWidth="1"/>
+    <col min="258" max="258" width="33.6640625" style="40" customWidth="1"/>
+    <col min="259" max="259" width="14.6640625" style="40" customWidth="1"/>
+    <col min="260" max="260" width="13.44140625" style="40" customWidth="1"/>
+    <col min="261" max="261" width="74.6640625" style="40" customWidth="1"/>
+    <col min="262" max="512" width="14.77734375" style="40"/>
+    <col min="513" max="513" width="56.6640625" style="40" bestFit="1" customWidth="1"/>
+    <col min="514" max="514" width="33.6640625" style="40" customWidth="1"/>
+    <col min="515" max="515" width="14.6640625" style="40" customWidth="1"/>
+    <col min="516" max="516" width="13.44140625" style="40" customWidth="1"/>
+    <col min="517" max="517" width="74.6640625" style="40" customWidth="1"/>
+    <col min="518" max="768" width="14.77734375" style="40"/>
+    <col min="769" max="769" width="56.6640625" style="40" bestFit="1" customWidth="1"/>
+    <col min="770" max="770" width="33.6640625" style="40" customWidth="1"/>
+    <col min="771" max="771" width="14.6640625" style="40" customWidth="1"/>
+    <col min="772" max="772" width="13.44140625" style="40" customWidth="1"/>
+    <col min="773" max="773" width="74.6640625" style="40" customWidth="1"/>
+    <col min="774" max="1024" width="14.77734375" style="40"/>
+    <col min="1025" max="1025" width="56.6640625" style="40" bestFit="1" customWidth="1"/>
+    <col min="1026" max="1026" width="33.6640625" style="40" customWidth="1"/>
+    <col min="1027" max="1027" width="14.6640625" style="40" customWidth="1"/>
+    <col min="1028" max="1028" width="13.44140625" style="40" customWidth="1"/>
+    <col min="1029" max="1029" width="74.6640625" style="40" customWidth="1"/>
+    <col min="1030" max="1280" width="14.77734375" style="40"/>
+    <col min="1281" max="1281" width="56.6640625" style="40" bestFit="1" customWidth="1"/>
+    <col min="1282" max="1282" width="33.6640625" style="40" customWidth="1"/>
+    <col min="1283" max="1283" width="14.6640625" style="40" customWidth="1"/>
+    <col min="1284" max="1284" width="13.44140625" style="40" customWidth="1"/>
+    <col min="1285" max="1285" width="74.6640625" style="40" customWidth="1"/>
+    <col min="1286" max="1536" width="14.77734375" style="40"/>
+    <col min="1537" max="1537" width="56.6640625" style="40" bestFit="1" customWidth="1"/>
+    <col min="1538" max="1538" width="33.6640625" style="40" customWidth="1"/>
+    <col min="1539" max="1539" width="14.6640625" style="40" customWidth="1"/>
+    <col min="1540" max="1540" width="13.44140625" style="40" customWidth="1"/>
+    <col min="1541" max="1541" width="74.6640625" style="40" customWidth="1"/>
+    <col min="1542" max="1792" width="14.77734375" style="40"/>
+    <col min="1793" max="1793" width="56.6640625" style="40" bestFit="1" customWidth="1"/>
+    <col min="1794" max="1794" width="33.6640625" style="40" customWidth="1"/>
+    <col min="1795" max="1795" width="14.6640625" style="40" customWidth="1"/>
+    <col min="1796" max="1796" width="13.44140625" style="40" customWidth="1"/>
+    <col min="1797" max="1797" width="74.6640625" style="40" customWidth="1"/>
+    <col min="1798" max="2048" width="14.77734375" style="40"/>
+    <col min="2049" max="2049" width="56.6640625" style="40" bestFit="1" customWidth="1"/>
+    <col min="2050" max="2050" width="33.6640625" style="40" customWidth="1"/>
+    <col min="2051" max="2051" width="14.6640625" style="40" customWidth="1"/>
+    <col min="2052" max="2052" width="13.44140625" style="40" customWidth="1"/>
+    <col min="2053" max="2053" width="74.6640625" style="40" customWidth="1"/>
+    <col min="2054" max="2304" width="14.77734375" style="40"/>
+    <col min="2305" max="2305" width="56.6640625" style="40" bestFit="1" customWidth="1"/>
+    <col min="2306" max="2306" width="33.6640625" style="40" customWidth="1"/>
+    <col min="2307" max="2307" width="14.6640625" style="40" customWidth="1"/>
+    <col min="2308" max="2308" width="13.44140625" style="40" customWidth="1"/>
+    <col min="2309" max="2309" width="74.6640625" style="40" customWidth="1"/>
+    <col min="2310" max="2560" width="14.77734375" style="40"/>
+    <col min="2561" max="2561" width="56.6640625" style="40" bestFit="1" customWidth="1"/>
+    <col min="2562" max="2562" width="33.6640625" style="40" customWidth="1"/>
+    <col min="2563" max="2563" width="14.6640625" style="40" customWidth="1"/>
+    <col min="2564" max="2564" width="13.44140625" style="40" customWidth="1"/>
+    <col min="2565" max="2565" width="74.6640625" style="40" customWidth="1"/>
+    <col min="2566" max="2816" width="14.77734375" style="40"/>
+    <col min="2817" max="2817" width="56.6640625" style="40" bestFit="1" customWidth="1"/>
+    <col min="2818" max="2818" width="33.6640625" style="40" customWidth="1"/>
+    <col min="2819" max="2819" width="14.6640625" style="40" customWidth="1"/>
+    <col min="2820" max="2820" width="13.44140625" style="40" customWidth="1"/>
+    <col min="2821" max="2821" width="74.6640625" style="40" customWidth="1"/>
+    <col min="2822" max="3072" width="14.77734375" style="40"/>
+    <col min="3073" max="3073" width="56.6640625" style="40" bestFit="1" customWidth="1"/>
+    <col min="3074" max="3074" width="33.6640625" style="40" customWidth="1"/>
+    <col min="3075" max="3075" width="14.6640625" style="40" customWidth="1"/>
+    <col min="3076" max="3076" width="13.44140625" style="40" customWidth="1"/>
+    <col min="3077" max="3077" width="74.6640625" style="40" customWidth="1"/>
+    <col min="3078" max="3328" width="14.77734375" style="40"/>
+    <col min="3329" max="3329" width="56.6640625" style="40" bestFit="1" customWidth="1"/>
+    <col min="3330" max="3330" width="33.6640625" style="40" customWidth="1"/>
+    <col min="3331" max="3331" width="14.6640625" style="40" customWidth="1"/>
+    <col min="3332" max="3332" width="13.44140625" style="40" customWidth="1"/>
+    <col min="3333" max="3333" width="74.6640625" style="40" customWidth="1"/>
+    <col min="3334" max="3584" width="14.77734375" style="40"/>
+    <col min="3585" max="3585" width="56.6640625" style="40" bestFit="1" customWidth="1"/>
+    <col min="3586" max="3586" width="33.6640625" style="40" customWidth="1"/>
+    <col min="3587" max="3587" width="14.6640625" style="40" customWidth="1"/>
+    <col min="3588" max="3588" width="13.44140625" style="40" customWidth="1"/>
+    <col min="3589" max="3589" width="74.6640625" style="40" customWidth="1"/>
+    <col min="3590" max="3840" width="14.77734375" style="40"/>
+    <col min="3841" max="3841" width="56.6640625" style="40" bestFit="1" customWidth="1"/>
+    <col min="3842" max="3842" width="33.6640625" style="40" customWidth="1"/>
+    <col min="3843" max="3843" width="14.6640625" style="40" customWidth="1"/>
+    <col min="3844" max="3844" width="13.44140625" style="40" customWidth="1"/>
+    <col min="3845" max="3845" width="74.6640625" style="40" customWidth="1"/>
+    <col min="3846" max="4096" width="14.77734375" style="40"/>
+    <col min="4097" max="4097" width="56.6640625" style="40" bestFit="1" customWidth="1"/>
+    <col min="4098" max="4098" width="33.6640625" style="40" customWidth="1"/>
+    <col min="4099" max="4099" width="14.6640625" style="40" customWidth="1"/>
+    <col min="4100" max="4100" width="13.44140625" style="40" customWidth="1"/>
+    <col min="4101" max="4101" width="74.6640625" style="40" customWidth="1"/>
+    <col min="4102" max="4352" width="14.77734375" style="40"/>
+    <col min="4353" max="4353" width="56.6640625" style="40" bestFit="1" customWidth="1"/>
+    <col min="4354" max="4354" width="33.6640625" style="40" customWidth="1"/>
+    <col min="4355" max="4355" width="14.6640625" style="40" customWidth="1"/>
+    <col min="4356" max="4356" width="13.44140625" style="40" customWidth="1"/>
+    <col min="4357" max="4357" width="74.6640625" style="40" customWidth="1"/>
+    <col min="4358" max="4608" width="14.77734375" style="40"/>
+    <col min="4609" max="4609" width="56.6640625" style="40" bestFit="1" customWidth="1"/>
+    <col min="4610" max="4610" width="33.6640625" style="40" customWidth="1"/>
+    <col min="4611" max="4611" width="14.6640625" style="40" customWidth="1"/>
+    <col min="4612" max="4612" width="13.44140625" style="40" customWidth="1"/>
+    <col min="4613" max="4613" width="74.6640625" style="40" customWidth="1"/>
+    <col min="4614" max="4864" width="14.77734375" style="40"/>
+    <col min="4865" max="4865" width="56.6640625" style="40" bestFit="1" customWidth="1"/>
+    <col min="4866" max="4866" width="33.6640625" style="40" customWidth="1"/>
+    <col min="4867" max="4867" width="14.6640625" style="40" customWidth="1"/>
+    <col min="4868" max="4868" width="13.44140625" style="40" customWidth="1"/>
+    <col min="4869" max="4869" width="74.6640625" style="40" customWidth="1"/>
+    <col min="4870" max="5120" width="14.77734375" style="40"/>
+    <col min="5121" max="5121" width="56.6640625" style="40" bestFit="1" customWidth="1"/>
+    <col min="5122" max="5122" width="33.6640625" style="40" customWidth="1"/>
+    <col min="5123" max="5123" width="14.6640625" style="40" customWidth="1"/>
+    <col min="5124" max="5124" width="13.44140625" style="40" customWidth="1"/>
+    <col min="5125" max="5125" width="74.6640625" style="40" customWidth="1"/>
+    <col min="5126" max="5376" width="14.77734375" style="40"/>
+    <col min="5377" max="5377" width="56.6640625" style="40" bestFit="1" customWidth="1"/>
+    <col min="5378" max="5378" width="33.6640625" style="40" customWidth="1"/>
+    <col min="5379" max="5379" width="14.6640625" style="40" customWidth="1"/>
+    <col min="5380" max="5380" width="13.44140625" style="40" customWidth="1"/>
+    <col min="5381" max="5381" width="74.6640625" style="40" customWidth="1"/>
+    <col min="5382" max="5632" width="14.77734375" style="40"/>
+    <col min="5633" max="5633" width="56.6640625" style="40" bestFit="1" customWidth="1"/>
+    <col min="5634" max="5634" width="33.6640625" style="40" customWidth="1"/>
+    <col min="5635" max="5635" width="14.6640625" style="40" customWidth="1"/>
+    <col min="5636" max="5636" width="13.44140625" style="40" customWidth="1"/>
+    <col min="5637" max="5637" width="74.6640625" style="40" customWidth="1"/>
+    <col min="5638" max="5888" width="14.77734375" style="40"/>
+    <col min="5889" max="5889" width="56.6640625" style="40" bestFit="1" customWidth="1"/>
+    <col min="5890" max="5890" width="33.6640625" style="40" customWidth="1"/>
+    <col min="5891" max="5891" width="14.6640625" style="40" customWidth="1"/>
+    <col min="5892" max="5892" width="13.44140625" style="40" customWidth="1"/>
+    <col min="5893" max="5893" width="74.6640625" style="40" customWidth="1"/>
+    <col min="5894" max="6144" width="14.77734375" style="40"/>
+    <col min="6145" max="6145" width="56.6640625" style="40" bestFit="1" customWidth="1"/>
+    <col min="6146" max="6146" width="33.6640625" style="40" customWidth="1"/>
+    <col min="6147" max="6147" width="14.6640625" style="40" customWidth="1"/>
+    <col min="6148" max="6148" width="13.44140625" style="40" customWidth="1"/>
+    <col min="6149" max="6149" width="74.6640625" style="40" customWidth="1"/>
+    <col min="6150" max="6400" width="14.77734375" style="40"/>
+    <col min="6401" max="6401" width="56.6640625" style="40" bestFit="1" customWidth="1"/>
+    <col min="6402" max="6402" width="33.6640625" style="40" customWidth="1"/>
+    <col min="6403" max="6403" width="14.6640625" style="40" customWidth="1"/>
+    <col min="6404" max="6404" width="13.44140625" style="40" customWidth="1"/>
+    <col min="6405" max="6405" width="74.6640625" style="40" customWidth="1"/>
+    <col min="6406" max="6656" width="14.77734375" style="40"/>
+    <col min="6657" max="6657" width="56.6640625" style="40" bestFit="1" customWidth="1"/>
+    <col min="6658" max="6658" width="33.6640625" style="40" customWidth="1"/>
+    <col min="6659" max="6659" width="14.6640625" style="40" customWidth="1"/>
+    <col min="6660" max="6660" width="13.44140625" style="40" customWidth="1"/>
+    <col min="6661" max="6661" width="74.6640625" style="40" customWidth="1"/>
+    <col min="6662" max="6912" width="14.77734375" style="40"/>
+    <col min="6913" max="6913" width="56.6640625" style="40" bestFit="1" customWidth="1"/>
+    <col min="6914" max="6914" width="33.6640625" style="40" customWidth="1"/>
+    <col min="6915" max="6915" width="14.6640625" style="40" customWidth="1"/>
+    <col min="6916" max="6916" width="13.44140625" style="40" customWidth="1"/>
+    <col min="6917" max="6917" width="74.6640625" style="40" customWidth="1"/>
+    <col min="6918" max="7168" width="14.77734375" style="40"/>
+    <col min="7169" max="7169" width="56.6640625" style="40" bestFit="1" customWidth="1"/>
+    <col min="7170" max="7170" width="33.6640625" style="40" customWidth="1"/>
+    <col min="7171" max="7171" width="14.6640625" style="40" customWidth="1"/>
+    <col min="7172" max="7172" width="13.44140625" style="40" customWidth="1"/>
+    <col min="7173" max="7173" width="74.6640625" style="40" customWidth="1"/>
+    <col min="7174" max="7424" width="14.77734375" style="40"/>
+    <col min="7425" max="7425" width="56.6640625" style="40" bestFit="1" customWidth="1"/>
+    <col min="7426" max="7426" width="33.6640625" style="40" customWidth="1"/>
+    <col min="7427" max="7427" width="14.6640625" style="40" customWidth="1"/>
+    <col min="7428" max="7428" width="13.44140625" style="40" customWidth="1"/>
+    <col min="7429" max="7429" width="74.6640625" style="40" customWidth="1"/>
+    <col min="7430" max="7680" width="14.77734375" style="40"/>
+    <col min="7681" max="7681" width="56.6640625" style="40" bestFit="1" customWidth="1"/>
+    <col min="7682" max="7682" width="33.6640625" style="40" customWidth="1"/>
+    <col min="7683" max="7683" width="14.6640625" style="40" customWidth="1"/>
+    <col min="7684" max="7684" width="13.44140625" style="40" customWidth="1"/>
+    <col min="7685" max="7685" width="74.6640625" style="40" customWidth="1"/>
+    <col min="7686" max="7936" width="14.77734375" style="40"/>
+    <col min="7937" max="7937" width="56.6640625" style="40" bestFit="1" customWidth="1"/>
+    <col min="7938" max="7938" width="33.6640625" style="40" customWidth="1"/>
+    <col min="7939" max="7939" width="14.6640625" style="40" customWidth="1"/>
+    <col min="7940" max="7940" width="13.44140625" style="40" customWidth="1"/>
+    <col min="7941" max="7941" width="74.6640625" style="40" customWidth="1"/>
+    <col min="7942" max="8192" width="14.77734375" style="40"/>
+    <col min="8193" max="8193" width="56.6640625" style="40" bestFit="1" customWidth="1"/>
+    <col min="8194" max="8194" width="33.6640625" style="40" customWidth="1"/>
+    <col min="8195" max="8195" width="14.6640625" style="40" customWidth="1"/>
+    <col min="8196" max="8196" width="13.44140625" style="40" customWidth="1"/>
+    <col min="8197" max="8197" width="74.6640625" style="40" customWidth="1"/>
+    <col min="8198" max="8448" width="14.77734375" style="40"/>
+    <col min="8449" max="8449" width="56.6640625" style="40" bestFit="1" customWidth="1"/>
+    <col min="8450" max="8450" width="33.6640625" style="40" customWidth="1"/>
+    <col min="8451" max="8451" width="14.6640625" style="40" customWidth="1"/>
+    <col min="8452" max="8452" width="13.44140625" style="40" customWidth="1"/>
+    <col min="8453" max="8453" width="74.6640625" style="40" customWidth="1"/>
+    <col min="8454" max="8704" width="14.77734375" style="40"/>
+    <col min="8705" max="8705" width="56.6640625" style="40" bestFit="1" customWidth="1"/>
+    <col min="8706" max="8706" width="33.6640625" style="40" customWidth="1"/>
+    <col min="8707" max="8707" width="14.6640625" style="40" customWidth="1"/>
+    <col min="8708" max="8708" width="13.44140625" style="40" customWidth="1"/>
+    <col min="8709" max="8709" width="74.6640625" style="40" customWidth="1"/>
+    <col min="8710" max="8960" width="14.77734375" style="40"/>
+    <col min="8961" max="8961" width="56.6640625" style="40" bestFit="1" customWidth="1"/>
+    <col min="8962" max="8962" width="33.6640625" style="40" customWidth="1"/>
+    <col min="8963" max="8963" width="14.6640625" style="40" customWidth="1"/>
+    <col min="8964" max="8964" width="13.44140625" style="40" customWidth="1"/>
+    <col min="8965" max="8965" width="74.6640625" style="40" customWidth="1"/>
+    <col min="8966" max="9216" width="14.77734375" style="40"/>
+    <col min="9217" max="9217" width="56.6640625" style="40" bestFit="1" customWidth="1"/>
+    <col min="9218" max="9218" width="33.6640625" style="40" customWidth="1"/>
+    <col min="9219" max="9219" width="14.6640625" style="40" customWidth="1"/>
+    <col min="9220" max="9220" width="13.44140625" style="40" customWidth="1"/>
+    <col min="9221" max="9221" width="74.6640625" style="40" customWidth="1"/>
+    <col min="9222" max="9472" width="14.77734375" style="40"/>
+    <col min="9473" max="9473" width="56.6640625" style="40" bestFit="1" customWidth="1"/>
+    <col min="9474" max="9474" width="33.6640625" style="40" customWidth="1"/>
+    <col min="9475" max="9475" width="14.6640625" style="40" customWidth="1"/>
+    <col min="9476" max="9476" width="13.44140625" style="40" customWidth="1"/>
+    <col min="9477" max="9477" width="74.6640625" style="40" customWidth="1"/>
+    <col min="9478" max="9728" width="14.77734375" style="40"/>
+    <col min="9729" max="9729" width="56.6640625" style="40" bestFit="1" customWidth="1"/>
+    <col min="9730" max="9730" width="33.6640625" style="40" customWidth="1"/>
+    <col min="9731" max="9731" width="14.6640625" style="40" customWidth="1"/>
+    <col min="9732" max="9732" width="13.44140625" style="40" customWidth="1"/>
+    <col min="9733" max="9733" width="74.6640625" style="40" customWidth="1"/>
+    <col min="9734" max="9984" width="14.77734375" style="40"/>
+    <col min="9985" max="9985" width="56.6640625" style="40" bestFit="1" customWidth="1"/>
+    <col min="9986" max="9986" width="33.6640625" style="40" customWidth="1"/>
+    <col min="9987" max="9987" width="14.6640625" style="40" customWidth="1"/>
+    <col min="9988" max="9988" width="13.44140625" style="40" customWidth="1"/>
+    <col min="9989" max="9989" width="74.6640625" style="40" customWidth="1"/>
+    <col min="9990" max="10240" width="14.77734375" style="40"/>
+    <col min="10241" max="10241" width="56.6640625" style="40" bestFit="1" customWidth="1"/>
+    <col min="10242" max="10242" width="33.6640625" style="40" customWidth="1"/>
+    <col min="10243" max="10243" width="14.6640625" style="40" customWidth="1"/>
+    <col min="10244" max="10244" width="13.44140625" style="40" customWidth="1"/>
+    <col min="10245" max="10245" width="74.6640625" style="40" customWidth="1"/>
+    <col min="10246" max="10496" width="14.77734375" style="40"/>
+    <col min="10497" max="10497" width="56.6640625" style="40" bestFit="1" customWidth="1"/>
+    <col min="10498" max="10498" width="33.6640625" style="40" customWidth="1"/>
+    <col min="10499" max="10499" width="14.6640625" style="40" customWidth="1"/>
+    <col min="10500" max="10500" width="13.44140625" style="40" customWidth="1"/>
+    <col min="10501" max="10501" width="74.6640625" style="40" customWidth="1"/>
+    <col min="10502" max="10752" width="14.77734375" style="40"/>
+    <col min="10753" max="10753" width="56.6640625" style="40" bestFit="1" customWidth="1"/>
+    <col min="10754" max="10754" width="33.6640625" style="40" customWidth="1"/>
+    <col min="10755" max="10755" width="14.6640625" style="40" customWidth="1"/>
+    <col min="10756" max="10756" width="13.44140625" style="40" customWidth="1"/>
+    <col min="10757" max="10757" width="74.6640625" style="40" customWidth="1"/>
+    <col min="10758" max="11008" width="14.77734375" style="40"/>
+    <col min="11009" max="11009" width="56.6640625" style="40" bestFit="1" customWidth="1"/>
+    <col min="11010" max="11010" width="33.6640625" style="40" customWidth="1"/>
+    <col min="11011" max="11011" width="14.6640625" style="40" customWidth="1"/>
+    <col min="11012" max="11012" width="13.44140625" style="40" customWidth="1"/>
+    <col min="11013" max="11013" width="74.6640625" style="40" customWidth="1"/>
+    <col min="11014" max="11264" width="14.77734375" style="40"/>
+    <col min="11265" max="11265" width="56.6640625" style="40" bestFit="1" customWidth="1"/>
+    <col min="11266" max="11266" width="33.6640625" style="40" customWidth="1"/>
+    <col min="11267" max="11267" width="14.6640625" style="40" customWidth="1"/>
+    <col min="11268" max="11268" width="13.44140625" style="40" customWidth="1"/>
+    <col min="11269" max="11269" width="74.6640625" style="40" customWidth="1"/>
+    <col min="11270" max="11520" width="14.77734375" style="40"/>
+    <col min="11521" max="11521" width="56.6640625" style="40" bestFit="1" customWidth="1"/>
+    <col min="11522" max="11522" width="33.6640625" style="40" customWidth="1"/>
+    <col min="11523" max="11523" width="14.6640625" style="40" customWidth="1"/>
+    <col min="11524" max="11524" width="13.44140625" style="40" customWidth="1"/>
+    <col min="11525" max="11525" width="74.6640625" style="40" customWidth="1"/>
+    <col min="11526" max="11776" width="14.77734375" style="40"/>
+    <col min="11777" max="11777" width="56.6640625" style="40" bestFit="1" customWidth="1"/>
+    <col min="11778" max="11778" width="33.6640625" style="40" customWidth="1"/>
+    <col min="11779" max="11779" width="14.6640625" style="40" customWidth="1"/>
+    <col min="11780" max="11780" width="13.44140625" style="40" customWidth="1"/>
+    <col min="11781" max="11781" width="74.6640625" style="40" customWidth="1"/>
+    <col min="11782" max="12032" width="14.77734375" style="40"/>
+    <col min="12033" max="12033" width="56.6640625" style="40" bestFit="1" customWidth="1"/>
+    <col min="12034" max="12034" width="33.6640625" style="40" customWidth="1"/>
+    <col min="12035" max="12035" width="14.6640625" style="40" customWidth="1"/>
+    <col min="12036" max="12036" width="13.44140625" style="40" customWidth="1"/>
+    <col min="12037" max="12037" width="74.6640625" style="40" customWidth="1"/>
+    <col min="12038" max="12288" width="14.77734375" style="40"/>
+    <col min="12289" max="12289" width="56.6640625" style="40" bestFit="1" customWidth="1"/>
+    <col min="12290" max="12290" width="33.6640625" style="40" customWidth="1"/>
+    <col min="12291" max="12291" width="14.6640625" style="40" customWidth="1"/>
+    <col min="12292" max="12292" width="13.44140625" style="40" customWidth="1"/>
+    <col min="12293" max="12293" width="74.6640625" style="40" customWidth="1"/>
+    <col min="12294" max="12544" width="14.77734375" style="40"/>
+    <col min="12545" max="12545" width="56.6640625" style="40" bestFit="1" customWidth="1"/>
+    <col min="12546" max="12546" width="33.6640625" style="40" customWidth="1"/>
+    <col min="12547" max="12547" width="14.6640625" style="40" customWidth="1"/>
+    <col min="12548" max="12548" width="13.44140625" style="40" customWidth="1"/>
+    <col min="12549" max="12549" width="74.6640625" style="40" customWidth="1"/>
+    <col min="12550" max="12800" width="14.77734375" style="40"/>
+    <col min="12801" max="12801" width="56.6640625" style="40" bestFit="1" customWidth="1"/>
+    <col min="12802" max="12802" width="33.6640625" style="40" customWidth="1"/>
+    <col min="12803" max="12803" width="14.6640625" style="40" customWidth="1"/>
+    <col min="12804" max="12804" width="13.44140625" style="40" customWidth="1"/>
+    <col min="12805" max="12805" width="74.6640625" style="40" customWidth="1"/>
+    <col min="12806" max="13056" width="14.77734375" style="40"/>
+    <col min="13057" max="13057" width="56.6640625" style="40" bestFit="1" customWidth="1"/>
+    <col min="13058" max="13058" width="33.6640625" style="40" customWidth="1"/>
+    <col min="13059" max="13059" width="14.6640625" style="40" customWidth="1"/>
+    <col min="13060" max="13060" width="13.44140625" style="40" customWidth="1"/>
+    <col min="13061" max="13061" width="74.6640625" style="40" customWidth="1"/>
+    <col min="13062" max="13312" width="14.77734375" style="40"/>
+    <col min="13313" max="13313" width="56.6640625" style="40" bestFit="1" customWidth="1"/>
+    <col min="13314" max="13314" width="33.6640625" style="40" customWidth="1"/>
+    <col min="13315" max="13315" width="14.6640625" style="40" customWidth="1"/>
+    <col min="13316" max="13316" width="13.44140625" style="40" customWidth="1"/>
+    <col min="13317" max="13317" width="74.6640625" style="40" customWidth="1"/>
+    <col min="13318" max="13568" width="14.77734375" style="40"/>
+    <col min="13569" max="13569" width="56.6640625" style="40" bestFit="1" customWidth="1"/>
+    <col min="13570" max="13570" width="33.6640625" style="40" customWidth="1"/>
+    <col min="13571" max="13571" width="14.6640625" style="40" customWidth="1"/>
+    <col min="13572" max="13572" width="13.44140625" style="40" customWidth="1"/>
+    <col min="13573" max="13573" width="74.6640625" style="40" customWidth="1"/>
+    <col min="13574" max="13824" width="14.77734375" style="40"/>
+    <col min="13825" max="13825" width="56.6640625" style="40" bestFit="1" customWidth="1"/>
+    <col min="13826" max="13826" width="33.6640625" style="40" customWidth="1"/>
+    <col min="13827" max="13827" width="14.6640625" style="40" customWidth="1"/>
+    <col min="13828" max="13828" width="13.44140625" style="40" customWidth="1"/>
+    <col min="13829" max="13829" width="74.6640625" style="40" customWidth="1"/>
+    <col min="13830" max="14080" width="14.77734375" style="40"/>
+    <col min="14081" max="14081" width="56.6640625" style="40" bestFit="1" customWidth="1"/>
+    <col min="14082" max="14082" width="33.6640625" style="40" customWidth="1"/>
+    <col min="14083" max="14083" width="14.6640625" style="40" customWidth="1"/>
+    <col min="14084" max="14084" width="13.44140625" style="40" customWidth="1"/>
+    <col min="14085" max="14085" width="74.6640625" style="40" customWidth="1"/>
+    <col min="14086" max="14336" width="14.77734375" style="40"/>
+    <col min="14337" max="14337" width="56.6640625" style="40" bestFit="1" customWidth="1"/>
+    <col min="14338" max="14338" width="33.6640625" style="40" customWidth="1"/>
+    <col min="14339" max="14339" width="14.6640625" style="40" customWidth="1"/>
+    <col min="14340" max="14340" width="13.44140625" style="40" customWidth="1"/>
+    <col min="14341" max="14341" width="74.6640625" style="40" customWidth="1"/>
+    <col min="14342" max="14592" width="14.77734375" style="40"/>
+    <col min="14593" max="14593" width="56.6640625" style="40" bestFit="1" customWidth="1"/>
+    <col min="14594" max="14594" width="33.6640625" style="40" customWidth="1"/>
+    <col min="14595" max="14595" width="14.6640625" style="40" customWidth="1"/>
+    <col min="14596" max="14596" width="13.44140625" style="40" customWidth="1"/>
+    <col min="14597" max="14597" width="74.6640625" style="40" customWidth="1"/>
+    <col min="14598" max="14848" width="14.77734375" style="40"/>
+    <col min="14849" max="14849" width="56.6640625" style="40" bestFit="1" customWidth="1"/>
+    <col min="14850" max="14850" width="33.6640625" style="40" customWidth="1"/>
+    <col min="14851" max="14851" width="14.6640625" style="40" customWidth="1"/>
+    <col min="14852" max="14852" width="13.44140625" style="40" customWidth="1"/>
+    <col min="14853" max="14853" width="74.6640625" style="40" customWidth="1"/>
+    <col min="14854" max="15104" width="14.77734375" style="40"/>
+    <col min="15105" max="15105" width="56.6640625" style="40" bestFit="1" customWidth="1"/>
+    <col min="15106" max="15106" width="33.6640625" style="40" customWidth="1"/>
+    <col min="15107" max="15107" width="14.6640625" style="40" customWidth="1"/>
+    <col min="15108" max="15108" width="13.44140625" style="40" customWidth="1"/>
+    <col min="15109" max="15109" width="74.6640625" style="40" customWidth="1"/>
+    <col min="15110" max="15360" width="14.77734375" style="40"/>
+    <col min="15361" max="15361" width="56.6640625" style="40" bestFit="1" customWidth="1"/>
+    <col min="15362" max="15362" width="33.6640625" style="40" customWidth="1"/>
+    <col min="15363" max="15363" width="14.6640625" style="40" customWidth="1"/>
+    <col min="15364" max="15364" width="13.44140625" style="40" customWidth="1"/>
+    <col min="15365" max="15365" width="74.6640625" style="40" customWidth="1"/>
+    <col min="15366" max="15616" width="14.77734375" style="40"/>
+    <col min="15617" max="15617" width="56.6640625" style="40" bestFit="1" customWidth="1"/>
+    <col min="15618" max="15618" width="33.6640625" style="40" customWidth="1"/>
+    <col min="15619" max="15619" width="14.6640625" style="40" customWidth="1"/>
+    <col min="15620" max="15620" width="13.44140625" style="40" customWidth="1"/>
+    <col min="15621" max="15621" width="74.6640625" style="40" customWidth="1"/>
+    <col min="15622" max="15872" width="14.77734375" style="40"/>
+    <col min="15873" max="15873" width="56.6640625" style="40" bestFit="1" customWidth="1"/>
+    <col min="15874" max="15874" width="33.6640625" style="40" customWidth="1"/>
+    <col min="15875" max="15875" width="14.6640625" style="40" customWidth="1"/>
+    <col min="15876" max="15876" width="13.44140625" style="40" customWidth="1"/>
+    <col min="15877" max="15877" width="74.6640625" style="40" customWidth="1"/>
+    <col min="15878" max="16128" width="14.77734375" style="40"/>
+    <col min="16129" max="16129" width="56.6640625" style="40" bestFit="1" customWidth="1"/>
+    <col min="16130" max="16130" width="33.6640625" style="40" customWidth="1"/>
+    <col min="16131" max="16131" width="14.6640625" style="40" customWidth="1"/>
+    <col min="16132" max="16132" width="13.44140625" style="40" customWidth="1"/>
+    <col min="16133" max="16133" width="74.6640625" style="40" customWidth="1"/>
+    <col min="16134" max="16384" width="14.77734375" style="40"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" s="2" customFormat="1" ht="40.25" customHeight="1" thickBot="1">
-      <c r="A1" s="108"/>
-      <c r="B1" s="109"/>
-      <c r="C1" s="109"/>
-      <c r="D1" s="109"/>
-      <c r="E1" s="109"/>
-    </row>
-    <row r="2" spans="1:5" ht="14" customHeight="1">
+    <row r="1" spans="1:5" s="2" customFormat="1" ht="40.200000000000003" customHeight="1" thickBot="1">
+      <c r="A1" s="93"/>
+      <c r="B1" s="94"/>
+      <c r="C1" s="94"/>
+      <c r="D1" s="94"/>
+      <c r="E1" s="94"/>
+    </row>
+    <row r="2" spans="1:5" ht="13.95" customHeight="1">
       <c r="A2" s="118" t="s">
         <v>64</v>
       </c>
-      <c r="B2" s="112" t="s">
+      <c r="B2" s="97" t="s">
         <v>65</v>
       </c>
       <c r="C2" s="119" t="s">
@@ -48206,16 +48243,16 @@
       <c r="D2" s="119" t="s">
         <v>67</v>
       </c>
-      <c r="E2" s="112" t="s">
+      <c r="E2" s="97" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="3" spans="1:5" ht="14.5" thickBot="1">
-      <c r="A3" s="111"/>
-      <c r="B3" s="113"/>
-      <c r="C3" s="115"/>
-      <c r="D3" s="115"/>
-      <c r="E3" s="113"/>
+    <row r="3" spans="1:5" ht="14.4" thickBot="1">
+      <c r="A3" s="96"/>
+      <c r="B3" s="98"/>
+      <c r="C3" s="100"/>
+      <c r="D3" s="100"/>
+      <c r="E3" s="98"/>
     </row>
     <row r="4" spans="1:5">
       <c r="A4" s="41" t="s">
@@ -48288,7 +48325,7 @@
         <v>389</v>
       </c>
     </row>
-    <row r="9" spans="1:5" ht="14.5" thickBot="1">
+    <row r="9" spans="1:5" ht="14.4" thickBot="1">
       <c r="A9" s="45" t="s">
         <v>153</v>
       </c>
@@ -48303,7 +48340,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="10" spans="1:5" ht="14.5" thickBot="1">
+    <row r="10" spans="1:5" ht="14.4" thickBot="1">
       <c r="A10" s="5"/>
       <c r="B10" s="5"/>
       <c r="C10" s="6"/>
@@ -48329,7 +48366,7 @@
       <c r="A12" s="49" t="s">
         <v>156</v>
       </c>
-      <c r="B12" s="101"/>
+      <c r="B12" s="102"/>
       <c r="C12" s="10" t="s">
         <v>228</v>
       </c>
@@ -48344,7 +48381,7 @@
       <c r="A13" s="51" t="s">
         <v>151</v>
       </c>
-      <c r="B13" s="101"/>
+      <c r="B13" s="102"/>
       <c r="C13" s="10" t="s">
         <v>229</v>
       </c>
@@ -48381,7 +48418,7 @@
         <v>391</v>
       </c>
     </row>
-    <row r="16" spans="1:5" ht="14.5" thickBot="1">
+    <row r="16" spans="1:5" ht="14.4" thickBot="1">
       <c r="A16" s="54" t="s">
         <v>153</v>
       </c>
@@ -48415,7 +48452,7 @@
       <c r="A18" s="51" t="s">
         <v>156</v>
       </c>
-      <c r="B18" s="101"/>
+      <c r="B18" s="102"/>
       <c r="C18" s="10">
         <v>737261</v>
       </c>
@@ -48430,7 +48467,7 @@
       <c r="A19" s="51" t="s">
         <v>151</v>
       </c>
-      <c r="B19" s="101"/>
+      <c r="B19" s="102"/>
       <c r="C19" s="10">
         <v>737262</v>
       </c>
@@ -48456,11 +48493,11 @@
         <v>162</v>
       </c>
     </row>
-    <row r="21" spans="1:5" ht="14.5" thickBot="1">
+    <row r="21" spans="1:5" ht="14.4" thickBot="1">
       <c r="A21" s="45" t="s">
         <v>153</v>
       </c>
-      <c r="B21" s="102"/>
+      <c r="B21" s="103"/>
       <c r="C21" s="16">
         <v>737263</v>
       </c>
@@ -48471,7 +48508,7 @@
         <v>163</v>
       </c>
     </row>
-    <row r="22" spans="1:5" ht="14.5" thickBot="1">
+    <row r="22" spans="1:5" ht="14.4" thickBot="1">
       <c r="A22" s="58"/>
       <c r="B22" s="59"/>
       <c r="C22" s="60"/>
@@ -48597,7 +48634,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="32" spans="1:5" ht="14.5" thickBot="1">
+    <row r="32" spans="1:5" ht="14.4" thickBot="1">
       <c r="A32" s="127"/>
       <c r="B32" s="130"/>
       <c r="C32" s="14">
@@ -48610,15 +48647,15 @@
         <v>174</v>
       </c>
     </row>
-    <row r="33" spans="1:5" ht="14.5" thickBot="1">
+    <row r="33" spans="1:5" ht="14.4" thickBot="1">
       <c r="A33" s="5"/>
       <c r="B33" s="68"/>
       <c r="C33" s="69"/>
       <c r="D33" s="69"/>
       <c r="E33" s="70"/>
     </row>
-    <row r="34" spans="1:5" ht="39.65" customHeight="1">
-      <c r="A34" s="107" t="s">
+    <row r="34" spans="1:5" ht="39.6" customHeight="1">
+      <c r="A34" s="113" t="s">
         <v>175</v>
       </c>
       <c r="B34" s="116"/>
@@ -48633,7 +48670,7 @@
       </c>
     </row>
     <row r="35" spans="1:5" ht="42" customHeight="1" thickBot="1">
-      <c r="A35" s="94"/>
+      <c r="A35" s="106"/>
       <c r="B35" s="117"/>
       <c r="C35" s="73">
         <v>734493</v>
@@ -48682,345 +48719,345 @@
       <selection activeCell="C17" sqref="C17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.81640625" defaultRowHeight="14"/>
+  <sheetFormatPr defaultColWidth="14.77734375" defaultRowHeight="13.8"/>
   <cols>
-    <col min="1" max="1" width="23.54296875" style="40" customWidth="1"/>
-    <col min="2" max="2" width="33.6328125" style="40" customWidth="1"/>
-    <col min="3" max="4" width="14.81640625" style="40" customWidth="1"/>
-    <col min="5" max="5" width="82.453125" style="40" customWidth="1"/>
-    <col min="6" max="256" width="14.81640625" style="40"/>
-    <col min="257" max="257" width="23.54296875" style="40" customWidth="1"/>
-    <col min="258" max="258" width="33.6328125" style="40" customWidth="1"/>
-    <col min="259" max="260" width="14.81640625" style="40" customWidth="1"/>
-    <col min="261" max="261" width="82.453125" style="40" customWidth="1"/>
-    <col min="262" max="512" width="14.81640625" style="40"/>
-    <col min="513" max="513" width="23.54296875" style="40" customWidth="1"/>
-    <col min="514" max="514" width="33.6328125" style="40" customWidth="1"/>
-    <col min="515" max="516" width="14.81640625" style="40" customWidth="1"/>
-    <col min="517" max="517" width="82.453125" style="40" customWidth="1"/>
-    <col min="518" max="768" width="14.81640625" style="40"/>
-    <col min="769" max="769" width="23.54296875" style="40" customWidth="1"/>
-    <col min="770" max="770" width="33.6328125" style="40" customWidth="1"/>
-    <col min="771" max="772" width="14.81640625" style="40" customWidth="1"/>
-    <col min="773" max="773" width="82.453125" style="40" customWidth="1"/>
-    <col min="774" max="1024" width="14.81640625" style="40"/>
-    <col min="1025" max="1025" width="23.54296875" style="40" customWidth="1"/>
-    <col min="1026" max="1026" width="33.6328125" style="40" customWidth="1"/>
-    <col min="1027" max="1028" width="14.81640625" style="40" customWidth="1"/>
-    <col min="1029" max="1029" width="82.453125" style="40" customWidth="1"/>
-    <col min="1030" max="1280" width="14.81640625" style="40"/>
-    <col min="1281" max="1281" width="23.54296875" style="40" customWidth="1"/>
-    <col min="1282" max="1282" width="33.6328125" style="40" customWidth="1"/>
-    <col min="1283" max="1284" width="14.81640625" style="40" customWidth="1"/>
-    <col min="1285" max="1285" width="82.453125" style="40" customWidth="1"/>
-    <col min="1286" max="1536" width="14.81640625" style="40"/>
-    <col min="1537" max="1537" width="23.54296875" style="40" customWidth="1"/>
-    <col min="1538" max="1538" width="33.6328125" style="40" customWidth="1"/>
-    <col min="1539" max="1540" width="14.81640625" style="40" customWidth="1"/>
-    <col min="1541" max="1541" width="82.453125" style="40" customWidth="1"/>
-    <col min="1542" max="1792" width="14.81640625" style="40"/>
-    <col min="1793" max="1793" width="23.54296875" style="40" customWidth="1"/>
-    <col min="1794" max="1794" width="33.6328125" style="40" customWidth="1"/>
-    <col min="1795" max="1796" width="14.81640625" style="40" customWidth="1"/>
-    <col min="1797" max="1797" width="82.453125" style="40" customWidth="1"/>
-    <col min="1798" max="2048" width="14.81640625" style="40"/>
-    <col min="2049" max="2049" width="23.54296875" style="40" customWidth="1"/>
-    <col min="2050" max="2050" width="33.6328125" style="40" customWidth="1"/>
-    <col min="2051" max="2052" width="14.81640625" style="40" customWidth="1"/>
-    <col min="2053" max="2053" width="82.453125" style="40" customWidth="1"/>
-    <col min="2054" max="2304" width="14.81640625" style="40"/>
-    <col min="2305" max="2305" width="23.54296875" style="40" customWidth="1"/>
-    <col min="2306" max="2306" width="33.6328125" style="40" customWidth="1"/>
-    <col min="2307" max="2308" width="14.81640625" style="40" customWidth="1"/>
-    <col min="2309" max="2309" width="82.453125" style="40" customWidth="1"/>
-    <col min="2310" max="2560" width="14.81640625" style="40"/>
-    <col min="2561" max="2561" width="23.54296875" style="40" customWidth="1"/>
-    <col min="2562" max="2562" width="33.6328125" style="40" customWidth="1"/>
-    <col min="2563" max="2564" width="14.81640625" style="40" customWidth="1"/>
-    <col min="2565" max="2565" width="82.453125" style="40" customWidth="1"/>
-    <col min="2566" max="2816" width="14.81640625" style="40"/>
-    <col min="2817" max="2817" width="23.54296875" style="40" customWidth="1"/>
-    <col min="2818" max="2818" width="33.6328125" style="40" customWidth="1"/>
-    <col min="2819" max="2820" width="14.81640625" style="40" customWidth="1"/>
-    <col min="2821" max="2821" width="82.453125" style="40" customWidth="1"/>
-    <col min="2822" max="3072" width="14.81640625" style="40"/>
-    <col min="3073" max="3073" width="23.54296875" style="40" customWidth="1"/>
-    <col min="3074" max="3074" width="33.6328125" style="40" customWidth="1"/>
-    <col min="3075" max="3076" width="14.81640625" style="40" customWidth="1"/>
-    <col min="3077" max="3077" width="82.453125" style="40" customWidth="1"/>
-    <col min="3078" max="3328" width="14.81640625" style="40"/>
-    <col min="3329" max="3329" width="23.54296875" style="40" customWidth="1"/>
-    <col min="3330" max="3330" width="33.6328125" style="40" customWidth="1"/>
-    <col min="3331" max="3332" width="14.81640625" style="40" customWidth="1"/>
-    <col min="3333" max="3333" width="82.453125" style="40" customWidth="1"/>
-    <col min="3334" max="3584" width="14.81640625" style="40"/>
-    <col min="3585" max="3585" width="23.54296875" style="40" customWidth="1"/>
-    <col min="3586" max="3586" width="33.6328125" style="40" customWidth="1"/>
-    <col min="3587" max="3588" width="14.81640625" style="40" customWidth="1"/>
-    <col min="3589" max="3589" width="82.453125" style="40" customWidth="1"/>
-    <col min="3590" max="3840" width="14.81640625" style="40"/>
-    <col min="3841" max="3841" width="23.54296875" style="40" customWidth="1"/>
-    <col min="3842" max="3842" width="33.6328125" style="40" customWidth="1"/>
-    <col min="3843" max="3844" width="14.81640625" style="40" customWidth="1"/>
-    <col min="3845" max="3845" width="82.453125" style="40" customWidth="1"/>
-    <col min="3846" max="4096" width="14.81640625" style="40"/>
-    <col min="4097" max="4097" width="23.54296875" style="40" customWidth="1"/>
-    <col min="4098" max="4098" width="33.6328125" style="40" customWidth="1"/>
-    <col min="4099" max="4100" width="14.81640625" style="40" customWidth="1"/>
-    <col min="4101" max="4101" width="82.453125" style="40" customWidth="1"/>
-    <col min="4102" max="4352" width="14.81640625" style="40"/>
-    <col min="4353" max="4353" width="23.54296875" style="40" customWidth="1"/>
-    <col min="4354" max="4354" width="33.6328125" style="40" customWidth="1"/>
-    <col min="4355" max="4356" width="14.81640625" style="40" customWidth="1"/>
-    <col min="4357" max="4357" width="82.453125" style="40" customWidth="1"/>
-    <col min="4358" max="4608" width="14.81640625" style="40"/>
-    <col min="4609" max="4609" width="23.54296875" style="40" customWidth="1"/>
-    <col min="4610" max="4610" width="33.6328125" style="40" customWidth="1"/>
-    <col min="4611" max="4612" width="14.81640625" style="40" customWidth="1"/>
-    <col min="4613" max="4613" width="82.453125" style="40" customWidth="1"/>
-    <col min="4614" max="4864" width="14.81640625" style="40"/>
-    <col min="4865" max="4865" width="23.54296875" style="40" customWidth="1"/>
-    <col min="4866" max="4866" width="33.6328125" style="40" customWidth="1"/>
-    <col min="4867" max="4868" width="14.81640625" style="40" customWidth="1"/>
-    <col min="4869" max="4869" width="82.453125" style="40" customWidth="1"/>
-    <col min="4870" max="5120" width="14.81640625" style="40"/>
-    <col min="5121" max="5121" width="23.54296875" style="40" customWidth="1"/>
-    <col min="5122" max="5122" width="33.6328125" style="40" customWidth="1"/>
-    <col min="5123" max="5124" width="14.81640625" style="40" customWidth="1"/>
-    <col min="5125" max="5125" width="82.453125" style="40" customWidth="1"/>
-    <col min="5126" max="5376" width="14.81640625" style="40"/>
-    <col min="5377" max="5377" width="23.54296875" style="40" customWidth="1"/>
-    <col min="5378" max="5378" width="33.6328125" style="40" customWidth="1"/>
-    <col min="5379" max="5380" width="14.81640625" style="40" customWidth="1"/>
-    <col min="5381" max="5381" width="82.453125" style="40" customWidth="1"/>
-    <col min="5382" max="5632" width="14.81640625" style="40"/>
-    <col min="5633" max="5633" width="23.54296875" style="40" customWidth="1"/>
-    <col min="5634" max="5634" width="33.6328125" style="40" customWidth="1"/>
-    <col min="5635" max="5636" width="14.81640625" style="40" customWidth="1"/>
-    <col min="5637" max="5637" width="82.453125" style="40" customWidth="1"/>
-    <col min="5638" max="5888" width="14.81640625" style="40"/>
-    <col min="5889" max="5889" width="23.54296875" style="40" customWidth="1"/>
-    <col min="5890" max="5890" width="33.6328125" style="40" customWidth="1"/>
-    <col min="5891" max="5892" width="14.81640625" style="40" customWidth="1"/>
-    <col min="5893" max="5893" width="82.453125" style="40" customWidth="1"/>
-    <col min="5894" max="6144" width="14.81640625" style="40"/>
-    <col min="6145" max="6145" width="23.54296875" style="40" customWidth="1"/>
-    <col min="6146" max="6146" width="33.6328125" style="40" customWidth="1"/>
-    <col min="6147" max="6148" width="14.81640625" style="40" customWidth="1"/>
-    <col min="6149" max="6149" width="82.453125" style="40" customWidth="1"/>
-    <col min="6150" max="6400" width="14.81640625" style="40"/>
-    <col min="6401" max="6401" width="23.54296875" style="40" customWidth="1"/>
-    <col min="6402" max="6402" width="33.6328125" style="40" customWidth="1"/>
-    <col min="6403" max="6404" width="14.81640625" style="40" customWidth="1"/>
-    <col min="6405" max="6405" width="82.453125" style="40" customWidth="1"/>
-    <col min="6406" max="6656" width="14.81640625" style="40"/>
-    <col min="6657" max="6657" width="23.54296875" style="40" customWidth="1"/>
-    <col min="6658" max="6658" width="33.6328125" style="40" customWidth="1"/>
-    <col min="6659" max="6660" width="14.81640625" style="40" customWidth="1"/>
-    <col min="6661" max="6661" width="82.453125" style="40" customWidth="1"/>
-    <col min="6662" max="6912" width="14.81640625" style="40"/>
-    <col min="6913" max="6913" width="23.54296875" style="40" customWidth="1"/>
-    <col min="6914" max="6914" width="33.6328125" style="40" customWidth="1"/>
-    <col min="6915" max="6916" width="14.81640625" style="40" customWidth="1"/>
-    <col min="6917" max="6917" width="82.453125" style="40" customWidth="1"/>
-    <col min="6918" max="7168" width="14.81640625" style="40"/>
-    <col min="7169" max="7169" width="23.54296875" style="40" customWidth="1"/>
-    <col min="7170" max="7170" width="33.6328125" style="40" customWidth="1"/>
-    <col min="7171" max="7172" width="14.81640625" style="40" customWidth="1"/>
-    <col min="7173" max="7173" width="82.453125" style="40" customWidth="1"/>
-    <col min="7174" max="7424" width="14.81640625" style="40"/>
-    <col min="7425" max="7425" width="23.54296875" style="40" customWidth="1"/>
-    <col min="7426" max="7426" width="33.6328125" style="40" customWidth="1"/>
-    <col min="7427" max="7428" width="14.81640625" style="40" customWidth="1"/>
-    <col min="7429" max="7429" width="82.453125" style="40" customWidth="1"/>
-    <col min="7430" max="7680" width="14.81640625" style="40"/>
-    <col min="7681" max="7681" width="23.54296875" style="40" customWidth="1"/>
-    <col min="7682" max="7682" width="33.6328125" style="40" customWidth="1"/>
-    <col min="7683" max="7684" width="14.81640625" style="40" customWidth="1"/>
-    <col min="7685" max="7685" width="82.453125" style="40" customWidth="1"/>
-    <col min="7686" max="7936" width="14.81640625" style="40"/>
-    <col min="7937" max="7937" width="23.54296875" style="40" customWidth="1"/>
-    <col min="7938" max="7938" width="33.6328125" style="40" customWidth="1"/>
-    <col min="7939" max="7940" width="14.81640625" style="40" customWidth="1"/>
-    <col min="7941" max="7941" width="82.453125" style="40" customWidth="1"/>
-    <col min="7942" max="8192" width="14.81640625" style="40"/>
-    <col min="8193" max="8193" width="23.54296875" style="40" customWidth="1"/>
-    <col min="8194" max="8194" width="33.6328125" style="40" customWidth="1"/>
-    <col min="8195" max="8196" width="14.81640625" style="40" customWidth="1"/>
-    <col min="8197" max="8197" width="82.453125" style="40" customWidth="1"/>
-    <col min="8198" max="8448" width="14.81640625" style="40"/>
-    <col min="8449" max="8449" width="23.54296875" style="40" customWidth="1"/>
-    <col min="8450" max="8450" width="33.6328125" style="40" customWidth="1"/>
-    <col min="8451" max="8452" width="14.81640625" style="40" customWidth="1"/>
-    <col min="8453" max="8453" width="82.453125" style="40" customWidth="1"/>
-    <col min="8454" max="8704" width="14.81640625" style="40"/>
-    <col min="8705" max="8705" width="23.54296875" style="40" customWidth="1"/>
-    <col min="8706" max="8706" width="33.6328125" style="40" customWidth="1"/>
-    <col min="8707" max="8708" width="14.81640625" style="40" customWidth="1"/>
-    <col min="8709" max="8709" width="82.453125" style="40" customWidth="1"/>
-    <col min="8710" max="8960" width="14.81640625" style="40"/>
-    <col min="8961" max="8961" width="23.54296875" style="40" customWidth="1"/>
-    <col min="8962" max="8962" width="33.6328125" style="40" customWidth="1"/>
-    <col min="8963" max="8964" width="14.81640625" style="40" customWidth="1"/>
-    <col min="8965" max="8965" width="82.453125" style="40" customWidth="1"/>
-    <col min="8966" max="9216" width="14.81640625" style="40"/>
-    <col min="9217" max="9217" width="23.54296875" style="40" customWidth="1"/>
-    <col min="9218" max="9218" width="33.6328125" style="40" customWidth="1"/>
-    <col min="9219" max="9220" width="14.81640625" style="40" customWidth="1"/>
-    <col min="9221" max="9221" width="82.453125" style="40" customWidth="1"/>
-    <col min="9222" max="9472" width="14.81640625" style="40"/>
-    <col min="9473" max="9473" width="23.54296875" style="40" customWidth="1"/>
-    <col min="9474" max="9474" width="33.6328125" style="40" customWidth="1"/>
-    <col min="9475" max="9476" width="14.81640625" style="40" customWidth="1"/>
-    <col min="9477" max="9477" width="82.453125" style="40" customWidth="1"/>
-    <col min="9478" max="9728" width="14.81640625" style="40"/>
-    <col min="9729" max="9729" width="23.54296875" style="40" customWidth="1"/>
-    <col min="9730" max="9730" width="33.6328125" style="40" customWidth="1"/>
-    <col min="9731" max="9732" width="14.81640625" style="40" customWidth="1"/>
-    <col min="9733" max="9733" width="82.453125" style="40" customWidth="1"/>
-    <col min="9734" max="9984" width="14.81640625" style="40"/>
-    <col min="9985" max="9985" width="23.54296875" style="40" customWidth="1"/>
-    <col min="9986" max="9986" width="33.6328125" style="40" customWidth="1"/>
-    <col min="9987" max="9988" width="14.81640625" style="40" customWidth="1"/>
-    <col min="9989" max="9989" width="82.453125" style="40" customWidth="1"/>
-    <col min="9990" max="10240" width="14.81640625" style="40"/>
-    <col min="10241" max="10241" width="23.54296875" style="40" customWidth="1"/>
-    <col min="10242" max="10242" width="33.6328125" style="40" customWidth="1"/>
-    <col min="10243" max="10244" width="14.81640625" style="40" customWidth="1"/>
-    <col min="10245" max="10245" width="82.453125" style="40" customWidth="1"/>
-    <col min="10246" max="10496" width="14.81640625" style="40"/>
-    <col min="10497" max="10497" width="23.54296875" style="40" customWidth="1"/>
-    <col min="10498" max="10498" width="33.6328125" style="40" customWidth="1"/>
-    <col min="10499" max="10500" width="14.81640625" style="40" customWidth="1"/>
-    <col min="10501" max="10501" width="82.453125" style="40" customWidth="1"/>
-    <col min="10502" max="10752" width="14.81640625" style="40"/>
-    <col min="10753" max="10753" width="23.54296875" style="40" customWidth="1"/>
-    <col min="10754" max="10754" width="33.6328125" style="40" customWidth="1"/>
-    <col min="10755" max="10756" width="14.81640625" style="40" customWidth="1"/>
-    <col min="10757" max="10757" width="82.453125" style="40" customWidth="1"/>
-    <col min="10758" max="11008" width="14.81640625" style="40"/>
-    <col min="11009" max="11009" width="23.54296875" style="40" customWidth="1"/>
-    <col min="11010" max="11010" width="33.6328125" style="40" customWidth="1"/>
-    <col min="11011" max="11012" width="14.81640625" style="40" customWidth="1"/>
-    <col min="11013" max="11013" width="82.453125" style="40" customWidth="1"/>
-    <col min="11014" max="11264" width="14.81640625" style="40"/>
-    <col min="11265" max="11265" width="23.54296875" style="40" customWidth="1"/>
-    <col min="11266" max="11266" width="33.6328125" style="40" customWidth="1"/>
-    <col min="11267" max="11268" width="14.81640625" style="40" customWidth="1"/>
-    <col min="11269" max="11269" width="82.453125" style="40" customWidth="1"/>
-    <col min="11270" max="11520" width="14.81640625" style="40"/>
-    <col min="11521" max="11521" width="23.54296875" style="40" customWidth="1"/>
-    <col min="11522" max="11522" width="33.6328125" style="40" customWidth="1"/>
-    <col min="11523" max="11524" width="14.81640625" style="40" customWidth="1"/>
-    <col min="11525" max="11525" width="82.453125" style="40" customWidth="1"/>
-    <col min="11526" max="11776" width="14.81640625" style="40"/>
-    <col min="11777" max="11777" width="23.54296875" style="40" customWidth="1"/>
-    <col min="11778" max="11778" width="33.6328125" style="40" customWidth="1"/>
-    <col min="11779" max="11780" width="14.81640625" style="40" customWidth="1"/>
-    <col min="11781" max="11781" width="82.453125" style="40" customWidth="1"/>
-    <col min="11782" max="12032" width="14.81640625" style="40"/>
-    <col min="12033" max="12033" width="23.54296875" style="40" customWidth="1"/>
-    <col min="12034" max="12034" width="33.6328125" style="40" customWidth="1"/>
-    <col min="12035" max="12036" width="14.81640625" style="40" customWidth="1"/>
-    <col min="12037" max="12037" width="82.453125" style="40" customWidth="1"/>
-    <col min="12038" max="12288" width="14.81640625" style="40"/>
-    <col min="12289" max="12289" width="23.54296875" style="40" customWidth="1"/>
-    <col min="12290" max="12290" width="33.6328125" style="40" customWidth="1"/>
-    <col min="12291" max="12292" width="14.81640625" style="40" customWidth="1"/>
-    <col min="12293" max="12293" width="82.453125" style="40" customWidth="1"/>
-    <col min="12294" max="12544" width="14.81640625" style="40"/>
-    <col min="12545" max="12545" width="23.54296875" style="40" customWidth="1"/>
-    <col min="12546" max="12546" width="33.6328125" style="40" customWidth="1"/>
-    <col min="12547" max="12548" width="14.81640625" style="40" customWidth="1"/>
-    <col min="12549" max="12549" width="82.453125" style="40" customWidth="1"/>
-    <col min="12550" max="12800" width="14.81640625" style="40"/>
-    <col min="12801" max="12801" width="23.54296875" style="40" customWidth="1"/>
-    <col min="12802" max="12802" width="33.6328125" style="40" customWidth="1"/>
-    <col min="12803" max="12804" width="14.81640625" style="40" customWidth="1"/>
-    <col min="12805" max="12805" width="82.453125" style="40" customWidth="1"/>
-    <col min="12806" max="13056" width="14.81640625" style="40"/>
-    <col min="13057" max="13057" width="23.54296875" style="40" customWidth="1"/>
-    <col min="13058" max="13058" width="33.6328125" style="40" customWidth="1"/>
-    <col min="13059" max="13060" width="14.81640625" style="40" customWidth="1"/>
-    <col min="13061" max="13061" width="82.453125" style="40" customWidth="1"/>
-    <col min="13062" max="13312" width="14.81640625" style="40"/>
-    <col min="13313" max="13313" width="23.54296875" style="40" customWidth="1"/>
-    <col min="13314" max="13314" width="33.6328125" style="40" customWidth="1"/>
-    <col min="13315" max="13316" width="14.81640625" style="40" customWidth="1"/>
-    <col min="13317" max="13317" width="82.453125" style="40" customWidth="1"/>
-    <col min="13318" max="13568" width="14.81640625" style="40"/>
-    <col min="13569" max="13569" width="23.54296875" style="40" customWidth="1"/>
-    <col min="13570" max="13570" width="33.6328125" style="40" customWidth="1"/>
-    <col min="13571" max="13572" width="14.81640625" style="40" customWidth="1"/>
-    <col min="13573" max="13573" width="82.453125" style="40" customWidth="1"/>
-    <col min="13574" max="13824" width="14.81640625" style="40"/>
-    <col min="13825" max="13825" width="23.54296875" style="40" customWidth="1"/>
-    <col min="13826" max="13826" width="33.6328125" style="40" customWidth="1"/>
-    <col min="13827" max="13828" width="14.81640625" style="40" customWidth="1"/>
-    <col min="13829" max="13829" width="82.453125" style="40" customWidth="1"/>
-    <col min="13830" max="14080" width="14.81640625" style="40"/>
-    <col min="14081" max="14081" width="23.54296875" style="40" customWidth="1"/>
-    <col min="14082" max="14082" width="33.6328125" style="40" customWidth="1"/>
-    <col min="14083" max="14084" width="14.81640625" style="40" customWidth="1"/>
-    <col min="14085" max="14085" width="82.453125" style="40" customWidth="1"/>
-    <col min="14086" max="14336" width="14.81640625" style="40"/>
-    <col min="14337" max="14337" width="23.54296875" style="40" customWidth="1"/>
-    <col min="14338" max="14338" width="33.6328125" style="40" customWidth="1"/>
-    <col min="14339" max="14340" width="14.81640625" style="40" customWidth="1"/>
-    <col min="14341" max="14341" width="82.453125" style="40" customWidth="1"/>
-    <col min="14342" max="14592" width="14.81640625" style="40"/>
-    <col min="14593" max="14593" width="23.54296875" style="40" customWidth="1"/>
-    <col min="14594" max="14594" width="33.6328125" style="40" customWidth="1"/>
-    <col min="14595" max="14596" width="14.81640625" style="40" customWidth="1"/>
-    <col min="14597" max="14597" width="82.453125" style="40" customWidth="1"/>
-    <col min="14598" max="14848" width="14.81640625" style="40"/>
-    <col min="14849" max="14849" width="23.54296875" style="40" customWidth="1"/>
-    <col min="14850" max="14850" width="33.6328125" style="40" customWidth="1"/>
-    <col min="14851" max="14852" width="14.81640625" style="40" customWidth="1"/>
-    <col min="14853" max="14853" width="82.453125" style="40" customWidth="1"/>
-    <col min="14854" max="15104" width="14.81640625" style="40"/>
-    <col min="15105" max="15105" width="23.54296875" style="40" customWidth="1"/>
-    <col min="15106" max="15106" width="33.6328125" style="40" customWidth="1"/>
-    <col min="15107" max="15108" width="14.81640625" style="40" customWidth="1"/>
-    <col min="15109" max="15109" width="82.453125" style="40" customWidth="1"/>
-    <col min="15110" max="15360" width="14.81640625" style="40"/>
-    <col min="15361" max="15361" width="23.54296875" style="40" customWidth="1"/>
-    <col min="15362" max="15362" width="33.6328125" style="40" customWidth="1"/>
-    <col min="15363" max="15364" width="14.81640625" style="40" customWidth="1"/>
-    <col min="15365" max="15365" width="82.453125" style="40" customWidth="1"/>
-    <col min="15366" max="15616" width="14.81640625" style="40"/>
-    <col min="15617" max="15617" width="23.54296875" style="40" customWidth="1"/>
-    <col min="15618" max="15618" width="33.6328125" style="40" customWidth="1"/>
-    <col min="15619" max="15620" width="14.81640625" style="40" customWidth="1"/>
-    <col min="15621" max="15621" width="82.453125" style="40" customWidth="1"/>
-    <col min="15622" max="15872" width="14.81640625" style="40"/>
-    <col min="15873" max="15873" width="23.54296875" style="40" customWidth="1"/>
-    <col min="15874" max="15874" width="33.6328125" style="40" customWidth="1"/>
-    <col min="15875" max="15876" width="14.81640625" style="40" customWidth="1"/>
-    <col min="15877" max="15877" width="82.453125" style="40" customWidth="1"/>
-    <col min="15878" max="16128" width="14.81640625" style="40"/>
-    <col min="16129" max="16129" width="23.54296875" style="40" customWidth="1"/>
-    <col min="16130" max="16130" width="33.6328125" style="40" customWidth="1"/>
-    <col min="16131" max="16132" width="14.81640625" style="40" customWidth="1"/>
-    <col min="16133" max="16133" width="82.453125" style="40" customWidth="1"/>
-    <col min="16134" max="16384" width="14.81640625" style="40"/>
+    <col min="1" max="1" width="23.5546875" style="40" customWidth="1"/>
+    <col min="2" max="2" width="33.6640625" style="40" customWidth="1"/>
+    <col min="3" max="4" width="14.77734375" style="40" customWidth="1"/>
+    <col min="5" max="5" width="82.44140625" style="40" customWidth="1"/>
+    <col min="6" max="256" width="14.77734375" style="40"/>
+    <col min="257" max="257" width="23.5546875" style="40" customWidth="1"/>
+    <col min="258" max="258" width="33.6640625" style="40" customWidth="1"/>
+    <col min="259" max="260" width="14.77734375" style="40" customWidth="1"/>
+    <col min="261" max="261" width="82.44140625" style="40" customWidth="1"/>
+    <col min="262" max="512" width="14.77734375" style="40"/>
+    <col min="513" max="513" width="23.5546875" style="40" customWidth="1"/>
+    <col min="514" max="514" width="33.6640625" style="40" customWidth="1"/>
+    <col min="515" max="516" width="14.77734375" style="40" customWidth="1"/>
+    <col min="517" max="517" width="82.44140625" style="40" customWidth="1"/>
+    <col min="518" max="768" width="14.77734375" style="40"/>
+    <col min="769" max="769" width="23.5546875" style="40" customWidth="1"/>
+    <col min="770" max="770" width="33.6640625" style="40" customWidth="1"/>
+    <col min="771" max="772" width="14.77734375" style="40" customWidth="1"/>
+    <col min="773" max="773" width="82.44140625" style="40" customWidth="1"/>
+    <col min="774" max="1024" width="14.77734375" style="40"/>
+    <col min="1025" max="1025" width="23.5546875" style="40" customWidth="1"/>
+    <col min="1026" max="1026" width="33.6640625" style="40" customWidth="1"/>
+    <col min="1027" max="1028" width="14.77734375" style="40" customWidth="1"/>
+    <col min="1029" max="1029" width="82.44140625" style="40" customWidth="1"/>
+    <col min="1030" max="1280" width="14.77734375" style="40"/>
+    <col min="1281" max="1281" width="23.5546875" style="40" customWidth="1"/>
+    <col min="1282" max="1282" width="33.6640625" style="40" customWidth="1"/>
+    <col min="1283" max="1284" width="14.77734375" style="40" customWidth="1"/>
+    <col min="1285" max="1285" width="82.44140625" style="40" customWidth="1"/>
+    <col min="1286" max="1536" width="14.77734375" style="40"/>
+    <col min="1537" max="1537" width="23.5546875" style="40" customWidth="1"/>
+    <col min="1538" max="1538" width="33.6640625" style="40" customWidth="1"/>
+    <col min="1539" max="1540" width="14.77734375" style="40" customWidth="1"/>
+    <col min="1541" max="1541" width="82.44140625" style="40" customWidth="1"/>
+    <col min="1542" max="1792" width="14.77734375" style="40"/>
+    <col min="1793" max="1793" width="23.5546875" style="40" customWidth="1"/>
+    <col min="1794" max="1794" width="33.6640625" style="40" customWidth="1"/>
+    <col min="1795" max="1796" width="14.77734375" style="40" customWidth="1"/>
+    <col min="1797" max="1797" width="82.44140625" style="40" customWidth="1"/>
+    <col min="1798" max="2048" width="14.77734375" style="40"/>
+    <col min="2049" max="2049" width="23.5546875" style="40" customWidth="1"/>
+    <col min="2050" max="2050" width="33.6640625" style="40" customWidth="1"/>
+    <col min="2051" max="2052" width="14.77734375" style="40" customWidth="1"/>
+    <col min="2053" max="2053" width="82.44140625" style="40" customWidth="1"/>
+    <col min="2054" max="2304" width="14.77734375" style="40"/>
+    <col min="2305" max="2305" width="23.5546875" style="40" customWidth="1"/>
+    <col min="2306" max="2306" width="33.6640625" style="40" customWidth="1"/>
+    <col min="2307" max="2308" width="14.77734375" style="40" customWidth="1"/>
+    <col min="2309" max="2309" width="82.44140625" style="40" customWidth="1"/>
+    <col min="2310" max="2560" width="14.77734375" style="40"/>
+    <col min="2561" max="2561" width="23.5546875" style="40" customWidth="1"/>
+    <col min="2562" max="2562" width="33.6640625" style="40" customWidth="1"/>
+    <col min="2563" max="2564" width="14.77734375" style="40" customWidth="1"/>
+    <col min="2565" max="2565" width="82.44140625" style="40" customWidth="1"/>
+    <col min="2566" max="2816" width="14.77734375" style="40"/>
+    <col min="2817" max="2817" width="23.5546875" style="40" customWidth="1"/>
+    <col min="2818" max="2818" width="33.6640625" style="40" customWidth="1"/>
+    <col min="2819" max="2820" width="14.77734375" style="40" customWidth="1"/>
+    <col min="2821" max="2821" width="82.44140625" style="40" customWidth="1"/>
+    <col min="2822" max="3072" width="14.77734375" style="40"/>
+    <col min="3073" max="3073" width="23.5546875" style="40" customWidth="1"/>
+    <col min="3074" max="3074" width="33.6640625" style="40" customWidth="1"/>
+    <col min="3075" max="3076" width="14.77734375" style="40" customWidth="1"/>
+    <col min="3077" max="3077" width="82.44140625" style="40" customWidth="1"/>
+    <col min="3078" max="3328" width="14.77734375" style="40"/>
+    <col min="3329" max="3329" width="23.5546875" style="40" customWidth="1"/>
+    <col min="3330" max="3330" width="33.6640625" style="40" customWidth="1"/>
+    <col min="3331" max="3332" width="14.77734375" style="40" customWidth="1"/>
+    <col min="3333" max="3333" width="82.44140625" style="40" customWidth="1"/>
+    <col min="3334" max="3584" width="14.77734375" style="40"/>
+    <col min="3585" max="3585" width="23.5546875" style="40" customWidth="1"/>
+    <col min="3586" max="3586" width="33.6640625" style="40" customWidth="1"/>
+    <col min="3587" max="3588" width="14.77734375" style="40" customWidth="1"/>
+    <col min="3589" max="3589" width="82.44140625" style="40" customWidth="1"/>
+    <col min="3590" max="3840" width="14.77734375" style="40"/>
+    <col min="3841" max="3841" width="23.5546875" style="40" customWidth="1"/>
+    <col min="3842" max="3842" width="33.6640625" style="40" customWidth="1"/>
+    <col min="3843" max="3844" width="14.77734375" style="40" customWidth="1"/>
+    <col min="3845" max="3845" width="82.44140625" style="40" customWidth="1"/>
+    <col min="3846" max="4096" width="14.77734375" style="40"/>
+    <col min="4097" max="4097" width="23.5546875" style="40" customWidth="1"/>
+    <col min="4098" max="4098" width="33.6640625" style="40" customWidth="1"/>
+    <col min="4099" max="4100" width="14.77734375" style="40" customWidth="1"/>
+    <col min="4101" max="4101" width="82.44140625" style="40" customWidth="1"/>
+    <col min="4102" max="4352" width="14.77734375" style="40"/>
+    <col min="4353" max="4353" width="23.5546875" style="40" customWidth="1"/>
+    <col min="4354" max="4354" width="33.6640625" style="40" customWidth="1"/>
+    <col min="4355" max="4356" width="14.77734375" style="40" customWidth="1"/>
+    <col min="4357" max="4357" width="82.44140625" style="40" customWidth="1"/>
+    <col min="4358" max="4608" width="14.77734375" style="40"/>
+    <col min="4609" max="4609" width="23.5546875" style="40" customWidth="1"/>
+    <col min="4610" max="4610" width="33.6640625" style="40" customWidth="1"/>
+    <col min="4611" max="4612" width="14.77734375" style="40" customWidth="1"/>
+    <col min="4613" max="4613" width="82.44140625" style="40" customWidth="1"/>
+    <col min="4614" max="4864" width="14.77734375" style="40"/>
+    <col min="4865" max="4865" width="23.5546875" style="40" customWidth="1"/>
+    <col min="4866" max="4866" width="33.6640625" style="40" customWidth="1"/>
+    <col min="4867" max="4868" width="14.77734375" style="40" customWidth="1"/>
+    <col min="4869" max="4869" width="82.44140625" style="40" customWidth="1"/>
+    <col min="4870" max="5120" width="14.77734375" style="40"/>
+    <col min="5121" max="5121" width="23.5546875" style="40" customWidth="1"/>
+    <col min="5122" max="5122" width="33.6640625" style="40" customWidth="1"/>
+    <col min="5123" max="5124" width="14.77734375" style="40" customWidth="1"/>
+    <col min="5125" max="5125" width="82.44140625" style="40" customWidth="1"/>
+    <col min="5126" max="5376" width="14.77734375" style="40"/>
+    <col min="5377" max="5377" width="23.5546875" style="40" customWidth="1"/>
+    <col min="5378" max="5378" width="33.6640625" style="40" customWidth="1"/>
+    <col min="5379" max="5380" width="14.77734375" style="40" customWidth="1"/>
+    <col min="5381" max="5381" width="82.44140625" style="40" customWidth="1"/>
+    <col min="5382" max="5632" width="14.77734375" style="40"/>
+    <col min="5633" max="5633" width="23.5546875" style="40" customWidth="1"/>
+    <col min="5634" max="5634" width="33.6640625" style="40" customWidth="1"/>
+    <col min="5635" max="5636" width="14.77734375" style="40" customWidth="1"/>
+    <col min="5637" max="5637" width="82.44140625" style="40" customWidth="1"/>
+    <col min="5638" max="5888" width="14.77734375" style="40"/>
+    <col min="5889" max="5889" width="23.5546875" style="40" customWidth="1"/>
+    <col min="5890" max="5890" width="33.6640625" style="40" customWidth="1"/>
+    <col min="5891" max="5892" width="14.77734375" style="40" customWidth="1"/>
+    <col min="5893" max="5893" width="82.44140625" style="40" customWidth="1"/>
+    <col min="5894" max="6144" width="14.77734375" style="40"/>
+    <col min="6145" max="6145" width="23.5546875" style="40" customWidth="1"/>
+    <col min="6146" max="6146" width="33.6640625" style="40" customWidth="1"/>
+    <col min="6147" max="6148" width="14.77734375" style="40" customWidth="1"/>
+    <col min="6149" max="6149" width="82.44140625" style="40" customWidth="1"/>
+    <col min="6150" max="6400" width="14.77734375" style="40"/>
+    <col min="6401" max="6401" width="23.5546875" style="40" customWidth="1"/>
+    <col min="6402" max="6402" width="33.6640625" style="40" customWidth="1"/>
+    <col min="6403" max="6404" width="14.77734375" style="40" customWidth="1"/>
+    <col min="6405" max="6405" width="82.44140625" style="40" customWidth="1"/>
+    <col min="6406" max="6656" width="14.77734375" style="40"/>
+    <col min="6657" max="6657" width="23.5546875" style="40" customWidth="1"/>
+    <col min="6658" max="6658" width="33.6640625" style="40" customWidth="1"/>
+    <col min="6659" max="6660" width="14.77734375" style="40" customWidth="1"/>
+    <col min="6661" max="6661" width="82.44140625" style="40" customWidth="1"/>
+    <col min="6662" max="6912" width="14.77734375" style="40"/>
+    <col min="6913" max="6913" width="23.5546875" style="40" customWidth="1"/>
+    <col min="6914" max="6914" width="33.6640625" style="40" customWidth="1"/>
+    <col min="6915" max="6916" width="14.77734375" style="40" customWidth="1"/>
+    <col min="6917" max="6917" width="82.44140625" style="40" customWidth="1"/>
+    <col min="6918" max="7168" width="14.77734375" style="40"/>
+    <col min="7169" max="7169" width="23.5546875" style="40" customWidth="1"/>
+    <col min="7170" max="7170" width="33.6640625" style="40" customWidth="1"/>
+    <col min="7171" max="7172" width="14.77734375" style="40" customWidth="1"/>
+    <col min="7173" max="7173" width="82.44140625" style="40" customWidth="1"/>
+    <col min="7174" max="7424" width="14.77734375" style="40"/>
+    <col min="7425" max="7425" width="23.5546875" style="40" customWidth="1"/>
+    <col min="7426" max="7426" width="33.6640625" style="40" customWidth="1"/>
+    <col min="7427" max="7428" width="14.77734375" style="40" customWidth="1"/>
+    <col min="7429" max="7429" width="82.44140625" style="40" customWidth="1"/>
+    <col min="7430" max="7680" width="14.77734375" style="40"/>
+    <col min="7681" max="7681" width="23.5546875" style="40" customWidth="1"/>
+    <col min="7682" max="7682" width="33.6640625" style="40" customWidth="1"/>
+    <col min="7683" max="7684" width="14.77734375" style="40" customWidth="1"/>
+    <col min="7685" max="7685" width="82.44140625" style="40" customWidth="1"/>
+    <col min="7686" max="7936" width="14.77734375" style="40"/>
+    <col min="7937" max="7937" width="23.5546875" style="40" customWidth="1"/>
+    <col min="7938" max="7938" width="33.6640625" style="40" customWidth="1"/>
+    <col min="7939" max="7940" width="14.77734375" style="40" customWidth="1"/>
+    <col min="7941" max="7941" width="82.44140625" style="40" customWidth="1"/>
+    <col min="7942" max="8192" width="14.77734375" style="40"/>
+    <col min="8193" max="8193" width="23.5546875" style="40" customWidth="1"/>
+    <col min="8194" max="8194" width="33.6640625" style="40" customWidth="1"/>
+    <col min="8195" max="8196" width="14.77734375" style="40" customWidth="1"/>
+    <col min="8197" max="8197" width="82.44140625" style="40" customWidth="1"/>
+    <col min="8198" max="8448" width="14.77734375" style="40"/>
+    <col min="8449" max="8449" width="23.5546875" style="40" customWidth="1"/>
+    <col min="8450" max="8450" width="33.6640625" style="40" customWidth="1"/>
+    <col min="8451" max="8452" width="14.77734375" style="40" customWidth="1"/>
+    <col min="8453" max="8453" width="82.44140625" style="40" customWidth="1"/>
+    <col min="8454" max="8704" width="14.77734375" style="40"/>
+    <col min="8705" max="8705" width="23.5546875" style="40" customWidth="1"/>
+    <col min="8706" max="8706" width="33.6640625" style="40" customWidth="1"/>
+    <col min="8707" max="8708" width="14.77734375" style="40" customWidth="1"/>
+    <col min="8709" max="8709" width="82.44140625" style="40" customWidth="1"/>
+    <col min="8710" max="8960" width="14.77734375" style="40"/>
+    <col min="8961" max="8961" width="23.5546875" style="40" customWidth="1"/>
+    <col min="8962" max="8962" width="33.6640625" style="40" customWidth="1"/>
+    <col min="8963" max="8964" width="14.77734375" style="40" customWidth="1"/>
+    <col min="8965" max="8965" width="82.44140625" style="40" customWidth="1"/>
+    <col min="8966" max="9216" width="14.77734375" style="40"/>
+    <col min="9217" max="9217" width="23.5546875" style="40" customWidth="1"/>
+    <col min="9218" max="9218" width="33.6640625" style="40" customWidth="1"/>
+    <col min="9219" max="9220" width="14.77734375" style="40" customWidth="1"/>
+    <col min="9221" max="9221" width="82.44140625" style="40" customWidth="1"/>
+    <col min="9222" max="9472" width="14.77734375" style="40"/>
+    <col min="9473" max="9473" width="23.5546875" style="40" customWidth="1"/>
+    <col min="9474" max="9474" width="33.6640625" style="40" customWidth="1"/>
+    <col min="9475" max="9476" width="14.77734375" style="40" customWidth="1"/>
+    <col min="9477" max="9477" width="82.44140625" style="40" customWidth="1"/>
+    <col min="9478" max="9728" width="14.77734375" style="40"/>
+    <col min="9729" max="9729" width="23.5546875" style="40" customWidth="1"/>
+    <col min="9730" max="9730" width="33.6640625" style="40" customWidth="1"/>
+    <col min="9731" max="9732" width="14.77734375" style="40" customWidth="1"/>
+    <col min="9733" max="9733" width="82.44140625" style="40" customWidth="1"/>
+    <col min="9734" max="9984" width="14.77734375" style="40"/>
+    <col min="9985" max="9985" width="23.5546875" style="40" customWidth="1"/>
+    <col min="9986" max="9986" width="33.6640625" style="40" customWidth="1"/>
+    <col min="9987" max="9988" width="14.77734375" style="40" customWidth="1"/>
+    <col min="9989" max="9989" width="82.44140625" style="40" customWidth="1"/>
+    <col min="9990" max="10240" width="14.77734375" style="40"/>
+    <col min="10241" max="10241" width="23.5546875" style="40" customWidth="1"/>
+    <col min="10242" max="10242" width="33.6640625" style="40" customWidth="1"/>
+    <col min="10243" max="10244" width="14.77734375" style="40" customWidth="1"/>
+    <col min="10245" max="10245" width="82.44140625" style="40" customWidth="1"/>
+    <col min="10246" max="10496" width="14.77734375" style="40"/>
+    <col min="10497" max="10497" width="23.5546875" style="40" customWidth="1"/>
+    <col min="10498" max="10498" width="33.6640625" style="40" customWidth="1"/>
+    <col min="10499" max="10500" width="14.77734375" style="40" customWidth="1"/>
+    <col min="10501" max="10501" width="82.44140625" style="40" customWidth="1"/>
+    <col min="10502" max="10752" width="14.77734375" style="40"/>
+    <col min="10753" max="10753" width="23.5546875" style="40" customWidth="1"/>
+    <col min="10754" max="10754" width="33.6640625" style="40" customWidth="1"/>
+    <col min="10755" max="10756" width="14.77734375" style="40" customWidth="1"/>
+    <col min="10757" max="10757" width="82.44140625" style="40" customWidth="1"/>
+    <col min="10758" max="11008" width="14.77734375" style="40"/>
+    <col min="11009" max="11009" width="23.5546875" style="40" customWidth="1"/>
+    <col min="11010" max="11010" width="33.6640625" style="40" customWidth="1"/>
+    <col min="11011" max="11012" width="14.77734375" style="40" customWidth="1"/>
+    <col min="11013" max="11013" width="82.44140625" style="40" customWidth="1"/>
+    <col min="11014" max="11264" width="14.77734375" style="40"/>
+    <col min="11265" max="11265" width="23.5546875" style="40" customWidth="1"/>
+    <col min="11266" max="11266" width="33.6640625" style="40" customWidth="1"/>
+    <col min="11267" max="11268" width="14.77734375" style="40" customWidth="1"/>
+    <col min="11269" max="11269" width="82.44140625" style="40" customWidth="1"/>
+    <col min="11270" max="11520" width="14.77734375" style="40"/>
+    <col min="11521" max="11521" width="23.5546875" style="40" customWidth="1"/>
+    <col min="11522" max="11522" width="33.6640625" style="40" customWidth="1"/>
+    <col min="11523" max="11524" width="14.77734375" style="40" customWidth="1"/>
+    <col min="11525" max="11525" width="82.44140625" style="40" customWidth="1"/>
+    <col min="11526" max="11776" width="14.77734375" style="40"/>
+    <col min="11777" max="11777" width="23.5546875" style="40" customWidth="1"/>
+    <col min="11778" max="11778" width="33.6640625" style="40" customWidth="1"/>
+    <col min="11779" max="11780" width="14.77734375" style="40" customWidth="1"/>
+    <col min="11781" max="11781" width="82.44140625" style="40" customWidth="1"/>
+    <col min="11782" max="12032" width="14.77734375" style="40"/>
+    <col min="12033" max="12033" width="23.5546875" style="40" customWidth="1"/>
+    <col min="12034" max="12034" width="33.6640625" style="40" customWidth="1"/>
+    <col min="12035" max="12036" width="14.77734375" style="40" customWidth="1"/>
+    <col min="12037" max="12037" width="82.44140625" style="40" customWidth="1"/>
+    <col min="12038" max="12288" width="14.77734375" style="40"/>
+    <col min="12289" max="12289" width="23.5546875" style="40" customWidth="1"/>
+    <col min="12290" max="12290" width="33.6640625" style="40" customWidth="1"/>
+    <col min="12291" max="12292" width="14.77734375" style="40" customWidth="1"/>
+    <col min="12293" max="12293" width="82.44140625" style="40" customWidth="1"/>
+    <col min="12294" max="12544" width="14.77734375" style="40"/>
+    <col min="12545" max="12545" width="23.5546875" style="40" customWidth="1"/>
+    <col min="12546" max="12546" width="33.6640625" style="40" customWidth="1"/>
+    <col min="12547" max="12548" width="14.77734375" style="40" customWidth="1"/>
+    <col min="12549" max="12549" width="82.44140625" style="40" customWidth="1"/>
+    <col min="12550" max="12800" width="14.77734375" style="40"/>
+    <col min="12801" max="12801" width="23.5546875" style="40" customWidth="1"/>
+    <col min="12802" max="12802" width="33.6640625" style="40" customWidth="1"/>
+    <col min="12803" max="12804" width="14.77734375" style="40" customWidth="1"/>
+    <col min="12805" max="12805" width="82.44140625" style="40" customWidth="1"/>
+    <col min="12806" max="13056" width="14.77734375" style="40"/>
+    <col min="13057" max="13057" width="23.5546875" style="40" customWidth="1"/>
+    <col min="13058" max="13058" width="33.6640625" style="40" customWidth="1"/>
+    <col min="13059" max="13060" width="14.77734375" style="40" customWidth="1"/>
+    <col min="13061" max="13061" width="82.44140625" style="40" customWidth="1"/>
+    <col min="13062" max="13312" width="14.77734375" style="40"/>
+    <col min="13313" max="13313" width="23.5546875" style="40" customWidth="1"/>
+    <col min="13314" max="13314" width="33.6640625" style="40" customWidth="1"/>
+    <col min="13315" max="13316" width="14.77734375" style="40" customWidth="1"/>
+    <col min="13317" max="13317" width="82.44140625" style="40" customWidth="1"/>
+    <col min="13318" max="13568" width="14.77734375" style="40"/>
+    <col min="13569" max="13569" width="23.5546875" style="40" customWidth="1"/>
+    <col min="13570" max="13570" width="33.6640625" style="40" customWidth="1"/>
+    <col min="13571" max="13572" width="14.77734375" style="40" customWidth="1"/>
+    <col min="13573" max="13573" width="82.44140625" style="40" customWidth="1"/>
+    <col min="13574" max="13824" width="14.77734375" style="40"/>
+    <col min="13825" max="13825" width="23.5546875" style="40" customWidth="1"/>
+    <col min="13826" max="13826" width="33.6640625" style="40" customWidth="1"/>
+    <col min="13827" max="13828" width="14.77734375" style="40" customWidth="1"/>
+    <col min="13829" max="13829" width="82.44140625" style="40" customWidth="1"/>
+    <col min="13830" max="14080" width="14.77734375" style="40"/>
+    <col min="14081" max="14081" width="23.5546875" style="40" customWidth="1"/>
+    <col min="14082" max="14082" width="33.6640625" style="40" customWidth="1"/>
+    <col min="14083" max="14084" width="14.77734375" style="40" customWidth="1"/>
+    <col min="14085" max="14085" width="82.44140625" style="40" customWidth="1"/>
+    <col min="14086" max="14336" width="14.77734375" style="40"/>
+    <col min="14337" max="14337" width="23.5546875" style="40" customWidth="1"/>
+    <col min="14338" max="14338" width="33.6640625" style="40" customWidth="1"/>
+    <col min="14339" max="14340" width="14.77734375" style="40" customWidth="1"/>
+    <col min="14341" max="14341" width="82.44140625" style="40" customWidth="1"/>
+    <col min="14342" max="14592" width="14.77734375" style="40"/>
+    <col min="14593" max="14593" width="23.5546875" style="40" customWidth="1"/>
+    <col min="14594" max="14594" width="33.6640625" style="40" customWidth="1"/>
+    <col min="14595" max="14596" width="14.77734375" style="40" customWidth="1"/>
+    <col min="14597" max="14597" width="82.44140625" style="40" customWidth="1"/>
+    <col min="14598" max="14848" width="14.77734375" style="40"/>
+    <col min="14849" max="14849" width="23.5546875" style="40" customWidth="1"/>
+    <col min="14850" max="14850" width="33.6640625" style="40" customWidth="1"/>
+    <col min="14851" max="14852" width="14.77734375" style="40" customWidth="1"/>
+    <col min="14853" max="14853" width="82.44140625" style="40" customWidth="1"/>
+    <col min="14854" max="15104" width="14.77734375" style="40"/>
+    <col min="15105" max="15105" width="23.5546875" style="40" customWidth="1"/>
+    <col min="15106" max="15106" width="33.6640625" style="40" customWidth="1"/>
+    <col min="15107" max="15108" width="14.77734375" style="40" customWidth="1"/>
+    <col min="15109" max="15109" width="82.44140625" style="40" customWidth="1"/>
+    <col min="15110" max="15360" width="14.77734375" style="40"/>
+    <col min="15361" max="15361" width="23.5546875" style="40" customWidth="1"/>
+    <col min="15362" max="15362" width="33.6640625" style="40" customWidth="1"/>
+    <col min="15363" max="15364" width="14.77734375" style="40" customWidth="1"/>
+    <col min="15365" max="15365" width="82.44140625" style="40" customWidth="1"/>
+    <col min="15366" max="15616" width="14.77734375" style="40"/>
+    <col min="15617" max="15617" width="23.5546875" style="40" customWidth="1"/>
+    <col min="15618" max="15618" width="33.6640625" style="40" customWidth="1"/>
+    <col min="15619" max="15620" width="14.77734375" style="40" customWidth="1"/>
+    <col min="15621" max="15621" width="82.44140625" style="40" customWidth="1"/>
+    <col min="15622" max="15872" width="14.77734375" style="40"/>
+    <col min="15873" max="15873" width="23.5546875" style="40" customWidth="1"/>
+    <col min="15874" max="15874" width="33.6640625" style="40" customWidth="1"/>
+    <col min="15875" max="15876" width="14.77734375" style="40" customWidth="1"/>
+    <col min="15877" max="15877" width="82.44140625" style="40" customWidth="1"/>
+    <col min="15878" max="16128" width="14.77734375" style="40"/>
+    <col min="16129" max="16129" width="23.5546875" style="40" customWidth="1"/>
+    <col min="16130" max="16130" width="33.6640625" style="40" customWidth="1"/>
+    <col min="16131" max="16132" width="14.77734375" style="40" customWidth="1"/>
+    <col min="16133" max="16133" width="82.44140625" style="40" customWidth="1"/>
+    <col min="16134" max="16384" width="14.77734375" style="40"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="18">
+    <row r="1" spans="1:5" ht="17.399999999999999">
       <c r="A1" s="76"/>
       <c r="B1" s="77"/>
       <c r="C1" s="77"/>
       <c r="D1" s="77"/>
       <c r="E1" s="77"/>
     </row>
-    <row r="2" spans="1:5" ht="14.5" thickBot="1">
+    <row r="2" spans="1:5" ht="14.4" thickBot="1">
       <c r="A2" s="77"/>
       <c r="B2" s="77"/>
       <c r="C2" s="77"/>
       <c r="D2" s="77"/>
       <c r="E2" s="77"/>
     </row>
-    <row r="3" spans="1:5" ht="14" customHeight="1">
+    <row r="3" spans="1:5" ht="13.95" customHeight="1">
       <c r="A3" s="160" t="s">
         <v>64</v>
       </c>
@@ -49037,14 +49074,14 @@
         <v>68</v>
       </c>
     </row>
-    <row r="4" spans="1:5" ht="14.5" thickBot="1">
+    <row r="4" spans="1:5" ht="14.4" thickBot="1">
       <c r="A4" s="161"/>
       <c r="B4" s="134"/>
       <c r="C4" s="134"/>
       <c r="D4" s="132"/>
       <c r="E4" s="134"/>
     </row>
-    <row r="5" spans="1:5" ht="14" customHeight="1">
+    <row r="5" spans="1:5" ht="13.95" customHeight="1">
       <c r="A5" s="153" t="s">
         <v>178</v>
       </c>
@@ -49098,7 +49135,7 @@
         <v>182</v>
       </c>
     </row>
-    <row r="9" spans="1:5" ht="14" customHeight="1">
+    <row r="9" spans="1:5" ht="13.95" customHeight="1">
       <c r="A9" s="137"/>
       <c r="B9" s="139"/>
       <c r="C9" s="79">
@@ -49256,7 +49293,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="21" spans="1:5" ht="14.5" thickBot="1">
+    <row r="21" spans="1:5" ht="14.4" thickBot="1">
       <c r="A21" s="138"/>
       <c r="B21" s="140"/>
       <c r="C21" s="81">
@@ -49269,7 +49306,7 @@
         <v>195</v>
       </c>
     </row>
-    <row r="22" spans="1:5" ht="14" customHeight="1">
+    <row r="22" spans="1:5" ht="13.95" customHeight="1">
       <c r="A22" s="141" t="s">
         <v>196</v>
       </c>
@@ -49349,7 +49386,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="28" spans="1:5" ht="14.5" thickBot="1">
+    <row r="28" spans="1:5" ht="14.4" thickBot="1">
       <c r="A28" s="142"/>
       <c r="B28" s="144"/>
       <c r="C28" s="80">
@@ -49585,7 +49622,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="46" spans="1:5" ht="14.5" thickBot="1">
+    <row r="46" spans="1:5" ht="14.4" thickBot="1">
       <c r="A46" s="148"/>
       <c r="B46" s="152"/>
       <c r="C46" s="81">
@@ -49614,8 +49651,8 @@
       </c>
     </row>
     <row r="48" spans="1:5">
-      <c r="A48" s="93"/>
-      <c r="B48" s="101"/>
+      <c r="A48" s="105"/>
+      <c r="B48" s="102"/>
       <c r="C48" s="79">
         <v>312832</v>
       </c>
@@ -49627,8 +49664,8 @@
       </c>
     </row>
     <row r="49" spans="1:5">
-      <c r="A49" s="93"/>
-      <c r="B49" s="101"/>
+      <c r="A49" s="105"/>
+      <c r="B49" s="102"/>
       <c r="C49" s="79">
         <v>312833</v>
       </c>
@@ -49640,8 +49677,8 @@
       </c>
     </row>
     <row r="50" spans="1:5">
-      <c r="A50" s="93"/>
-      <c r="B50" s="101"/>
+      <c r="A50" s="105"/>
+      <c r="B50" s="102"/>
       <c r="C50" s="79">
         <v>337802</v>
       </c>
@@ -49653,8 +49690,8 @@
       </c>
     </row>
     <row r="51" spans="1:5">
-      <c r="A51" s="93"/>
-      <c r="B51" s="101"/>
+      <c r="A51" s="105"/>
+      <c r="B51" s="102"/>
       <c r="C51" s="79">
         <v>312834</v>
       </c>
@@ -49666,8 +49703,8 @@
       </c>
     </row>
     <row r="52" spans="1:5">
-      <c r="A52" s="93"/>
-      <c r="B52" s="101"/>
+      <c r="A52" s="105"/>
+      <c r="B52" s="102"/>
       <c r="C52" s="79">
         <v>312835</v>
       </c>
@@ -49679,8 +49716,8 @@
       </c>
     </row>
     <row r="53" spans="1:5">
-      <c r="A53" s="93"/>
-      <c r="B53" s="101"/>
+      <c r="A53" s="105"/>
+      <c r="B53" s="102"/>
       <c r="C53" s="79">
         <v>312836</v>
       </c>
@@ -49691,9 +49728,9 @@
         <v>221</v>
       </c>
     </row>
-    <row r="54" spans="1:5" ht="14.5" thickBot="1">
-      <c r="A54" s="94"/>
-      <c r="B54" s="102"/>
+    <row r="54" spans="1:5" ht="14.4" thickBot="1">
+      <c r="A54" s="106"/>
+      <c r="B54" s="103"/>
       <c r="C54" s="81">
         <v>337803</v>
       </c>
@@ -49738,16 +49775,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A5:E367"/>
   <sheetViews>
-    <sheetView topLeftCell="B40" workbookViewId="0">
-      <selection activeCell="C45" sqref="C45"/>
+    <sheetView topLeftCell="A340" workbookViewId="0">
+      <selection activeCell="B353" sqref="B353"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="29.1796875" customWidth="1"/>
-    <col min="2" max="2" width="68.90625" customWidth="1"/>
-    <col min="3" max="3" width="20.6328125" customWidth="1"/>
-    <col min="5" max="5" width="22.1796875" customWidth="1"/>
+    <col min="1" max="1" width="29.21875" customWidth="1"/>
+    <col min="2" max="2" width="68.88671875" customWidth="1"/>
+    <col min="3" max="3" width="20.6640625" customWidth="1"/>
+    <col min="5" max="5" width="22.21875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="5" spans="1:5">
@@ -53004,7 +53041,7 @@
     </row>
     <row r="346" spans="1:4">
       <c r="B346" s="1" t="s">
-        <v>149</v>
+        <v>457</v>
       </c>
       <c r="C346" s="1">
         <v>768893</v>
@@ -53258,10 +53295,10 @@
       <selection activeCell="D75" sqref="D75"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="3" max="3" width="28.36328125" customWidth="1"/>
-    <col min="4" max="4" width="79.1796875" customWidth="1"/>
+    <col min="3" max="3" width="28.33203125" customWidth="1"/>
+    <col min="4" max="4" width="79.21875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="4" spans="3:4">
@@ -54090,10 +54127,10 @@
       <selection activeCell="G16" sqref="G16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="4" max="4" width="21.6328125" customWidth="1"/>
-    <col min="5" max="5" width="84.90625" customWidth="1"/>
+    <col min="4" max="4" width="21.6640625" customWidth="1"/>
+    <col min="5" max="5" width="84.88671875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="6" spans="4:5">
@@ -54398,11 +54435,11 @@
       <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="24.36328125" customWidth="1"/>
-    <col min="2" max="2" width="69.453125" customWidth="1"/>
-    <col min="3" max="3" width="22.08984375" customWidth="1"/>
+    <col min="1" max="1" width="24.33203125" customWidth="1"/>
+    <col min="2" max="2" width="69.44140625" customWidth="1"/>
+    <col min="3" max="3" width="22.109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="5" spans="1:5">
@@ -57913,12 +57950,12 @@
       <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="32.36328125" customWidth="1"/>
-    <col min="2" max="2" width="68.453125" customWidth="1"/>
-    <col min="3" max="3" width="23.08984375" customWidth="1"/>
-    <col min="5" max="5" width="10.54296875" customWidth="1"/>
+    <col min="1" max="1" width="32.33203125" customWidth="1"/>
+    <col min="2" max="2" width="68.44140625" customWidth="1"/>
+    <col min="3" max="3" width="23.109375" customWidth="1"/>
+    <col min="5" max="5" width="10.5546875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="5" spans="1:5">
@@ -61286,12 +61323,12 @@
       <selection activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="25.81640625" customWidth="1"/>
-    <col min="2" max="2" width="67.453125" customWidth="1"/>
-    <col min="3" max="3" width="22.81640625" customWidth="1"/>
-    <col min="4" max="4" width="11.54296875" customWidth="1"/>
+    <col min="1" max="1" width="25.77734375" customWidth="1"/>
+    <col min="2" max="2" width="67.44140625" customWidth="1"/>
+    <col min="3" max="3" width="22.77734375" customWidth="1"/>
+    <col min="4" max="4" width="11.5546875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="5" spans="1:5">
@@ -64850,15 +64887,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A5:E367"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E6" sqref="E6"/>
+    <sheetView tabSelected="1" topLeftCell="A337" workbookViewId="0">
+      <selection activeCell="B351" sqref="B351"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="22.90625" customWidth="1"/>
-    <col min="2" max="2" width="68.90625" customWidth="1"/>
-    <col min="3" max="3" width="20.6328125" customWidth="1"/>
+    <col min="1" max="1" width="22.88671875" customWidth="1"/>
+    <col min="2" max="2" width="68.88671875" customWidth="1"/>
+    <col min="3" max="3" width="20.6640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="5" spans="1:5">
@@ -68115,7 +68152,7 @@
     </row>
     <row r="346" spans="1:4">
       <c r="B346" s="1" t="s">
-        <v>149</v>
+        <v>457</v>
       </c>
       <c r="C346" s="1">
         <v>768893</v>
@@ -68369,11 +68406,11 @@
       <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="24.453125" customWidth="1"/>
-    <col min="2" max="2" width="69.453125" customWidth="1"/>
-    <col min="3" max="3" width="22.08984375" customWidth="1"/>
+    <col min="1" max="1" width="24.44140625" customWidth="1"/>
+    <col min="2" max="2" width="69.44140625" customWidth="1"/>
+    <col min="3" max="3" width="22.109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="5" spans="1:5">
@@ -71884,12 +71921,12 @@
       <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="27.1796875" customWidth="1"/>
-    <col min="2" max="2" width="68.453125" customWidth="1"/>
-    <col min="3" max="3" width="23.08984375" customWidth="1"/>
-    <col min="5" max="5" width="10.453125" customWidth="1"/>
+    <col min="1" max="1" width="27.21875" customWidth="1"/>
+    <col min="2" max="2" width="68.44140625" customWidth="1"/>
+    <col min="3" max="3" width="23.109375" customWidth="1"/>
+    <col min="5" max="5" width="10.44140625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="5" spans="1:5">
@@ -75257,12 +75294,12 @@
       <selection activeCell="H7" sqref="H7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="32.453125" customWidth="1"/>
-    <col min="2" max="2" width="67.453125" customWidth="1"/>
-    <col min="3" max="3" width="22.81640625" customWidth="1"/>
-    <col min="4" max="4" width="11.54296875" customWidth="1"/>
+    <col min="1" max="1" width="32.44140625" customWidth="1"/>
+    <col min="2" max="2" width="67.44140625" customWidth="1"/>
+    <col min="3" max="3" width="22.77734375" customWidth="1"/>
+    <col min="4" max="4" width="11.5546875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="5" spans="1:6">

</xml_diff>